<commit_message>
NAV-88 Update Estimates 22 graph
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="597">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -340,7 +340,23 @@
     <t xml:space="preserve">The majority of delays and challenges with the estimates process are related to the preparation of data inputs. Best practice suggests that high quality data inputs should be prepared prior to beginning your estimates. Ensure all programme data are available in your country's national health management information system (e.g., DHIS2), reviewed for quality, validated by the relevant authorities, and ready for use in this year's estimates process. To learn more about the programme data required, see Guide 8, Data Quality, Indicator Element Matrix. </t>
   </si>
   <si>
-    <t>Guide 8, Data Quality, Indicator Element Matrix (https://hivtools.unaids.org/hiv-estimates-training-material-en/)</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Guide 8, Data Quality, Indicator Element Matrix </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <sz val="8.0"/>
+        <u/>
+      </rPr>
+      <t>https://hivtools.unaids.org/hiv-estimates-training-material-en/</t>
+    </r>
   </si>
   <si>
     <t>MM: Add sheet to HIV tools page and put link to that sheet here
@@ -362,7 +378,23 @@
     <t>The greatest impediment to a successful estimates process is poor quality programme data. The most important thing you can do before you begin is review the quality of your programme data. There are specific analyses recommended to assess the quality of your program data. These analyses are available in Guide 6, Data Quality Standards of Practice. Table 2 provides specific analyses for the different programme inputs to ensure you start the estimates process with high quality inputs. ShinyRob is another tool available to users for assessing data quality. This step will be completed after data are uploaded to ADR.</t>
   </si>
   <si>
-    <t>Guide 6, Data Quality Standards of Practice (https://hivtools.unaids.org/hiv-estimates-training-material-en/)</t>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF000000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Guide 6, Data Quality Standards of Practice </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FF1155CC"/>
+        <sz val="8.0"/>
+        <u/>
+      </rPr>
+      <t>https://hivtools.unaids.org/hiv-estimates-training-material-en/</t>
+    </r>
   </si>
   <si>
     <t>MM: training materials ID: D.8</t>
@@ -383,7 +415,7 @@
     <t>Some HIV estimates models require data inputs to be in a specific format. They are a part of the Inputs to UNAIDS Estimates Package for this year. Data inputs include programme data such as ANC, HIV testing, and ART data, survey data, population data, and an area boundary file. Note models may require similar data, but in slightly different formats. For example, Shiny 90 requires survey data at the level of your Spectrum estimates file. UNAIDS has provided the templates required by the models in the AIDS Data Repository.</t>
   </si>
   <si>
-    <t>Data Input Templates on the AIDS Data Repository - https://adr.unaids.org/en/pages/inputs-unaids</t>
+    <t>Data Input Templates on the AIDS Data Repository https://adr.unaids.org/en/pages/inputs-unaids</t>
   </si>
   <si>
     <t xml:space="preserve">MM: @S4 I think this should be deleted given question GEN-05.  We don't want them starting fresh they should update previously used sheets
@@ -408,7 +440,7 @@
     <t>Before you upload your data inputs package to ADR, ensure you have prepopulated all of them and reviewed the quality of data. Complete each of the required templates: i) Population, ii) area boundary, iii) Naomi survey, iv) HIV testing, v) ART, and vi) ANC?</t>
   </si>
   <si>
-    <t>AIDS Data Repository - https://adr.unaids.org/</t>
+    <t>AIDS Data Repository https://adr.unaids.org/</t>
   </si>
   <si>
     <r>
@@ -805,9 +837,6 @@
   </si>
   <si>
     <t>In order to use ShinyRob, you must upload three files to your estimates inputs package for this year. To upload your files, access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format. Be sure to confirm the green "Valid" badge next to each file. If any files are missing the green "valid" badge, be sure to review the data issues identified by ADR and correct them. If any changes are made to the data in the estimates templates, ensure changes are cascaded to the source systems (e.g., DHIS2) as needed. Once data are uploaded and valid in ADR, you may proceed to ShinyRob to conduct thorough data quality reviews.</t>
-  </si>
-  <si>
-    <t>AIDS Data Repository https://adr.unaids.org/</t>
   </si>
   <si>
     <t>@UNAIDS - I've tagged everything here as mandatory right now. This means the user will not be able to proceed to Spectrum data entry until this process is complete. Are we okay with that order of operations to help avoid data quality problems downstream?</t>
@@ -2656,7 +2685,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="30">
+  <fonts count="27">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2688,17 +2717,6 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
     </font>
     <font>
       <b/>
@@ -2740,6 +2758,12 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="8.0"/>
       <color theme="9"/>
       <name val="Calibri"/>
@@ -2748,12 +2772,6 @@
       <sz val="11.0"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="8.0"/>
@@ -2974,7 +2992,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="133">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3013,16 +3031,16 @@
     <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3034,14 +3052,14 @@
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3060,10 +3078,10 @@
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3075,126 +3093,125 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="13" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="49" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="5" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3203,22 +3220,22 @@
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -3228,11 +3245,11 @@
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="10" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -3241,20 +3258,20 @@
     <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="6" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3263,42 +3280,42 @@
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="21" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="28" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -32613,7 +32630,7 @@
     <col customWidth="1" min="2" max="2" width="24.29"/>
     <col customWidth="1" min="3" max="3" width="34.57"/>
     <col customWidth="1" min="4" max="4" width="43.14"/>
-    <col customWidth="1" min="5" max="5" width="15.14"/>
+    <col customWidth="1" min="5" max="5" width="69.86"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
     <col customWidth="1" hidden="1" min="7" max="7" width="37.29"/>
     <col customWidth="1" hidden="1" min="8" max="8" width="26.86"/>
@@ -32716,11 +32733,11 @@
       <c r="D5" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="59" t="s">
+      <c r="E5" s="60" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61">
+      <c r="F5" s="61"/>
+      <c r="G5" s="62">
         <v>0.0</v>
       </c>
       <c r="H5" s="58" t="s">
@@ -32745,11 +32762,11 @@
       <c r="D6" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="E6" s="58" t="s">
+      <c r="E6" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="62"/>
-      <c r="G6" s="63">
+      <c r="F6" s="63"/>
+      <c r="G6" s="64">
         <v>1.0</v>
       </c>
       <c r="H6" s="58" t="s">
@@ -32774,17 +32791,17 @@
       <c r="D7" s="58" t="s">
         <v>73</v>
       </c>
-      <c r="E7" s="58" t="s">
+      <c r="E7" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61">
+      <c r="F7" s="61"/>
+      <c r="G7" s="62">
         <v>1.0</v>
       </c>
-      <c r="H7" s="64" t="s">
+      <c r="H7" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="I7" s="65" t="s">
+      <c r="I7" s="66" t="s">
         <v>76</v>
       </c>
       <c r="J7" s="22"/>
@@ -32805,17 +32822,17 @@
       <c r="D8" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61">
+      <c r="F8" s="61"/>
+      <c r="G8" s="62">
         <v>1.0</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="I8" s="65"/>
+      <c r="I8" s="66"/>
       <c r="J8" s="22"/>
       <c r="K8" s="22" t="s">
         <v>84</v>
@@ -32835,16 +32852,16 @@
         <v>88</v>
       </c>
       <c r="E9" s="58"/>
-      <c r="F9" s="60">
+      <c r="F9" s="61">
         <v>1.0</v>
       </c>
-      <c r="G9" s="61">
+      <c r="G9" s="62">
         <v>1.0</v>
       </c>
-      <c r="H9" s="65" t="s">
+      <c r="H9" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="65" t="s">
+      <c r="I9" s="66" t="s">
         <v>90</v>
       </c>
       <c r="J9" s="22"/>
@@ -32866,14 +32883,14 @@
         <v>95</v>
       </c>
       <c r="E10" s="58"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61">
+      <c r="F10" s="61"/>
+      <c r="G10" s="62">
         <v>0.0</v>
       </c>
-      <c r="H10" s="65" t="s">
+      <c r="H10" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="I10" s="65" t="s">
+      <c r="I10" s="66" t="s">
         <v>97</v>
       </c>
       <c r="J10" s="22"/>
@@ -32895,14 +32912,14 @@
         <v>102</v>
       </c>
       <c r="E11" s="58"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61">
+      <c r="F11" s="61"/>
+      <c r="G11" s="62">
         <v>0.0</v>
       </c>
       <c r="H11" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="I11" s="66" t="s">
+      <c r="I11" s="67" t="s">
         <v>104</v>
       </c>
       <c r="J11" s="22"/>
@@ -32924,8 +32941,8 @@
         <v>109</v>
       </c>
       <c r="E12" s="58"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="68">
+      <c r="F12" s="68"/>
+      <c r="G12" s="69">
         <v>0.0</v>
       </c>
       <c r="H12" s="44"/>
@@ -32936,7 +32953,7 @@
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
-      <c r="C13" s="69"/>
+      <c r="C13" s="70"/>
       <c r="H13" s="39"/>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -34177,10 +34194,14 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E5"/>
+    <hyperlink r:id="rId2" ref="E6"/>
+  </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -34197,7 +34218,7 @@
     <col customWidth="1" min="1" max="2" width="10.43"/>
     <col customWidth="1" min="3" max="3" width="24.43"/>
     <col customWidth="1" min="4" max="4" width="51.29"/>
-    <col customWidth="1" min="5" max="5" width="46.57"/>
+    <col customWidth="1" min="5" max="5" width="85.29"/>
     <col customWidth="1" min="6" max="6" width="12.0"/>
     <col customWidth="1" min="7" max="7" width="27.0"/>
     <col customWidth="1" hidden="1" min="8" max="8" width="37.86"/>
@@ -34217,7 +34238,7 @@
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
@@ -34233,20 +34254,20 @@
       <c r="D2" s="46" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="71"/>
+      <c r="E2" s="72"/>
       <c r="F2" s="47">
         <v>0.1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="72"/>
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
     </row>
     <row r="4">
       <c r="A4" s="55" t="s">
@@ -34261,7 +34282,7 @@
       <c r="D4" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="75" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="54" t="s">
@@ -34284,7 +34305,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="76" t="s">
         <v>114</v>
       </c>
       <c r="B5" s="58" t="s">
@@ -34296,7 +34317,7 @@
       <c r="D5" s="58" t="s">
         <v>117</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="60" t="s">
         <v>118</v>
       </c>
       <c r="F5" s="77">
@@ -34315,7 +34336,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="76" t="s">
         <v>121</v>
       </c>
       <c r="B6" s="58" t="s">
@@ -34334,17 +34355,17 @@
       <c r="G6" s="77">
         <v>0.0</v>
       </c>
-      <c r="H6" s="65" t="s">
+      <c r="H6" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="65"/>
+      <c r="I6" s="66"/>
       <c r="J6" s="22"/>
       <c r="K6" s="22" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="76" t="s">
         <v>127</v>
       </c>
       <c r="B7" s="58" t="s">
@@ -34356,7 +34377,7 @@
       <c r="D7" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="E7" s="60" t="s">
         <v>130</v>
       </c>
       <c r="F7" s="78">
@@ -34375,7 +34396,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="76" t="s">
         <v>133</v>
       </c>
       <c r="B8" s="58" t="s">
@@ -34419,7 +34440,7 @@
       <c r="Z8" s="80"/>
     </row>
     <row r="9">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="76" t="s">
         <v>139</v>
       </c>
       <c r="B9" s="58" t="s">
@@ -34431,7 +34452,7 @@
       <c r="D9" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="60" t="s">
         <v>143</v>
       </c>
       <c r="F9" s="59">
@@ -34499,7 +34520,7 @@
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
@@ -34576,57 +34597,57 @@
         <v>151</v>
       </c>
       <c r="E5" s="59" t="s">
+        <v>82</v>
+      </c>
+      <c r="F5" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="61">
+        <v>0.0</v>
+      </c>
+      <c r="H5" s="79" t="s">
         <v>152</v>
-      </c>
-      <c r="F5" s="60">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="60">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="79" t="s">
-        <v>153</v>
       </c>
       <c r="I5" s="38"/>
       <c r="J5" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="58" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="C6" s="58" t="s">
         <v>156</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="D6" s="58" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="E6" s="59" t="s">
         <v>158</v>
       </c>
-      <c r="E6" s="59" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="60">
+      <c r="F6" s="61">
         <v>1.0</v>
       </c>
-      <c r="G6" s="60">
+      <c r="G6" s="61">
         <v>0.0</v>
       </c>
-      <c r="H6" s="62"/>
+      <c r="H6" s="63"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="82" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" s="82"/>
       <c r="C7" s="82" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
@@ -34637,93 +34658,93 @@
         <v>1.0</v>
       </c>
       <c r="H7" s="84" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I7" s="85"/>
       <c r="J7" s="85" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B8" s="58" t="s">
         <v>165</v>
       </c>
-      <c r="B8" s="58" t="s">
+      <c r="C8" s="58" t="s">
         <v>166</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="D8" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="E8" s="59" t="s">
         <v>168</v>
       </c>
-      <c r="E8" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="F8" s="60">
+      <c r="F8" s="61">
         <v>1.0</v>
       </c>
-      <c r="G8" s="60">
+      <c r="G8" s="61">
         <v>0.0</v>
       </c>
-      <c r="H8" s="62"/>
+      <c r="H8" s="63"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="58" t="s">
         <v>171</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="C9" s="58" t="s">
         <v>172</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="D9" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="58" t="s">
+      <c r="E9" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="F9" s="63">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="63">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="63"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="38" t="s">
         <v>174</v>
-      </c>
-      <c r="E9" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="F9" s="62">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="62">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="62"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="38" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="58" t="s">
         <v>176</v>
       </c>
-      <c r="B10" s="58" t="s">
+      <c r="C10" s="58" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="D10" s="58" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="58" t="s">
+      <c r="E10" s="58"/>
+      <c r="F10" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="61">
+        <v>0.0</v>
+      </c>
+      <c r="H10" s="58"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="38" t="s">
         <v>179</v>
-      </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="60">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="60">
-        <v>0.0</v>
-      </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="87"/>
-      <c r="J10" s="38" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -35842,21 +35863,21 @@
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>181</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>182</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -35865,31 +35886,31 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="89" t="s">
-        <v>184</v>
-      </c>
-      <c r="C4" s="88" t="s">
+      <c r="B4" s="88" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="88" t="s">
+      <c r="H4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="88" t="s">
+      <c r="I4" s="87" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="52" t="s">
@@ -35904,48 +35925,48 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="91"/>
+      <c r="C5" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="E5" s="92" t="s">
         <v>187</v>
       </c>
-      <c r="E5" s="93" t="s">
+      <c r="F5" s="93" t="s">
         <v>188</v>
-      </c>
-      <c r="F5" s="94" t="s">
-        <v>189</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37">
         <v>1.0</v>
       </c>
-      <c r="I5" s="87"/>
+      <c r="I5" s="86"/>
       <c r="J5" s="58"/>
-      <c r="K5" s="95" t="s">
-        <v>190</v>
+      <c r="K5" s="94" t="s">
+        <v>189</v>
       </c>
       <c r="L5" s="38"/>
       <c r="M5" s="38" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="95"/>
+      <c r="C6" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="B6" s="96"/>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="E6" s="96" t="s">
         <v>194</v>
-      </c>
-      <c r="E6" s="97" t="s">
-        <v>195</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37">
@@ -35955,34 +35976,34 @@
         <v>1.0</v>
       </c>
       <c r="I6" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="J6" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="J6" s="58" t="s">
+      <c r="K6" s="94" t="s">
         <v>197</v>
-      </c>
-      <c r="K6" s="95" t="s">
-        <v>198</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" s="91" t="s">
         <v>200</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="C7" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="D7" s="37" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="E7" s="96" t="s">
         <v>203</v>
-      </c>
-      <c r="E7" s="97" t="s">
-        <v>204</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
@@ -35990,32 +36011,32 @@
         <v>1.0</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J7" s="58"/>
       <c r="L7" s="38"/>
       <c r="M7" s="38" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="B8" s="97">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="B8" s="98">
-        <v>1.0</v>
-      </c>
-      <c r="C8" s="37" t="s">
+      <c r="D8" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="E8" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="F8" s="93" t="s">
         <v>210</v>
-      </c>
-      <c r="F8" s="94" t="s">
-        <v>211</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="37">
@@ -36025,170 +36046,170 @@
       <c r="J8" s="58"/>
       <c r="L8" s="38"/>
       <c r="M8" s="38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="95"/>
+      <c r="C9" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="E9" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="E9" s="93" t="s">
-        <v>216</v>
-      </c>
-      <c r="F9" s="99"/>
+      <c r="F9" s="98"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37">
         <v>0.0</v>
       </c>
-      <c r="I9" s="100" t="s">
+      <c r="I9" s="99" t="s">
+        <v>216</v>
+      </c>
+      <c r="J9" s="58"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="38" t="s">
         <v>217</v>
-      </c>
-      <c r="J9" s="58"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="38" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" s="95"/>
+      <c r="C10" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="E10" s="92" t="s">
         <v>221</v>
       </c>
-      <c r="E10" s="93" t="s">
+      <c r="F10" s="38" t="s">
         <v>222</v>
-      </c>
-      <c r="F10" s="38" t="s">
-        <v>223</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="37">
         <v>1.0</v>
       </c>
-      <c r="I10" s="101"/>
+      <c r="I10" s="100"/>
       <c r="J10" s="58"/>
-      <c r="L10" s="87"/>
+      <c r="L10" s="86"/>
       <c r="M10" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="B11" s="97" t="s">
         <v>225</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="C11" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D11" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="E11" s="92" t="s">
         <v>228</v>
       </c>
-      <c r="E11" s="93" t="s">
-        <v>229</v>
-      </c>
       <c r="F11" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="37"/>
       <c r="H11" s="37">
         <v>1.0</v>
       </c>
-      <c r="I11" s="100" t="s">
+      <c r="I11" s="99" t="s">
+        <v>229</v>
+      </c>
+      <c r="J11" s="58" t="s">
         <v>230</v>
-      </c>
-      <c r="J11" s="58" t="s">
-        <v>231</v>
       </c>
       <c r="L11" s="38"/>
       <c r="M11" s="38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" s="97"/>
+      <c r="C12" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="B12" s="98"/>
-      <c r="C12" s="37" t="s">
+      <c r="D12" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="E12" s="92" t="s">
         <v>235</v>
-      </c>
-      <c r="E12" s="93" t="s">
-        <v>236</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37">
         <v>0.0</v>
       </c>
-      <c r="I12" s="100" t="s">
-        <v>237</v>
+      <c r="I12" s="99" t="s">
+        <v>236</v>
       </c>
       <c r="J12" s="58"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="97">
+        <v>2.0</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="B13" s="98">
-        <v>2.0</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="D13" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="E13" s="92" t="s">
         <v>241</v>
       </c>
-      <c r="E13" s="93" t="s">
-        <v>242</v>
-      </c>
       <c r="F13" s="38" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="37">
         <v>1.0</v>
       </c>
-      <c r="I13" s="100"/>
+      <c r="I13" s="99"/>
       <c r="J13" s="58"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="101"/>
+      <c r="C14" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="B14" s="102"/>
-      <c r="C14" s="37" t="s">
+      <c r="D14" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="E14" s="37" t="s">
         <v>246</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>247</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
@@ -36196,253 +36217,253 @@
         <v>1.0</v>
       </c>
       <c r="I14" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="J14" s="37"/>
+      <c r="K14" s="102" t="s">
         <v>248</v>
-      </c>
-      <c r="J14" s="37"/>
-      <c r="K14" s="103" t="s">
-        <v>249</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="103" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="104" t="s">
+      <c r="B15" s="104"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="103" t="s">
         <v>251</v>
       </c>
-      <c r="B15" s="105"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104" t="s">
+      <c r="E15" s="105"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="103">
+        <v>1.0</v>
+      </c>
+      <c r="H15" s="103"/>
+      <c r="I15" s="106" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="106"/>
-      <c r="F15" s="104"/>
-      <c r="G15" s="104">
-        <v>1.0</v>
-      </c>
-      <c r="H15" s="104"/>
-      <c r="I15" s="107" t="s">
+      <c r="J15" s="82"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="85" t="s">
         <v>253</v>
-      </c>
-      <c r="J15" s="82"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="85" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
+        <v>254</v>
+      </c>
+      <c r="B16" s="97" t="s">
         <v>255</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="C16" s="107" t="s">
         <v>256</v>
       </c>
-      <c r="C16" s="108" t="s">
+      <c r="D16" s="107" t="s">
         <v>257</v>
       </c>
-      <c r="D16" s="108" t="s">
+      <c r="E16" s="108" t="s">
         <v>258</v>
       </c>
-      <c r="E16" s="109" t="s">
+      <c r="F16" s="109" t="s">
         <v>259</v>
       </c>
-      <c r="F16" s="110" t="s">
+      <c r="G16" s="107"/>
+      <c r="H16" s="107">
+        <v>1.0</v>
+      </c>
+      <c r="I16" s="110" t="s">
         <v>260</v>
       </c>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108">
-        <v>1.0</v>
-      </c>
-      <c r="I16" s="111" t="s">
+      <c r="J16" s="111" t="s">
         <v>261</v>
-      </c>
-      <c r="J16" s="112" t="s">
-        <v>262</v>
       </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
+        <v>263</v>
+      </c>
+      <c r="B17" s="95" t="s">
         <v>264</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="C17" s="107" t="s">
         <v>265</v>
       </c>
-      <c r="C17" s="108" t="s">
+      <c r="D17" s="107" t="s">
         <v>266</v>
       </c>
-      <c r="D17" s="108" t="s">
+      <c r="E17" s="108" t="s">
         <v>267</v>
       </c>
-      <c r="E17" s="109" t="s">
+      <c r="F17" s="109" t="s">
+        <v>259</v>
+      </c>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107">
+        <v>1.0</v>
+      </c>
+      <c r="I17" s="110" t="s">
         <v>268</v>
       </c>
-      <c r="F17" s="110" t="s">
-        <v>260</v>
-      </c>
-      <c r="G17" s="108"/>
-      <c r="H17" s="108">
-        <v>1.0</v>
-      </c>
-      <c r="I17" s="111" t="s">
+      <c r="J17" s="111" t="s">
         <v>269</v>
-      </c>
-      <c r="J17" s="112" t="s">
-        <v>270</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="38" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="95" t="s">
         <v>272</v>
       </c>
-      <c r="B18" s="96" t="s">
+      <c r="C18" s="37" t="s">
         <v>273</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="E18" s="92" t="s">
         <v>275</v>
       </c>
-      <c r="E18" s="93" t="s">
-        <v>276</v>
-      </c>
-      <c r="F18" s="113" t="s">
-        <v>260</v>
+      <c r="F18" s="112" t="s">
+        <v>259</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="37">
         <v>1.0</v>
       </c>
-      <c r="I18" s="101"/>
+      <c r="I18" s="100"/>
       <c r="J18" s="58"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="95">
+        <v>19.0</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>278</v>
       </c>
-      <c r="B19" s="96">
-        <v>19.0</v>
-      </c>
-      <c r="C19" s="37" t="s">
+      <c r="D19" s="37" t="s">
         <v>279</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="E19" s="92" t="s">
         <v>280</v>
       </c>
-      <c r="E19" s="93" t="s">
+      <c r="F19" s="112" t="s">
         <v>281</v>
-      </c>
-      <c r="F19" s="113" t="s">
-        <v>282</v>
       </c>
       <c r="G19" s="37"/>
       <c r="H19" s="37">
         <v>1.0</v>
       </c>
-      <c r="I19" s="101"/>
+      <c r="I19" s="100"/>
       <c r="J19" s="58"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="37" t="s">
+        <v>283</v>
+      </c>
+      <c r="B20" s="95">
+        <v>20.0</v>
+      </c>
+      <c r="C20" s="37" t="s">
         <v>284</v>
       </c>
-      <c r="B20" s="96">
-        <v>20.0</v>
-      </c>
-      <c r="C20" s="37" t="s">
+      <c r="D20" s="37" t="s">
         <v>285</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="E20" s="92" t="s">
         <v>286</v>
       </c>
-      <c r="E20" s="93" t="s">
-        <v>287</v>
-      </c>
-      <c r="F20" s="113" t="s">
-        <v>260</v>
+      <c r="F20" s="112" t="s">
+        <v>259</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="37">
         <v>1.0</v>
       </c>
-      <c r="I20" s="101" t="s">
+      <c r="I20" s="100" t="s">
+        <v>287</v>
+      </c>
+      <c r="J20" s="58"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="J20" s="58"/>
-      <c r="L20" s="86"/>
-      <c r="M20" s="38" t="s">
+    </row>
+    <row r="21">
+      <c r="A21" s="103" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="104" t="s">
+      <c r="B21" s="113"/>
+      <c r="C21" s="103"/>
+      <c r="D21" s="103" t="s">
         <v>290</v>
       </c>
-      <c r="B21" s="114"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104" t="s">
+      <c r="E21" s="105"/>
+      <c r="F21" s="114"/>
+      <c r="G21" s="115">
+        <v>1.0</v>
+      </c>
+      <c r="H21" s="115"/>
+      <c r="I21" s="106" t="s">
         <v>291</v>
-      </c>
-      <c r="E21" s="106"/>
-      <c r="F21" s="115"/>
-      <c r="G21" s="116">
-        <v>1.0</v>
-      </c>
-      <c r="H21" s="116"/>
-      <c r="I21" s="107" t="s">
-        <v>292</v>
       </c>
       <c r="J21" s="82"/>
       <c r="L21" s="38"/>
       <c r="M21" s="85" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
+        <v>293</v>
+      </c>
+      <c r="B22" s="95" t="s">
         <v>294</v>
       </c>
-      <c r="B22" s="96" t="s">
+      <c r="C22" s="37" t="s">
         <v>295</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="D22" s="37" t="s">
         <v>296</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="E22" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="E22" s="37" t="s">
+      <c r="F22" s="116"/>
+      <c r="G22" s="116"/>
+      <c r="H22" s="116">
+        <v>1.0</v>
+      </c>
+      <c r="I22" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="F22" s="117"/>
-      <c r="G22" s="117"/>
-      <c r="H22" s="117">
-        <v>1.0</v>
-      </c>
-      <c r="I22" s="79" t="s">
+      <c r="J22" s="58"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="38" t="s">
         <v>299</v>
-      </c>
-      <c r="J22" s="58"/>
-      <c r="L22" s="86"/>
-      <c r="M22" s="38" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -37530,21 +37551,21 @@
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="84.0" customHeight="1">
       <c r="A2" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>301</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>302</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -37553,31 +37574,31 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="88" t="s">
-        <v>304</v>
-      </c>
-      <c r="I4" s="118" t="s">
+      <c r="H4" s="87" t="s">
+        <v>303</v>
+      </c>
+      <c r="I4" s="117" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -37589,97 +37610,97 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
+        <v>304</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>305</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="C5" s="38" t="s">
         <v>306</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="37" t="s">
         <v>307</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>308</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37">
         <v>0.0</v>
       </c>
-      <c r="H5" s="93" t="s">
-        <v>309</v>
-      </c>
-      <c r="I5" s="100"/>
+      <c r="H5" s="92" t="s">
+        <v>308</v>
+      </c>
+      <c r="I5" s="99"/>
       <c r="J5" s="38"/>
       <c r="K5" s="38" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>311</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="37" t="s">
         <v>313</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>314</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37">
         <v>1.0</v>
       </c>
-      <c r="H6" s="93" t="s">
-        <v>315</v>
+      <c r="H6" s="92" t="s">
+        <v>314</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>317</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="C7" s="37" t="s">
         <v>318</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="D7" s="37" t="s">
         <v>319</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>320</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37">
         <v>1.0</v>
       </c>
-      <c r="H7" s="93" t="s">
-        <v>315</v>
+      <c r="H7" s="92" t="s">
+        <v>314</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="38"/>
       <c r="K7" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>322</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="C8" s="37" t="s">
         <v>323</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="D8" s="37" t="s">
         <v>324</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>325</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37">
@@ -37688,28 +37709,28 @@
       <c r="G8" s="37">
         <v>1.0</v>
       </c>
-      <c r="H8" s="93"/>
+      <c r="H8" s="92"/>
       <c r="I8" s="37"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="C9" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="E9" s="118" t="s">
         <v>330</v>
-      </c>
-      <c r="E9" s="119" t="s">
-        <v>331</v>
       </c>
       <c r="F9" s="37">
         <v>1.0</v>
@@ -37717,54 +37738,54 @@
       <c r="G9" s="37">
         <v>1.0</v>
       </c>
-      <c r="H9" s="93"/>
+      <c r="H9" s="92"/>
       <c r="I9" s="37" t="s">
+        <v>331</v>
+      </c>
+      <c r="J9" s="28"/>
+      <c r="K9" s="38" t="s">
         <v>332</v>
-      </c>
-      <c r="J9" s="86"/>
-      <c r="K9" s="38" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="C10" s="37" t="s">
         <v>335</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="37" t="s">
         <v>336</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>337</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37">
         <v>1.0</v>
       </c>
-      <c r="H10" s="120" t="s">
+      <c r="H10" s="119" t="s">
+        <v>337</v>
+      </c>
+      <c r="I10" s="37"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="38" t="s">
         <v>338</v>
-      </c>
-      <c r="I10" s="37"/>
-      <c r="J10" s="87"/>
-      <c r="K10" s="38" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
+        <v>339</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>340</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="C11" s="37" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D11" s="37" t="s">
         <v>342</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>343</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37">
@@ -37774,14 +37795,14 @@
         <v>1.0</v>
       </c>
       <c r="H11" s="37" t="s">
+        <v>343</v>
+      </c>
+      <c r="I11" s="37" t="s">
         <v>344</v>
-      </c>
-      <c r="I11" s="37" t="s">
-        <v>345</v>
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="38" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L11" s="80"/>
       <c r="M11" s="80"/>
@@ -38817,21 +38838,21 @@
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>347</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>348</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -38839,25 +38860,25 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="K3" s="121"/>
+      <c r="K3" s="120"/>
     </row>
     <row r="4">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="87" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -38866,134 +38887,134 @@
       <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="88" t="s">
+      <c r="I4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="88" t="s">
-        <v>304</v>
-      </c>
-      <c r="K4" s="118" t="s">
+      <c r="J4" s="87" t="s">
+        <v>303</v>
+      </c>
+      <c r="K4" s="117" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="C5" s="99" t="s">
         <v>351</v>
       </c>
-      <c r="C5" s="100" t="s">
+      <c r="D5" s="99" t="s">
         <v>352</v>
       </c>
-      <c r="D5" s="100" t="s">
-        <v>353</v>
-      </c>
-      <c r="E5" s="101"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="38" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I5" s="37">
         <v>0.0</v>
       </c>
-      <c r="J5" s="120" t="s">
-        <v>355</v>
-      </c>
-      <c r="K5" s="100"/>
+      <c r="J5" s="119" t="s">
+        <v>354</v>
+      </c>
+      <c r="K5" s="99"/>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
+        <v>355</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>356</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="37" t="s">
         <v>357</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="37" t="s">
         <v>358</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="E6" s="38" t="s">
         <v>359</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>360</v>
       </c>
       <c r="F6" s="37">
         <v>1.0</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="38" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I6" s="37">
         <v>1.0</v>
       </c>
-      <c r="J6" s="93"/>
+      <c r="J6" s="92"/>
       <c r="K6" s="37"/>
     </row>
     <row r="7">
-      <c r="A7" s="122" t="s">
+      <c r="A7" s="121" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121" t="s">
         <v>362</v>
       </c>
-      <c r="B7" s="122"/>
-      <c r="C7" s="122" t="s">
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="85" t="s">
         <v>363</v>
       </c>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="85" t="s">
+      <c r="I7" s="121">
+        <v>1.0</v>
+      </c>
+      <c r="J7" s="122" t="s">
         <v>364</v>
       </c>
-      <c r="I7" s="122">
-        <v>1.0</v>
-      </c>
-      <c r="J7" s="123" t="s">
-        <v>365</v>
-      </c>
-      <c r="K7" s="124"/>
+      <c r="K7" s="123"/>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>366</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="C8" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="D8" s="37" t="s">
         <v>368</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>369</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="I8" s="37">
         <v>1.0</v>
       </c>
-      <c r="J8" s="93" t="s">
-        <v>371</v>
-      </c>
-      <c r="K8" s="125"/>
+      <c r="J8" s="92" t="s">
+        <v>370</v>
+      </c>
+      <c r="K8" s="124"/>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
+        <v>371</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>372</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="C9" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="37" t="s">
         <v>374</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>375</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37">
@@ -39001,107 +39022,107 @@
       </c>
       <c r="G9" s="37"/>
       <c r="H9" s="38" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I9" s="37">
         <v>1.0</v>
       </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="125"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="124"/>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
+        <v>376</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>377</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="C10" s="37" t="s">
         <v>378</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="37" t="s">
         <v>379</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>380</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I10" s="37">
         <v>0.0</v>
       </c>
-      <c r="J10" s="93" t="s">
-        <v>382</v>
-      </c>
-      <c r="K10" s="125"/>
+      <c r="J10" s="92" t="s">
+        <v>381</v>
+      </c>
+      <c r="K10" s="124"/>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
+        <v>382</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>383</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="C11" s="37" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D11" s="37" t="s">
         <v>385</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>386</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="38" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I11" s="37">
         <v>0.0</v>
       </c>
-      <c r="J11" s="93" t="s">
-        <v>388</v>
+      <c r="J11" s="92" t="s">
+        <v>387</v>
       </c>
       <c r="K11" s="37"/>
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>389</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="C12" s="37" t="s">
         <v>390</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="D12" s="37" t="s">
         <v>391</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>392</v>
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I12" s="37">
         <v>0.0</v>
       </c>
-      <c r="J12" s="93" t="s">
-        <v>394</v>
-      </c>
-      <c r="K12" s="125"/>
+      <c r="J12" s="92" t="s">
+        <v>393</v>
+      </c>
+      <c r="K12" s="124"/>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
+        <v>394</v>
+      </c>
+      <c r="B13" s="37" t="s">
         <v>395</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="C13" s="37" t="s">
         <v>396</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="D13" s="37" t="s">
         <v>397</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>398</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37">
@@ -39109,53 +39130,53 @@
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I13" s="37">
         <v>1.0</v>
       </c>
-      <c r="J13" s="93" t="s">
-        <v>400</v>
-      </c>
-      <c r="K13" s="125"/>
+      <c r="J13" s="92" t="s">
+        <v>399</v>
+      </c>
+      <c r="K13" s="124"/>
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
+        <v>400</v>
+      </c>
+      <c r="B14" s="37" t="s">
         <v>401</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="C14" s="37" t="s">
         <v>402</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="D14" s="37" t="s">
         <v>403</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>404</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="38" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I14" s="37">
         <v>0.0</v>
       </c>
-      <c r="J14" s="93"/>
-      <c r="K14" s="125"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="124"/>
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
+        <v>405</v>
+      </c>
+      <c r="B15" s="37" t="s">
         <v>406</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="C15" s="37" t="s">
         <v>407</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="D15" s="37" t="s">
         <v>408</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>409</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37">
@@ -39163,53 +39184,53 @@
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="93" t="s">
-        <v>411</v>
-      </c>
-      <c r="K15" s="125"/>
+      <c r="J15" s="92" t="s">
+        <v>410</v>
+      </c>
+      <c r="K15" s="124"/>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
+        <v>411</v>
+      </c>
+      <c r="B16" s="37" t="s">
         <v>412</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="C16" s="37" t="s">
         <v>413</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="D16" s="37" t="s">
         <v>414</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>415</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I16" s="37">
         <v>0.0</v>
       </c>
-      <c r="J16" s="93"/>
-      <c r="K16" s="125"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="124"/>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
+        <v>416</v>
+      </c>
+      <c r="B17" s="37" t="s">
         <v>417</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="C17" s="37" t="s">
         <v>418</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="D17" s="37" t="s">
         <v>419</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>420</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37">
@@ -39217,38 +39238,38 @@
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I17" s="37">
         <v>1.0</v>
       </c>
-      <c r="J17" s="93"/>
-      <c r="K17" s="125"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="124"/>
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
+        <v>421</v>
+      </c>
+      <c r="B18" s="37" t="s">
         <v>422</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="C18" s="37" t="s">
         <v>423</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="37" t="s">
         <v>424</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>425</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="38" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I18" s="37">
         <v>0.0</v>
       </c>
-      <c r="J18" s="93"/>
-      <c r="K18" s="125"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="124"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="C19" s="39"/>
@@ -40290,28 +40311,28 @@
       <c r="A1" s="81" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="125" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="44" t="s">
+        <v>426</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>427</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="126" t="s">
         <v>428</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="127" t="s">
-        <v>429</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -40320,25 +40341,25 @@
     </row>
     <row r="3" ht="13.5" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="128" t="s">
-        <v>184</v>
-      </c>
-      <c r="C4" s="88" t="s">
+      <c r="B4" s="127" t="s">
+        <v>183</v>
+      </c>
+      <c r="C4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="88" t="s">
+      <c r="E4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="88" t="s">
+      <c r="G4" s="87" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="17" t="s">
@@ -40347,87 +40368,87 @@
       <c r="I4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="88" t="s">
+      <c r="J4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="88" t="s">
+      <c r="K4" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="118" t="s">
+      <c r="L4" s="117" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="38" t="s">
+        <v>429</v>
+      </c>
+      <c r="B5" s="101"/>
+      <c r="C5" s="37" t="s">
         <v>430</v>
       </c>
-      <c r="B5" s="102"/>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="37" t="s">
         <v>431</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="E5" s="37" t="s">
         <v>432</v>
-      </c>
-      <c r="E5" s="37" t="s">
-        <v>433</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
       <c r="I5" s="38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J5" s="37">
         <v>0.0</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="L5" s="37"/>
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
+        <v>435</v>
+      </c>
+      <c r="B6" s="101"/>
+      <c r="C6" s="37" t="s">
         <v>436</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="37" t="s">
         <v>437</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="E6" s="37" t="s">
         <v>438</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>439</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="J6" s="37">
         <v>0.0</v>
       </c>
       <c r="K6" s="37" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="L6" s="37"/>
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="B7" s="101">
+        <v>21.0</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>442</v>
       </c>
-      <c r="B7" s="102">
-        <v>21.0</v>
-      </c>
-      <c r="C7" s="37" t="s">
+      <c r="D7" s="37" t="s">
         <v>443</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="E7" s="37" t="s">
         <v>444</v>
-      </c>
-      <c r="E7" s="37" t="s">
-        <v>445</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37">
@@ -40435,32 +40456,32 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="38" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J7" s="37">
         <v>1.0</v>
       </c>
       <c r="K7" s="37" t="s">
+        <v>446</v>
+      </c>
+      <c r="L7" s="37"/>
+      <c r="M7" s="128" t="s">
         <v>447</v>
-      </c>
-      <c r="L7" s="37"/>
-      <c r="M7" s="129" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="38" t="s">
+        <v>448</v>
+      </c>
+      <c r="B8" s="101"/>
+      <c r="C8" s="37" t="s">
         <v>449</v>
       </c>
-      <c r="B8" s="102"/>
-      <c r="C8" s="37" t="s">
+      <c r="D8" s="37" t="s">
         <v>450</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="E8" s="37" t="s">
         <v>451</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>452</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="37">
@@ -40468,98 +40489,98 @@
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J8" s="37">
         <v>1.0</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="L8" s="37"/>
     </row>
     <row r="9">
       <c r="A9" s="38" t="s">
+        <v>454</v>
+      </c>
+      <c r="B9" s="101"/>
+      <c r="C9" s="37" t="s">
         <v>455</v>
       </c>
-      <c r="B9" s="102"/>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="37" t="s">
         <v>456</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="E9" s="37" t="s">
         <v>457</v>
-      </c>
-      <c r="E9" s="37" t="s">
-        <v>458</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J9" s="37">
         <v>0.0</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="L9" s="37"/>
-      <c r="M9" s="129" t="s">
-        <v>448</v>
+      <c r="M9" s="128" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
+        <v>460</v>
+      </c>
+      <c r="B10" s="101"/>
+      <c r="C10" s="37" t="s">
         <v>461</v>
       </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="37" t="s">
         <v>462</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="E10" s="37" t="s">
         <v>463</v>
-      </c>
-      <c r="E10" s="37" t="s">
-        <v>464</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="J10" s="37">
         <v>0.0</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="L10" s="37"/>
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
+        <v>466</v>
+      </c>
+      <c r="B11" s="101" t="s">
         <v>467</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="C11" s="37" t="s">
         <v>468</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D11" s="37" t="s">
         <v>469</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="E11" s="37" t="s">
         <v>470</v>
       </c>
-      <c r="E11" s="37" t="s">
-        <v>471</v>
-      </c>
-      <c r="F11" s="101"/>
+      <c r="F11" s="100"/>
       <c r="G11" s="37">
         <v>1.0</v>
       </c>
       <c r="H11" s="37"/>
       <c r="I11" s="38" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="J11" s="37">
         <v>1.0</v>
@@ -40569,47 +40590,47 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
+        <v>472</v>
+      </c>
+      <c r="B12" s="101"/>
+      <c r="C12" s="37" t="s">
         <v>473</v>
       </c>
-      <c r="B12" s="102"/>
-      <c r="C12" s="37" t="s">
+      <c r="D12" s="37" t="s">
         <v>474</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="E12" s="37" t="s">
         <v>475</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>476</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="J12" s="37">
         <v>0.0</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="L12" s="37"/>
     </row>
     <row r="13">
       <c r="A13" s="38" t="s">
+        <v>478</v>
+      </c>
+      <c r="B13" s="101">
+        <v>22.0</v>
+      </c>
+      <c r="C13" s="37" t="s">
         <v>479</v>
       </c>
-      <c r="B13" s="102">
-        <v>22.0</v>
-      </c>
-      <c r="C13" s="37" t="s">
+      <c r="D13" s="37" t="s">
         <v>480</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="E13" s="37" t="s">
         <v>481</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>482</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37">
@@ -40617,35 +40638,35 @@
       </c>
       <c r="H13" s="37"/>
       <c r="I13" s="38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="J13" s="37">
         <v>1.0</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="L13" s="37"/>
     </row>
     <row r="14">
       <c r="A14" s="38" t="s">
+        <v>484</v>
+      </c>
+      <c r="B14" s="101"/>
+      <c r="C14" s="37" t="s">
         <v>485</v>
       </c>
-      <c r="B14" s="102"/>
-      <c r="C14" s="37" t="s">
+      <c r="D14" s="37" t="s">
         <v>486</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="E14" s="37" t="s">
         <v>487</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>488</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J14" s="37">
         <v>0.0</v>
@@ -40655,23 +40676,23 @@
     </row>
     <row r="15">
       <c r="A15" s="38" t="s">
+        <v>489</v>
+      </c>
+      <c r="B15" s="101"/>
+      <c r="C15" s="37" t="s">
         <v>490</v>
       </c>
-      <c r="B15" s="102"/>
-      <c r="C15" s="37" t="s">
+      <c r="D15" s="37" t="s">
         <v>491</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="E15" s="37" t="s">
         <v>492</v>
-      </c>
-      <c r="E15" s="37" t="s">
-        <v>493</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="J15" s="37">
         <v>0.0</v>
@@ -40681,105 +40702,105 @@
     </row>
     <row r="16">
       <c r="A16" s="38" t="s">
+        <v>494</v>
+      </c>
+      <c r="B16" s="101"/>
+      <c r="C16" s="37" t="s">
         <v>495</v>
       </c>
-      <c r="B16" s="102"/>
-      <c r="C16" s="37" t="s">
+      <c r="D16" s="37" t="s">
         <v>496</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="E16" s="37" t="s">
         <v>497</v>
       </c>
-      <c r="E16" s="37" t="s">
+      <c r="F16" s="93" t="s">
         <v>498</v>
-      </c>
-      <c r="F16" s="94" t="s">
-        <v>499</v>
       </c>
       <c r="G16" s="37">
         <v>1.0</v>
       </c>
       <c r="H16" s="37"/>
       <c r="I16" s="38" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="J16" s="37">
         <v>1.0</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="L16" s="37"/>
     </row>
     <row r="17">
       <c r="A17" s="38" t="s">
+        <v>501</v>
+      </c>
+      <c r="B17" s="101"/>
+      <c r="C17" s="37" t="s">
+        <v>455</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>431</v>
+      </c>
+      <c r="E17" s="37" t="s">
         <v>502</v>
-      </c>
-      <c r="B17" s="102"/>
-      <c r="C17" s="37" t="s">
-        <v>456</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>432</v>
-      </c>
-      <c r="E17" s="37" t="s">
-        <v>503</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="38" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J17" s="37">
         <v>1.0</v>
       </c>
       <c r="K17" s="37" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L17" s="37"/>
     </row>
     <row r="18">
       <c r="A18" s="38" t="s">
+        <v>505</v>
+      </c>
+      <c r="B18" s="101"/>
+      <c r="C18" s="37" t="s">
         <v>506</v>
       </c>
-      <c r="B18" s="102"/>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="37" t="s">
         <v>507</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="E18" s="37" t="s">
         <v>508</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>509</v>
       </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="38" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J18" s="37">
         <v>1.0</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L18" s="37"/>
     </row>
     <row r="19">
       <c r="A19" s="38" t="s">
+        <v>511</v>
+      </c>
+      <c r="B19" s="101"/>
+      <c r="C19" s="37" t="s">
         <v>512</v>
       </c>
-      <c r="B19" s="102"/>
-      <c r="C19" s="37" t="s">
+      <c r="D19" s="37" t="s">
         <v>513</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="E19" s="37" t="s">
         <v>514</v>
-      </c>
-      <c r="E19" s="37" t="s">
-        <v>515</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37">
@@ -40787,7 +40808,7 @@
       </c>
       <c r="H19" s="37"/>
       <c r="I19" s="38" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J19" s="37">
         <v>1.0</v>
@@ -41825,48 +41846,48 @@
       <c r="D1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="71"/>
       <c r="F1" s="43" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="49.5" customHeight="1">
       <c r="A2" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" s="46" t="s">
         <v>517</v>
-      </c>
-      <c r="B2" s="46" t="s">
-        <v>518</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>519</v>
-      </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="130">
+        <v>518</v>
+      </c>
+      <c r="E2" s="72"/>
+      <c r="F2" s="129">
         <v>0.1</v>
       </c>
-      <c r="G2" s="131"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="88" t="s">
+      <c r="C4" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="88" t="s">
+      <c r="D4" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="91" t="s">
+      <c r="E4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="88" t="s">
+      <c r="F4" s="87" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -41875,28 +41896,28 @@
       <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="88" t="s">
+      <c r="I4" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="88" t="s">
+      <c r="J4" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="118" t="s">
+      <c r="K4" s="117" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
+        <v>519</v>
+      </c>
+      <c r="B5" s="37" t="s">
         <v>520</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="C5" s="37" t="s">
         <v>521</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="D5" s="37" t="s">
         <v>522</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>523</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37">
@@ -41904,34 +41925,34 @@
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="38" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="I5" s="37">
         <v>0.0</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K5" s="37"/>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
+        <v>525</v>
+      </c>
+      <c r="B6" s="37" t="s">
         <v>526</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="C6" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="D6" s="37" t="s">
         <v>528</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>529</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="38" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="I6" s="37">
         <v>0.0</v>
@@ -41941,49 +41962,49 @@
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
+        <v>530</v>
+      </c>
+      <c r="B7" s="37" t="s">
         <v>531</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="C7" s="37" t="s">
         <v>532</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="D7" s="37" t="s">
         <v>533</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>534</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="38" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="I7" s="37">
         <v>0.0</v>
       </c>
-      <c r="J7" s="101" t="s">
-        <v>536</v>
+      <c r="J7" s="100" t="s">
+        <v>535</v>
       </c>
       <c r="K7" s="37"/>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
+        <v>536</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>537</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="C8" s="37" t="s">
         <v>538</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="D8" s="37" t="s">
         <v>539</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>540</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I8" s="37">
         <v>0.0</v>
@@ -41993,22 +42014,22 @@
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
+        <v>541</v>
+      </c>
+      <c r="B9" s="37" t="s">
         <v>542</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="C9" s="37" t="s">
         <v>543</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="37" t="s">
         <v>544</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>545</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="38" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I9" s="37">
         <v>1.0</v>
@@ -42018,26 +42039,26 @@
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
+        <v>546</v>
+      </c>
+      <c r="B10" s="37" t="s">
         <v>547</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="C10" s="37" t="s">
         <v>548</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="37" t="s">
         <v>549</v>
       </c>
-      <c r="D10" s="37" t="s">
-        <v>550</v>
-      </c>
-      <c r="E10" s="113" t="s">
-        <v>223</v>
+      <c r="E10" s="112" t="s">
+        <v>222</v>
       </c>
       <c r="F10" s="37">
         <v>1.0</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="I10" s="37">
         <v>1.0</v>
@@ -42047,24 +42068,24 @@
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
+        <v>551</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>552</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="C11" s="37" t="s">
         <v>553</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="D11" s="37" t="s">
         <v>554</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="E11" s="112" t="s">
         <v>555</v>
-      </c>
-      <c r="E11" s="113" t="s">
-        <v>556</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="38" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="I11" s="37">
         <v>0.0</v>
@@ -42074,49 +42095,49 @@
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
+        <v>557</v>
+      </c>
+      <c r="B12" s="37" t="s">
         <v>558</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="C12" s="37" t="s">
         <v>559</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="D12" s="132" t="s">
         <v>560</v>
       </c>
-      <c r="D12" s="133" t="s">
+      <c r="E12" s="38" t="s">
         <v>561</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>562</v>
       </c>
       <c r="F12" s="37">
         <v>1.0</v>
       </c>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I12" s="37">
         <v>1.0</v>
       </c>
       <c r="J12" s="37" t="s">
+        <v>563</v>
+      </c>
+      <c r="K12" s="37" t="s">
         <v>564</v>
-      </c>
-      <c r="K12" s="37" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
+        <v>565</v>
+      </c>
+      <c r="B13" s="37" t="s">
         <v>566</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="C13" s="37" t="s">
         <v>567</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="D13" s="37" t="s">
         <v>568</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>569</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37">
@@ -42124,7 +42145,7 @@
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="I13" s="37">
         <v>1.0</v>
@@ -42134,26 +42155,26 @@
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
+        <v>570</v>
+      </c>
+      <c r="B14" s="37" t="s">
         <v>571</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="C14" s="37" t="s">
         <v>572</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="D14" s="37" t="s">
         <v>573</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="E14" s="38" t="s">
         <v>574</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>575</v>
       </c>
       <c r="F14" s="37">
         <v>1.0</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="38" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I14" s="37">
         <v>1.0</v>
@@ -42163,16 +42184,16 @@
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
+        <v>576</v>
+      </c>
+      <c r="B15" s="37" t="s">
         <v>577</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="C15" s="37" t="s">
         <v>578</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>579</v>
-      </c>
       <c r="D15" s="37" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37">
@@ -42180,34 +42201,34 @@
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="101" t="s">
-        <v>581</v>
+      <c r="J15" s="100" t="s">
+        <v>580</v>
       </c>
       <c r="K15" s="37"/>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
+        <v>581</v>
+      </c>
+      <c r="B16" s="37" t="s">
         <v>582</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="C16" s="37" t="s">
         <v>583</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="D16" s="37" t="s">
         <v>584</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>585</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="38" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="I16" s="37">
         <v>0.0</v>
@@ -42217,16 +42238,16 @@
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
+        <v>586</v>
+      </c>
+      <c r="B17" s="37" t="s">
         <v>587</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="C17" s="37" t="s">
         <v>588</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="D17" s="37" t="s">
         <v>589</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>590</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37">
@@ -42234,7 +42255,7 @@
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="I17" s="37">
         <v>1.0</v>
@@ -42244,26 +42265,26 @@
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
+        <v>591</v>
+      </c>
+      <c r="B18" s="37" t="s">
         <v>592</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="C18" s="37" t="s">
         <v>593</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="D18" s="37" t="s">
         <v>594</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="E18" s="38" t="s">
         <v>595</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>596</v>
       </c>
       <c r="F18" s="37">
         <v>1.0</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="38" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="I18" s="37">
         <v>1.0</v>

</xml_diff>

<commit_message>
NAV-91 Add ADR auto checks
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -26,6 +26,13 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="E16">
+      <text>
+        <t xml:space="preserve">@jonathan@fjelltopp.org ADD LINK DIRECTLY TO USER'S ORGANIZATION PAGE / INPUTS PACKAGE FOR THIS YEAR.
+_Assigned to Jonathan Berry_
+	-Jonathan Berry</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="E9">
       <text>
         <t xml:space="preserve">@jonathan@fjelltopp.org ADD LINK DIRECTLY TO USER'S ORGANIZATION PAGE / INPUTS PACKAGE FOR THIS YEAR.
@@ -33,14 +40,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E7">
-      <text>
-        <t xml:space="preserve">@jonathan@fjelltopp.org ADD LINK DIRECTLY TO USER'S ORGANIZATION PAGE / INPUTS PACKAGE FOR THIS YEAR.
-_Assigned to Jonathan Berry_
-	-Jonathan Berry</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D8">
+    <comment authorId="0" ref="D15">
       <text>
         <t xml:space="preserve">Unaids to add justification for why uploading data is important.
 	-Jonathan Berry</t>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="631">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -704,6 +704,54 @@
     <t>check_manual_confirmation('EST-ADR-03-A')</t>
   </si>
   <si>
+    <t>ADR-03A</t>
+  </si>
+  <si>
+    <t>Upload your Shiny 90 Survey template to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a Shiny90 survey testing template?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your Shiny90 survey file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your Shiny90 Survey template to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Shiny90 Survey Data" and click *Add Data*
+- Drag your Shiny90 template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-shiny90-survey', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-03B</t>
+  </si>
+  <si>
+    <t>Upload your Shiny 90 HIV Testing template to ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a Shiny90 HIV Testing template?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your Shiny90 HIV Testing template to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your Shiny90 HIV Testing template to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Shiny90 Survey Data" and click *Add Data*
+- Drag your Shiny90 template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-hiv-testing', 'url', '.*')</t>
+  </si>
+  <si>
     <t>ADR-04</t>
   </si>
   <si>
@@ -740,6 +788,126 @@
     <t>check_manual_confirmation('EST-ADR-04-A')</t>
   </si>
   <si>
+    <t>ADR-04A</t>
+  </si>
+  <si>
+    <t>Upload your area boundaries data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a Geographic data file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your Geographic area boundaries file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your  Geographic area boundaries data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Geographic Data" and click *Add Data*
+- Drag your Geographic areas boundaries file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-geographic', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04B</t>
+  </si>
+  <si>
+    <t>Upload your population data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a population template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your population template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your population data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Population Data" and click *Add Data*
+- Drag your population template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-population', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04C</t>
+  </si>
+  <si>
+    <t>Upload your Naomi survey data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a survey template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your survey template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your  Naomi survey data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Survey Data" and click *Add Data*
+- Drag your Naomi survey template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-survey', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04D</t>
+  </si>
+  <si>
+    <t>Upload your ART data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded an ART template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your ART template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your  ART data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "ART Data" and click *Add Data*
+- Drag your ART template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-art', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04E</t>
+  </si>
+  <si>
+    <t>Upload your ANC survey data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded an  ANC template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your ANC template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your ANC data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "ANC Data" and click *Add Data*
+- Drag your ANC template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-anc', 'url', '.*')</t>
+  </si>
+  <si>
     <t>ADR-05</t>
   </si>
   <si>
@@ -789,7 +957,7 @@
     </r>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-ADR-06-A')</t>
+    <t>check_dataset_valid()</t>
   </si>
   <si>
     <t>Review quality of programme data inputs in ShinyRob</t>
@@ -842,7 +1010,7 @@
     <t>@UNAIDS - I've tagged everything here as mandatory right now. This means the user will not be able to proceed to Spectrum data entry until this process is complete. Are we okay with that order of operations to help avoid data quality problems downstream?</t>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-ROB-01-A')</t>
+    <t>check_not_skipped(['EST-ADR-04-A', 'EST-ADR-04A-A', 'EST-ADR-04B-A', 'EST-ADR-04C-A', 'EST-ADR-04D-A', 'EST-ADR-04E-A', 'EST-ADR-06-A'])</t>
   </si>
   <si>
     <t>ROB-02</t>
@@ -871,9 +1039,6 @@
   </si>
   <si>
     <t>not a user-facing task check; required to import data from ADR</t>
-  </si>
-  <si>
-    <t>check_not_skipped(['EST-ADR-04-A', 'EST-ADR-06-A'])</t>
   </si>
   <si>
     <t>ROB-03</t>
@@ -2827,7 +2992,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2838,6 +3003,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -2856,12 +3033,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
         <bgColor rgb="FFD8D8D8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -2992,7 +3163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="145">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3184,6 +3355,35 @@
     <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="6" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3191,21 +3391,24 @@
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3214,7 +3417,7 @@
     <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3224,11 +3427,11 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3238,43 +3441,43 @@
     <xf borderId="1" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3288,13 +3491,13 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="8" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -3302,7 +3505,7 @@
     <xf borderId="2" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
@@ -32630,7 +32833,7 @@
     <col customWidth="1" min="2" max="2" width="24.29"/>
     <col customWidth="1" min="3" max="3" width="34.57"/>
     <col customWidth="1" min="4" max="4" width="43.14"/>
-    <col customWidth="1" min="5" max="5" width="69.86"/>
+    <col customWidth="1" min="5" max="5" width="41.57"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
     <col customWidth="1" hidden="1" min="7" max="7" width="37.29"/>
     <col customWidth="1" hidden="1" min="8" max="8" width="26.86"/>
@@ -34364,108 +34567,395 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="76" t="s">
+    <row r="7" ht="87.0" customHeight="1">
+      <c r="A7" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="80" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="60" t="s">
+      <c r="D7" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="78">
+      <c r="E7" s="81"/>
+      <c r="F7" s="82">
         <v>0.0</v>
       </c>
-      <c r="G7" s="77">
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="86" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="87"/>
+      <c r="Z7" s="87"/>
+      <c r="AA7" s="87"/>
+    </row>
+    <row r="8" ht="87.0" customHeight="1">
+      <c r="A8" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="80" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="81"/>
+      <c r="F8" s="82">
         <v>0.0</v>
       </c>
-      <c r="H7" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="59" t="s">
+      <c r="G8" s="83"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="78">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="77">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="80"/>
-      <c r="S8" s="80"/>
-      <c r="T8" s="80"/>
-      <c r="U8" s="80"/>
-      <c r="V8" s="80"/>
-      <c r="W8" s="80"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="80"/>
-      <c r="Z8" s="80"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
+      <c r="X8" s="87"/>
+      <c r="Y8" s="87"/>
+      <c r="Z8" s="87"/>
+      <c r="AA8" s="87"/>
     </row>
     <row r="9">
       <c r="A9" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="D9" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="F9" s="78">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="77">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="59">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="58">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="58"/>
       <c r="I9" s="58"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="80" t="s">
         <v>144</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="88"/>
+      <c r="F10" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="83"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="88"/>
+      <c r="F11" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="83"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="89"/>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="79" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="88"/>
+      <c r="F12" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="83"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85" t="s">
+        <v>157</v>
+      </c>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="88"/>
+      <c r="F13" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="83"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
+      <c r="X13" s="89"/>
+      <c r="Y13" s="89"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="88"/>
+      <c r="F14" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="83"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="58"/>
+      <c r="F15" s="78">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="77">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="90" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" s="58"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="91"/>
+      <c r="X15" s="91"/>
+      <c r="Y15" s="91"/>
+      <c r="Z15" s="91"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="59">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="58">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -34475,8 +34965,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="E5"/>
-    <hyperlink r:id="rId3" ref="E7"/>
-    <hyperlink r:id="rId4" ref="E9"/>
+    <hyperlink r:id="rId3" ref="E9"/>
+    <hyperlink r:id="rId4" ref="E16"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -34510,7 +35000,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -34527,14 +35017,14 @@
     </row>
     <row r="2" ht="48.0" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -34585,16 +35075,16 @@
     </row>
     <row r="5">
       <c r="A5" s="58" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="E5" s="59" t="s">
         <v>82</v>
@@ -34605,29 +35095,29 @@
       <c r="G5" s="61">
         <v>0.0</v>
       </c>
-      <c r="H5" s="79" t="s">
-        <v>152</v>
+      <c r="H5" s="90" t="s">
+        <v>187</v>
       </c>
       <c r="I5" s="38"/>
-      <c r="J5" s="38" t="s">
-        <v>153</v>
+      <c r="J5" s="93" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="58" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="F6" s="61">
         <v>1.0</v>
@@ -34638,48 +35128,48 @@
       <c r="H6" s="63"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="82" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83">
+      <c r="A7" s="94" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95">
         <v>1.0</v>
       </c>
-      <c r="G7" s="83">
+      <c r="G7" s="95">
         <v>1.0</v>
       </c>
-      <c r="H7" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85" t="s">
-        <v>163</v>
+      <c r="H7" s="96" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="58" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="F8" s="61">
         <v>1.0</v>
@@ -34690,24 +35180,24 @@
       <c r="H8" s="63"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="58" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="F9" s="63">
         <v>1.0</v>
@@ -34718,21 +35208,21 @@
       <c r="H9" s="63"/>
       <c r="I9" s="28"/>
       <c r="J9" s="38" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="58" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="61">
@@ -34742,9 +35232,9 @@
         <v>0.0</v>
       </c>
       <c r="H10" s="58"/>
-      <c r="I10" s="86"/>
+      <c r="I10" s="98"/>
       <c r="J10" s="38" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -35853,7 +36343,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -35870,14 +36360,14 @@
     </row>
     <row r="2">
       <c r="A2" s="44" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -35886,31 +36376,31 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="87" t="s">
+      <c r="B4" s="100" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="87" t="s">
+      <c r="H4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="99" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="52" t="s">
@@ -35925,48 +36415,48 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="91"/>
+        <v>218</v>
+      </c>
+      <c r="B5" s="103"/>
       <c r="C5" s="37" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="92" t="s">
-        <v>187</v>
-      </c>
-      <c r="F5" s="93" t="s">
-        <v>188</v>
+        <v>220</v>
+      </c>
+      <c r="E5" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>222</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37">
         <v>1.0</v>
       </c>
-      <c r="I5" s="86"/>
+      <c r="I5" s="98"/>
       <c r="J5" s="58"/>
-      <c r="K5" s="94" t="s">
-        <v>189</v>
+      <c r="K5" s="106" t="s">
+        <v>223</v>
       </c>
       <c r="L5" s="38"/>
       <c r="M5" s="38" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="95"/>
+        <v>225</v>
+      </c>
+      <c r="B6" s="107"/>
       <c r="C6" s="37" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="96" t="s">
-        <v>194</v>
+        <v>227</v>
+      </c>
+      <c r="E6" s="108" t="s">
+        <v>228</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37">
@@ -35976,34 +36466,34 @@
         <v>1.0</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
       <c r="J6" s="58" t="s">
-        <v>196</v>
-      </c>
-      <c r="K6" s="94" t="s">
-        <v>197</v>
+        <v>230</v>
+      </c>
+      <c r="K6" s="106" t="s">
+        <v>231</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="91" t="s">
-        <v>200</v>
+        <v>233</v>
+      </c>
+      <c r="B7" s="103" t="s">
+        <v>234</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="96" t="s">
-        <v>203</v>
+        <v>236</v>
+      </c>
+      <c r="E7" s="108" t="s">
+        <v>237</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
@@ -36011,32 +36501,32 @@
         <v>1.0</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="J7" s="58"/>
       <c r="L7" s="38"/>
       <c r="M7" s="38" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="B8" s="97">
+        <v>240</v>
+      </c>
+      <c r="B8" s="109">
         <v>1.0</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="E8" s="92" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" s="93" t="s">
-        <v>210</v>
+        <v>242</v>
+      </c>
+      <c r="E8" s="104" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="105" t="s">
+        <v>244</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="37">
@@ -36046,170 +36536,170 @@
       <c r="J8" s="58"/>
       <c r="L8" s="38"/>
       <c r="M8" s="38" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="95"/>
+        <v>246</v>
+      </c>
+      <c r="B9" s="107"/>
       <c r="C9" s="37" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="E9" s="92" t="s">
-        <v>215</v>
-      </c>
-      <c r="F9" s="98"/>
+        <v>248</v>
+      </c>
+      <c r="E9" s="104" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="110"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37">
         <v>0.0</v>
       </c>
-      <c r="I9" s="99" t="s">
-        <v>216</v>
+      <c r="I9" s="111" t="s">
+        <v>250</v>
       </c>
       <c r="J9" s="58"/>
       <c r="L9" s="28"/>
       <c r="M9" s="38" t="s">
-        <v>217</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="B10" s="95"/>
+        <v>252</v>
+      </c>
+      <c r="B10" s="107"/>
       <c r="C10" s="37" t="s">
-        <v>219</v>
+        <v>253</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="E10" s="92" t="s">
-        <v>221</v>
+        <v>254</v>
+      </c>
+      <c r="E10" s="104" t="s">
+        <v>255</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="37">
         <v>1.0</v>
       </c>
-      <c r="I10" s="100"/>
+      <c r="I10" s="112"/>
       <c r="J10" s="58"/>
-      <c r="L10" s="86"/>
+      <c r="L10" s="98"/>
       <c r="M10" s="38" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="B11" s="97" t="s">
-        <v>225</v>
+        <v>258</v>
+      </c>
+      <c r="B11" s="109" t="s">
+        <v>259</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" s="92" t="s">
-        <v>228</v>
+        <v>261</v>
+      </c>
+      <c r="E11" s="104" t="s">
+        <v>262</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="G11" s="37"/>
       <c r="H11" s="37">
         <v>1.0</v>
       </c>
-      <c r="I11" s="99" t="s">
-        <v>229</v>
+      <c r="I11" s="111" t="s">
+        <v>263</v>
       </c>
       <c r="J11" s="58" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
       <c r="L11" s="38"/>
       <c r="M11" s="38" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="97"/>
+        <v>266</v>
+      </c>
+      <c r="B12" s="109"/>
       <c r="C12" s="37" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E12" s="92" t="s">
-        <v>235</v>
+        <v>268</v>
+      </c>
+      <c r="E12" s="104" t="s">
+        <v>269</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37">
         <v>0.0</v>
       </c>
-      <c r="I12" s="99" t="s">
-        <v>236</v>
+      <c r="I12" s="111" t="s">
+        <v>270</v>
       </c>
       <c r="J12" s="58"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38" t="s">
-        <v>237</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="B13" s="97">
+        <v>272</v>
+      </c>
+      <c r="B13" s="109">
         <v>2.0</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="E13" s="92" t="s">
-        <v>241</v>
+        <v>274</v>
+      </c>
+      <c r="E13" s="104" t="s">
+        <v>275</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="37">
         <v>1.0</v>
       </c>
-      <c r="I13" s="99"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="58"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="B14" s="101"/>
+        <v>277</v>
+      </c>
+      <c r="B14" s="113"/>
       <c r="C14" s="37" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
@@ -36217,253 +36707,253 @@
         <v>1.0</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
       <c r="J14" s="37"/>
-      <c r="K14" s="102" t="s">
-        <v>248</v>
+      <c r="K14" s="114" t="s">
+        <v>282</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38" t="s">
-        <v>249</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="103" t="s">
-        <v>250</v>
-      </c>
-      <c r="B15" s="104"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="103" t="s">
-        <v>251</v>
-      </c>
-      <c r="E15" s="105"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103">
+      <c r="A15" s="115" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="116"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" s="117"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115">
         <v>1.0</v>
       </c>
-      <c r="H15" s="103"/>
-      <c r="I15" s="106" t="s">
-        <v>252</v>
-      </c>
-      <c r="J15" s="82"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="118" t="s">
+        <v>286</v>
+      </c>
+      <c r="J15" s="94"/>
       <c r="L15" s="28"/>
-      <c r="M15" s="85" t="s">
-        <v>253</v>
+      <c r="M15" s="97" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="B16" s="97" t="s">
-        <v>255</v>
-      </c>
-      <c r="C16" s="107" t="s">
-        <v>256</v>
-      </c>
-      <c r="D16" s="107" t="s">
-        <v>257</v>
-      </c>
-      <c r="E16" s="108" t="s">
-        <v>258</v>
-      </c>
-      <c r="F16" s="109" t="s">
-        <v>259</v>
-      </c>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107">
+        <v>288</v>
+      </c>
+      <c r="B16" s="109" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="119" t="s">
+        <v>290</v>
+      </c>
+      <c r="D16" s="119" t="s">
+        <v>291</v>
+      </c>
+      <c r="E16" s="120" t="s">
+        <v>292</v>
+      </c>
+      <c r="F16" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119">
         <v>1.0</v>
       </c>
-      <c r="I16" s="110" t="s">
-        <v>260</v>
-      </c>
-      <c r="J16" s="111" t="s">
-        <v>261</v>
+      <c r="I16" s="122" t="s">
+        <v>294</v>
+      </c>
+      <c r="J16" s="123" t="s">
+        <v>295</v>
       </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="B17" s="95" t="s">
-        <v>264</v>
-      </c>
-      <c r="C17" s="107" t="s">
-        <v>265</v>
-      </c>
-      <c r="D17" s="107" t="s">
-        <v>266</v>
-      </c>
-      <c r="E17" s="108" t="s">
-        <v>267</v>
-      </c>
-      <c r="F17" s="109" t="s">
-        <v>259</v>
-      </c>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107">
+        <v>297</v>
+      </c>
+      <c r="B17" s="107" t="s">
+        <v>298</v>
+      </c>
+      <c r="C17" s="119" t="s">
+        <v>299</v>
+      </c>
+      <c r="D17" s="119" t="s">
+        <v>300</v>
+      </c>
+      <c r="E17" s="120" t="s">
+        <v>301</v>
+      </c>
+      <c r="F17" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119">
         <v>1.0</v>
       </c>
-      <c r="I17" s="110" t="s">
-        <v>268</v>
-      </c>
-      <c r="J17" s="111" t="s">
-        <v>269</v>
+      <c r="I17" s="122" t="s">
+        <v>302</v>
+      </c>
+      <c r="J17" s="123" t="s">
+        <v>303</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="38" t="s">
-        <v>270</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="B18" s="95" t="s">
-        <v>272</v>
+        <v>305</v>
+      </c>
+      <c r="B18" s="107" t="s">
+        <v>306</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="E18" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="F18" s="112" t="s">
-        <v>259</v>
+        <v>308</v>
+      </c>
+      <c r="E18" s="104" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="124" t="s">
+        <v>293</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="37">
         <v>1.0</v>
       </c>
-      <c r="I18" s="100"/>
+      <c r="I18" s="112"/>
       <c r="J18" s="58"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="B19" s="95">
+        <v>311</v>
+      </c>
+      <c r="B19" s="107">
         <v>19.0</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="E19" s="92" t="s">
-        <v>280</v>
-      </c>
-      <c r="F19" s="112" t="s">
-        <v>281</v>
+        <v>313</v>
+      </c>
+      <c r="E19" s="104" t="s">
+        <v>314</v>
+      </c>
+      <c r="F19" s="124" t="s">
+        <v>315</v>
       </c>
       <c r="G19" s="37"/>
       <c r="H19" s="37">
         <v>1.0</v>
       </c>
-      <c r="I19" s="100"/>
+      <c r="I19" s="112"/>
       <c r="J19" s="58"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="B20" s="95">
+        <v>317</v>
+      </c>
+      <c r="B20" s="107">
         <v>20.0</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>284</v>
+        <v>318</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>285</v>
-      </c>
-      <c r="E20" s="92" t="s">
-        <v>286</v>
-      </c>
-      <c r="F20" s="112" t="s">
-        <v>259</v>
+        <v>319</v>
+      </c>
+      <c r="E20" s="104" t="s">
+        <v>320</v>
+      </c>
+      <c r="F20" s="124" t="s">
+        <v>293</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="37">
         <v>1.0</v>
       </c>
-      <c r="I20" s="100" t="s">
-        <v>287</v>
+      <c r="I20" s="112" t="s">
+        <v>321</v>
       </c>
       <c r="J20" s="58"/>
       <c r="L20" s="28"/>
       <c r="M20" s="38" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="103" t="s">
-        <v>289</v>
-      </c>
-      <c r="B21" s="113"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="103" t="s">
-        <v>290</v>
-      </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="115">
+      <c r="A21" s="115" t="s">
+        <v>323</v>
+      </c>
+      <c r="B21" s="125"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115" t="s">
+        <v>324</v>
+      </c>
+      <c r="E21" s="117"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="127">
         <v>1.0</v>
       </c>
-      <c r="H21" s="115"/>
-      <c r="I21" s="106" t="s">
-        <v>291</v>
-      </c>
-      <c r="J21" s="82"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="118" t="s">
+        <v>325</v>
+      </c>
+      <c r="J21" s="94"/>
       <c r="L21" s="38"/>
-      <c r="M21" s="85" t="s">
-        <v>292</v>
+      <c r="M21" s="97" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="B22" s="95" t="s">
-        <v>294</v>
+        <v>327</v>
+      </c>
+      <c r="B22" s="107" t="s">
+        <v>328</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>295</v>
+        <v>329</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>296</v>
+        <v>330</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>297</v>
-      </c>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116">
+        <v>331</v>
+      </c>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128">
         <v>1.0</v>
       </c>
-      <c r="I22" s="79" t="s">
-        <v>298</v>
+      <c r="I22" s="90" t="s">
+        <v>332</v>
       </c>
       <c r="J22" s="58"/>
       <c r="L22" s="28"/>
       <c r="M22" s="38" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -37541,7 +38031,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -37558,14 +38048,14 @@
     </row>
     <row r="2" ht="84.0" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -37574,31 +38064,31 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="87" t="s">
-        <v>303</v>
-      </c>
-      <c r="I4" s="117" t="s">
+      <c r="H4" s="99" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" s="129" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -37610,97 +38100,97 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>305</v>
+        <v>339</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>306</v>
+        <v>340</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37">
         <v>0.0</v>
       </c>
-      <c r="H5" s="92" t="s">
-        <v>308</v>
-      </c>
-      <c r="I5" s="99"/>
+      <c r="H5" s="104" t="s">
+        <v>342</v>
+      </c>
+      <c r="I5" s="111"/>
       <c r="J5" s="38"/>
       <c r="K5" s="38" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>312</v>
+        <v>346</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>313</v>
+        <v>347</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37">
         <v>1.0</v>
       </c>
-      <c r="H6" s="92" t="s">
-        <v>314</v>
+      <c r="H6" s="104" t="s">
+        <v>348</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38" t="s">
-        <v>315</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
-        <v>316</v>
+        <v>350</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>317</v>
+        <v>351</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>318</v>
+        <v>352</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>319</v>
+        <v>353</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37">
         <v>1.0</v>
       </c>
-      <c r="H7" s="92" t="s">
-        <v>314</v>
+      <c r="H7" s="104" t="s">
+        <v>348</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="38"/>
       <c r="K7" s="38" t="s">
-        <v>320</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>321</v>
+        <v>355</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>323</v>
+        <v>357</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>324</v>
+        <v>358</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37">
@@ -37709,28 +38199,28 @@
       <c r="G8" s="37">
         <v>1.0</v>
       </c>
-      <c r="H8" s="92"/>
+      <c r="H8" s="104"/>
       <c r="I8" s="37"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38" t="s">
-        <v>325</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>326</v>
+        <v>360</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>327</v>
+        <v>361</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>328</v>
+        <v>362</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>329</v>
-      </c>
-      <c r="E9" s="118" t="s">
-        <v>330</v>
+        <v>363</v>
+      </c>
+      <c r="E9" s="130" t="s">
+        <v>364</v>
       </c>
       <c r="F9" s="37">
         <v>1.0</v>
@@ -37738,54 +38228,54 @@
       <c r="G9" s="37">
         <v>1.0</v>
       </c>
-      <c r="H9" s="92"/>
+      <c r="H9" s="104"/>
       <c r="I9" s="37" t="s">
-        <v>331</v>
+        <v>365</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="38" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>333</v>
+        <v>367</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>334</v>
+        <v>368</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>335</v>
+        <v>369</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37">
         <v>1.0</v>
       </c>
-      <c r="H10" s="119" t="s">
-        <v>337</v>
+      <c r="H10" s="131" t="s">
+        <v>371</v>
       </c>
       <c r="I10" s="37"/>
-      <c r="J10" s="86"/>
+      <c r="J10" s="98"/>
       <c r="K10" s="38" t="s">
-        <v>338</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>339</v>
+        <v>373</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>340</v>
+        <v>374</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>341</v>
+        <v>375</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>342</v>
+        <v>376</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37">
@@ -37795,31 +38285,31 @@
         <v>1.0</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="I11" s="37" t="s">
-        <v>344</v>
+        <v>378</v>
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="38" t="s">
-        <v>345</v>
-      </c>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="80"/>
-      <c r="Q11" s="80"/>
-      <c r="R11" s="80"/>
-      <c r="S11" s="80"/>
-      <c r="T11" s="80"/>
-      <c r="U11" s="80"/>
-      <c r="V11" s="80"/>
-      <c r="W11" s="80"/>
-      <c r="X11" s="80"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="80"/>
-      <c r="AA11" s="80"/>
+        <v>379</v>
+      </c>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="91"/>
+      <c r="Q11" s="91"/>
+      <c r="R11" s="91"/>
+      <c r="S11" s="91"/>
+      <c r="T11" s="91"/>
+      <c r="U11" s="91"/>
+      <c r="V11" s="91"/>
+      <c r="W11" s="91"/>
+      <c r="X11" s="91"/>
+      <c r="Y11" s="91"/>
+      <c r="Z11" s="91"/>
+      <c r="AA11" s="91"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -38828,7 +39318,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -38845,14 +39335,14 @@
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>346</v>
+        <v>380</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -38860,25 +39350,25 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="K3" s="120"/>
+      <c r="K3" s="132"/>
     </row>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -38887,134 +39377,134 @@
       <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="87" t="s">
-        <v>303</v>
-      </c>
-      <c r="K4" s="117" t="s">
+      <c r="J4" s="99" t="s">
+        <v>337</v>
+      </c>
+      <c r="K4" s="129" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>349</v>
+        <v>383</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>350</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>351</v>
-      </c>
-      <c r="D5" s="99" t="s">
-        <v>352</v>
-      </c>
-      <c r="E5" s="100"/>
+        <v>384</v>
+      </c>
+      <c r="C5" s="111" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" s="112"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="38" t="s">
-        <v>353</v>
+        <v>387</v>
       </c>
       <c r="I5" s="37">
         <v>0.0</v>
       </c>
-      <c r="J5" s="119" t="s">
-        <v>354</v>
-      </c>
-      <c r="K5" s="99"/>
+      <c r="J5" s="131" t="s">
+        <v>388</v>
+      </c>
+      <c r="K5" s="111"/>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>355</v>
+        <v>389</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>356</v>
+        <v>390</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>357</v>
+        <v>391</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>358</v>
+        <v>392</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>359</v>
+        <v>393</v>
       </c>
       <c r="F6" s="37">
         <v>1.0</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="38" t="s">
-        <v>360</v>
+        <v>394</v>
       </c>
       <c r="I6" s="37">
         <v>1.0</v>
       </c>
-      <c r="J6" s="92"/>
+      <c r="J6" s="104"/>
       <c r="K6" s="37"/>
     </row>
     <row r="7">
-      <c r="A7" s="121" t="s">
-        <v>361</v>
-      </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121" t="s">
-        <v>362</v>
-      </c>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="85" t="s">
-        <v>363</v>
-      </c>
-      <c r="I7" s="121">
+      <c r="A7" s="133" t="s">
+        <v>395</v>
+      </c>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="97" t="s">
+        <v>397</v>
+      </c>
+      <c r="I7" s="133">
         <v>1.0</v>
       </c>
-      <c r="J7" s="122" t="s">
-        <v>364</v>
-      </c>
-      <c r="K7" s="123"/>
+      <c r="J7" s="134" t="s">
+        <v>398</v>
+      </c>
+      <c r="K7" s="135"/>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>365</v>
+        <v>399</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>366</v>
+        <v>400</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>367</v>
+        <v>401</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>368</v>
+        <v>402</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>369</v>
+        <v>403</v>
       </c>
       <c r="I8" s="37">
         <v>1.0</v>
       </c>
-      <c r="J8" s="92" t="s">
-        <v>370</v>
-      </c>
-      <c r="K8" s="124"/>
+      <c r="J8" s="104" t="s">
+        <v>404</v>
+      </c>
+      <c r="K8" s="136"/>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>371</v>
+        <v>405</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>372</v>
+        <v>406</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37">
@@ -39022,107 +39512,107 @@
       </c>
       <c r="G9" s="37"/>
       <c r="H9" s="38" t="s">
-        <v>375</v>
+        <v>409</v>
       </c>
       <c r="I9" s="37">
         <v>1.0</v>
       </c>
-      <c r="J9" s="92"/>
-      <c r="K9" s="124"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="136"/>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>377</v>
+        <v>411</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>378</v>
+        <v>412</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>379</v>
+        <v>413</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>380</v>
+        <v>414</v>
       </c>
       <c r="I10" s="37">
         <v>0.0</v>
       </c>
-      <c r="J10" s="92" t="s">
-        <v>381</v>
-      </c>
-      <c r="K10" s="124"/>
+      <c r="J10" s="104" t="s">
+        <v>415</v>
+      </c>
+      <c r="K10" s="136"/>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>382</v>
+        <v>416</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>383</v>
+        <v>417</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>384</v>
+        <v>418</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>385</v>
+        <v>419</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="38" t="s">
-        <v>386</v>
+        <v>420</v>
       </c>
       <c r="I11" s="37">
         <v>0.0</v>
       </c>
-      <c r="J11" s="92" t="s">
-        <v>387</v>
+      <c r="J11" s="104" t="s">
+        <v>421</v>
       </c>
       <c r="K11" s="37"/>
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>388</v>
+        <v>422</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>389</v>
+        <v>423</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>390</v>
+        <v>424</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>391</v>
+        <v>425</v>
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>392</v>
+        <v>426</v>
       </c>
       <c r="I12" s="37">
         <v>0.0</v>
       </c>
-      <c r="J12" s="92" t="s">
-        <v>393</v>
-      </c>
-      <c r="K12" s="124"/>
+      <c r="J12" s="104" t="s">
+        <v>427</v>
+      </c>
+      <c r="K12" s="136"/>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>394</v>
+        <v>428</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>395</v>
+        <v>429</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>396</v>
+        <v>430</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>397</v>
+        <v>431</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37">
@@ -39130,53 +39620,53 @@
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38" t="s">
-        <v>398</v>
+        <v>432</v>
       </c>
       <c r="I13" s="37">
         <v>1.0</v>
       </c>
-      <c r="J13" s="92" t="s">
-        <v>399</v>
-      </c>
-      <c r="K13" s="124"/>
+      <c r="J13" s="104" t="s">
+        <v>433</v>
+      </c>
+      <c r="K13" s="136"/>
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
-        <v>400</v>
+        <v>434</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>401</v>
+        <v>435</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>403</v>
+        <v>437</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="38" t="s">
-        <v>404</v>
+        <v>438</v>
       </c>
       <c r="I14" s="37">
         <v>0.0</v>
       </c>
-      <c r="J14" s="92"/>
-      <c r="K14" s="124"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="136"/>
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
-        <v>405</v>
+        <v>439</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>406</v>
+        <v>440</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>407</v>
+        <v>441</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>408</v>
+        <v>442</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37">
@@ -39184,53 +39674,53 @@
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38" t="s">
-        <v>409</v>
+        <v>443</v>
       </c>
       <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="92" t="s">
-        <v>410</v>
-      </c>
-      <c r="K15" s="124"/>
+      <c r="J15" s="104" t="s">
+        <v>444</v>
+      </c>
+      <c r="K15" s="136"/>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>411</v>
+        <v>445</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>412</v>
+        <v>446</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>413</v>
+        <v>447</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>414</v>
+        <v>448</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="38" t="s">
-        <v>415</v>
+        <v>449</v>
       </c>
       <c r="I16" s="37">
         <v>0.0</v>
       </c>
-      <c r="J16" s="92"/>
-      <c r="K16" s="124"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="136"/>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
-        <v>416</v>
+        <v>450</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>417</v>
+        <v>451</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>418</v>
+        <v>452</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>419</v>
+        <v>453</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37">
@@ -39238,38 +39728,38 @@
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>420</v>
+        <v>454</v>
       </c>
       <c r="I17" s="37">
         <v>1.0</v>
       </c>
-      <c r="J17" s="92"/>
-      <c r="K17" s="124"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="136"/>
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>422</v>
+        <v>456</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>423</v>
+        <v>457</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="38" t="s">
-        <v>425</v>
+        <v>459</v>
       </c>
       <c r="I18" s="37">
         <v>0.0</v>
       </c>
-      <c r="J18" s="92"/>
-      <c r="K18" s="124"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="136"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="C19" s="39"/>
@@ -40308,10 +40798,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="125" t="s">
+      <c r="B1" s="137" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
@@ -40325,14 +40815,14 @@
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>426</v>
+        <v>460</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>427</v>
+        <v>461</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="126" t="s">
-        <v>428</v>
+      <c r="D2" s="138" t="s">
+        <v>462</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -40341,25 +40831,25 @@
     </row>
     <row r="3" ht="13.5" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="127" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="87" t="s">
+      <c r="B4" s="139" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="17" t="s">
@@ -40368,87 +40858,87 @@
       <c r="I4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="87" t="s">
+      <c r="K4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="117" t="s">
+      <c r="L4" s="129" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="38" t="s">
-        <v>429</v>
-      </c>
-      <c r="B5" s="101"/>
+        <v>463</v>
+      </c>
+      <c r="B5" s="113"/>
       <c r="C5" s="37" t="s">
-        <v>430</v>
+        <v>464</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>431</v>
+        <v>465</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>432</v>
+        <v>466</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
       <c r="I5" s="38" t="s">
-        <v>433</v>
+        <v>467</v>
       </c>
       <c r="J5" s="37">
         <v>0.0</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>434</v>
+        <v>468</v>
       </c>
       <c r="L5" s="37"/>
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="B6" s="101"/>
+        <v>469</v>
+      </c>
+      <c r="B6" s="113"/>
       <c r="C6" s="37" t="s">
-        <v>436</v>
+        <v>470</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>437</v>
+        <v>471</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>438</v>
+        <v>472</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38" t="s">
-        <v>439</v>
+        <v>473</v>
       </c>
       <c r="J6" s="37">
         <v>0.0</v>
       </c>
       <c r="K6" s="37" t="s">
-        <v>440</v>
+        <v>474</v>
       </c>
       <c r="L6" s="37"/>
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="B7" s="101">
+        <v>475</v>
+      </c>
+      <c r="B7" s="113">
         <v>21.0</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>442</v>
+        <v>476</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>443</v>
+        <v>477</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>444</v>
+        <v>478</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37">
@@ -40456,32 +40946,32 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="38" t="s">
-        <v>445</v>
+        <v>479</v>
       </c>
       <c r="J7" s="37">
         <v>1.0</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>446</v>
+        <v>480</v>
       </c>
       <c r="L7" s="37"/>
-      <c r="M7" s="128" t="s">
-        <v>447</v>
+      <c r="M7" s="140" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="38" t="s">
-        <v>448</v>
-      </c>
-      <c r="B8" s="101"/>
+        <v>482</v>
+      </c>
+      <c r="B8" s="113"/>
       <c r="C8" s="37" t="s">
-        <v>449</v>
+        <v>483</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>450</v>
+        <v>484</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>451</v>
+        <v>485</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="37">
@@ -40489,98 +40979,98 @@
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="38" t="s">
-        <v>452</v>
+        <v>486</v>
       </c>
       <c r="J8" s="37">
         <v>1.0</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>453</v>
+        <v>487</v>
       </c>
       <c r="L8" s="37"/>
     </row>
     <row r="9">
       <c r="A9" s="38" t="s">
-        <v>454</v>
-      </c>
-      <c r="B9" s="101"/>
+        <v>488</v>
+      </c>
+      <c r="B9" s="113"/>
       <c r="C9" s="37" t="s">
-        <v>455</v>
+        <v>489</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>456</v>
+        <v>490</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>457</v>
+        <v>491</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38" t="s">
-        <v>458</v>
+        <v>492</v>
       </c>
       <c r="J9" s="37">
         <v>0.0</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>459</v>
+        <v>493</v>
       </c>
       <c r="L9" s="37"/>
-      <c r="M9" s="128" t="s">
-        <v>447</v>
+      <c r="M9" s="140" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>460</v>
-      </c>
-      <c r="B10" s="101"/>
+        <v>494</v>
+      </c>
+      <c r="B10" s="113"/>
       <c r="C10" s="37" t="s">
-        <v>461</v>
+        <v>495</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>462</v>
+        <v>496</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>463</v>
+        <v>497</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38" t="s">
-        <v>464</v>
+        <v>498</v>
       </c>
       <c r="J10" s="37">
         <v>0.0</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>465</v>
+        <v>499</v>
       </c>
       <c r="L10" s="37"/>
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
-        <v>466</v>
-      </c>
-      <c r="B11" s="101" t="s">
-        <v>467</v>
+        <v>500</v>
+      </c>
+      <c r="B11" s="113" t="s">
+        <v>501</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>468</v>
+        <v>502</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>469</v>
+        <v>503</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>470</v>
-      </c>
-      <c r="F11" s="100"/>
+        <v>504</v>
+      </c>
+      <c r="F11" s="112"/>
       <c r="G11" s="37">
         <v>1.0</v>
       </c>
       <c r="H11" s="37"/>
       <c r="I11" s="38" t="s">
-        <v>471</v>
+        <v>505</v>
       </c>
       <c r="J11" s="37">
         <v>1.0</v>
@@ -40590,47 +41080,47 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>472</v>
-      </c>
-      <c r="B12" s="101"/>
+        <v>506</v>
+      </c>
+      <c r="B12" s="113"/>
       <c r="C12" s="37" t="s">
-        <v>473</v>
+        <v>507</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>474</v>
+        <v>508</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>475</v>
+        <v>509</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="J12" s="37">
         <v>0.0</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>477</v>
+        <v>511</v>
       </c>
       <c r="L12" s="37"/>
     </row>
     <row r="13">
       <c r="A13" s="38" t="s">
-        <v>478</v>
-      </c>
-      <c r="B13" s="101">
+        <v>512</v>
+      </c>
+      <c r="B13" s="113">
         <v>22.0</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>479</v>
+        <v>513</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>480</v>
+        <v>514</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>481</v>
+        <v>515</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37">
@@ -40638,35 +41128,35 @@
       </c>
       <c r="H13" s="37"/>
       <c r="I13" s="38" t="s">
-        <v>482</v>
+        <v>516</v>
       </c>
       <c r="J13" s="37">
         <v>1.0</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>483</v>
+        <v>517</v>
       </c>
       <c r="L13" s="37"/>
     </row>
     <row r="14">
       <c r="A14" s="38" t="s">
-        <v>484</v>
-      </c>
-      <c r="B14" s="101"/>
+        <v>518</v>
+      </c>
+      <c r="B14" s="113"/>
       <c r="C14" s="37" t="s">
-        <v>485</v>
+        <v>519</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>486</v>
+        <v>520</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38" t="s">
-        <v>488</v>
+        <v>522</v>
       </c>
       <c r="J14" s="37">
         <v>0.0</v>
@@ -40676,23 +41166,23 @@
     </row>
     <row r="15">
       <c r="A15" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="B15" s="101"/>
+        <v>523</v>
+      </c>
+      <c r="B15" s="113"/>
       <c r="C15" s="37" t="s">
-        <v>490</v>
+        <v>524</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>491</v>
+        <v>525</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>492</v>
+        <v>526</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="38" t="s">
-        <v>493</v>
+        <v>527</v>
       </c>
       <c r="J15" s="37">
         <v>0.0</v>
@@ -40702,105 +41192,105 @@
     </row>
     <row r="16">
       <c r="A16" s="38" t="s">
-        <v>494</v>
-      </c>
-      <c r="B16" s="101"/>
+        <v>528</v>
+      </c>
+      <c r="B16" s="113"/>
       <c r="C16" s="37" t="s">
-        <v>495</v>
+        <v>529</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>496</v>
+        <v>530</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>497</v>
-      </c>
-      <c r="F16" s="93" t="s">
-        <v>498</v>
+        <v>531</v>
+      </c>
+      <c r="F16" s="105" t="s">
+        <v>532</v>
       </c>
       <c r="G16" s="37">
         <v>1.0</v>
       </c>
       <c r="H16" s="37"/>
       <c r="I16" s="38" t="s">
-        <v>499</v>
+        <v>533</v>
       </c>
       <c r="J16" s="37">
         <v>1.0</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>500</v>
+        <v>534</v>
       </c>
       <c r="L16" s="37"/>
     </row>
     <row r="17">
       <c r="A17" s="38" t="s">
-        <v>501</v>
-      </c>
-      <c r="B17" s="101"/>
+        <v>535</v>
+      </c>
+      <c r="B17" s="113"/>
       <c r="C17" s="37" t="s">
-        <v>455</v>
+        <v>489</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>431</v>
+        <v>465</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>502</v>
+        <v>536</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="38" t="s">
-        <v>503</v>
+        <v>537</v>
       </c>
       <c r="J17" s="37">
         <v>1.0</v>
       </c>
       <c r="K17" s="37" t="s">
-        <v>504</v>
+        <v>538</v>
       </c>
       <c r="L17" s="37"/>
     </row>
     <row r="18">
       <c r="A18" s="38" t="s">
-        <v>505</v>
-      </c>
-      <c r="B18" s="101"/>
+        <v>539</v>
+      </c>
+      <c r="B18" s="113"/>
       <c r="C18" s="37" t="s">
-        <v>506</v>
+        <v>540</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>507</v>
+        <v>541</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>508</v>
+        <v>542</v>
       </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="38" t="s">
-        <v>509</v>
+        <v>543</v>
       </c>
       <c r="J18" s="37">
         <v>1.0</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>510</v>
+        <v>544</v>
       </c>
       <c r="L18" s="37"/>
     </row>
     <row r="19">
       <c r="A19" s="38" t="s">
-        <v>511</v>
-      </c>
-      <c r="B19" s="101"/>
+        <v>545</v>
+      </c>
+      <c r="B19" s="113"/>
       <c r="C19" s="37" t="s">
-        <v>512</v>
+        <v>546</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>513</v>
+        <v>547</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>514</v>
+        <v>548</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37">
@@ -40808,7 +41298,7 @@
       </c>
       <c r="H19" s="37"/>
       <c r="I19" s="38" t="s">
-        <v>515</v>
+        <v>549</v>
       </c>
       <c r="J19" s="37">
         <v>1.0</v>
@@ -41836,7 +42326,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -41853,41 +42343,41 @@
     </row>
     <row r="2" ht="49.5" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>516</v>
+        <v>550</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>517</v>
+        <v>551</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>518</v>
+        <v>552</v>
       </c>
       <c r="E2" s="72"/>
-      <c r="F2" s="129">
+      <c r="F2" s="141">
         <v>0.1</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -41896,28 +42386,28 @@
       <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="117" t="s">
+      <c r="K4" s="129" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>519</v>
+        <v>553</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>520</v>
+        <v>554</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>521</v>
+        <v>555</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>522</v>
+        <v>556</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37">
@@ -41925,34 +42415,34 @@
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="38" t="s">
-        <v>523</v>
+        <v>557</v>
       </c>
       <c r="I5" s="37">
         <v>0.0</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>524</v>
+        <v>558</v>
       </c>
       <c r="K5" s="37"/>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>525</v>
+        <v>559</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>526</v>
+        <v>560</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>527</v>
+        <v>561</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>528</v>
+        <v>562</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="38" t="s">
-        <v>529</v>
+        <v>563</v>
       </c>
       <c r="I6" s="37">
         <v>0.0</v>
@@ -41962,49 +42452,49 @@
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
-        <v>530</v>
+        <v>564</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>531</v>
+        <v>565</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>532</v>
+        <v>566</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>533</v>
+        <v>567</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="38" t="s">
-        <v>534</v>
+        <v>568</v>
       </c>
       <c r="I7" s="37">
         <v>0.0</v>
       </c>
-      <c r="J7" s="100" t="s">
-        <v>535</v>
+      <c r="J7" s="112" t="s">
+        <v>569</v>
       </c>
       <c r="K7" s="37"/>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>536</v>
+        <v>570</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>537</v>
+        <v>571</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>538</v>
+        <v>572</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>539</v>
+        <v>573</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>540</v>
+        <v>574</v>
       </c>
       <c r="I8" s="37">
         <v>0.0</v>
@@ -42014,22 +42504,22 @@
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>541</v>
+        <v>575</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>542</v>
+        <v>576</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>543</v>
+        <v>577</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>544</v>
+        <v>578</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="38" t="s">
-        <v>545</v>
+        <v>579</v>
       </c>
       <c r="I9" s="37">
         <v>1.0</v>
@@ -42039,26 +42529,26 @@
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>546</v>
+        <v>580</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>547</v>
+        <v>581</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>548</v>
+        <v>582</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>549</v>
-      </c>
-      <c r="E10" s="112" t="s">
-        <v>222</v>
+        <v>583</v>
+      </c>
+      <c r="E10" s="124" t="s">
+        <v>256</v>
       </c>
       <c r="F10" s="37">
         <v>1.0</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>550</v>
+        <v>584</v>
       </c>
       <c r="I10" s="37">
         <v>1.0</v>
@@ -42068,24 +42558,24 @@
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>551</v>
+        <v>585</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>552</v>
+        <v>586</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>553</v>
+        <v>587</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>554</v>
-      </c>
-      <c r="E11" s="112" t="s">
-        <v>555</v>
+        <v>588</v>
+      </c>
+      <c r="E11" s="124" t="s">
+        <v>589</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="38" t="s">
-        <v>556</v>
+        <v>590</v>
       </c>
       <c r="I11" s="37">
         <v>0.0</v>
@@ -42095,49 +42585,49 @@
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>557</v>
+        <v>591</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>558</v>
+        <v>592</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>559</v>
-      </c>
-      <c r="D12" s="132" t="s">
-        <v>560</v>
+        <v>593</v>
+      </c>
+      <c r="D12" s="144" t="s">
+        <v>594</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>561</v>
+        <v>595</v>
       </c>
       <c r="F12" s="37">
         <v>1.0</v>
       </c>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>562</v>
+        <v>596</v>
       </c>
       <c r="I12" s="37">
         <v>1.0</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>563</v>
+        <v>597</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>564</v>
+        <v>598</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>565</v>
+        <v>599</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>566</v>
+        <v>600</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>567</v>
+        <v>601</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>568</v>
+        <v>602</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37">
@@ -42145,7 +42635,7 @@
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38" t="s">
-        <v>569</v>
+        <v>603</v>
       </c>
       <c r="I13" s="37">
         <v>1.0</v>
@@ -42155,26 +42645,26 @@
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
-        <v>570</v>
+        <v>604</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>571</v>
+        <v>605</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>572</v>
+        <v>606</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>573</v>
+        <v>607</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>574</v>
+        <v>608</v>
       </c>
       <c r="F14" s="37">
         <v>1.0</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="38" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="I14" s="37">
         <v>1.0</v>
@@ -42184,16 +42674,16 @@
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
-        <v>576</v>
+        <v>610</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>577</v>
+        <v>611</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>502</v>
+        <v>536</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37">
@@ -42201,34 +42691,34 @@
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38" t="s">
-        <v>579</v>
+        <v>613</v>
       </c>
       <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="100" t="s">
-        <v>580</v>
+      <c r="J15" s="112" t="s">
+        <v>614</v>
       </c>
       <c r="K15" s="37"/>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>581</v>
+        <v>615</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>583</v>
+        <v>617</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>584</v>
+        <v>618</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="38" t="s">
-        <v>585</v>
+        <v>619</v>
       </c>
       <c r="I16" s="37">
         <v>0.0</v>
@@ -42238,16 +42728,16 @@
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>587</v>
+        <v>621</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>588</v>
+        <v>622</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>589</v>
+        <v>623</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37">
@@ -42255,7 +42745,7 @@
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>590</v>
+        <v>624</v>
       </c>
       <c r="I17" s="37">
         <v>1.0</v>
@@ -42265,26 +42755,26 @@
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>591</v>
+        <v>625</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>592</v>
+        <v>626</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>593</v>
+        <v>627</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>594</v>
+        <v>628</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>595</v>
+        <v>629</v>
       </c>
       <c r="F18" s="37">
         <v>1.0</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="38" t="s">
-        <v>596</v>
+        <v>630</v>
       </c>
       <c r="I18" s="37">
         <v>1.0</v>

</xml_diff>

<commit_message>
NAV-91 Add automatic ADR checks to the ADR milestone (#44)
* NAV-91 Dataset valid check

* NAV-91 Add ADR auto checks

* NAV-91 Fix flake8
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -26,6 +26,13 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="E16">
+      <text>
+        <t xml:space="preserve">@jonathan@fjelltopp.org ADD LINK DIRECTLY TO USER'S ORGANIZATION PAGE / INPUTS PACKAGE FOR THIS YEAR.
+_Assigned to Jonathan Berry_
+	-Jonathan Berry</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="E9">
       <text>
         <t xml:space="preserve">@jonathan@fjelltopp.org ADD LINK DIRECTLY TO USER'S ORGANIZATION PAGE / INPUTS PACKAGE FOR THIS YEAR.
@@ -33,14 +40,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E7">
-      <text>
-        <t xml:space="preserve">@jonathan@fjelltopp.org ADD LINK DIRECTLY TO USER'S ORGANIZATION PAGE / INPUTS PACKAGE FOR THIS YEAR.
-_Assigned to Jonathan Berry_
-	-Jonathan Berry</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="D8">
+    <comment authorId="0" ref="D15">
       <text>
         <t xml:space="preserve">Unaids to add justification for why uploading data is important.
 	-Jonathan Berry</t>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="631">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -704,6 +704,54 @@
     <t>check_manual_confirmation('EST-ADR-03-A')</t>
   </si>
   <si>
+    <t>ADR-03A</t>
+  </si>
+  <si>
+    <t>Upload your Shiny 90 Survey template to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a Shiny90 survey testing template?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your Shiny90 survey file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your Shiny90 Survey template to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Shiny90 Survey Data" and click *Add Data*
+- Drag your Shiny90 template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-shiny90-survey', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-03B</t>
+  </si>
+  <si>
+    <t>Upload your Shiny 90 HIV Testing template to ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a Shiny90 HIV Testing template?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your Shiny90 HIV Testing template to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your Shiny90 HIV Testing template to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Shiny90 Survey Data" and click *Add Data*
+- Drag your Shiny90 template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-hiv-testing', 'url', '.*')</t>
+  </si>
+  <si>
     <t>ADR-04</t>
   </si>
   <si>
@@ -740,6 +788,126 @@
     <t>check_manual_confirmation('EST-ADR-04-A')</t>
   </si>
   <si>
+    <t>ADR-04A</t>
+  </si>
+  <si>
+    <t>Upload your area boundaries data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a Geographic data file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your Geographic area boundaries file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your  Geographic area boundaries data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Geographic Data" and click *Add Data*
+- Drag your Geographic areas boundaries file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-geographic', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04B</t>
+  </si>
+  <si>
+    <t>Upload your population data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a population template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your population template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your population data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Population Data" and click *Add Data*
+- Drag your population template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-population', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04C</t>
+  </si>
+  <si>
+    <t>Upload your Naomi survey data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded a survey template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your survey template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your  Naomi survey data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "Survey Data" and click *Add Data*
+- Drag your Naomi survey template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-survey', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04D</t>
+  </si>
+  <si>
+    <t>Upload your ART data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded an ART template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your ART template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your  ART data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "ART Data" and click *Add Data*
+- Drag your ART template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-art', 'url', '.*')</t>
+  </si>
+  <si>
+    <t>ADR-04E</t>
+  </si>
+  <si>
+    <t>Upload your ANC survey data to the ADR</t>
+  </si>
+  <si>
+    <t>Has the user uploaded an  ANC template file?</t>
+  </si>
+  <si>
+    <t>It looks like you have not uploaded your ANC template file to the ADR.
+UNAIDS strongly recommends the use of the AIDS Data Repository (ADR) to store your estimates data, both inputs and outputs. Using ADR provides a number of advantages and efficiencies for your estimates process, including a secure location to store your data files as well as automated validation function to ensure your data meet formatting and minimum data quality requirements before beginning the data. Access your organization on ADR and find this year's inputs package. Upload each of the required files for this year's estimates process in the required format.
+**To upload your ANC data to the ADR:**
+- Open your estimates 2022 dataset in the ADR
+- Under *Missing Resources* find "ANC Data" and click *Add Data*
+- Drag your ANC template file into the file upload zone
+- Add any useful notes about the file under *Description* 
+- Confirm the format field is correct
+- If you wish to share the file with someone outside your organisation you can do so under *Access Restriction* 
+- Click "Add" to upload the file</t>
+  </si>
+  <si>
+    <t>check_resource_key('inputs-unaids-anc', 'url', '.*')</t>
+  </si>
+  <si>
     <t>ADR-05</t>
   </si>
   <si>
@@ -789,7 +957,7 @@
     </r>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-ADR-06-A')</t>
+    <t>check_dataset_valid()</t>
   </si>
   <si>
     <t>Review quality of programme data inputs in ShinyRob</t>
@@ -842,7 +1010,7 @@
     <t>@UNAIDS - I've tagged everything here as mandatory right now. This means the user will not be able to proceed to Spectrum data entry until this process is complete. Are we okay with that order of operations to help avoid data quality problems downstream?</t>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-ROB-01-A')</t>
+    <t>check_not_skipped(['EST-ADR-04-A', 'EST-ADR-04A-A', 'EST-ADR-04B-A', 'EST-ADR-04C-A', 'EST-ADR-04D-A', 'EST-ADR-04E-A', 'EST-ADR-06-A'])</t>
   </si>
   <si>
     <t>ROB-02</t>
@@ -871,9 +1039,6 @@
   </si>
   <si>
     <t>not a user-facing task check; required to import data from ADR</t>
-  </si>
-  <si>
-    <t>check_not_skipped(['EST-ADR-04-A', 'EST-ADR-06-A'])</t>
   </si>
   <si>
     <t>ROB-03</t>
@@ -2827,7 +2992,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2838,6 +3003,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6D7A8"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -2856,12 +3033,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD8D8D8"/>
         <bgColor rgb="FFD8D8D8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -2992,7 +3163,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="145">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3184,6 +3355,35 @@
     <xf borderId="5" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="6" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="5" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="5" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3191,21 +3391,24 @@
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf borderId="9" fillId="3" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="5" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3214,7 +3417,7 @@
     <xf borderId="1" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3224,11 +3427,11 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="4" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="6" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3238,43 +3441,43 @@
     <xf borderId="1" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="10" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="10" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="9" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="9" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="3" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="11" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3288,13 +3491,13 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="8" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -3302,7 +3505,7 @@
     <xf borderId="2" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
@@ -32630,7 +32833,7 @@
     <col customWidth="1" min="2" max="2" width="24.29"/>
     <col customWidth="1" min="3" max="3" width="34.57"/>
     <col customWidth="1" min="4" max="4" width="43.14"/>
-    <col customWidth="1" min="5" max="5" width="69.86"/>
+    <col customWidth="1" min="5" max="5" width="41.57"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
     <col customWidth="1" hidden="1" min="7" max="7" width="37.29"/>
     <col customWidth="1" hidden="1" min="8" max="8" width="26.86"/>
@@ -34364,108 +34567,395 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="76" t="s">
+    <row r="7" ht="87.0" customHeight="1">
+      <c r="A7" s="79" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="80" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="80" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="60" t="s">
+      <c r="D7" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="78">
+      <c r="E7" s="81"/>
+      <c r="F7" s="82">
         <v>0.0</v>
       </c>
-      <c r="G7" s="77">
+      <c r="G7" s="83"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="86" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" s="87"/>
+      <c r="M7" s="87"/>
+      <c r="N7" s="87"/>
+      <c r="O7" s="87"/>
+      <c r="P7" s="87"/>
+      <c r="Q7" s="87"/>
+      <c r="R7" s="87"/>
+      <c r="S7" s="87"/>
+      <c r="T7" s="87"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="87"/>
+      <c r="W7" s="87"/>
+      <c r="X7" s="87"/>
+      <c r="Y7" s="87"/>
+      <c r="Z7" s="87"/>
+      <c r="AA7" s="87"/>
+    </row>
+    <row r="8" ht="87.0" customHeight="1">
+      <c r="A8" s="79" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="80" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="80" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="80" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="81"/>
+      <c r="F8" s="82">
         <v>0.0</v>
       </c>
-      <c r="H7" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="58"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="76" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>135</v>
-      </c>
-      <c r="D8" s="59" t="s">
+      <c r="G8" s="83"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85" t="s">
         <v>136</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="78">
-        <v>0.0</v>
-      </c>
-      <c r="G8" s="77">
-        <v>0.0</v>
-      </c>
-      <c r="H8" s="79" t="s">
-        <v>137</v>
-      </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="80"/>
-      <c r="P8" s="80"/>
-      <c r="Q8" s="80"/>
-      <c r="R8" s="80"/>
-      <c r="S8" s="80"/>
-      <c r="T8" s="80"/>
-      <c r="U8" s="80"/>
-      <c r="V8" s="80"/>
-      <c r="W8" s="80"/>
-      <c r="X8" s="80"/>
-      <c r="Y8" s="80"/>
-      <c r="Z8" s="80"/>
+      <c r="L8" s="87"/>
+      <c r="M8" s="87"/>
+      <c r="N8" s="87"/>
+      <c r="O8" s="87"/>
+      <c r="P8" s="87"/>
+      <c r="Q8" s="87"/>
+      <c r="R8" s="87"/>
+      <c r="S8" s="87"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="87"/>
+      <c r="V8" s="87"/>
+      <c r="W8" s="87"/>
+      <c r="X8" s="87"/>
+      <c r="Y8" s="87"/>
+      <c r="Z8" s="87"/>
+      <c r="AA8" s="87"/>
     </row>
     <row r="9">
       <c r="A9" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="58" t="s">
+      <c r="D9" s="58" t="s">
+        <v>124</v>
+      </c>
+      <c r="E9" s="60" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="F9" s="78">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="77">
+        <v>0.0</v>
+      </c>
+      <c r="H9" s="58" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="58" t="s">
-        <v>142</v>
-      </c>
-      <c r="E9" s="60" t="s">
-        <v>143</v>
-      </c>
-      <c r="F9" s="59">
-        <v>0.0</v>
-      </c>
-      <c r="G9" s="58">
-        <v>0.0</v>
-      </c>
-      <c r="H9" s="58"/>
       <c r="I9" s="58"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="80" t="s">
         <v>144</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="88"/>
+      <c r="F10" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="83"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="85"/>
+      <c r="K10" s="85" t="s">
+        <v>147</v>
+      </c>
+      <c r="L10" s="89"/>
+      <c r="M10" s="89"/>
+      <c r="N10" s="89"/>
+      <c r="O10" s="89"/>
+      <c r="P10" s="89"/>
+      <c r="Q10" s="89"/>
+      <c r="R10" s="89"/>
+      <c r="S10" s="89"/>
+      <c r="T10" s="89"/>
+      <c r="U10" s="89"/>
+      <c r="V10" s="89"/>
+      <c r="W10" s="89"/>
+      <c r="X10" s="89"/>
+      <c r="Y10" s="89"/>
+      <c r="Z10" s="89"/>
+      <c r="AA10" s="89"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="80" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="80" t="s">
+        <v>150</v>
+      </c>
+      <c r="D11" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="E11" s="88"/>
+      <c r="F11" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="83"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85" t="s">
+        <v>152</v>
+      </c>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="89"/>
+      <c r="Q11" s="89"/>
+      <c r="R11" s="89"/>
+      <c r="S11" s="89"/>
+      <c r="T11" s="89"/>
+      <c r="U11" s="89"/>
+      <c r="V11" s="89"/>
+      <c r="W11" s="89"/>
+      <c r="X11" s="89"/>
+      <c r="Y11" s="89"/>
+      <c r="Z11" s="89"/>
+      <c r="AA11" s="89"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="79" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" s="80" t="s">
+        <v>154</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12" s="80" t="s">
+        <v>156</v>
+      </c>
+      <c r="E12" s="88"/>
+      <c r="F12" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="83"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="85"/>
+      <c r="K12" s="85" t="s">
+        <v>157</v>
+      </c>
+      <c r="L12" s="89"/>
+      <c r="M12" s="89"/>
+      <c r="N12" s="89"/>
+      <c r="O12" s="89"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
+      <c r="R12" s="89"/>
+      <c r="S12" s="89"/>
+      <c r="T12" s="89"/>
+      <c r="U12" s="89"/>
+      <c r="V12" s="89"/>
+      <c r="W12" s="89"/>
+      <c r="X12" s="89"/>
+      <c r="Y12" s="89"/>
+      <c r="Z12" s="89"/>
+      <c r="AA12" s="89"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="79" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="80" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="80" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="88"/>
+      <c r="F13" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="83"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85" t="s">
+        <v>162</v>
+      </c>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="89"/>
+      <c r="O13" s="89"/>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
+      <c r="R13" s="89"/>
+      <c r="S13" s="89"/>
+      <c r="T13" s="89"/>
+      <c r="U13" s="89"/>
+      <c r="V13" s="89"/>
+      <c r="W13" s="89"/>
+      <c r="X13" s="89"/>
+      <c r="Y13" s="89"/>
+      <c r="Z13" s="89"/>
+      <c r="AA13" s="89"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="79" t="s">
+        <v>163</v>
+      </c>
+      <c r="B14" s="80" t="s">
+        <v>164</v>
+      </c>
+      <c r="C14" s="80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D14" s="80" t="s">
+        <v>166</v>
+      </c>
+      <c r="E14" s="88"/>
+      <c r="F14" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="83"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85" t="s">
+        <v>167</v>
+      </c>
+      <c r="L14" s="89"/>
+      <c r="M14" s="89"/>
+      <c r="N14" s="89"/>
+      <c r="O14" s="89"/>
+      <c r="P14" s="89"/>
+      <c r="Q14" s="89"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="89"/>
+      <c r="T14" s="89"/>
+      <c r="U14" s="89"/>
+      <c r="V14" s="89"/>
+      <c r="W14" s="89"/>
+      <c r="X14" s="89"/>
+      <c r="Y14" s="89"/>
+      <c r="Z14" s="89"/>
+      <c r="AA14" s="89"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C15" s="58" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="58"/>
+      <c r="F15" s="78">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="77">
+        <v>0.0</v>
+      </c>
+      <c r="H15" s="90" t="s">
+        <v>172</v>
+      </c>
+      <c r="I15" s="58"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+      <c r="R15" s="91"/>
+      <c r="S15" s="91"/>
+      <c r="T15" s="91"/>
+      <c r="U15" s="91"/>
+      <c r="V15" s="91"/>
+      <c r="W15" s="91"/>
+      <c r="X15" s="91"/>
+      <c r="Y15" s="91"/>
+      <c r="Z15" s="91"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="76" t="s">
+        <v>174</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="F16" s="59">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="58">
+        <v>0.0</v>
+      </c>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -34475,8 +34965,8 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="E5"/>
-    <hyperlink r:id="rId3" ref="E7"/>
-    <hyperlink r:id="rId4" ref="E9"/>
+    <hyperlink r:id="rId3" ref="E9"/>
+    <hyperlink r:id="rId4" ref="E16"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -34510,7 +35000,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -34527,14 +35017,14 @@
     </row>
     <row r="2" ht="48.0" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -34585,16 +35075,16 @@
     </row>
     <row r="5">
       <c r="A5" s="58" t="s">
-        <v>148</v>
+        <v>183</v>
       </c>
       <c r="B5" s="58" t="s">
-        <v>149</v>
+        <v>184</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="E5" s="59" t="s">
         <v>82</v>
@@ -34605,29 +35095,29 @@
       <c r="G5" s="61">
         <v>0.0</v>
       </c>
-      <c r="H5" s="79" t="s">
-        <v>152</v>
+      <c r="H5" s="90" t="s">
+        <v>187</v>
       </c>
       <c r="I5" s="38"/>
-      <c r="J5" s="38" t="s">
-        <v>153</v>
+      <c r="J5" s="93" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="58" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="B6" s="58" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="D6" s="58" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="F6" s="61">
         <v>1.0</v>
@@ -34638,48 +35128,48 @@
       <c r="H6" s="63"/>
       <c r="I6" s="38"/>
       <c r="J6" s="38" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="82" t="s">
-        <v>160</v>
-      </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82" t="s">
-        <v>161</v>
-      </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83">
+      <c r="A7" s="94" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="95">
         <v>1.0</v>
       </c>
-      <c r="G7" s="83">
+      <c r="G7" s="95">
         <v>1.0</v>
       </c>
-      <c r="H7" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85" t="s">
-        <v>163</v>
+      <c r="H7" s="96" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="58" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="E8" s="59" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="F8" s="61">
         <v>1.0</v>
@@ -34690,24 +35180,24 @@
       <c r="H8" s="63"/>
       <c r="I8" s="38"/>
       <c r="J8" s="38" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="58" t="s">
-        <v>170</v>
+        <v>204</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>171</v>
+        <v>205</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>172</v>
+        <v>206</v>
       </c>
       <c r="D9" s="58" t="s">
-        <v>173</v>
+        <v>207</v>
       </c>
       <c r="E9" s="59" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
       <c r="F9" s="63">
         <v>1.0</v>
@@ -34718,21 +35208,21 @@
       <c r="H9" s="63"/>
       <c r="I9" s="28"/>
       <c r="J9" s="38" t="s">
-        <v>174</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="58" t="s">
-        <v>175</v>
+        <v>209</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>176</v>
+        <v>210</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>177</v>
+        <v>211</v>
       </c>
       <c r="D10" s="58" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
       <c r="E10" s="58"/>
       <c r="F10" s="61">
@@ -34742,9 +35232,9 @@
         <v>0.0</v>
       </c>
       <c r="H10" s="58"/>
-      <c r="I10" s="86"/>
+      <c r="I10" s="98"/>
       <c r="J10" s="38" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -35853,7 +36343,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -35870,14 +36360,14 @@
     </row>
     <row r="2">
       <c r="A2" s="44" t="s">
-        <v>180</v>
+        <v>214</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -35886,31 +36376,31 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="88" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="87" t="s">
+      <c r="B4" s="100" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="101" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="87" t="s">
+      <c r="H4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="99" t="s">
         <v>17</v>
       </c>
       <c r="J4" s="52" t="s">
@@ -35925,48 +36415,48 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="91"/>
+        <v>218</v>
+      </c>
+      <c r="B5" s="103"/>
       <c r="C5" s="37" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E5" s="92" t="s">
-        <v>187</v>
-      </c>
-      <c r="F5" s="93" t="s">
-        <v>188</v>
+        <v>220</v>
+      </c>
+      <c r="E5" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" s="105" t="s">
+        <v>222</v>
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="37">
         <v>1.0</v>
       </c>
-      <c r="I5" s="86"/>
+      <c r="I5" s="98"/>
       <c r="J5" s="58"/>
-      <c r="K5" s="94" t="s">
-        <v>189</v>
+      <c r="K5" s="106" t="s">
+        <v>223</v>
       </c>
       <c r="L5" s="38"/>
       <c r="M5" s="38" t="s">
-        <v>190</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="B6" s="95"/>
+        <v>225</v>
+      </c>
+      <c r="B6" s="107"/>
       <c r="C6" s="37" t="s">
-        <v>192</v>
+        <v>226</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="E6" s="96" t="s">
-        <v>194</v>
+        <v>227</v>
+      </c>
+      <c r="E6" s="108" t="s">
+        <v>228</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37">
@@ -35976,34 +36466,34 @@
         <v>1.0</v>
       </c>
       <c r="I6" s="37" t="s">
-        <v>195</v>
+        <v>229</v>
       </c>
       <c r="J6" s="58" t="s">
-        <v>196</v>
-      </c>
-      <c r="K6" s="94" t="s">
-        <v>197</v>
+        <v>230</v>
+      </c>
+      <c r="K6" s="106" t="s">
+        <v>231</v>
       </c>
       <c r="L6" s="38"/>
       <c r="M6" s="38" t="s">
-        <v>198</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="91" t="s">
-        <v>200</v>
+        <v>233</v>
+      </c>
+      <c r="B7" s="103" t="s">
+        <v>234</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>201</v>
+        <v>235</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="96" t="s">
-        <v>203</v>
+        <v>236</v>
+      </c>
+      <c r="E7" s="108" t="s">
+        <v>237</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
@@ -36011,32 +36501,32 @@
         <v>1.0</v>
       </c>
       <c r="I7" s="37" t="s">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="J7" s="58"/>
       <c r="L7" s="38"/>
       <c r="M7" s="38" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="B8" s="97">
+        <v>240</v>
+      </c>
+      <c r="B8" s="109">
         <v>1.0</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>207</v>
+        <v>241</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="E8" s="92" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" s="93" t="s">
-        <v>210</v>
+        <v>242</v>
+      </c>
+      <c r="E8" s="104" t="s">
+        <v>243</v>
+      </c>
+      <c r="F8" s="105" t="s">
+        <v>244</v>
       </c>
       <c r="G8" s="37"/>
       <c r="H8" s="37">
@@ -36046,170 +36536,170 @@
       <c r="J8" s="58"/>
       <c r="L8" s="38"/>
       <c r="M8" s="38" t="s">
-        <v>211</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>212</v>
-      </c>
-      <c r="B9" s="95"/>
+        <v>246</v>
+      </c>
+      <c r="B9" s="107"/>
       <c r="C9" s="37" t="s">
-        <v>213</v>
+        <v>247</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>214</v>
-      </c>
-      <c r="E9" s="92" t="s">
-        <v>215</v>
-      </c>
-      <c r="F9" s="98"/>
+        <v>248</v>
+      </c>
+      <c r="E9" s="104" t="s">
+        <v>249</v>
+      </c>
+      <c r="F9" s="110"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37">
         <v>0.0</v>
       </c>
-      <c r="I9" s="99" t="s">
-        <v>216</v>
+      <c r="I9" s="111" t="s">
+        <v>250</v>
       </c>
       <c r="J9" s="58"/>
       <c r="L9" s="28"/>
       <c r="M9" s="38" t="s">
-        <v>217</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="B10" s="95"/>
+        <v>252</v>
+      </c>
+      <c r="B10" s="107"/>
       <c r="C10" s="37" t="s">
-        <v>219</v>
+        <v>253</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="E10" s="92" t="s">
-        <v>221</v>
+        <v>254</v>
+      </c>
+      <c r="E10" s="104" t="s">
+        <v>255</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="37">
         <v>1.0</v>
       </c>
-      <c r="I10" s="100"/>
+      <c r="I10" s="112"/>
       <c r="J10" s="58"/>
-      <c r="L10" s="86"/>
+      <c r="L10" s="98"/>
       <c r="M10" s="38" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>224</v>
-      </c>
-      <c r="B11" s="97" t="s">
-        <v>225</v>
+        <v>258</v>
+      </c>
+      <c r="B11" s="109" t="s">
+        <v>259</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>226</v>
+        <v>260</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" s="92" t="s">
-        <v>228</v>
+        <v>261</v>
+      </c>
+      <c r="E11" s="104" t="s">
+        <v>262</v>
       </c>
       <c r="F11" s="38" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="G11" s="37"/>
       <c r="H11" s="37">
         <v>1.0</v>
       </c>
-      <c r="I11" s="99" t="s">
-        <v>229</v>
+      <c r="I11" s="111" t="s">
+        <v>263</v>
       </c>
       <c r="J11" s="58" t="s">
-        <v>230</v>
+        <v>264</v>
       </c>
       <c r="L11" s="38"/>
       <c r="M11" s="38" t="s">
-        <v>231</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>232</v>
-      </c>
-      <c r="B12" s="97"/>
+        <v>266</v>
+      </c>
+      <c r="B12" s="109"/>
       <c r="C12" s="37" t="s">
-        <v>233</v>
+        <v>267</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E12" s="92" t="s">
-        <v>235</v>
+        <v>268</v>
+      </c>
+      <c r="E12" s="104" t="s">
+        <v>269</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37">
         <v>0.0</v>
       </c>
-      <c r="I12" s="99" t="s">
-        <v>236</v>
+      <c r="I12" s="111" t="s">
+        <v>270</v>
       </c>
       <c r="J12" s="58"/>
       <c r="L12" s="38"/>
       <c r="M12" s="38" t="s">
-        <v>237</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="B13" s="97">
+        <v>272</v>
+      </c>
+      <c r="B13" s="109">
         <v>2.0</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>240</v>
-      </c>
-      <c r="E13" s="92" t="s">
-        <v>241</v>
+        <v>274</v>
+      </c>
+      <c r="E13" s="104" t="s">
+        <v>275</v>
       </c>
       <c r="F13" s="38" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="37">
         <v>1.0</v>
       </c>
-      <c r="I13" s="99"/>
+      <c r="I13" s="111"/>
       <c r="J13" s="58"/>
       <c r="L13" s="38"/>
       <c r="M13" s="38" t="s">
-        <v>242</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
-        <v>243</v>
-      </c>
-      <c r="B14" s="101"/>
+        <v>277</v>
+      </c>
+      <c r="B14" s="113"/>
       <c r="C14" s="37" t="s">
-        <v>244</v>
+        <v>278</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>245</v>
+        <v>279</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>246</v>
+        <v>280</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
@@ -36217,253 +36707,253 @@
         <v>1.0</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>247</v>
+        <v>281</v>
       </c>
       <c r="J14" s="37"/>
-      <c r="K14" s="102" t="s">
-        <v>248</v>
+      <c r="K14" s="114" t="s">
+        <v>282</v>
       </c>
       <c r="L14" s="38"/>
       <c r="M14" s="38" t="s">
-        <v>249</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="103" t="s">
-        <v>250</v>
-      </c>
-      <c r="B15" s="104"/>
-      <c r="C15" s="103"/>
-      <c r="D15" s="103" t="s">
-        <v>251</v>
-      </c>
-      <c r="E15" s="105"/>
-      <c r="F15" s="103"/>
-      <c r="G15" s="103">
+      <c r="A15" s="115" t="s">
+        <v>284</v>
+      </c>
+      <c r="B15" s="116"/>
+      <c r="C15" s="115"/>
+      <c r="D15" s="115" t="s">
+        <v>285</v>
+      </c>
+      <c r="E15" s="117"/>
+      <c r="F15" s="115"/>
+      <c r="G15" s="115">
         <v>1.0</v>
       </c>
-      <c r="H15" s="103"/>
-      <c r="I15" s="106" t="s">
-        <v>252</v>
-      </c>
-      <c r="J15" s="82"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="118" t="s">
+        <v>286</v>
+      </c>
+      <c r="J15" s="94"/>
       <c r="L15" s="28"/>
-      <c r="M15" s="85" t="s">
-        <v>253</v>
+      <c r="M15" s="97" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>254</v>
-      </c>
-      <c r="B16" s="97" t="s">
-        <v>255</v>
-      </c>
-      <c r="C16" s="107" t="s">
-        <v>256</v>
-      </c>
-      <c r="D16" s="107" t="s">
-        <v>257</v>
-      </c>
-      <c r="E16" s="108" t="s">
-        <v>258</v>
-      </c>
-      <c r="F16" s="109" t="s">
-        <v>259</v>
-      </c>
-      <c r="G16" s="107"/>
-      <c r="H16" s="107">
+        <v>288</v>
+      </c>
+      <c r="B16" s="109" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" s="119" t="s">
+        <v>290</v>
+      </c>
+      <c r="D16" s="119" t="s">
+        <v>291</v>
+      </c>
+      <c r="E16" s="120" t="s">
+        <v>292</v>
+      </c>
+      <c r="F16" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119">
         <v>1.0</v>
       </c>
-      <c r="I16" s="110" t="s">
-        <v>260</v>
-      </c>
-      <c r="J16" s="111" t="s">
-        <v>261</v>
+      <c r="I16" s="122" t="s">
+        <v>294</v>
+      </c>
+      <c r="J16" s="123" t="s">
+        <v>295</v>
       </c>
       <c r="L16" s="38"/>
       <c r="M16" s="38" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
-        <v>263</v>
-      </c>
-      <c r="B17" s="95" t="s">
-        <v>264</v>
-      </c>
-      <c r="C17" s="107" t="s">
-        <v>265</v>
-      </c>
-      <c r="D17" s="107" t="s">
-        <v>266</v>
-      </c>
-      <c r="E17" s="108" t="s">
-        <v>267</v>
-      </c>
-      <c r="F17" s="109" t="s">
-        <v>259</v>
-      </c>
-      <c r="G17" s="107"/>
-      <c r="H17" s="107">
+        <v>297</v>
+      </c>
+      <c r="B17" s="107" t="s">
+        <v>298</v>
+      </c>
+      <c r="C17" s="119" t="s">
+        <v>299</v>
+      </c>
+      <c r="D17" s="119" t="s">
+        <v>300</v>
+      </c>
+      <c r="E17" s="120" t="s">
+        <v>301</v>
+      </c>
+      <c r="F17" s="121" t="s">
+        <v>293</v>
+      </c>
+      <c r="G17" s="119"/>
+      <c r="H17" s="119">
         <v>1.0</v>
       </c>
-      <c r="I17" s="110" t="s">
-        <v>268</v>
-      </c>
-      <c r="J17" s="111" t="s">
-        <v>269</v>
+      <c r="I17" s="122" t="s">
+        <v>302</v>
+      </c>
+      <c r="J17" s="123" t="s">
+        <v>303</v>
       </c>
       <c r="L17" s="38"/>
       <c r="M17" s="38" t="s">
-        <v>270</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>271</v>
-      </c>
-      <c r="B18" s="95" t="s">
-        <v>272</v>
+        <v>305</v>
+      </c>
+      <c r="B18" s="107" t="s">
+        <v>306</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>273</v>
+        <v>307</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>274</v>
-      </c>
-      <c r="E18" s="92" t="s">
-        <v>275</v>
-      </c>
-      <c r="F18" s="112" t="s">
-        <v>259</v>
+        <v>308</v>
+      </c>
+      <c r="E18" s="104" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="124" t="s">
+        <v>293</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="37">
         <v>1.0</v>
       </c>
-      <c r="I18" s="100"/>
+      <c r="I18" s="112"/>
       <c r="J18" s="58"/>
       <c r="L18" s="38"/>
       <c r="M18" s="38" t="s">
-        <v>276</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="37" t="s">
-        <v>277</v>
-      </c>
-      <c r="B19" s="95">
+        <v>311</v>
+      </c>
+      <c r="B19" s="107">
         <v>19.0</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>278</v>
+        <v>312</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>279</v>
-      </c>
-      <c r="E19" s="92" t="s">
-        <v>280</v>
-      </c>
-      <c r="F19" s="112" t="s">
-        <v>281</v>
+        <v>313</v>
+      </c>
+      <c r="E19" s="104" t="s">
+        <v>314</v>
+      </c>
+      <c r="F19" s="124" t="s">
+        <v>315</v>
       </c>
       <c r="G19" s="37"/>
       <c r="H19" s="37">
         <v>1.0</v>
       </c>
-      <c r="I19" s="100"/>
+      <c r="I19" s="112"/>
       <c r="J19" s="58"/>
       <c r="L19" s="38"/>
       <c r="M19" s="38" t="s">
-        <v>282</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="37" t="s">
-        <v>283</v>
-      </c>
-      <c r="B20" s="95">
+        <v>317</v>
+      </c>
+      <c r="B20" s="107">
         <v>20.0</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>284</v>
+        <v>318</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>285</v>
-      </c>
-      <c r="E20" s="92" t="s">
-        <v>286</v>
-      </c>
-      <c r="F20" s="112" t="s">
-        <v>259</v>
+        <v>319</v>
+      </c>
+      <c r="E20" s="104" t="s">
+        <v>320</v>
+      </c>
+      <c r="F20" s="124" t="s">
+        <v>293</v>
       </c>
       <c r="G20" s="37"/>
       <c r="H20" s="37">
         <v>1.0</v>
       </c>
-      <c r="I20" s="100" t="s">
-        <v>287</v>
+      <c r="I20" s="112" t="s">
+        <v>321</v>
       </c>
       <c r="J20" s="58"/>
       <c r="L20" s="28"/>
       <c r="M20" s="38" t="s">
-        <v>288</v>
+        <v>322</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="103" t="s">
-        <v>289</v>
-      </c>
-      <c r="B21" s="113"/>
-      <c r="C21" s="103"/>
-      <c r="D21" s="103" t="s">
-        <v>290</v>
-      </c>
-      <c r="E21" s="105"/>
-      <c r="F21" s="114"/>
-      <c r="G21" s="115">
+      <c r="A21" s="115" t="s">
+        <v>323</v>
+      </c>
+      <c r="B21" s="125"/>
+      <c r="C21" s="115"/>
+      <c r="D21" s="115" t="s">
+        <v>324</v>
+      </c>
+      <c r="E21" s="117"/>
+      <c r="F21" s="126"/>
+      <c r="G21" s="127">
         <v>1.0</v>
       </c>
-      <c r="H21" s="115"/>
-      <c r="I21" s="106" t="s">
-        <v>291</v>
-      </c>
-      <c r="J21" s="82"/>
+      <c r="H21" s="127"/>
+      <c r="I21" s="118" t="s">
+        <v>325</v>
+      </c>
+      <c r="J21" s="94"/>
       <c r="L21" s="38"/>
-      <c r="M21" s="85" t="s">
-        <v>292</v>
+      <c r="M21" s="97" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>293</v>
-      </c>
-      <c r="B22" s="95" t="s">
-        <v>294</v>
+        <v>327</v>
+      </c>
+      <c r="B22" s="107" t="s">
+        <v>328</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>295</v>
+        <v>329</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>296</v>
+        <v>330</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>297</v>
-      </c>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116">
+        <v>331</v>
+      </c>
+      <c r="F22" s="128"/>
+      <c r="G22" s="128"/>
+      <c r="H22" s="128">
         <v>1.0</v>
       </c>
-      <c r="I22" s="79" t="s">
-        <v>298</v>
+      <c r="I22" s="90" t="s">
+        <v>332</v>
       </c>
       <c r="J22" s="58"/>
       <c r="L22" s="28"/>
       <c r="M22" s="38" t="s">
-        <v>299</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -37541,7 +38031,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -37558,14 +38048,14 @@
     </row>
     <row r="2" ht="84.0" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>300</v>
+        <v>334</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>301</v>
+        <v>335</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>302</v>
+        <v>336</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -37574,31 +38064,31 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="87" t="s">
-        <v>303</v>
-      </c>
-      <c r="I4" s="117" t="s">
+      <c r="H4" s="99" t="s">
+        <v>337</v>
+      </c>
+      <c r="I4" s="129" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="17" t="s">
@@ -37610,97 +38100,97 @@
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>305</v>
+        <v>339</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>306</v>
+        <v>340</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>307</v>
+        <v>341</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37">
         <v>0.0</v>
       </c>
-      <c r="H5" s="92" t="s">
-        <v>308</v>
-      </c>
-      <c r="I5" s="99"/>
+      <c r="H5" s="104" t="s">
+        <v>342</v>
+      </c>
+      <c r="I5" s="111"/>
       <c r="J5" s="38"/>
       <c r="K5" s="38" t="s">
-        <v>309</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>310</v>
+        <v>344</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>311</v>
+        <v>345</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>312</v>
+        <v>346</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>313</v>
+        <v>347</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37">
         <v>1.0</v>
       </c>
-      <c r="H6" s="92" t="s">
-        <v>314</v>
+      <c r="H6" s="104" t="s">
+        <v>348</v>
       </c>
       <c r="I6" s="37"/>
       <c r="J6" s="38"/>
       <c r="K6" s="38" t="s">
-        <v>315</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
-        <v>316</v>
+        <v>350</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>317</v>
+        <v>351</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>318</v>
+        <v>352</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>319</v>
+        <v>353</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37">
         <v>1.0</v>
       </c>
-      <c r="H7" s="92" t="s">
-        <v>314</v>
+      <c r="H7" s="104" t="s">
+        <v>348</v>
       </c>
       <c r="I7" s="37"/>
       <c r="J7" s="38"/>
       <c r="K7" s="38" t="s">
-        <v>320</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>321</v>
+        <v>355</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>323</v>
+        <v>357</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>324</v>
+        <v>358</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37">
@@ -37709,28 +38199,28 @@
       <c r="G8" s="37">
         <v>1.0</v>
       </c>
-      <c r="H8" s="92"/>
+      <c r="H8" s="104"/>
       <c r="I8" s="37"/>
       <c r="J8" s="38"/>
       <c r="K8" s="38" t="s">
-        <v>325</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>326</v>
+        <v>360</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>327</v>
+        <v>361</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>328</v>
+        <v>362</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>329</v>
-      </c>
-      <c r="E9" s="118" t="s">
-        <v>330</v>
+        <v>363</v>
+      </c>
+      <c r="E9" s="130" t="s">
+        <v>364</v>
       </c>
       <c r="F9" s="37">
         <v>1.0</v>
@@ -37738,54 +38228,54 @@
       <c r="G9" s="37">
         <v>1.0</v>
       </c>
-      <c r="H9" s="92"/>
+      <c r="H9" s="104"/>
       <c r="I9" s="37" t="s">
-        <v>331</v>
+        <v>365</v>
       </c>
       <c r="J9" s="28"/>
       <c r="K9" s="38" t="s">
-        <v>332</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>333</v>
+        <v>367</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>334</v>
+        <v>368</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>335</v>
+        <v>369</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>336</v>
+        <v>370</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37">
         <v>1.0</v>
       </c>
-      <c r="H10" s="119" t="s">
-        <v>337</v>
+      <c r="H10" s="131" t="s">
+        <v>371</v>
       </c>
       <c r="I10" s="37"/>
-      <c r="J10" s="86"/>
+      <c r="J10" s="98"/>
       <c r="K10" s="38" t="s">
-        <v>338</v>
+        <v>372</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>339</v>
+        <v>373</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>340</v>
+        <v>374</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>341</v>
+        <v>375</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>342</v>
+        <v>376</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37">
@@ -37795,31 +38285,31 @@
         <v>1.0</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="I11" s="37" t="s">
-        <v>344</v>
+        <v>378</v>
       </c>
       <c r="J11" s="38"/>
       <c r="K11" s="38" t="s">
-        <v>345</v>
-      </c>
-      <c r="L11" s="80"/>
-      <c r="M11" s="80"/>
-      <c r="N11" s="80"/>
-      <c r="O11" s="80"/>
-      <c r="P11" s="80"/>
-      <c r="Q11" s="80"/>
-      <c r="R11" s="80"/>
-      <c r="S11" s="80"/>
-      <c r="T11" s="80"/>
-      <c r="U11" s="80"/>
-      <c r="V11" s="80"/>
-      <c r="W11" s="80"/>
-      <c r="X11" s="80"/>
-      <c r="Y11" s="80"/>
-      <c r="Z11" s="80"/>
-      <c r="AA11" s="80"/>
+        <v>379</v>
+      </c>
+      <c r="L11" s="91"/>
+      <c r="M11" s="91"/>
+      <c r="N11" s="91"/>
+      <c r="O11" s="91"/>
+      <c r="P11" s="91"/>
+      <c r="Q11" s="91"/>
+      <c r="R11" s="91"/>
+      <c r="S11" s="91"/>
+      <c r="T11" s="91"/>
+      <c r="U11" s="91"/>
+      <c r="V11" s="91"/>
+      <c r="W11" s="91"/>
+      <c r="X11" s="91"/>
+      <c r="Y11" s="91"/>
+      <c r="Z11" s="91"/>
+      <c r="AA11" s="91"/>
     </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -38828,7 +39318,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -38845,14 +39335,14 @@
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>346</v>
+        <v>380</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>347</v>
+        <v>381</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -38860,25 +39350,25 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="K3" s="120"/>
+      <c r="K3" s="132"/>
     </row>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -38887,134 +39377,134 @@
       <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="87" t="s">
-        <v>303</v>
-      </c>
-      <c r="K4" s="117" t="s">
+      <c r="J4" s="99" t="s">
+        <v>337</v>
+      </c>
+      <c r="K4" s="129" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>349</v>
+        <v>383</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>350</v>
-      </c>
-      <c r="C5" s="99" t="s">
-        <v>351</v>
-      </c>
-      <c r="D5" s="99" t="s">
-        <v>352</v>
-      </c>
-      <c r="E5" s="100"/>
+        <v>384</v>
+      </c>
+      <c r="C5" s="111" t="s">
+        <v>385</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>386</v>
+      </c>
+      <c r="E5" s="112"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="38" t="s">
-        <v>353</v>
+        <v>387</v>
       </c>
       <c r="I5" s="37">
         <v>0.0</v>
       </c>
-      <c r="J5" s="119" t="s">
-        <v>354</v>
-      </c>
-      <c r="K5" s="99"/>
+      <c r="J5" s="131" t="s">
+        <v>388</v>
+      </c>
+      <c r="K5" s="111"/>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>355</v>
+        <v>389</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>356</v>
+        <v>390</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>357</v>
+        <v>391</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>358</v>
+        <v>392</v>
       </c>
       <c r="E6" s="38" t="s">
-        <v>359</v>
+        <v>393</v>
       </c>
       <c r="F6" s="37">
         <v>1.0</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="38" t="s">
-        <v>360</v>
+        <v>394</v>
       </c>
       <c r="I6" s="37">
         <v>1.0</v>
       </c>
-      <c r="J6" s="92"/>
+      <c r="J6" s="104"/>
       <c r="K6" s="37"/>
     </row>
     <row r="7">
-      <c r="A7" s="121" t="s">
-        <v>361</v>
-      </c>
-      <c r="B7" s="121"/>
-      <c r="C7" s="121" t="s">
-        <v>362</v>
-      </c>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="85" t="s">
-        <v>363</v>
-      </c>
-      <c r="I7" s="121">
+      <c r="A7" s="133" t="s">
+        <v>395</v>
+      </c>
+      <c r="B7" s="133"/>
+      <c r="C7" s="133" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="133"/>
+      <c r="G7" s="133"/>
+      <c r="H7" s="97" t="s">
+        <v>397</v>
+      </c>
+      <c r="I7" s="133">
         <v>1.0</v>
       </c>
-      <c r="J7" s="122" t="s">
-        <v>364</v>
-      </c>
-      <c r="K7" s="123"/>
+      <c r="J7" s="134" t="s">
+        <v>398</v>
+      </c>
+      <c r="K7" s="135"/>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>365</v>
+        <v>399</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>366</v>
+        <v>400</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>367</v>
+        <v>401</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>368</v>
+        <v>402</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>369</v>
+        <v>403</v>
       </c>
       <c r="I8" s="37">
         <v>1.0</v>
       </c>
-      <c r="J8" s="92" t="s">
-        <v>370</v>
-      </c>
-      <c r="K8" s="124"/>
+      <c r="J8" s="104" t="s">
+        <v>404</v>
+      </c>
+      <c r="K8" s="136"/>
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>371</v>
+        <v>405</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>372</v>
+        <v>406</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>373</v>
+        <v>407</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37">
@@ -39022,107 +39512,107 @@
       </c>
       <c r="G9" s="37"/>
       <c r="H9" s="38" t="s">
-        <v>375</v>
+        <v>409</v>
       </c>
       <c r="I9" s="37">
         <v>1.0</v>
       </c>
-      <c r="J9" s="92"/>
-      <c r="K9" s="124"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="136"/>
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>376</v>
+        <v>410</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>377</v>
+        <v>411</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>378</v>
+        <v>412</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>379</v>
+        <v>413</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>380</v>
+        <v>414</v>
       </c>
       <c r="I10" s="37">
         <v>0.0</v>
       </c>
-      <c r="J10" s="92" t="s">
-        <v>381</v>
-      </c>
-      <c r="K10" s="124"/>
+      <c r="J10" s="104" t="s">
+        <v>415</v>
+      </c>
+      <c r="K10" s="136"/>
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>382</v>
+        <v>416</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>383</v>
+        <v>417</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>384</v>
+        <v>418</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>385</v>
+        <v>419</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="38" t="s">
-        <v>386</v>
+        <v>420</v>
       </c>
       <c r="I11" s="37">
         <v>0.0</v>
       </c>
-      <c r="J11" s="92" t="s">
-        <v>387</v>
+      <c r="J11" s="104" t="s">
+        <v>421</v>
       </c>
       <c r="K11" s="37"/>
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>388</v>
+        <v>422</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>389</v>
+        <v>423</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>390</v>
+        <v>424</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>391</v>
+        <v>425</v>
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>392</v>
+        <v>426</v>
       </c>
       <c r="I12" s="37">
         <v>0.0</v>
       </c>
-      <c r="J12" s="92" t="s">
-        <v>393</v>
-      </c>
-      <c r="K12" s="124"/>
+      <c r="J12" s="104" t="s">
+        <v>427</v>
+      </c>
+      <c r="K12" s="136"/>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>394</v>
+        <v>428</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>395</v>
+        <v>429</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>396</v>
+        <v>430</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>397</v>
+        <v>431</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37">
@@ -39130,53 +39620,53 @@
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38" t="s">
-        <v>398</v>
+        <v>432</v>
       </c>
       <c r="I13" s="37">
         <v>1.0</v>
       </c>
-      <c r="J13" s="92" t="s">
-        <v>399</v>
-      </c>
-      <c r="K13" s="124"/>
+      <c r="J13" s="104" t="s">
+        <v>433</v>
+      </c>
+      <c r="K13" s="136"/>
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
-        <v>400</v>
+        <v>434</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>401</v>
+        <v>435</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>402</v>
+        <v>436</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>403</v>
+        <v>437</v>
       </c>
       <c r="E14" s="37"/>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="38" t="s">
-        <v>404</v>
+        <v>438</v>
       </c>
       <c r="I14" s="37">
         <v>0.0</v>
       </c>
-      <c r="J14" s="92"/>
-      <c r="K14" s="124"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="136"/>
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
-        <v>405</v>
+        <v>439</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>406</v>
+        <v>440</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>407</v>
+        <v>441</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>408</v>
+        <v>442</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37">
@@ -39184,53 +39674,53 @@
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38" t="s">
-        <v>409</v>
+        <v>443</v>
       </c>
       <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="92" t="s">
-        <v>410</v>
-      </c>
-      <c r="K15" s="124"/>
+      <c r="J15" s="104" t="s">
+        <v>444</v>
+      </c>
+      <c r="K15" s="136"/>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>411</v>
+        <v>445</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>412</v>
+        <v>446</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>413</v>
+        <v>447</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>414</v>
+        <v>448</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="38" t="s">
-        <v>415</v>
+        <v>449</v>
       </c>
       <c r="I16" s="37">
         <v>0.0</v>
       </c>
-      <c r="J16" s="92"/>
-      <c r="K16" s="124"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="136"/>
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
-        <v>416</v>
+        <v>450</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>417</v>
+        <v>451</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>418</v>
+        <v>452</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>419</v>
+        <v>453</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37">
@@ -39238,38 +39728,38 @@
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>420</v>
+        <v>454</v>
       </c>
       <c r="I17" s="37">
         <v>1.0</v>
       </c>
-      <c r="J17" s="92"/>
-      <c r="K17" s="124"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="136"/>
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>421</v>
+        <v>455</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>422</v>
+        <v>456</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>423</v>
+        <v>457</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>424</v>
+        <v>458</v>
       </c>
       <c r="E18" s="37"/>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="38" t="s">
-        <v>425</v>
+        <v>459</v>
       </c>
       <c r="I18" s="37">
         <v>0.0</v>
       </c>
-      <c r="J18" s="92"/>
-      <c r="K18" s="124"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="136"/>
     </row>
     <row r="19" ht="14.25" customHeight="1">
       <c r="C19" s="39"/>
@@ -40308,10 +40798,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="125" t="s">
+      <c r="B1" s="137" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
@@ -40325,14 +40815,14 @@
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>426</v>
+        <v>460</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>427</v>
+        <v>461</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="126" t="s">
-        <v>428</v>
+      <c r="D2" s="138" t="s">
+        <v>462</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -40341,25 +40831,25 @@
     </row>
     <row r="3" ht="13.5" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="127" t="s">
-        <v>183</v>
-      </c>
-      <c r="C4" s="87" t="s">
+      <c r="B4" s="139" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="87" t="s">
+      <c r="G4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="17" t="s">
@@ -40368,87 +40858,87 @@
       <c r="I4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="87" t="s">
+      <c r="K4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="117" t="s">
+      <c r="L4" s="129" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="38" t="s">
-        <v>429</v>
-      </c>
-      <c r="B5" s="101"/>
+        <v>463</v>
+      </c>
+      <c r="B5" s="113"/>
       <c r="C5" s="37" t="s">
-        <v>430</v>
+        <v>464</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>431</v>
+        <v>465</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>432</v>
+        <v>466</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
       <c r="I5" s="38" t="s">
-        <v>433</v>
+        <v>467</v>
       </c>
       <c r="J5" s="37">
         <v>0.0</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>434</v>
+        <v>468</v>
       </c>
       <c r="L5" s="37"/>
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="B6" s="101"/>
+        <v>469</v>
+      </c>
+      <c r="B6" s="113"/>
       <c r="C6" s="37" t="s">
-        <v>436</v>
+        <v>470</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>437</v>
+        <v>471</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>438</v>
+        <v>472</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
       <c r="I6" s="38" t="s">
-        <v>439</v>
+        <v>473</v>
       </c>
       <c r="J6" s="37">
         <v>0.0</v>
       </c>
       <c r="K6" s="37" t="s">
-        <v>440</v>
+        <v>474</v>
       </c>
       <c r="L6" s="37"/>
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
-        <v>441</v>
-      </c>
-      <c r="B7" s="101">
+        <v>475</v>
+      </c>
+      <c r="B7" s="113">
         <v>21.0</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>442</v>
+        <v>476</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>443</v>
+        <v>477</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>444</v>
+        <v>478</v>
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37">
@@ -40456,32 +40946,32 @@
       </c>
       <c r="H7" s="37"/>
       <c r="I7" s="38" t="s">
-        <v>445</v>
+        <v>479</v>
       </c>
       <c r="J7" s="37">
         <v>1.0</v>
       </c>
       <c r="K7" s="37" t="s">
-        <v>446</v>
+        <v>480</v>
       </c>
       <c r="L7" s="37"/>
-      <c r="M7" s="128" t="s">
-        <v>447</v>
+      <c r="M7" s="140" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="38" t="s">
-        <v>448</v>
-      </c>
-      <c r="B8" s="101"/>
+        <v>482</v>
+      </c>
+      <c r="B8" s="113"/>
       <c r="C8" s="37" t="s">
-        <v>449</v>
+        <v>483</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>450</v>
+        <v>484</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>451</v>
+        <v>485</v>
       </c>
       <c r="F8" s="37"/>
       <c r="G8" s="37">
@@ -40489,98 +40979,98 @@
       </c>
       <c r="H8" s="37"/>
       <c r="I8" s="38" t="s">
-        <v>452</v>
+        <v>486</v>
       </c>
       <c r="J8" s="37">
         <v>1.0</v>
       </c>
       <c r="K8" s="37" t="s">
-        <v>453</v>
+        <v>487</v>
       </c>
       <c r="L8" s="37"/>
     </row>
     <row r="9">
       <c r="A9" s="38" t="s">
-        <v>454</v>
-      </c>
-      <c r="B9" s="101"/>
+        <v>488</v>
+      </c>
+      <c r="B9" s="113"/>
       <c r="C9" s="37" t="s">
-        <v>455</v>
+        <v>489</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>456</v>
+        <v>490</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>457</v>
+        <v>491</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="37"/>
       <c r="I9" s="38" t="s">
-        <v>458</v>
+        <v>492</v>
       </c>
       <c r="J9" s="37">
         <v>0.0</v>
       </c>
       <c r="K9" s="38" t="s">
-        <v>459</v>
+        <v>493</v>
       </c>
       <c r="L9" s="37"/>
-      <c r="M9" s="128" t="s">
-        <v>447</v>
+      <c r="M9" s="140" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>460</v>
-      </c>
-      <c r="B10" s="101"/>
+        <v>494</v>
+      </c>
+      <c r="B10" s="113"/>
       <c r="C10" s="37" t="s">
-        <v>461</v>
+        <v>495</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>462</v>
+        <v>496</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>463</v>
+        <v>497</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="37"/>
       <c r="H10" s="37"/>
       <c r="I10" s="38" t="s">
-        <v>464</v>
+        <v>498</v>
       </c>
       <c r="J10" s="37">
         <v>0.0</v>
       </c>
       <c r="K10" s="37" t="s">
-        <v>465</v>
+        <v>499</v>
       </c>
       <c r="L10" s="37"/>
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
-        <v>466</v>
-      </c>
-      <c r="B11" s="101" t="s">
-        <v>467</v>
+        <v>500</v>
+      </c>
+      <c r="B11" s="113" t="s">
+        <v>501</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>468</v>
+        <v>502</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>469</v>
+        <v>503</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>470</v>
-      </c>
-      <c r="F11" s="100"/>
+        <v>504</v>
+      </c>
+      <c r="F11" s="112"/>
       <c r="G11" s="37">
         <v>1.0</v>
       </c>
       <c r="H11" s="37"/>
       <c r="I11" s="38" t="s">
-        <v>471</v>
+        <v>505</v>
       </c>
       <c r="J11" s="37">
         <v>1.0</v>
@@ -40590,47 +41080,47 @@
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>472</v>
-      </c>
-      <c r="B12" s="101"/>
+        <v>506</v>
+      </c>
+      <c r="B12" s="113"/>
       <c r="C12" s="37" t="s">
-        <v>473</v>
+        <v>507</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>474</v>
+        <v>508</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>475</v>
+        <v>509</v>
       </c>
       <c r="F12" s="37"/>
       <c r="G12" s="37"/>
       <c r="H12" s="37"/>
       <c r="I12" s="38" t="s">
-        <v>476</v>
+        <v>510</v>
       </c>
       <c r="J12" s="37">
         <v>0.0</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>477</v>
+        <v>511</v>
       </c>
       <c r="L12" s="37"/>
     </row>
     <row r="13">
       <c r="A13" s="38" t="s">
-        <v>478</v>
-      </c>
-      <c r="B13" s="101">
+        <v>512</v>
+      </c>
+      <c r="B13" s="113">
         <v>22.0</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>479</v>
+        <v>513</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>480</v>
+        <v>514</v>
       </c>
       <c r="E13" s="37" t="s">
-        <v>481</v>
+        <v>515</v>
       </c>
       <c r="F13" s="37"/>
       <c r="G13" s="37">
@@ -40638,35 +41128,35 @@
       </c>
       <c r="H13" s="37"/>
       <c r="I13" s="38" t="s">
-        <v>482</v>
+        <v>516</v>
       </c>
       <c r="J13" s="37">
         <v>1.0</v>
       </c>
       <c r="K13" s="37" t="s">
-        <v>483</v>
+        <v>517</v>
       </c>
       <c r="L13" s="37"/>
     </row>
     <row r="14">
       <c r="A14" s="38" t="s">
-        <v>484</v>
-      </c>
-      <c r="B14" s="101"/>
+        <v>518</v>
+      </c>
+      <c r="B14" s="113"/>
       <c r="C14" s="37" t="s">
-        <v>485</v>
+        <v>519</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>486</v>
+        <v>520</v>
       </c>
       <c r="E14" s="37" t="s">
-        <v>487</v>
+        <v>521</v>
       </c>
       <c r="F14" s="37"/>
       <c r="G14" s="37"/>
       <c r="H14" s="37"/>
       <c r="I14" s="38" t="s">
-        <v>488</v>
+        <v>522</v>
       </c>
       <c r="J14" s="37">
         <v>0.0</v>
@@ -40676,23 +41166,23 @@
     </row>
     <row r="15">
       <c r="A15" s="38" t="s">
-        <v>489</v>
-      </c>
-      <c r="B15" s="101"/>
+        <v>523</v>
+      </c>
+      <c r="B15" s="113"/>
       <c r="C15" s="37" t="s">
-        <v>490</v>
+        <v>524</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>491</v>
+        <v>525</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>492</v>
+        <v>526</v>
       </c>
       <c r="F15" s="37"/>
       <c r="G15" s="37"/>
       <c r="H15" s="37"/>
       <c r="I15" s="38" t="s">
-        <v>493</v>
+        <v>527</v>
       </c>
       <c r="J15" s="37">
         <v>0.0</v>
@@ -40702,105 +41192,105 @@
     </row>
     <row r="16">
       <c r="A16" s="38" t="s">
-        <v>494</v>
-      </c>
-      <c r="B16" s="101"/>
+        <v>528</v>
+      </c>
+      <c r="B16" s="113"/>
       <c r="C16" s="37" t="s">
-        <v>495</v>
+        <v>529</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>496</v>
+        <v>530</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>497</v>
-      </c>
-      <c r="F16" s="93" t="s">
-        <v>498</v>
+        <v>531</v>
+      </c>
+      <c r="F16" s="105" t="s">
+        <v>532</v>
       </c>
       <c r="G16" s="37">
         <v>1.0</v>
       </c>
       <c r="H16" s="37"/>
       <c r="I16" s="38" t="s">
-        <v>499</v>
+        <v>533</v>
       </c>
       <c r="J16" s="37">
         <v>1.0</v>
       </c>
       <c r="K16" s="37" t="s">
-        <v>500</v>
+        <v>534</v>
       </c>
       <c r="L16" s="37"/>
     </row>
     <row r="17">
       <c r="A17" s="38" t="s">
-        <v>501</v>
-      </c>
-      <c r="B17" s="101"/>
+        <v>535</v>
+      </c>
+      <c r="B17" s="113"/>
       <c r="C17" s="37" t="s">
-        <v>455</v>
+        <v>489</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>431</v>
+        <v>465</v>
       </c>
       <c r="E17" s="37" t="s">
-        <v>502</v>
+        <v>536</v>
       </c>
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
       <c r="H17" s="37"/>
       <c r="I17" s="38" t="s">
-        <v>503</v>
+        <v>537</v>
       </c>
       <c r="J17" s="37">
         <v>1.0</v>
       </c>
       <c r="K17" s="37" t="s">
-        <v>504</v>
+        <v>538</v>
       </c>
       <c r="L17" s="37"/>
     </row>
     <row r="18">
       <c r="A18" s="38" t="s">
-        <v>505</v>
-      </c>
-      <c r="B18" s="101"/>
+        <v>539</v>
+      </c>
+      <c r="B18" s="113"/>
       <c r="C18" s="37" t="s">
-        <v>506</v>
+        <v>540</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>507</v>
+        <v>541</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>508</v>
+        <v>542</v>
       </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="38" t="s">
-        <v>509</v>
+        <v>543</v>
       </c>
       <c r="J18" s="37">
         <v>1.0</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>510</v>
+        <v>544</v>
       </c>
       <c r="L18" s="37"/>
     </row>
     <row r="19">
       <c r="A19" s="38" t="s">
-        <v>511</v>
-      </c>
-      <c r="B19" s="101"/>
+        <v>545</v>
+      </c>
+      <c r="B19" s="113"/>
       <c r="C19" s="37" t="s">
-        <v>512</v>
+        <v>546</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>513</v>
+        <v>547</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>514</v>
+        <v>548</v>
       </c>
       <c r="F19" s="37"/>
       <c r="G19" s="37">
@@ -40808,7 +41298,7 @@
       </c>
       <c r="H19" s="37"/>
       <c r="I19" s="38" t="s">
-        <v>515</v>
+        <v>549</v>
       </c>
       <c r="J19" s="37">
         <v>1.0</v>
@@ -41836,7 +42326,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="42" t="s">
@@ -41853,41 +42343,41 @@
     </row>
     <row r="2" ht="49.5" customHeight="1">
       <c r="A2" s="44" t="s">
-        <v>516</v>
+        <v>550</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>517</v>
+        <v>551</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>518</v>
+        <v>552</v>
       </c>
       <c r="E2" s="72"/>
-      <c r="F2" s="129">
+      <c r="F2" s="141">
         <v>0.1</v>
       </c>
-      <c r="G2" s="130"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="143"/>
+      <c r="I2" s="143"/>
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="87" t="s">
+      <c r="B4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="99" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="99" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -41896,28 +42386,28 @@
       <c r="H4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="117" t="s">
+      <c r="K4" s="129" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="37" t="s">
-        <v>519</v>
+        <v>553</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>520</v>
+        <v>554</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>521</v>
+        <v>555</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>522</v>
+        <v>556</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="37">
@@ -41925,34 +42415,34 @@
       </c>
       <c r="G5" s="37"/>
       <c r="H5" s="38" t="s">
-        <v>523</v>
+        <v>557</v>
       </c>
       <c r="I5" s="37">
         <v>0.0</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>524</v>
+        <v>558</v>
       </c>
       <c r="K5" s="37"/>
     </row>
     <row r="6">
       <c r="A6" s="37" t="s">
-        <v>525</v>
+        <v>559</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>526</v>
+        <v>560</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>527</v>
+        <v>561</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>528</v>
+        <v>562</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="38" t="s">
-        <v>529</v>
+        <v>563</v>
       </c>
       <c r="I6" s="37">
         <v>0.0</v>
@@ -41962,49 +42452,49 @@
     </row>
     <row r="7">
       <c r="A7" s="37" t="s">
-        <v>530</v>
+        <v>564</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>531</v>
+        <v>565</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>532</v>
+        <v>566</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>533</v>
+        <v>567</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="G7" s="37"/>
       <c r="H7" s="38" t="s">
-        <v>534</v>
+        <v>568</v>
       </c>
       <c r="I7" s="37">
         <v>0.0</v>
       </c>
-      <c r="J7" s="100" t="s">
-        <v>535</v>
+      <c r="J7" s="112" t="s">
+        <v>569</v>
       </c>
       <c r="K7" s="37"/>
     </row>
     <row r="8">
       <c r="A8" s="37" t="s">
-        <v>536</v>
+        <v>570</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>537</v>
+        <v>571</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>538</v>
+        <v>572</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>539</v>
+        <v>573</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
       <c r="G8" s="37"/>
       <c r="H8" s="38" t="s">
-        <v>540</v>
+        <v>574</v>
       </c>
       <c r="I8" s="37">
         <v>0.0</v>
@@ -42014,22 +42504,22 @@
     </row>
     <row r="9">
       <c r="A9" s="37" t="s">
-        <v>541</v>
+        <v>575</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>542</v>
+        <v>576</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>543</v>
+        <v>577</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>544</v>
+        <v>578</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
       <c r="H9" s="38" t="s">
-        <v>545</v>
+        <v>579</v>
       </c>
       <c r="I9" s="37">
         <v>1.0</v>
@@ -42039,26 +42529,26 @@
     </row>
     <row r="10">
       <c r="A10" s="37" t="s">
-        <v>546</v>
+        <v>580</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>547</v>
+        <v>581</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>548</v>
+        <v>582</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>549</v>
-      </c>
-      <c r="E10" s="112" t="s">
-        <v>222</v>
+        <v>583</v>
+      </c>
+      <c r="E10" s="124" t="s">
+        <v>256</v>
       </c>
       <c r="F10" s="37">
         <v>1.0</v>
       </c>
       <c r="G10" s="37"/>
       <c r="H10" s="38" t="s">
-        <v>550</v>
+        <v>584</v>
       </c>
       <c r="I10" s="37">
         <v>1.0</v>
@@ -42068,24 +42558,24 @@
     </row>
     <row r="11">
       <c r="A11" s="37" t="s">
-        <v>551</v>
+        <v>585</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>552</v>
+        <v>586</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>553</v>
+        <v>587</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>554</v>
-      </c>
-      <c r="E11" s="112" t="s">
-        <v>555</v>
+        <v>588</v>
+      </c>
+      <c r="E11" s="124" t="s">
+        <v>589</v>
       </c>
       <c r="F11" s="37"/>
       <c r="G11" s="37"/>
       <c r="H11" s="38" t="s">
-        <v>556</v>
+        <v>590</v>
       </c>
       <c r="I11" s="37">
         <v>0.0</v>
@@ -42095,49 +42585,49 @@
     </row>
     <row r="12">
       <c r="A12" s="37" t="s">
-        <v>557</v>
+        <v>591</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>558</v>
+        <v>592</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>559</v>
-      </c>
-      <c r="D12" s="132" t="s">
-        <v>560</v>
+        <v>593</v>
+      </c>
+      <c r="D12" s="144" t="s">
+        <v>594</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>561</v>
+        <v>595</v>
       </c>
       <c r="F12" s="37">
         <v>1.0</v>
       </c>
       <c r="G12" s="37"/>
       <c r="H12" s="38" t="s">
-        <v>562</v>
+        <v>596</v>
       </c>
       <c r="I12" s="37">
         <v>1.0</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>563</v>
+        <v>597</v>
       </c>
       <c r="K12" s="37" t="s">
-        <v>564</v>
+        <v>598</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="37" t="s">
-        <v>565</v>
+        <v>599</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>566</v>
+        <v>600</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>567</v>
+        <v>601</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>568</v>
+        <v>602</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37">
@@ -42145,7 +42635,7 @@
       </c>
       <c r="G13" s="37"/>
       <c r="H13" s="38" t="s">
-        <v>569</v>
+        <v>603</v>
       </c>
       <c r="I13" s="37">
         <v>1.0</v>
@@ -42155,26 +42645,26 @@
     </row>
     <row r="14">
       <c r="A14" s="37" t="s">
-        <v>570</v>
+        <v>604</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>571</v>
+        <v>605</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>572</v>
+        <v>606</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>573</v>
+        <v>607</v>
       </c>
       <c r="E14" s="38" t="s">
-        <v>574</v>
+        <v>608</v>
       </c>
       <c r="F14" s="37">
         <v>1.0</v>
       </c>
       <c r="G14" s="37"/>
       <c r="H14" s="38" t="s">
-        <v>575</v>
+        <v>609</v>
       </c>
       <c r="I14" s="37">
         <v>1.0</v>
@@ -42184,16 +42674,16 @@
     </row>
     <row r="15">
       <c r="A15" s="37" t="s">
-        <v>576</v>
+        <v>610</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>577</v>
+        <v>611</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>578</v>
+        <v>612</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>502</v>
+        <v>536</v>
       </c>
       <c r="E15" s="37"/>
       <c r="F15" s="37">
@@ -42201,34 +42691,34 @@
       </c>
       <c r="G15" s="37"/>
       <c r="H15" s="38" t="s">
-        <v>579</v>
+        <v>613</v>
       </c>
       <c r="I15" s="37">
         <v>1.0</v>
       </c>
-      <c r="J15" s="100" t="s">
-        <v>580</v>
+      <c r="J15" s="112" t="s">
+        <v>614</v>
       </c>
       <c r="K15" s="37"/>
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>581</v>
+        <v>615</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>582</v>
+        <v>616</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>583</v>
+        <v>617</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>584</v>
+        <v>618</v>
       </c>
       <c r="E16" s="37"/>
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
       <c r="H16" s="38" t="s">
-        <v>585</v>
+        <v>619</v>
       </c>
       <c r="I16" s="37">
         <v>0.0</v>
@@ -42238,16 +42728,16 @@
     </row>
     <row r="17">
       <c r="A17" s="37" t="s">
-        <v>586</v>
+        <v>620</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>587</v>
+        <v>621</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>588</v>
+        <v>622</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>589</v>
+        <v>623</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="37">
@@ -42255,7 +42745,7 @@
       </c>
       <c r="G17" s="37"/>
       <c r="H17" s="38" t="s">
-        <v>590</v>
+        <v>624</v>
       </c>
       <c r="I17" s="37">
         <v>1.0</v>
@@ -42265,26 +42755,26 @@
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>591</v>
+        <v>625</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>592</v>
+        <v>626</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>593</v>
+        <v>627</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>594</v>
+        <v>628</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>595</v>
+        <v>629</v>
       </c>
       <c r="F18" s="37">
         <v>1.0</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="38" t="s">
-        <v>596</v>
+        <v>630</v>
       </c>
       <c r="I18" s="37">
         <v>1.0</v>

</xml_diff>

<commit_message>
NAV-172 Update to the BDG
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhXm71E5VMdC1qXIcBprYdxJCNlxg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjiNpm5AzZuJU2TnI9xV+4aLknm9A=="/>
     </ext>
   </extLst>
 </workbook>
@@ -77,7 +77,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miSs3mMnk0YBVYPSxILsEYFzGTiMQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mj819Io1FNxZ4HoiNPoz9tksp3vbA=="/>
     </ext>
   </extLst>
 </comments>
@@ -89,7 +89,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E8">
+    <comment authorId="0" ref="E9">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5eY
@@ -99,7 +99,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E11">
+    <comment authorId="0" ref="E12">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5d8
@@ -109,7 +109,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E10">
+    <comment authorId="0" ref="E11">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5d0
@@ -119,7 +119,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E9">
+    <comment authorId="0" ref="E10">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5dw
@@ -158,7 +158,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjo22ZfdbVCXMI1MMT0aasqHkGbpw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgHlTMUvHUTre4T4ahVahmEueX3vg=="/>
     </ext>
   </extLst>
 </comments>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="603">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -686,6 +686,27 @@
     <t>ADR-01-10</t>
   </si>
   <si>
+    <t>Associate your ADR account with an organization as an editor</t>
+  </si>
+  <si>
+    <t>Is user a member of an organization (country) with an "editor" role on ADR?</t>
+  </si>
+  <si>
+    <t>In order to take advantage of the features available to users on the AIDS Data Repository, you must register an account. It is a quick and simple process. There is an instructional video available on Youtube which will demonstrate how to register and join an organization. Typically, the organization is your country. In order to upload and edit data, you must be an "editor" or "admin". Request the one most appropriate for your estimates role when you are requesting access to the organization.</t>
+  </si>
+  <si>
+    <t>Registering and Joining an Organisation - The AIDS Data Repository https://www.youtube.com/watch?v=O34wTKvn1xI</t>
+  </si>
+  <si>
+    <t>MM Would recomend linking to training manuals instead of youtube</t>
+  </si>
+  <si>
+    <t>check_manual_confirmation('EST-ADR-01-10-A')</t>
+  </si>
+  <si>
+    <t>ADR-01-11</t>
+  </si>
+  <si>
     <t>Check that the required data has been preloaded into your ADR dataset</t>
   </si>
   <si>
@@ -707,7 +728,7 @@
     <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum'], 'url', '.*')</t>
   </si>
   <si>
-    <t>ADR-01-11</t>
+    <t>ADR-01-12</t>
   </si>
   <si>
     <t>Upload data inputs to the ADR using the required templates</t>
@@ -729,7 +750,7 @@
 - Click "Upload Files"</t>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-ADR-01-11-A')</t>
+    <t>check_manual_confirmation('EST-ADR-01-12-A')</t>
   </si>
   <si>
     <t>ADR-02-01</t>
@@ -2997,7 +3018,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="116">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3110,14 +3131,20 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -10188,7 +10215,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -10205,44 +10232,44 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="30">
         <v>0.2</v>
       </c>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="115"/>
+      <c r="I2" s="115"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="109" t="s">
-        <v>520</v>
-      </c>
-      <c r="C4" s="81" t="s">
+      <c r="B4" s="111" t="s">
+        <v>527</v>
+      </c>
+      <c r="C4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="81" t="s">
+      <c r="G4" s="83" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="34" t="s">
@@ -10251,26 +10278,26 @@
       <c r="I4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="81" t="s">
+      <c r="J4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>521</v>
-      </c>
-      <c r="B5" s="110"/>
+        <v>528</v>
+      </c>
+      <c r="B5" s="112"/>
       <c r="C5" s="15" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15">
@@ -10278,26 +10305,26 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="23" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>526</v>
-      </c>
-      <c r="B6" s="110" t="s">
-        <v>527</v>
+        <v>533</v>
+      </c>
+      <c r="B6" s="112" t="s">
+        <v>534</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15">
@@ -10305,186 +10332,186 @@
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="23" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>533</v>
-      </c>
-      <c r="B7" s="110"/>
+        <v>540</v>
+      </c>
+      <c r="B7" s="112"/>
       <c r="C7" s="15" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>535</v>
-      </c>
-      <c r="J7" s="90"/>
+        <v>542</v>
+      </c>
+      <c r="J7" s="92"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>536</v>
-      </c>
-      <c r="B8" s="110"/>
+        <v>543</v>
+      </c>
+      <c r="B8" s="112"/>
       <c r="C8" s="15" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="23" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="B9" s="110" t="s">
-        <v>539</v>
+        <v>545</v>
+      </c>
+      <c r="B9" s="112" t="s">
+        <v>546</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>542</v>
-      </c>
-      <c r="B10" s="110" t="s">
-        <v>543</v>
+        <v>549</v>
+      </c>
+      <c r="B10" s="112" t="s">
+        <v>550</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="F10" s="97" t="s">
-        <v>267</v>
+        <v>553</v>
+      </c>
+      <c r="F10" s="99" t="s">
+        <v>274</v>
       </c>
       <c r="G10" s="15">
         <v>1.0</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="23" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>548</v>
-      </c>
-      <c r="B11" s="110"/>
+        <v>555</v>
+      </c>
+      <c r="B11" s="112"/>
       <c r="C11" s="15" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>551</v>
-      </c>
-      <c r="F11" s="97" t="s">
-        <v>552</v>
+        <v>558</v>
+      </c>
+      <c r="F11" s="99" t="s">
+        <v>559</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="23" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>554</v>
-      </c>
-      <c r="B12" s="110" t="s">
-        <v>555</v>
+        <v>561</v>
+      </c>
+      <c r="B12" s="112" t="s">
+        <v>562</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>557</v>
-      </c>
-      <c r="E12" s="87" t="s">
-        <v>558</v>
+        <v>564</v>
+      </c>
+      <c r="E12" s="89" t="s">
+        <v>565</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="G12" s="15">
         <v>1.0</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="K12" s="15"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>562</v>
-      </c>
-      <c r="B13" s="110" t="s">
-        <v>563</v>
+        <v>569</v>
+      </c>
+      <c r="B13" s="112" t="s">
+        <v>570</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15">
@@ -10492,53 +10519,53 @@
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="23" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>568</v>
-      </c>
-      <c r="B14" s="110" t="s">
-        <v>569</v>
+        <v>575</v>
+      </c>
+      <c r="B14" s="112" t="s">
+        <v>576</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="G14" s="15">
         <v>1.0</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="23" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>575</v>
-      </c>
-      <c r="B15" s="110"/>
+        <v>582</v>
+      </c>
+      <c r="B15" s="112"/>
       <c r="C15" s="15" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15">
@@ -10546,47 +10573,47 @@
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="23" t="s">
-        <v>579</v>
-      </c>
-      <c r="J15" s="90"/>
+        <v>586</v>
+      </c>
+      <c r="J15" s="92"/>
       <c r="K15" s="15"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>580</v>
-      </c>
-      <c r="B16" s="110"/>
+        <v>587</v>
+      </c>
+      <c r="B16" s="112"/>
       <c r="C16" s="15" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="23" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>585</v>
-      </c>
-      <c r="B17" s="110"/>
+        <v>592</v>
+      </c>
+      <c r="B17" s="112"/>
       <c r="C17" s="15" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>587</v>
+        <v>594</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15">
@@ -10594,34 +10621,34 @@
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="23" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>590</v>
-      </c>
-      <c r="B18" s="110"/>
+        <v>597</v>
+      </c>
+      <c r="B18" s="112"/>
       <c r="C18" s="15" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>594</v>
+        <v>601</v>
       </c>
       <c r="G18" s="15">
         <v>1.0</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="23" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -13235,7 +13262,7 @@
       <c r="F3" s="48"/>
       <c r="G3" s="48"/>
     </row>
-    <row r="4" ht="12.0" customHeight="1">
+    <row r="4" ht="11.25" customHeight="1">
       <c r="A4" s="49" t="s">
         <v>9</v>
       </c>
@@ -13264,7 +13291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="12.0" customHeight="1">
+    <row r="5" ht="92.25" customHeight="1">
       <c r="A5" s="50" t="s">
         <v>116</v>
       </c>
@@ -13277,148 +13304,134 @@
       <c r="D5" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="52" t="s">
+      <c r="E5" s="51" t="s">
         <v>120</v>
       </c>
+      <c r="F5" s="52">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="53" t="s">
+        <v>121</v>
+      </c>
       <c r="H5" s="18"/>
-      <c r="I5" s="17" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" ht="69.0" customHeight="1">
-      <c r="A6" s="50" t="s">
+      <c r="I5" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="53" t="s">
+    </row>
+    <row r="6" ht="12.0" customHeight="1">
+      <c r="A6" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="B6" s="51" t="s">
         <v>124</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="C6" s="51" t="s">
         <v>125</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>126</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="39"/>
-      <c r="G6" s="54"/>
+      <c r="G6" s="53" t="s">
+        <v>127</v>
+      </c>
       <c r="H6" s="18"/>
-      <c r="I6" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
-      <c r="N6" s="56"/>
-      <c r="O6" s="56"/>
-      <c r="P6" s="56"/>
-      <c r="Q6" s="56"/>
-      <c r="R6" s="56"/>
-      <c r="S6" s="56"/>
-      <c r="T6" s="56"/>
-      <c r="U6" s="56"/>
-      <c r="V6" s="56"/>
-      <c r="W6" s="56"/>
-      <c r="X6" s="56"/>
-      <c r="Y6" s="56"/>
-    </row>
-    <row r="7" ht="12.0" customHeight="1">
-      <c r="A7" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="37" t="s">
+      <c r="I6" s="17" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="37" t="s">
+    </row>
+    <row r="7" ht="69.0" customHeight="1">
+      <c r="A7" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="B7" s="55" t="s">
         <v>130</v>
       </c>
+      <c r="C7" s="55" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>132</v>
+      </c>
       <c r="E7" s="37"/>
-      <c r="F7" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="54"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="56"/>
       <c r="H7" s="18"/>
-      <c r="I7" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
-      <c r="X7" s="56"/>
-      <c r="Y7" s="56"/>
-    </row>
-    <row r="8" ht="26.25" customHeight="1">
-      <c r="A8" s="57" t="s">
-        <v>132</v>
+      <c r="I7" s="57" t="s">
+        <v>133</v>
+      </c>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+      <c r="L7" s="58"/>
+      <c r="M7" s="58"/>
+      <c r="N7" s="58"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="58"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="58"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="58"/>
+      <c r="X7" s="58"/>
+      <c r="Y7" s="58"/>
+    </row>
+    <row r="8" ht="12.0" customHeight="1">
+      <c r="A8" s="59" t="s">
+        <v>134</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>136</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="E8" s="37"/>
       <c r="F8" s="39">
         <v>1.0</v>
       </c>
-      <c r="G8" s="37"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="18"/>
-      <c r="I8" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-    </row>
-    <row r="9" ht="99.75" customHeight="1">
-      <c r="A9" s="57" t="s">
+      <c r="I8" s="17" t="s">
         <v>138</v>
       </c>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="58"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="58"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="58"/>
+      <c r="Y8" s="58"/>
+    </row>
+    <row r="9" ht="26.25" customHeight="1">
+      <c r="A9" s="59" t="s">
+        <v>139</v>
+      </c>
       <c r="B9" s="37" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E9" s="42" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F9" s="39">
         <v>1.0</v>
@@ -13426,7 +13439,7 @@
       <c r="G9" s="37"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -13445,29 +13458,29 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" ht="12.0" customHeight="1">
-      <c r="A10" s="58" t="s">
-        <v>144</v>
-      </c>
-      <c r="B10" s="59" t="s">
+    <row r="10" ht="99.75" customHeight="1">
+      <c r="A10" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="B10" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="C10" s="37" t="s">
         <v>147</v>
       </c>
-      <c r="E10" s="60" t="s">
+      <c r="D10" s="51" t="s">
         <v>148</v>
       </c>
-      <c r="F10" s="61">
+      <c r="E10" s="42" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="39">
         <v>1.0</v>
       </c>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64" t="s">
-        <v>149</v>
+      <c r="G10" s="37"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18" t="s">
+        <v>150</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -13487,46 +13500,86 @@
       <c r="Y10" s="6"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="A11" s="57" t="s">
-        <v>150</v>
-      </c>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="60" t="s">
         <v>151</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="B11" s="61" t="s">
         <v>152</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="C11" s="61" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="D11" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="F11" s="37">
+      <c r="E11" s="62" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" s="63">
         <v>1.0</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="J11" s="65"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="65"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
-      <c r="U11" s="65"/>
-      <c r="V11" s="65"/>
-      <c r="W11" s="65"/>
-      <c r="X11" s="65"/>
-    </row>
-    <row r="12" ht="12.0" customHeight="1"/>
+      <c r="G11" s="64"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="66" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" ht="12.0" customHeight="1">
+      <c r="A12" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="37">
+        <v>1.0</v>
+      </c>
+      <c r="G12" s="37"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="J12" s="67"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="67"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="67"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="67"/>
+      <c r="R12" s="67"/>
+      <c r="S12" s="67"/>
+      <c r="T12" s="67"/>
+      <c r="U12" s="67"/>
+      <c r="V12" s="67"/>
+      <c r="W12" s="67"/>
+      <c r="X12" s="67"/>
+    </row>
     <row r="13" ht="12.0" customHeight="1"/>
     <row r="14" ht="12.0" customHeight="1"/>
     <row r="15" ht="12.0" customHeight="1"/>
@@ -14511,6 +14564,7 @@
     <row r="994" ht="12.0" customHeight="1"/>
     <row r="995" ht="12.0" customHeight="1"/>
     <row r="996" ht="12.0" customHeight="1"/>
+    <row r="997" ht="12.0" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -14518,10 +14572,10 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="E8"/>
-    <hyperlink r:id="rId3" ref="E9"/>
-    <hyperlink r:id="rId4" ref="E10"/>
-    <hyperlink r:id="rId5" ref="E11"/>
+    <hyperlink r:id="rId2" ref="E9"/>
+    <hyperlink r:id="rId3" ref="E10"/>
+    <hyperlink r:id="rId4" ref="E11"/>
+    <hyperlink r:id="rId5" ref="E12"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -14554,7 +14608,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -14571,14 +14625,14 @@
     </row>
     <row r="2" ht="48.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -14624,143 +14678,143 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="67" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="68" t="s">
-        <v>160</v>
-      </c>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="69">
+      <c r="A5" s="69" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="71">
         <v>1.0</v>
       </c>
-      <c r="G5" s="70" t="s">
-        <v>161</v>
-      </c>
-      <c r="H5" s="71"/>
-      <c r="I5" s="72" t="s">
-        <v>162</v>
+      <c r="G5" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="73"/>
+      <c r="I5" s="74" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="37" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F6" s="73">
+        <v>174</v>
+      </c>
+      <c r="F6" s="75">
         <v>1.0</v>
       </c>
-      <c r="G6" s="74"/>
+      <c r="G6" s="76"/>
       <c r="H6" s="15"/>
       <c r="I6" s="23" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="37" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="73">
+      <c r="F7" s="75">
         <v>1.0</v>
       </c>
-      <c r="G7" s="74"/>
+      <c r="G7" s="76"/>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="73">
+      <c r="F8" s="75">
         <v>1.0</v>
       </c>
-      <c r="G8" s="74"/>
+      <c r="G8" s="76"/>
       <c r="H8" s="15"/>
       <c r="I8" s="23" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="37" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="75">
         <v>1.0</v>
       </c>
-      <c r="G9" s="74"/>
+      <c r="G9" s="76"/>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="37" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="E10" s="37"/>
-      <c r="F10" s="74">
+      <c r="F10" s="76">
         <v>1.0</v>
       </c>
-      <c r="G10" s="75"/>
+      <c r="G10" s="77"/>
       <c r="H10" s="21"/>
       <c r="I10" s="23" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -15861,7 +15915,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -15877,15 +15931,15 @@
       </c>
     </row>
     <row r="2" ht="48.0" customHeight="1">
-      <c r="A2" s="76" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="77" t="s">
-        <v>190</v>
+      <c r="A2" s="78" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>197</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="77" t="s">
-        <v>158</v>
+      <c r="D2" s="79" t="s">
+        <v>165</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -15902,8 +15956,8 @@
       <c r="G3" s="32"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="78" t="s">
-        <v>191</v>
+      <c r="A4" s="80" t="s">
+        <v>198</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>9</v>
@@ -15935,166 +15989,166 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="37" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="73">
+      <c r="G5" s="75">
         <v>1.0</v>
       </c>
-      <c r="H5" s="75"/>
+      <c r="H5" s="77"/>
       <c r="I5" s="15"/>
-      <c r="J5" s="79" t="s">
-        <v>197</v>
+      <c r="J5" s="81" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="37" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="G6" s="73">
+        <v>209</v>
+      </c>
+      <c r="G6" s="75">
         <v>1.0</v>
       </c>
-      <c r="H6" s="74"/>
+      <c r="H6" s="76"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="69" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="71">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="72" t="s">
+        <v>168</v>
+      </c>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73" t="s">
         <v>204</v>
-      </c>
-      <c r="B7" s="67" t="s">
-        <v>205</v>
-      </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67" t="s">
-        <v>206</v>
-      </c>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="69">
-        <v>1.0</v>
-      </c>
-      <c r="H7" s="70" t="s">
-        <v>161</v>
-      </c>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="E8" s="37" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="G8" s="73">
+        <v>216</v>
+      </c>
+      <c r="G8" s="75">
         <v>1.0</v>
       </c>
-      <c r="H8" s="74"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="37" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="G9" s="74">
+        <v>216</v>
+      </c>
+      <c r="G9" s="76">
         <v>1.0</v>
       </c>
-      <c r="H9" s="80" t="s">
-        <v>215</v>
+      <c r="H9" s="82" t="s">
+        <v>222</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="15" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="37" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F10" s="37"/>
-      <c r="G10" s="73">
+      <c r="G10" s="75">
         <v>1.0</v>
       </c>
       <c r="H10" s="37"/>
       <c r="I10" s="19"/>
       <c r="J10" s="15" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -17187,7 +17241,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="9.29"/>
-    <col customWidth="1" min="2" max="2" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="25.57"/>
     <col customWidth="1" min="3" max="3" width="14.57"/>
     <col customWidth="1" min="4" max="4" width="20.0"/>
     <col customWidth="1" min="5" max="5" width="70.43"/>
@@ -17199,7 +17253,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -17216,14 +17270,14 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -17232,31 +17286,31 @@
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="82" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="81" t="s">
+      <c r="B4" s="84" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="81" t="s">
+      <c r="G4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="81" t="s">
+      <c r="H4" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="84" t="s">
+      <c r="I4" s="86" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="34" t="s">
@@ -17265,46 +17319,46 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>226</v>
-      </c>
-      <c r="B5" s="85"/>
+        <v>233</v>
+      </c>
+      <c r="B5" s="87"/>
       <c r="C5" s="15" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="E5" s="86" t="s">
-        <v>229</v>
-      </c>
-      <c r="F5" s="87" t="s">
-        <v>230</v>
+        <v>235</v>
+      </c>
+      <c r="E5" s="88" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" s="89" t="s">
+        <v>237</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="23" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B6" s="85"/>
+        <v>240</v>
+      </c>
+      <c r="B6" s="87"/>
       <c r="C6" s="15" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E6" s="86" t="s">
-        <v>236</v>
+        <v>242</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>243</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="G6" s="15">
         <v>1.0</v>
@@ -17312,22 +17366,22 @@
       <c r="H6" s="19"/>
       <c r="I6" s="15"/>
       <c r="J6" s="23" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="88"/>
+        <v>246</v>
+      </c>
+      <c r="B7" s="90"/>
       <c r="C7" s="15" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="E7" s="86" t="s">
-        <v>242</v>
+        <v>248</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>249</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
@@ -17336,381 +17390,381 @@
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="23" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="B8" s="85"/>
+        <v>251</v>
+      </c>
+      <c r="B8" s="87"/>
       <c r="C8" s="15" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="E8" s="86" t="s">
-        <v>247</v>
+        <v>253</v>
+      </c>
+      <c r="E8" s="88" t="s">
+        <v>254</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="23" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="B9" s="88" t="s">
-        <v>251</v>
+        <v>257</v>
+      </c>
+      <c r="B9" s="90" t="s">
+        <v>258</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="E9" s="86" t="s">
-        <v>254</v>
-      </c>
-      <c r="F9" s="87" t="s">
-        <v>255</v>
+        <v>260</v>
+      </c>
+      <c r="E9" s="88" t="s">
+        <v>261</v>
+      </c>
+      <c r="F9" s="89" t="s">
+        <v>262</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="23" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="B10" s="88"/>
+        <v>264</v>
+      </c>
+      <c r="B10" s="90"/>
       <c r="C10" s="15" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>259</v>
-      </c>
-      <c r="E10" s="86" t="s">
-        <v>260</v>
-      </c>
-      <c r="F10" s="89"/>
+        <v>266</v>
+      </c>
+      <c r="E10" s="88" t="s">
+        <v>267</v>
+      </c>
+      <c r="F10" s="91"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="57" t="s">
-        <v>261</v>
+      <c r="H10" s="59" t="s">
+        <v>268</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="23" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" ht="57.0" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>263</v>
-      </c>
-      <c r="B11" s="88"/>
+        <v>270</v>
+      </c>
+      <c r="B11" s="90"/>
       <c r="C11" s="15" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="E11" s="86" t="s">
-        <v>266</v>
+        <v>272</v>
+      </c>
+      <c r="E11" s="88" t="s">
+        <v>273</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="90"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="19"/>
       <c r="J11" s="23" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" ht="12.0" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="B12" s="85" t="s">
-        <v>270</v>
+        <v>276</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>277</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="E12" s="86" t="s">
-        <v>273</v>
+        <v>279</v>
+      </c>
+      <c r="E12" s="88" t="s">
+        <v>280</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="57"/>
+      <c r="H12" s="59"/>
       <c r="I12" s="15"/>
       <c r="J12" s="23" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>275</v>
-      </c>
-      <c r="B13" s="91"/>
+        <v>282</v>
+      </c>
+      <c r="B13" s="93"/>
       <c r="C13" s="15" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="E13" s="86" t="s">
-        <v>278</v>
+        <v>284</v>
+      </c>
+      <c r="E13" s="88" t="s">
+        <v>285</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="57" t="s">
-        <v>279</v>
+      <c r="H13" s="59" t="s">
+        <v>286</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="23" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="B14" s="88" t="s">
-        <v>282</v>
+        <v>288</v>
+      </c>
+      <c r="B14" s="90" t="s">
+        <v>289</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="E14" s="86" t="s">
-        <v>285</v>
+        <v>291</v>
+      </c>
+      <c r="E14" s="88" t="s">
+        <v>292</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="57"/>
+      <c r="H14" s="59"/>
       <c r="I14" s="15"/>
       <c r="J14" s="23" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="B15" s="88" t="s">
-        <v>288</v>
+        <v>294</v>
+      </c>
+      <c r="B15" s="90" t="s">
+        <v>295</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="E15" s="86" t="s">
-        <v>291</v>
+        <v>297</v>
+      </c>
+      <c r="E15" s="88" t="s">
+        <v>298</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="23" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="A16" s="71" t="s">
-        <v>294</v>
-      </c>
-      <c r="B16" s="88"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71" t="s">
-        <v>295</v>
-      </c>
-      <c r="E16" s="92"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71">
+      <c r="A16" s="73" t="s">
+        <v>301</v>
+      </c>
+      <c r="B16" s="90"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73" t="s">
+        <v>302</v>
+      </c>
+      <c r="E16" s="94"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73">
         <v>1.0</v>
       </c>
-      <c r="H16" s="93" t="s">
-        <v>296</v>
+      <c r="H16" s="95" t="s">
+        <v>303</v>
       </c>
       <c r="I16" s="21"/>
-      <c r="J16" s="72" t="s">
-        <v>297</v>
+      <c r="J16" s="74" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="B17" s="88" t="s">
-        <v>299</v>
-      </c>
-      <c r="C17" s="79" t="s">
-        <v>300</v>
-      </c>
-      <c r="D17" s="79" t="s">
-        <v>301</v>
-      </c>
-      <c r="E17" s="94" t="s">
-        <v>302</v>
-      </c>
-      <c r="F17" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="G17" s="79"/>
-      <c r="H17" s="96"/>
+        <v>305</v>
+      </c>
+      <c r="B17" s="90" t="s">
+        <v>306</v>
+      </c>
+      <c r="C17" s="81" t="s">
+        <v>307</v>
+      </c>
+      <c r="D17" s="81" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" s="96" t="s">
+        <v>309</v>
+      </c>
+      <c r="F17" s="97" t="s">
+        <v>310</v>
+      </c>
+      <c r="G17" s="81"/>
+      <c r="H17" s="98"/>
       <c r="I17" s="15"/>
       <c r="J17" s="23" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B18" s="88" t="s">
-        <v>306</v>
-      </c>
-      <c r="C18" s="79" t="s">
-        <v>307</v>
-      </c>
-      <c r="D18" s="79" t="s">
-        <v>308</v>
-      </c>
-      <c r="E18" s="94" t="s">
-        <v>309</v>
-      </c>
-      <c r="F18" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="G18" s="79"/>
-      <c r="H18" s="96"/>
+        <v>312</v>
+      </c>
+      <c r="B18" s="90" t="s">
+        <v>313</v>
+      </c>
+      <c r="C18" s="81" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="81" t="s">
+        <v>315</v>
+      </c>
+      <c r="E18" s="96" t="s">
+        <v>316</v>
+      </c>
+      <c r="F18" s="97" t="s">
+        <v>310</v>
+      </c>
+      <c r="G18" s="81"/>
+      <c r="H18" s="98"/>
       <c r="I18" s="15"/>
       <c r="J18" s="23" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="B19" s="88" t="s">
-        <v>312</v>
+        <v>318</v>
+      </c>
+      <c r="B19" s="90" t="s">
+        <v>319</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>314</v>
-      </c>
-      <c r="E19" s="86" t="s">
-        <v>315</v>
-      </c>
-      <c r="F19" s="97" t="s">
-        <v>303</v>
+        <v>321</v>
+      </c>
+      <c r="E19" s="88" t="s">
+        <v>322</v>
+      </c>
+      <c r="F19" s="99" t="s">
+        <v>310</v>
       </c>
       <c r="G19" s="15"/>
-      <c r="H19" s="90"/>
+      <c r="H19" s="92"/>
       <c r="I19" s="15"/>
       <c r="J19" s="23" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
     </row>
     <row r="20" ht="12.0" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="B20" s="88" t="s">
-        <v>318</v>
+        <v>324</v>
+      </c>
+      <c r="B20" s="90" t="s">
+        <v>325</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="E20" s="86" t="s">
-        <v>321</v>
-      </c>
-      <c r="F20" s="97" t="s">
-        <v>322</v>
+        <v>327</v>
+      </c>
+      <c r="E20" s="88" t="s">
+        <v>328</v>
+      </c>
+      <c r="F20" s="99" t="s">
+        <v>329</v>
       </c>
       <c r="G20" s="15"/>
-      <c r="H20" s="90"/>
+      <c r="H20" s="92"/>
       <c r="I20" s="15"/>
       <c r="J20" s="23" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="B21" s="88" t="s">
-        <v>325</v>
+        <v>331</v>
+      </c>
+      <c r="B21" s="90" t="s">
+        <v>332</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="E21" s="86" t="s">
-        <v>328</v>
-      </c>
-      <c r="F21" s="97" t="s">
-        <v>303</v>
+        <v>334</v>
+      </c>
+      <c r="E21" s="88" t="s">
+        <v>335</v>
+      </c>
+      <c r="F21" s="99" t="s">
+        <v>310</v>
       </c>
       <c r="G21" s="15"/>
-      <c r="H21" s="90"/>
+      <c r="H21" s="92"/>
       <c r="I21" s="21"/>
       <c r="J21" s="23" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" ht="12.0" customHeight="1">
-      <c r="A22" s="71" t="s">
-        <v>330</v>
-      </c>
-      <c r="B22" s="98"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="71" t="s">
-        <v>331</v>
-      </c>
-      <c r="E22" s="92"/>
-      <c r="F22" s="99"/>
-      <c r="G22" s="100">
+      <c r="A22" s="73" t="s">
+        <v>337</v>
+      </c>
+      <c r="B22" s="100"/>
+      <c r="C22" s="73"/>
+      <c r="D22" s="73" t="s">
+        <v>338</v>
+      </c>
+      <c r="E22" s="94"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="102">
         <v>1.0</v>
       </c>
-      <c r="H22" s="93" t="s">
-        <v>332</v>
+      <c r="H22" s="95" t="s">
+        <v>339</v>
       </c>
       <c r="I22" s="15"/>
-      <c r="J22" s="72" t="s">
-        <v>333</v>
+      <c r="J22" s="74" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="23" ht="12.0" customHeight="1">
@@ -18781,7 +18835,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -18797,15 +18851,15 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="76" t="s">
-        <v>334</v>
-      </c>
-      <c r="B2" s="77" t="s">
-        <v>335</v>
+      <c r="A2" s="78" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2" s="79" t="s">
+        <v>342</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="77" t="s">
-        <v>336</v>
+      <c r="D2" s="79" t="s">
+        <v>343</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -18814,29 +18868,29 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="81" t="s">
-        <v>337</v>
+      <c r="G4" s="83" t="s">
+        <v>344</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="I4" s="34" t="s">
         <v>16</v>
@@ -18847,138 +18901,138 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="57"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="59"/>
       <c r="I5" s="15"/>
       <c r="J5" s="23" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="86" t="s">
-        <v>348</v>
+      <c r="G6" s="88" t="s">
+        <v>355</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="23" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="86" t="s">
-        <v>348</v>
+      <c r="G7" s="88" t="s">
+        <v>355</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="23" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15">
         <v>1.0</v>
       </c>
-      <c r="G8" s="86"/>
+      <c r="G8" s="88"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="23" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>363</v>
-      </c>
-      <c r="E9" s="101" t="s">
-        <v>364</v>
+        <v>370</v>
+      </c>
+      <c r="E9" s="103" t="s">
+        <v>371</v>
       </c>
       <c r="F9" s="15">
         <v>1.0</v>
       </c>
-      <c r="G9" s="86" t="s">
-        <v>365</v>
+      <c r="G9" s="88" t="s">
+        <v>372</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="21"/>
       <c r="J9" s="23" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15">
@@ -18988,24 +19042,24 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="23" t="s">
-        <v>371</v>
-      </c>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
-      <c r="U10" s="65"/>
-      <c r="V10" s="65"/>
-      <c r="W10" s="65"/>
-      <c r="X10" s="65"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="65"/>
+        <v>378</v>
+      </c>
+      <c r="K10" s="67"/>
+      <c r="L10" s="67"/>
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="O10" s="67"/>
+      <c r="P10" s="67"/>
+      <c r="Q10" s="67"/>
+      <c r="R10" s="67"/>
+      <c r="S10" s="67"/>
+      <c r="T10" s="67"/>
+      <c r="U10" s="67"/>
+      <c r="V10" s="67"/>
+      <c r="W10" s="67"/>
+      <c r="X10" s="67"/>
+      <c r="Y10" s="67"/>
+      <c r="Z10" s="67"/>
     </row>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>
@@ -20036,7 +20090,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -20053,14 +20107,14 @@
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -20068,25 +20122,25 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="J3" s="102"/>
+      <c r="J3" s="104"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="34" t="s">
@@ -20095,93 +20149,93 @@
       <c r="H4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="81" t="s">
-        <v>337</v>
+      <c r="I4" s="83" t="s">
+        <v>344</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>377</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>378</v>
-      </c>
-      <c r="E5" s="90"/>
+        <v>383</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5" s="59" t="s">
+        <v>385</v>
+      </c>
+      <c r="E5" s="92"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="23" t="s">
-        <v>379</v>
-      </c>
-      <c r="I5" s="103"/>
-      <c r="J5" s="57"/>
+        <v>386</v>
+      </c>
+      <c r="I5" s="105"/>
+      <c r="J5" s="59"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="F6" s="15">
         <v>1.0</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="23" t="s">
-        <v>385</v>
-      </c>
-      <c r="I6" s="86"/>
+        <v>392</v>
+      </c>
+      <c r="I6" s="88"/>
       <c r="J6" s="15"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="104" t="s">
-        <v>386</v>
-      </c>
-      <c r="B7" s="104"/>
-      <c r="C7" s="104" t="s">
-        <v>387</v>
-      </c>
-      <c r="D7" s="104"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="104"/>
-      <c r="G7" s="104"/>
-      <c r="H7" s="72" t="s">
-        <v>388</v>
-      </c>
-      <c r="I7" s="105" t="s">
-        <v>389</v>
-      </c>
-      <c r="J7" s="106"/>
+      <c r="A7" s="106" t="s">
+        <v>393</v>
+      </c>
+      <c r="B7" s="106"/>
+      <c r="C7" s="106" t="s">
+        <v>394</v>
+      </c>
+      <c r="D7" s="106"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
+      <c r="G7" s="106"/>
+      <c r="H7" s="74" t="s">
+        <v>395</v>
+      </c>
+      <c r="I7" s="107" t="s">
+        <v>396</v>
+      </c>
+      <c r="J7" s="108"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15">
@@ -20189,45 +20243,45 @@
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="23" t="s">
-        <v>394</v>
-      </c>
-      <c r="I8" s="86"/>
-      <c r="J8" s="107"/>
+        <v>401</v>
+      </c>
+      <c r="I8" s="88"/>
+      <c r="J8" s="109"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="23" t="s">
-        <v>399</v>
-      </c>
-      <c r="I9" s="86"/>
-      <c r="J9" s="107"/>
+        <v>406</v>
+      </c>
+      <c r="I9" s="88"/>
+      <c r="J9" s="109"/>
     </row>
     <row r="10" ht="115.5" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15">
@@ -20235,47 +20289,47 @@
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="23" t="s">
-        <v>404</v>
-      </c>
-      <c r="I10" s="86" t="s">
-        <v>405</v>
-      </c>
-      <c r="J10" s="107"/>
+        <v>411</v>
+      </c>
+      <c r="I10" s="88" t="s">
+        <v>412</v>
+      </c>
+      <c r="J10" s="109"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="23" t="s">
-        <v>410</v>
-      </c>
-      <c r="I11" s="86"/>
-      <c r="J11" s="107"/>
+        <v>417</v>
+      </c>
+      <c r="I11" s="88"/>
+      <c r="J11" s="109"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15">
@@ -20283,47 +20337,47 @@
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="23" t="s">
-        <v>415</v>
-      </c>
-      <c r="I12" s="86" t="s">
-        <v>416</v>
-      </c>
-      <c r="J12" s="107"/>
+        <v>422</v>
+      </c>
+      <c r="I12" s="88" t="s">
+        <v>423</v>
+      </c>
+      <c r="J12" s="109"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="23" t="s">
-        <v>421</v>
-      </c>
-      <c r="I13" s="86"/>
-      <c r="J13" s="107"/>
+        <v>428</v>
+      </c>
+      <c r="I13" s="88"/>
+      <c r="J13" s="109"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15">
@@ -20331,32 +20385,32 @@
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="23" t="s">
-        <v>426</v>
-      </c>
-      <c r="I14" s="86"/>
-      <c r="J14" s="107"/>
+        <v>433</v>
+      </c>
+      <c r="I14" s="88"/>
+      <c r="J14" s="109"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="23" t="s">
-        <v>431</v>
-      </c>
-      <c r="I15" s="86"/>
-      <c r="J15" s="107"/>
+        <v>438</v>
+      </c>
+      <c r="I15" s="88"/>
+      <c r="J15" s="109"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="C16" s="26"/>
@@ -21380,7 +21434,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="19.43"/>
-    <col customWidth="1" min="2" max="2" width="9.29"/>
+    <col customWidth="1" min="2" max="2" width="28.86"/>
     <col customWidth="1" min="3" max="3" width="10.86"/>
     <col customWidth="1" min="4" max="4" width="17.43"/>
     <col customWidth="1" min="5" max="5" width="17.0"/>
@@ -21394,10 +21448,10 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="110" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
@@ -21411,14 +21465,14 @@
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="8" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -21427,25 +21481,25 @@
     </row>
     <row r="3" ht="13.5" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="109" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="81" t="s">
+      <c r="B4" s="111" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="81" t="s">
+      <c r="E4" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="81" t="s">
+      <c r="F4" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="81" t="s">
+      <c r="G4" s="83" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="34" t="s">
@@ -21454,78 +21508,78 @@
       <c r="I4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="81" t="s">
+      <c r="J4" s="83" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="B5" s="110"/>
+        <v>442</v>
+      </c>
+      <c r="B5" s="112"/>
       <c r="C5" s="15" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="23" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="K5" s="15"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>441</v>
-      </c>
-      <c r="B6" s="110"/>
+        <v>448</v>
+      </c>
+      <c r="B6" s="112"/>
       <c r="C6" s="15" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="23" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>447</v>
-      </c>
-      <c r="B7" s="110" t="s">
-        <v>448</v>
+        <v>454</v>
+      </c>
+      <c r="B7" s="112" t="s">
+        <v>455</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
@@ -21533,29 +21587,29 @@
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="K7" s="15"/>
-      <c r="L7" s="111" t="s">
-        <v>454</v>
+      <c r="L7" s="113" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>455</v>
-      </c>
-      <c r="B8" s="110"/>
+        <v>462</v>
+      </c>
+      <c r="B8" s="112"/>
       <c r="C8" s="15" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
@@ -21563,26 +21617,26 @@
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="23" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="K8" s="15"/>
     </row>
     <row r="9" ht="199.5" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="B9" s="110"/>
+        <v>468</v>
+      </c>
+      <c r="B9" s="112"/>
       <c r="C9" s="15" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
@@ -21590,78 +21644,78 @@
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>466</v>
-      </c>
-      <c r="B10" s="110" t="s">
-        <v>467</v>
+        <v>473</v>
+      </c>
+      <c r="B10" s="112" t="s">
+        <v>474</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="F10" s="90"/>
+        <v>477</v>
+      </c>
+      <c r="F10" s="92"/>
       <c r="G10" s="15">
         <v>1.0</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="23" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>472</v>
-      </c>
-      <c r="B11" s="110"/>
+        <v>479</v>
+      </c>
+      <c r="B11" s="112"/>
       <c r="C11" s="15" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="23" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="K11" s="15"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>478</v>
-      </c>
-      <c r="B12" s="110" t="s">
-        <v>479</v>
+        <v>485</v>
+      </c>
+      <c r="B12" s="112" t="s">
+        <v>486</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15">
@@ -21669,149 +21723,149 @@
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="B13" s="110"/>
+        <v>491</v>
+      </c>
+      <c r="B13" s="112"/>
       <c r="C13" s="15" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="23" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>489</v>
-      </c>
-      <c r="B14" s="110"/>
+        <v>496</v>
+      </c>
+      <c r="B14" s="112"/>
       <c r="C14" s="15" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>494</v>
-      </c>
-      <c r="B15" s="110"/>
+        <v>501</v>
+      </c>
+      <c r="B15" s="112"/>
       <c r="C15" s="15" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>497</v>
-      </c>
-      <c r="F15" s="87" t="s">
-        <v>498</v>
+        <v>504</v>
+      </c>
+      <c r="F15" s="89" t="s">
+        <v>505</v>
       </c>
       <c r="G15" s="15">
         <v>1.0</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="23" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="K15" s="15"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>501</v>
-      </c>
-      <c r="B16" s="110"/>
+        <v>508</v>
+      </c>
+      <c r="B16" s="112"/>
       <c r="C16" s="15" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="23" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="K16" s="15"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>506</v>
-      </c>
-      <c r="B17" s="110"/>
+        <v>513</v>
+      </c>
+      <c r="B17" s="112"/>
       <c r="C17" s="15" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="23" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="K17" s="15"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>512</v>
-      </c>
-      <c r="B18" s="110"/>
+        <v>519</v>
+      </c>
+      <c r="B18" s="112"/>
       <c r="C18" s="15" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15">
@@ -21819,7 +21873,7 @@
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="23" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>

</xml_diff>

<commit_message>
NAV-172 Remove first ADR task
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mjiNpm5AzZuJU2TnI9xV+4aLknm9A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhXm71E5VMdC1qXIcBprYdxJCNlxg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -77,7 +77,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mj819Io1FNxZ4HoiNPoz9tksp3vbA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjRTiHm/bb3hoFY4mbh/FCIGzfI2Q=="/>
     </ext>
   </extLst>
 </comments>
@@ -89,7 +89,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="E9">
+    <comment authorId="0" ref="E8">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5eY
@@ -99,7 +99,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E12">
+    <comment authorId="0" ref="E11">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5d8
@@ -109,7 +109,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E11">
+    <comment authorId="0" ref="E10">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5d0
@@ -119,7 +119,7 @@
 	-Jonathan Berry</t>
       </text>
     </comment>
-    <comment authorId="0" ref="E10">
+    <comment authorId="0" ref="E9">
       <text>
         <t xml:space="preserve">======
 ID#AAAASYjj5dw
@@ -158,7 +158,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgHlTMUvHUTre4T4ahVahmEueX3vg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgYos0niKmTsh4KflH2MPzKEKqG+w=="/>
     </ext>
   </extLst>
 </comments>
@@ -240,7 +240,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="596">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -686,27 +686,6 @@
     <t>ADR-01-10</t>
   </si>
   <si>
-    <t>Associate your ADR account with an organization as an editor</t>
-  </si>
-  <si>
-    <t>Is user a member of an organization (country) with an "editor" role on ADR?</t>
-  </si>
-  <si>
-    <t>In order to take advantage of the features available to users on the AIDS Data Repository, you must register an account. It is a quick and simple process. There is an instructional video available on Youtube which will demonstrate how to register and join an organization. Typically, the organization is your country. In order to upload and edit data, you must be an "editor" or "admin". Request the one most appropriate for your estimates role when you are requesting access to the organization.</t>
-  </si>
-  <si>
-    <t>Registering and Joining an Organisation - The AIDS Data Repository https://www.youtube.com/watch?v=O34wTKvn1xI</t>
-  </si>
-  <si>
-    <t>MM Would recomend linking to training manuals instead of youtube</t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-ADR-01-10-A')</t>
-  </si>
-  <si>
-    <t>ADR-01-11</t>
-  </si>
-  <si>
     <t>Check that the required data has been preloaded into your ADR dataset</t>
   </si>
   <si>
@@ -728,7 +707,7 @@
     <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum'], 'url', '.*')</t>
   </si>
   <si>
-    <t>ADR-01-12</t>
+    <t>ADR-01-11</t>
   </si>
   <si>
     <t>Upload data inputs to the ADR using the required templates</t>
@@ -750,7 +729,7 @@
 - Click "Upload Files"</t>
   </si>
   <si>
-    <t>check_manual_confirmation('EST-ADR-01-12-A')</t>
+    <t>check_manual_confirmation('EST-ADR-01-11-A')</t>
   </si>
   <si>
     <t>ADR-02-01</t>
@@ -3018,7 +2997,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="114">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3131,20 +3110,14 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -10215,7 +10188,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -10232,44 +10205,44 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="30">
         <v>0.2</v>
       </c>
-      <c r="G2" s="114"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="111" t="s">
-        <v>527</v>
-      </c>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="109" t="s">
+        <v>520</v>
+      </c>
+      <c r="C4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="81" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="34" t="s">
@@ -10278,26 +10251,26 @@
       <c r="I4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="83" t="s">
+      <c r="J4" s="81" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>528</v>
-      </c>
-      <c r="B5" s="112"/>
+        <v>521</v>
+      </c>
+      <c r="B5" s="110"/>
       <c r="C5" s="15" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15">
@@ -10305,26 +10278,26 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="23" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>533</v>
-      </c>
-      <c r="B6" s="112" t="s">
-        <v>534</v>
+        <v>526</v>
+      </c>
+      <c r="B6" s="110" t="s">
+        <v>527</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15">
@@ -10332,186 +10305,186 @@
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="23" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="B7" s="112"/>
+        <v>533</v>
+      </c>
+      <c r="B7" s="110"/>
       <c r="C7" s="15" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>542</v>
-      </c>
-      <c r="J7" s="92"/>
+        <v>535</v>
+      </c>
+      <c r="J7" s="90"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>543</v>
-      </c>
-      <c r="B8" s="112"/>
+        <v>536</v>
+      </c>
+      <c r="B8" s="110"/>
       <c r="C8" s="15" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="23" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>545</v>
-      </c>
-      <c r="B9" s="112" t="s">
-        <v>546</v>
+        <v>538</v>
+      </c>
+      <c r="B9" s="110" t="s">
+        <v>539</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>549</v>
-      </c>
-      <c r="B10" s="112" t="s">
-        <v>550</v>
+        <v>542</v>
+      </c>
+      <c r="B10" s="110" t="s">
+        <v>543</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>553</v>
-      </c>
-      <c r="F10" s="99" t="s">
-        <v>274</v>
+        <v>546</v>
+      </c>
+      <c r="F10" s="97" t="s">
+        <v>267</v>
       </c>
       <c r="G10" s="15">
         <v>1.0</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="23" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>555</v>
-      </c>
-      <c r="B11" s="112"/>
+        <v>548</v>
+      </c>
+      <c r="B11" s="110"/>
       <c r="C11" s="15" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>558</v>
-      </c>
-      <c r="F11" s="99" t="s">
-        <v>559</v>
+        <v>551</v>
+      </c>
+      <c r="F11" s="97" t="s">
+        <v>552</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="23" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>561</v>
-      </c>
-      <c r="B12" s="112" t="s">
-        <v>562</v>
+        <v>554</v>
+      </c>
+      <c r="B12" s="110" t="s">
+        <v>555</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>564</v>
-      </c>
-      <c r="E12" s="89" t="s">
-        <v>565</v>
+        <v>557</v>
+      </c>
+      <c r="E12" s="87" t="s">
+        <v>558</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="G12" s="15">
         <v>1.0</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="K12" s="15"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>569</v>
-      </c>
-      <c r="B13" s="112" t="s">
-        <v>570</v>
+        <v>562</v>
+      </c>
+      <c r="B13" s="110" t="s">
+        <v>563</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15">
@@ -10519,53 +10492,53 @@
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="23" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>575</v>
-      </c>
-      <c r="B14" s="112" t="s">
-        <v>576</v>
+        <v>568</v>
+      </c>
+      <c r="B14" s="110" t="s">
+        <v>569</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="G14" s="15">
         <v>1.0</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="23" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>582</v>
-      </c>
-      <c r="B15" s="112"/>
+        <v>575</v>
+      </c>
+      <c r="B15" s="110"/>
       <c r="C15" s="15" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15">
@@ -10573,47 +10546,47 @@
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="23" t="s">
-        <v>586</v>
-      </c>
-      <c r="J15" s="92"/>
+        <v>579</v>
+      </c>
+      <c r="J15" s="90"/>
       <c r="K15" s="15"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>587</v>
-      </c>
-      <c r="B16" s="112"/>
+        <v>580</v>
+      </c>
+      <c r="B16" s="110"/>
       <c r="C16" s="15" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="23" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>592</v>
-      </c>
-      <c r="B17" s="112"/>
+        <v>585</v>
+      </c>
+      <c r="B17" s="110"/>
       <c r="C17" s="15" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15">
@@ -10621,34 +10594,34 @@
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="23" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>597</v>
-      </c>
-      <c r="B18" s="112"/>
+        <v>590</v>
+      </c>
+      <c r="B18" s="110"/>
       <c r="C18" s="15" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="G18" s="15">
         <v>1.0</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="23" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
@@ -13291,7 +13264,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="92.25" customHeight="1">
+    <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="50" t="s">
         <v>116</v>
       </c>
@@ -13304,134 +13277,148 @@
       <c r="D5" s="51" t="s">
         <v>119</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="37"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="52">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="53" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="51" t="s">
+    </row>
+    <row r="6" ht="168.0" customHeight="1">
+      <c r="A6" s="50" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="6" ht="12.0" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="C6" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="D6" s="53" t="s">
         <v>125</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>126</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="39"/>
-      <c r="G6" s="53" t="s">
+      <c r="G6" s="54"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="55" t="s">
+        <v>126</v>
+      </c>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="56"/>
+      <c r="W6" s="56"/>
+      <c r="X6" s="56"/>
+      <c r="Y6" s="56"/>
+    </row>
+    <row r="7" ht="12.0" customHeight="1">
+      <c r="A7" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="17" t="s">
+      <c r="B7" s="37" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" ht="69.0" customHeight="1">
-      <c r="A7" s="54" t="s">
+      <c r="C7" s="37" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="D7" s="51" t="s">
         <v>130</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="E7" s="37"/>
+      <c r="F7" s="39">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="54"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="56"/>
+      <c r="U7" s="56"/>
+      <c r="V7" s="56"/>
+      <c r="W7" s="56"/>
+      <c r="X7" s="56"/>
+      <c r="Y7" s="56"/>
+    </row>
+    <row r="8" ht="26.25" customHeight="1">
+      <c r="A8" s="57" t="s">
         <v>132</v>
       </c>
-      <c r="E7" s="37"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="57" t="s">
+      <c r="B8" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-    </row>
-    <row r="8" ht="12.0" customHeight="1">
-      <c r="A8" s="59" t="s">
+      <c r="C8" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="D8" s="51" t="s">
         <v>135</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="E8" s="42" t="s">
         <v>136</v>
       </c>
-      <c r="D8" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="37"/>
       <c r="F8" s="39">
         <v>1.0</v>
       </c>
-      <c r="G8" s="56"/>
+      <c r="G8" s="37"/>
       <c r="H8" s="18"/>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" ht="99.75" customHeight="1">
+      <c r="A9" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="58"/>
-    </row>
-    <row r="9" ht="26.25" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="B9" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="C9" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="51" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="E9" s="42" t="s">
         <v>142</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>143</v>
       </c>
       <c r="F9" s="39">
         <v>1.0</v>
@@ -13439,7 +13426,7 @@
       <c r="G9" s="37"/>
       <c r="H9" s="18"/>
       <c r="I9" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
@@ -13458,29 +13445,29 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
     </row>
-    <row r="10" ht="99.75" customHeight="1">
-      <c r="A10" s="59" t="s">
+    <row r="10" ht="12.0" customHeight="1">
+      <c r="A10" s="58" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="C10" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="D10" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="E10" s="60" t="s">
         <v>148</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="F10" s="61">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="62"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="64" t="s">
         <v>149</v>
-      </c>
-      <c r="F10" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="37"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18" t="s">
-        <v>150</v>
       </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
@@ -13500,86 +13487,46 @@
       <c r="Y10" s="6"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>151</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="C11" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="61" t="s">
+      <c r="D11" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="E11" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="F11" s="37">
+        <v>1.0</v>
+      </c>
+      <c r="G11" s="37"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="F11" s="63">
-        <v>1.0</v>
-      </c>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="66" t="s">
-        <v>156</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="6"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-      <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-    </row>
-    <row r="12" ht="12.0" customHeight="1">
-      <c r="A12" s="59" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="F12" s="37">
-        <v>1.0</v>
-      </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="67"/>
-      <c r="O12" s="67"/>
-      <c r="P12" s="67"/>
-      <c r="Q12" s="67"/>
-      <c r="R12" s="67"/>
-      <c r="S12" s="67"/>
-      <c r="T12" s="67"/>
-      <c r="U12" s="67"/>
-      <c r="V12" s="67"/>
-      <c r="W12" s="67"/>
-      <c r="X12" s="67"/>
-    </row>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+      <c r="S11" s="65"/>
+      <c r="T11" s="65"/>
+      <c r="U11" s="65"/>
+      <c r="V11" s="65"/>
+      <c r="W11" s="65"/>
+      <c r="X11" s="65"/>
+    </row>
+    <row r="12" ht="12.0" customHeight="1"/>
     <row r="13" ht="12.0" customHeight="1"/>
     <row r="14" ht="12.0" customHeight="1"/>
     <row r="15" ht="12.0" customHeight="1"/>
@@ -14564,7 +14511,6 @@
     <row r="994" ht="12.0" customHeight="1"/>
     <row r="995" ht="12.0" customHeight="1"/>
     <row r="996" ht="12.0" customHeight="1"/>
-    <row r="997" ht="12.0" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -14572,10 +14518,10 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="E9"/>
-    <hyperlink r:id="rId3" ref="E10"/>
-    <hyperlink r:id="rId4" ref="E11"/>
-    <hyperlink r:id="rId5" ref="E12"/>
+    <hyperlink r:id="rId2" ref="E8"/>
+    <hyperlink r:id="rId3" ref="E9"/>
+    <hyperlink r:id="rId4" ref="E10"/>
+    <hyperlink r:id="rId5" ref="E11"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -14608,7 +14554,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -14625,14 +14571,14 @@
     </row>
     <row r="2" ht="48.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -14678,143 +14624,143 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="69" t="s">
-        <v>166</v>
-      </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="70" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="71">
+      <c r="A5" s="67" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="67"/>
+      <c r="C5" s="68" t="s">
+        <v>160</v>
+      </c>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="69">
         <v>1.0</v>
       </c>
-      <c r="G5" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74" t="s">
-        <v>169</v>
+      <c r="G5" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="H5" s="71"/>
+      <c r="I5" s="72" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="37" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="F6" s="75">
+        <v>167</v>
+      </c>
+      <c r="F6" s="73">
         <v>1.0</v>
       </c>
-      <c r="G6" s="76"/>
+      <c r="G6" s="74"/>
       <c r="H6" s="15"/>
       <c r="I6" s="23" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="37" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="75">
+      <c r="F7" s="73">
         <v>1.0</v>
       </c>
-      <c r="G7" s="76"/>
+      <c r="G7" s="74"/>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E8" s="18"/>
-      <c r="F8" s="75">
+      <c r="F8" s="73">
         <v>1.0</v>
       </c>
-      <c r="G8" s="76"/>
+      <c r="G8" s="74"/>
       <c r="H8" s="15"/>
       <c r="I8" s="23" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="37" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="73">
         <v>1.0</v>
       </c>
-      <c r="G9" s="76"/>
+      <c r="G9" s="74"/>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="37" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E10" s="37"/>
-      <c r="F10" s="76">
+      <c r="F10" s="74">
         <v>1.0</v>
       </c>
-      <c r="G10" s="77"/>
+      <c r="G10" s="75"/>
       <c r="H10" s="21"/>
       <c r="I10" s="23" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -15915,7 +15861,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -15931,15 +15877,15 @@
       </c>
     </row>
     <row r="2" ht="48.0" customHeight="1">
-      <c r="A2" s="78" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>197</v>
+      <c r="A2" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>190</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="79" t="s">
-        <v>165</v>
+      <c r="D2" s="77" t="s">
+        <v>158</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -15956,8 +15902,8 @@
       <c r="G3" s="32"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="80" t="s">
-        <v>198</v>
+      <c r="A4" s="78" t="s">
+        <v>191</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>9</v>
@@ -15989,166 +15935,166 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="37" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="75">
+      <c r="G5" s="73">
         <v>1.0</v>
       </c>
-      <c r="H5" s="77"/>
+      <c r="H5" s="75"/>
       <c r="I5" s="15"/>
-      <c r="J5" s="81" t="s">
-        <v>204</v>
+      <c r="J5" s="79" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="37" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="G6" s="75">
+        <v>202</v>
+      </c>
+      <c r="G6" s="73">
         <v>1.0</v>
       </c>
-      <c r="H6" s="76"/>
+      <c r="H6" s="74"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="69" t="s">
-        <v>211</v>
-      </c>
-      <c r="B7" s="69" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69" t="s">
-        <v>213</v>
-      </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="71">
+      <c r="A7" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="69">
         <v>1.0</v>
       </c>
-      <c r="H7" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73" t="s">
-        <v>204</v>
+      <c r="H7" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="B8" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>188</v>
-      </c>
       <c r="E8" s="37" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="G8" s="75">
+        <v>209</v>
+      </c>
+      <c r="G8" s="73">
         <v>1.0</v>
       </c>
-      <c r="H8" s="76"/>
+      <c r="H8" s="74"/>
       <c r="I8" s="15"/>
       <c r="J8" s="15" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="37" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="E9" s="37" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" s="76">
+        <v>209</v>
+      </c>
+      <c r="G9" s="74">
         <v>1.0</v>
       </c>
-      <c r="H9" s="82" t="s">
-        <v>222</v>
+      <c r="H9" s="80" t="s">
+        <v>215</v>
       </c>
       <c r="I9" s="21"/>
       <c r="J9" s="15" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="37" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="B10" s="37" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E10" s="37" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="F10" s="37"/>
-      <c r="G10" s="75">
+      <c r="G10" s="73">
         <v>1.0</v>
       </c>
       <c r="H10" s="37"/>
       <c r="I10" s="19"/>
       <c r="J10" s="15" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -17253,7 +17199,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="12.0" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -17270,14 +17216,14 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -17286,31 +17232,31 @@
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="84" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="82" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="83" t="s">
+      <c r="H4" s="81" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="86" t="s">
+      <c r="I4" s="84" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="34" t="s">
@@ -17319,46 +17265,46 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="B5" s="87"/>
+        <v>226</v>
+      </c>
+      <c r="B5" s="85"/>
       <c r="C5" s="15" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E5" s="88" t="s">
-        <v>236</v>
-      </c>
-      <c r="F5" s="89" t="s">
-        <v>237</v>
+        <v>228</v>
+      </c>
+      <c r="E5" s="86" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" s="87" t="s">
+        <v>230</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="B6" s="87"/>
+        <v>233</v>
+      </c>
+      <c r="B6" s="85"/>
       <c r="C6" s="15" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E6" s="88" t="s">
-        <v>243</v>
+        <v>235</v>
+      </c>
+      <c r="E6" s="86" t="s">
+        <v>236</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="G6" s="15">
         <v>1.0</v>
@@ -17366,22 +17312,22 @@
       <c r="H6" s="19"/>
       <c r="I6" s="15"/>
       <c r="J6" s="23" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="B7" s="90"/>
+        <v>239</v>
+      </c>
+      <c r="B7" s="88"/>
       <c r="C7" s="15" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E7" s="88" t="s">
-        <v>249</v>
+        <v>241</v>
+      </c>
+      <c r="E7" s="86" t="s">
+        <v>242</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
@@ -17390,381 +17336,381 @@
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="23" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="B8" s="87"/>
+        <v>244</v>
+      </c>
+      <c r="B8" s="85"/>
       <c r="C8" s="15" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>253</v>
-      </c>
-      <c r="E8" s="88" t="s">
-        <v>254</v>
+        <v>246</v>
+      </c>
+      <c r="E8" s="86" t="s">
+        <v>247</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="23" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="B9" s="90" t="s">
-        <v>258</v>
+        <v>250</v>
+      </c>
+      <c r="B9" s="88" t="s">
+        <v>251</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="E9" s="88" t="s">
-        <v>261</v>
-      </c>
-      <c r="F9" s="89" t="s">
-        <v>262</v>
+        <v>253</v>
+      </c>
+      <c r="E9" s="86" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" s="87" t="s">
+        <v>255</v>
       </c>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="23" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>264</v>
-      </c>
-      <c r="B10" s="90"/>
+        <v>257</v>
+      </c>
+      <c r="B10" s="88"/>
       <c r="C10" s="15" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="E10" s="88" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="91"/>
+        <v>259</v>
+      </c>
+      <c r="E10" s="86" t="s">
+        <v>260</v>
+      </c>
+      <c r="F10" s="89"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="59" t="s">
-        <v>268</v>
+      <c r="H10" s="57" t="s">
+        <v>261</v>
       </c>
       <c r="I10" s="21"/>
       <c r="J10" s="23" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" ht="57.0" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="B11" s="90"/>
+        <v>263</v>
+      </c>
+      <c r="B11" s="88"/>
       <c r="C11" s="15" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>272</v>
-      </c>
-      <c r="E11" s="88" t="s">
-        <v>273</v>
+        <v>265</v>
+      </c>
+      <c r="E11" s="86" t="s">
+        <v>266</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="92"/>
+      <c r="H11" s="90"/>
       <c r="I11" s="19"/>
       <c r="J11" s="23" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" ht="12.0" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>276</v>
-      </c>
-      <c r="B12" s="87" t="s">
-        <v>277</v>
+        <v>269</v>
+      </c>
+      <c r="B12" s="85" t="s">
+        <v>270</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>279</v>
-      </c>
-      <c r="E12" s="88" t="s">
-        <v>280</v>
+        <v>272</v>
+      </c>
+      <c r="E12" s="86" t="s">
+        <v>273</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G12" s="15"/>
-      <c r="H12" s="59"/>
+      <c r="H12" s="57"/>
       <c r="I12" s="15"/>
       <c r="J12" s="23" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="B13" s="93"/>
+        <v>275</v>
+      </c>
+      <c r="B13" s="91"/>
       <c r="C13" s="15" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="E13" s="88" t="s">
-        <v>285</v>
+        <v>277</v>
+      </c>
+      <c r="E13" s="86" t="s">
+        <v>278</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
-      <c r="H13" s="59" t="s">
-        <v>286</v>
+      <c r="H13" s="57" t="s">
+        <v>279</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="23" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="B14" s="90" t="s">
-        <v>289</v>
+        <v>281</v>
+      </c>
+      <c r="B14" s="88" t="s">
+        <v>282</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>291</v>
-      </c>
-      <c r="E14" s="88" t="s">
-        <v>292</v>
+        <v>284</v>
+      </c>
+      <c r="E14" s="86" t="s">
+        <v>285</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G14" s="15"/>
-      <c r="H14" s="59"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="15"/>
       <c r="J14" s="23" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="B15" s="90" t="s">
-        <v>295</v>
+        <v>287</v>
+      </c>
+      <c r="B15" s="88" t="s">
+        <v>288</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>297</v>
-      </c>
-      <c r="E15" s="88" t="s">
-        <v>298</v>
+        <v>290</v>
+      </c>
+      <c r="E15" s="86" t="s">
+        <v>291</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="15" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="23" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" ht="12.0" customHeight="1">
-      <c r="A16" s="73" t="s">
-        <v>301</v>
-      </c>
-      <c r="B16" s="90"/>
-      <c r="C16" s="73"/>
-      <c r="D16" s="73" t="s">
-        <v>302</v>
-      </c>
-      <c r="E16" s="94"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="73">
+      <c r="A16" s="71" t="s">
+        <v>294</v>
+      </c>
+      <c r="B16" s="88"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71" t="s">
+        <v>295</v>
+      </c>
+      <c r="E16" s="92"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71">
         <v>1.0</v>
       </c>
-      <c r="H16" s="95" t="s">
-        <v>303</v>
+      <c r="H16" s="93" t="s">
+        <v>296</v>
       </c>
       <c r="I16" s="21"/>
-      <c r="J16" s="74" t="s">
-        <v>304</v>
+      <c r="J16" s="72" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="B17" s="90" t="s">
-        <v>306</v>
-      </c>
-      <c r="C17" s="81" t="s">
-        <v>307</v>
-      </c>
-      <c r="D17" s="81" t="s">
-        <v>308</v>
-      </c>
-      <c r="E17" s="96" t="s">
-        <v>309</v>
-      </c>
-      <c r="F17" s="97" t="s">
-        <v>310</v>
-      </c>
-      <c r="G17" s="81"/>
-      <c r="H17" s="98"/>
+        <v>298</v>
+      </c>
+      <c r="B17" s="88" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>300</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>301</v>
+      </c>
+      <c r="E17" s="94" t="s">
+        <v>302</v>
+      </c>
+      <c r="F17" s="95" t="s">
+        <v>303</v>
+      </c>
+      <c r="G17" s="79"/>
+      <c r="H17" s="96"/>
       <c r="I17" s="15"/>
       <c r="J17" s="23" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="B18" s="90" t="s">
-        <v>313</v>
-      </c>
-      <c r="C18" s="81" t="s">
-        <v>314</v>
-      </c>
-      <c r="D18" s="81" t="s">
-        <v>315</v>
-      </c>
-      <c r="E18" s="96" t="s">
-        <v>316</v>
-      </c>
-      <c r="F18" s="97" t="s">
-        <v>310</v>
-      </c>
-      <c r="G18" s="81"/>
-      <c r="H18" s="98"/>
+        <v>305</v>
+      </c>
+      <c r="B18" s="88" t="s">
+        <v>306</v>
+      </c>
+      <c r="C18" s="79" t="s">
+        <v>307</v>
+      </c>
+      <c r="D18" s="79" t="s">
+        <v>308</v>
+      </c>
+      <c r="E18" s="94" t="s">
+        <v>309</v>
+      </c>
+      <c r="F18" s="95" t="s">
+        <v>303</v>
+      </c>
+      <c r="G18" s="79"/>
+      <c r="H18" s="96"/>
       <c r="I18" s="15"/>
       <c r="J18" s="23" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="15" t="s">
-        <v>318</v>
-      </c>
-      <c r="B19" s="90" t="s">
-        <v>319</v>
+        <v>311</v>
+      </c>
+      <c r="B19" s="88" t="s">
+        <v>312</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="E19" s="88" t="s">
-        <v>322</v>
-      </c>
-      <c r="F19" s="99" t="s">
-        <v>310</v>
+        <v>314</v>
+      </c>
+      <c r="E19" s="86" t="s">
+        <v>315</v>
+      </c>
+      <c r="F19" s="97" t="s">
+        <v>303</v>
       </c>
       <c r="G19" s="15"/>
-      <c r="H19" s="92"/>
+      <c r="H19" s="90"/>
       <c r="I19" s="15"/>
       <c r="J19" s="23" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
     </row>
     <row r="20" ht="12.0" customHeight="1">
       <c r="A20" s="15" t="s">
-        <v>324</v>
-      </c>
-      <c r="B20" s="90" t="s">
-        <v>325</v>
+        <v>317</v>
+      </c>
+      <c r="B20" s="88" t="s">
+        <v>318</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>327</v>
-      </c>
-      <c r="E20" s="88" t="s">
-        <v>328</v>
-      </c>
-      <c r="F20" s="99" t="s">
-        <v>329</v>
+        <v>320</v>
+      </c>
+      <c r="E20" s="86" t="s">
+        <v>321</v>
+      </c>
+      <c r="F20" s="97" t="s">
+        <v>322</v>
       </c>
       <c r="G20" s="15"/>
-      <c r="H20" s="92"/>
+      <c r="H20" s="90"/>
       <c r="I20" s="15"/>
       <c r="J20" s="23" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="15" t="s">
-        <v>331</v>
-      </c>
-      <c r="B21" s="90" t="s">
-        <v>332</v>
+        <v>324</v>
+      </c>
+      <c r="B21" s="88" t="s">
+        <v>325</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>334</v>
-      </c>
-      <c r="E21" s="88" t="s">
-        <v>335</v>
-      </c>
-      <c r="F21" s="99" t="s">
-        <v>310</v>
+        <v>327</v>
+      </c>
+      <c r="E21" s="86" t="s">
+        <v>328</v>
+      </c>
+      <c r="F21" s="97" t="s">
+        <v>303</v>
       </c>
       <c r="G21" s="15"/>
-      <c r="H21" s="92"/>
+      <c r="H21" s="90"/>
       <c r="I21" s="21"/>
       <c r="J21" s="23" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
     </row>
     <row r="22" ht="12.0" customHeight="1">
-      <c r="A22" s="73" t="s">
-        <v>337</v>
-      </c>
-      <c r="B22" s="100"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73" t="s">
-        <v>338</v>
-      </c>
-      <c r="E22" s="94"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="102">
+      <c r="A22" s="71" t="s">
+        <v>330</v>
+      </c>
+      <c r="B22" s="98"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71" t="s">
+        <v>331</v>
+      </c>
+      <c r="E22" s="92"/>
+      <c r="F22" s="99"/>
+      <c r="G22" s="100">
         <v>1.0</v>
       </c>
-      <c r="H22" s="95" t="s">
-        <v>339</v>
+      <c r="H22" s="93" t="s">
+        <v>332</v>
       </c>
       <c r="I22" s="15"/>
-      <c r="J22" s="74" t="s">
-        <v>340</v>
+      <c r="J22" s="72" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="23" ht="12.0" customHeight="1">
@@ -18835,7 +18781,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -18851,15 +18797,15 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="78" t="s">
-        <v>341</v>
-      </c>
-      <c r="B2" s="79" t="s">
-        <v>342</v>
+      <c r="A2" s="76" t="s">
+        <v>334</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>335</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="79" t="s">
-        <v>343</v>
+      <c r="D2" s="77" t="s">
+        <v>336</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -18868,29 +18814,29 @@
     </row>
     <row r="3" ht="14.25" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="83" t="s">
-        <v>344</v>
+      <c r="G4" s="81" t="s">
+        <v>337</v>
       </c>
       <c r="H4" s="49" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="I4" s="34" t="s">
         <v>16</v>
@@ -18901,138 +18847,138 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="59"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="15"/>
       <c r="J5" s="23" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="88" t="s">
-        <v>355</v>
+      <c r="G6" s="86" t="s">
+        <v>348</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="23" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="88" t="s">
-        <v>355</v>
+      <c r="G7" s="86" t="s">
+        <v>348</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="15"/>
       <c r="J7" s="23" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15">
         <v>1.0</v>
       </c>
-      <c r="G8" s="88"/>
+      <c r="G8" s="86"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15"/>
       <c r="J8" s="23" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="E9" s="103" t="s">
-        <v>371</v>
+        <v>363</v>
+      </c>
+      <c r="E9" s="101" t="s">
+        <v>364</v>
       </c>
       <c r="F9" s="15">
         <v>1.0</v>
       </c>
-      <c r="G9" s="88" t="s">
-        <v>372</v>
+      <c r="G9" s="86" t="s">
+        <v>365</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="21"/>
       <c r="J9" s="23" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15">
@@ -19042,24 +18988,24 @@
       <c r="H10" s="15"/>
       <c r="I10" s="15"/>
       <c r="J10" s="23" t="s">
-        <v>378</v>
-      </c>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="67"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="67"/>
-      <c r="Y10" s="67"/>
-      <c r="Z10" s="67"/>
+        <v>371</v>
+      </c>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="65"/>
+      <c r="X10" s="65"/>
+      <c r="Y10" s="65"/>
+      <c r="Z10" s="65"/>
     </row>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>
@@ -20090,7 +20036,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
@@ -20107,14 +20053,14 @@
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="30" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -20122,25 +20068,25 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="J3" s="104"/>
+      <c r="J3" s="102"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="83" t="s">
+      <c r="C4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="81" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="34" t="s">
@@ -20149,93 +20095,93 @@
       <c r="H4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="83" t="s">
-        <v>344</v>
+      <c r="I4" s="81" t="s">
+        <v>337</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="C5" s="59" t="s">
-        <v>384</v>
-      </c>
-      <c r="D5" s="59" t="s">
-        <v>385</v>
-      </c>
-      <c r="E5" s="92"/>
+        <v>376</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>377</v>
+      </c>
+      <c r="D5" s="57" t="s">
+        <v>378</v>
+      </c>
+      <c r="E5" s="90"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="23" t="s">
-        <v>386</v>
-      </c>
-      <c r="I5" s="105"/>
-      <c r="J5" s="59"/>
+        <v>379</v>
+      </c>
+      <c r="I5" s="103"/>
+      <c r="J5" s="57"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="F6" s="15">
         <v>1.0</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="23" t="s">
-        <v>392</v>
-      </c>
-      <c r="I6" s="88"/>
+        <v>385</v>
+      </c>
+      <c r="I6" s="86"/>
       <c r="J6" s="15"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="106" t="s">
-        <v>393</v>
-      </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106" t="s">
-        <v>394</v>
-      </c>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
-      <c r="G7" s="106"/>
-      <c r="H7" s="74" t="s">
-        <v>395</v>
-      </c>
-      <c r="I7" s="107" t="s">
-        <v>396</v>
-      </c>
-      <c r="J7" s="108"/>
+      <c r="A7" s="104" t="s">
+        <v>386</v>
+      </c>
+      <c r="B7" s="104"/>
+      <c r="C7" s="104" t="s">
+        <v>387</v>
+      </c>
+      <c r="D7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="104"/>
+      <c r="G7" s="104"/>
+      <c r="H7" s="72" t="s">
+        <v>388</v>
+      </c>
+      <c r="I7" s="105" t="s">
+        <v>389</v>
+      </c>
+      <c r="J7" s="106"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E8" s="15"/>
       <c r="F8" s="15">
@@ -20243,45 +20189,45 @@
       </c>
       <c r="G8" s="15"/>
       <c r="H8" s="23" t="s">
-        <v>401</v>
-      </c>
-      <c r="I8" s="88"/>
-      <c r="J8" s="109"/>
+        <v>394</v>
+      </c>
+      <c r="I8" s="86"/>
+      <c r="J8" s="107"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="23" t="s">
-        <v>406</v>
-      </c>
-      <c r="I9" s="88"/>
-      <c r="J9" s="109"/>
+        <v>399</v>
+      </c>
+      <c r="I9" s="86"/>
+      <c r="J9" s="107"/>
     </row>
     <row r="10" ht="115.5" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="E10" s="15"/>
       <c r="F10" s="15">
@@ -20289,47 +20235,47 @@
       </c>
       <c r="G10" s="15"/>
       <c r="H10" s="23" t="s">
-        <v>411</v>
-      </c>
-      <c r="I10" s="88" t="s">
-        <v>412</v>
-      </c>
-      <c r="J10" s="109"/>
+        <v>404</v>
+      </c>
+      <c r="I10" s="86" t="s">
+        <v>405</v>
+      </c>
+      <c r="J10" s="107"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="23" t="s">
-        <v>417</v>
-      </c>
-      <c r="I11" s="88"/>
-      <c r="J11" s="109"/>
+        <v>410</v>
+      </c>
+      <c r="I11" s="86"/>
+      <c r="J11" s="107"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="15">
@@ -20337,47 +20283,47 @@
       </c>
       <c r="G12" s="15"/>
       <c r="H12" s="23" t="s">
-        <v>422</v>
-      </c>
-      <c r="I12" s="88" t="s">
-        <v>423</v>
-      </c>
-      <c r="J12" s="109"/>
+        <v>415</v>
+      </c>
+      <c r="I12" s="86" t="s">
+        <v>416</v>
+      </c>
+      <c r="J12" s="107"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="23" t="s">
-        <v>428</v>
-      </c>
-      <c r="I13" s="88"/>
-      <c r="J13" s="109"/>
+        <v>421</v>
+      </c>
+      <c r="I13" s="86"/>
+      <c r="J13" s="107"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="15">
@@ -20385,32 +20331,32 @@
       </c>
       <c r="G14" s="15"/>
       <c r="H14" s="23" t="s">
-        <v>433</v>
-      </c>
-      <c r="I14" s="88"/>
-      <c r="J14" s="109"/>
+        <v>426</v>
+      </c>
+      <c r="I14" s="86"/>
+      <c r="J14" s="107"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
       <c r="H15" s="23" t="s">
-        <v>438</v>
-      </c>
-      <c r="I15" s="88"/>
-      <c r="J15" s="109"/>
+        <v>431</v>
+      </c>
+      <c r="I15" s="86"/>
+      <c r="J15" s="107"/>
     </row>
     <row r="16" ht="14.25" customHeight="1">
       <c r="C16" s="26"/>
@@ -21448,10 +21394,10 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="108" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3"/>
@@ -21465,14 +21411,14 @@
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="29" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="8" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="29">
@@ -21481,25 +21427,25 @@
     </row>
     <row r="3" ht="13.5" customHeight="1"/>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="83" t="s">
+      <c r="A4" s="81" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="111" t="s">
-        <v>232</v>
-      </c>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="109" t="s">
+        <v>225</v>
+      </c>
+      <c r="C4" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="83" t="s">
+      <c r="D4" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="83" t="s">
+      <c r="E4" s="81" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="83" t="s">
+      <c r="F4" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="83" t="s">
+      <c r="G4" s="81" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="34" t="s">
@@ -21508,78 +21454,78 @@
       <c r="I4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="83" t="s">
+      <c r="J4" s="81" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>442</v>
-      </c>
-      <c r="B5" s="112"/>
+        <v>435</v>
+      </c>
+      <c r="B5" s="110"/>
       <c r="C5" s="15" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
       <c r="I5" s="23" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="K5" s="15"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>448</v>
-      </c>
-      <c r="B6" s="112"/>
+        <v>441</v>
+      </c>
+      <c r="B6" s="110"/>
       <c r="C6" s="15" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
       <c r="I6" s="23" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>454</v>
-      </c>
-      <c r="B7" s="112" t="s">
-        <v>455</v>
+        <v>447</v>
+      </c>
+      <c r="B7" s="110" t="s">
+        <v>448</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="F7" s="15"/>
       <c r="G7" s="15">
@@ -21587,29 +21533,29 @@
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="23" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="K7" s="15"/>
-      <c r="L7" s="113" t="s">
-        <v>461</v>
+      <c r="L7" s="111" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>462</v>
-      </c>
-      <c r="B8" s="112"/>
+        <v>455</v>
+      </c>
+      <c r="B8" s="110"/>
       <c r="C8" s="15" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="F8" s="15"/>
       <c r="G8" s="15">
@@ -21617,26 +21563,26 @@
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="23" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="K8" s="15"/>
     </row>
     <row r="9" ht="199.5" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>468</v>
-      </c>
-      <c r="B9" s="112"/>
+        <v>461</v>
+      </c>
+      <c r="B9" s="110"/>
       <c r="C9" s="15" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15">
@@ -21644,78 +21590,78 @@
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="23" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>473</v>
-      </c>
-      <c r="B10" s="112" t="s">
-        <v>474</v>
+        <v>466</v>
+      </c>
+      <c r="B10" s="110" t="s">
+        <v>467</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>477</v>
-      </c>
-      <c r="F10" s="92"/>
+        <v>470</v>
+      </c>
+      <c r="F10" s="90"/>
       <c r="G10" s="15">
         <v>1.0</v>
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="23" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>479</v>
-      </c>
-      <c r="B11" s="112"/>
+        <v>472</v>
+      </c>
+      <c r="B11" s="110"/>
       <c r="C11" s="15" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="23" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="K11" s="15"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>485</v>
-      </c>
-      <c r="B12" s="112" t="s">
-        <v>486</v>
+        <v>478</v>
+      </c>
+      <c r="B12" s="110" t="s">
+        <v>479</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15">
@@ -21723,149 +21669,149 @@
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="23" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>491</v>
-      </c>
-      <c r="B13" s="112"/>
+        <v>484</v>
+      </c>
+      <c r="B13" s="110"/>
       <c r="C13" s="15" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="23" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>496</v>
-      </c>
-      <c r="B14" s="112"/>
+        <v>489</v>
+      </c>
+      <c r="B14" s="110"/>
       <c r="C14" s="15" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="23" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>501</v>
-      </c>
-      <c r="B15" s="112"/>
+        <v>494</v>
+      </c>
+      <c r="B15" s="110"/>
       <c r="C15" s="15" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>504</v>
-      </c>
-      <c r="F15" s="89" t="s">
-        <v>505</v>
+        <v>497</v>
+      </c>
+      <c r="F15" s="87" t="s">
+        <v>498</v>
       </c>
       <c r="G15" s="15">
         <v>1.0</v>
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="23" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="K15" s="15"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>508</v>
-      </c>
-      <c r="B16" s="112"/>
+        <v>501</v>
+      </c>
+      <c r="B16" s="110"/>
       <c r="C16" s="15" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="23" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="K16" s="15"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>513</v>
-      </c>
-      <c r="B17" s="112"/>
+        <v>506</v>
+      </c>
+      <c r="B17" s="110"/>
       <c r="C17" s="15" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>515</v>
+        <v>508</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="15"/>
       <c r="I17" s="23" t="s">
-        <v>517</v>
+        <v>510</v>
       </c>
       <c r="J17" s="15" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="K17" s="15"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>519</v>
-      </c>
-      <c r="B18" s="112"/>
+        <v>512</v>
+      </c>
+      <c r="B18" s="110"/>
       <c r="C18" s="15" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15">
@@ -21873,7 +21819,7 @@
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="23" t="s">
-        <v>523</v>
+        <v>516</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>

</xml_diff>

<commit_message>
NAV-177 New BDG passing validation
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -17,7 +17,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgEhANcLrUpyZbCn7chYtIRKNp4gA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mivM8sG1k7DW4Sc/ZFrJn+y6qp9XQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -29,6 +29,24 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D7">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASRXWHKM
+Jonathan Berry    (2021-11-29 13:56:32)
+@jonathan@strategy4ward.com Is "Upload your inputs package to the ADR" a bit misleading here... maybe "Before you upload your input data to the ADR"
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D6">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASRXWHKE
+Jonathan Berry    (2021-11-29 13:54:06)
+@jonathan@strategy4ward.com Should we be removing all references to ShinyRob?
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="E12">
       <text>
         <t xml:space="preserve">======
@@ -76,7 +94,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjRTiHm/bb3hoFY4mbh/FCIGzfI2Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgV2/fB1ZeWyrbYgf80fCN/yrLt0Q=="/>
     </ext>
   </extLst>
 </comments>
@@ -88,6 +106,15 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A2">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASRXWHKQ
+Jonathan Berry    (2021-11-29 14:00:29)
+@jonathan@strategy4ward.com I would suggest a slightly different milestone title "Upload Estimates Input Data to the ADR" I'd suggest being careful how we use the word "package".
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="E8">
       <text>
         <t xml:space="preserve">======
@@ -131,13 +158,38 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miWk+6zpVG89196YJLo8CF9SnorYQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjnnOISAjCwMQqK7fkn9NXYxGUPyQ=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A2">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASQZYp8Y
+Jonathan Berry    (2021-11-29 16:13:01)
+@jonathan@strategy4ward.com Unfortunately Markdown can only be used in the task content, not the milestone titles.  I would suggest shortening this milestone name, maybe: "Review 
+quality of data inputs in Naomi" Also we need to be consistent in our capitalisation of milestones.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjQLChH7kssFiYviT8L8Yx8jDWCvw=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -162,7 +214,31 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B15">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASQZYp8s
+Jonathan Berry    (2021-11-29 16:19:26)
+@jonathan@strategy4ward.com Unfortunately we are only supporting markdown in the task content, not the task title.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miach7Q1bggrDq+3B9RkyZJqWtEJg=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -187,12 +263,21 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C15">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASQZYp80
+Jonathan Berry    (2021-11-29 16:27:24)
+@jonathan@strategy4ward.com  Unfortunately we don't support markdown in task titles, only in task content.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F18">
       <text>
         <t xml:space="preserve">======
@@ -206,7 +291,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJslj5uvmHEvEMtEDbwbds5MVx3A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi5EQmflitcDFgvxHNOZnt5sdaLkg=="/>
     </ext>
   </extLst>
 </comments>
@@ -677,7 +762,7 @@
 Can easily remove.</t>
   </si>
   <si>
-    <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum'], 'url', '.*')</t>
+    <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum-file'], 'url', '.*')</t>
   </si>
   <si>
     <t>ADR-01-11</t>
@@ -3342,14 +3427,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.29"/>
+    <col customWidth="1" min="1" max="1" width="14.0"/>
+    <col customWidth="1" min="2" max="2" width="49.0"/>
     <col customWidth="1" min="3" max="3" width="21.86"/>
     <col customWidth="1" min="4" max="4" width="43.71"/>
-    <col customWidth="1" min="5" max="5" width="39.14"/>
+    <col customWidth="1" min="5" max="5" width="18.29"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
     <col customWidth="1" min="7" max="7" width="31.86"/>
-    <col customWidth="1" min="8" max="8" width="36.86"/>
+    <col customWidth="1" min="8" max="8" width="14.14"/>
     <col customWidth="1" min="9" max="9" width="26.86"/>
     <col customWidth="1" min="10" max="10" width="31.86"/>
     <col customWidth="1" min="11" max="24" width="8.71"/>
@@ -14189,7 +14274,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -18385,7 +18471,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -19856,7 +19943,7 @@
     <col customWidth="1" min="2" max="2" width="11.43"/>
     <col customWidth="1" min="3" max="3" width="12.29"/>
     <col customWidth="1" min="4" max="4" width="19.43"/>
-    <col customWidth="1" min="5" max="5" width="13.29"/>
+    <col customWidth="1" min="5" max="5" width="63.0"/>
     <col customWidth="1" min="6" max="6" width="52.86"/>
     <col customWidth="1" min="7" max="7" width="11.29"/>
     <col customWidth="1" min="8" max="8" width="20.57"/>

</xml_diff>

<commit_message>
NAV 177 Validate check_resource_key calls (#61)
* NAV-177 Explicitly validate referenced resource_types

* NAV-177 Debug check_resource_key validation

* NAV-177 New BDG passing validation

* NAV-177 Fix linting issues
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -17,7 +17,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgEhANcLrUpyZbCn7chYtIRKNp4gA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mivM8sG1k7DW4Sc/ZFrJn+y6qp9XQ=="/>
     </ext>
   </extLst>
 </workbook>
@@ -29,6 +29,24 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D7">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASRXWHKM
+Jonathan Berry    (2021-11-29 13:56:32)
+@jonathan@strategy4ward.com Is "Upload your inputs package to the ADR" a bit misleading here... maybe "Before you upload your input data to the ADR"
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="D6">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASRXWHKE
+Jonathan Berry    (2021-11-29 13:54:06)
+@jonathan@strategy4ward.com Should we be removing all references to ShinyRob?
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="E12">
       <text>
         <t xml:space="preserve">======
@@ -76,7 +94,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjRTiHm/bb3hoFY4mbh/FCIGzfI2Q=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgV2/fB1ZeWyrbYgf80fCN/yrLt0Q=="/>
     </ext>
   </extLst>
 </comments>
@@ -88,6 +106,15 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A2">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASRXWHKQ
+Jonathan Berry    (2021-11-29 14:00:29)
+@jonathan@strategy4ward.com I would suggest a slightly different milestone title "Upload Estimates Input Data to the ADR" I'd suggest being careful how we use the word "package".
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="E8">
       <text>
         <t xml:space="preserve">======
@@ -131,13 +158,38 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miWk+6zpVG89196YJLo8CF9SnorYQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjnnOISAjCwMQqK7fkn9NXYxGUPyQ=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A2">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASQZYp8Y
+Jonathan Berry    (2021-11-29 16:13:01)
+@jonathan@strategy4ward.com Unfortunately Markdown can only be used in the task content, not the milestone titles.  I would suggest shortening this milestone name, maybe: "Review 
+quality of data inputs in Naomi" Also we need to be consistent in our capitalisation of milestones.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjQLChH7kssFiYviT8L8Yx8jDWCvw=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -162,7 +214,31 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="B15">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASQZYp8s
+Jonathan Berry    (2021-11-29 16:19:26)
+@jonathan@strategy4ward.com Unfortunately we are only supporting markdown in the task content, not the task title.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miach7Q1bggrDq+3B9RkyZJqWtEJg=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -187,12 +263,21 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="C15">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASQZYp80
+Jonathan Berry    (2021-11-29 16:27:24)
+@jonathan@strategy4ward.com  Unfortunately we don't support markdown in task titles, only in task content.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F18">
       <text>
         <t xml:space="preserve">======
@@ -206,7 +291,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJslj5uvmHEvEMtEDbwbds5MVx3A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mi5EQmflitcDFgvxHNOZnt5sdaLkg=="/>
     </ext>
   </extLst>
 </comments>
@@ -677,7 +762,7 @@
 Can easily remove.</t>
   </si>
   <si>
-    <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum'], 'url', '.*')</t>
+    <t>check_resource_key(['inputs-unaids-geographic', 'inputs-unaids-survey', 'inputs-unaids-population', 'inputs-unaids-spectrum-file'], 'url', '.*')</t>
   </si>
   <si>
     <t>ADR-01-11</t>
@@ -3342,14 +3427,14 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.71"/>
-    <col customWidth="1" min="2" max="2" width="19.29"/>
+    <col customWidth="1" min="1" max="1" width="14.0"/>
+    <col customWidth="1" min="2" max="2" width="49.0"/>
     <col customWidth="1" min="3" max="3" width="21.86"/>
     <col customWidth="1" min="4" max="4" width="43.71"/>
-    <col customWidth="1" min="5" max="5" width="39.14"/>
+    <col customWidth="1" min="5" max="5" width="18.29"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
     <col customWidth="1" min="7" max="7" width="31.86"/>
-    <col customWidth="1" min="8" max="8" width="36.86"/>
+    <col customWidth="1" min="8" max="8" width="14.14"/>
     <col customWidth="1" min="9" max="9" width="26.86"/>
     <col customWidth="1" min="10" max="10" width="31.86"/>
     <col customWidth="1" min="11" max="24" width="8.71"/>
@@ -14189,7 +14274,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -18385,7 +18471,8 @@
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -19856,7 +19943,7 @@
     <col customWidth="1" min="2" max="2" width="11.43"/>
     <col customWidth="1" min="3" max="3" width="12.29"/>
     <col customWidth="1" min="4" max="4" width="19.43"/>
-    <col customWidth="1" min="5" max="5" width="13.29"/>
+    <col customWidth="1" min="5" max="5" width="63.0"/>
     <col customWidth="1" min="6" max="6" width="52.86"/>
     <col customWidth="1" min="7" max="7" width="11.29"/>
     <col customWidth="1" min="8" max="8" width="20.57"/>

</xml_diff>

<commit_message>
NAV-172 Debug BDG (#71)
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="00-Oveview" sheetId="1" state="visible" r:id="rId2"/>
@@ -3233,13 +3233,13 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49"/>
@@ -10012,7 +10012,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
@@ -11557,11 +11557,11 @@
   </sheetPr>
   <dimension ref="A1:Y996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
@@ -11720,9 +11720,7 @@
         <v>143</v>
       </c>
       <c r="E7" s="15"/>
-      <c r="F7" s="29" t="n">
-        <v>1</v>
-      </c>
+      <c r="F7" s="29"/>
       <c r="G7" s="21"/>
       <c r="H7" s="15"/>
       <c r="I7" s="15" t="s">
@@ -11761,9 +11759,7 @@
       <c r="E8" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="F8" s="29" t="n">
-        <v>1</v>
-      </c>
+      <c r="F8" s="29"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="15" t="s">
@@ -11802,9 +11798,7 @@
       <c r="E9" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="29" t="n">
-        <v>1</v>
-      </c>
+      <c r="F9" s="29"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="15" t="s">
@@ -11882,9 +11876,7 @@
       <c r="E11" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="F11" s="15" t="n">
-        <v>1</v>
-      </c>
+      <c r="F11" s="15"/>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="15" t="s">
@@ -12925,7 +12917,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
@@ -14237,7 +14229,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -15823,7 +15815,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -17085,7 +17077,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.41"/>
@@ -18448,7 +18440,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.3"/>
@@ -21883,7 +21875,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>

</xml_diff>

<commit_message>
NAV-188 Add data loader to the BDG
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="00-Oveview" sheetId="1" state="visible" r:id="rId2"/>
@@ -387,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="572">
   <si>
     <t xml:space="preserve">Milestone Title (Visible to User):</t>
   </si>
@@ -1881,6 +1881,9 @@
     <t xml:space="preserve">check_manual_confirmation('EST-S90-11-01-A')</t>
   </si>
   <si>
+    <t xml:space="preserve">Data Loader:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finalize National HIV Estimates in Spectrum</t>
   </si>
   <si>
@@ -1888,6 +1891,9 @@
   </si>
   <si>
     <t xml:space="preserve">Milestones, 1, 2, 3, 4, 5 and 6 are completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load_csv_from_zipped_resource('inputs-unaids-spectrum-file', '.*_check.CSV', 'spectrum-validation-file ')</t>
   </si>
   <si>
     <t xml:space="preserve">SPF-01-10</t>
@@ -3239,7 +3245,7 @@
       <selection pane="bottomLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49"/>
@@ -10012,7 +10018,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
@@ -11557,11 +11563,11 @@
   </sheetPr>
   <dimension ref="A1:Y996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
@@ -12917,7 +12923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
@@ -14229,7 +14235,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -15815,7 +15821,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -17077,7 +17083,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.41"/>
@@ -18436,18 +18442,19 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.43"/>
@@ -18470,21 +18477,27 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>407</v>
+      </c>
       <c r="I1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>0.2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>411</v>
       </c>
       <c r="I2" s="30"/>
     </row>
@@ -18528,66 +18541,66 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="I5" s="80"/>
       <c r="J5" s="13" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="K5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I6" s="80"/>
       <c r="J6" s="13" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="n">
@@ -18595,31 +18608,31 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="I7" s="80" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="81" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="n">
@@ -18627,26 +18640,26 @@
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="I8" s="80"/>
       <c r="J8" s="13" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="K8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="199.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="n">
@@ -18654,7 +18667,7 @@
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I9" s="80"/>
       <c r="J9" s="13"/>
@@ -18662,16 +18675,16 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E10" s="61"/>
       <c r="F10" s="13" t="n">
@@ -18679,51 +18692,51 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="I10" s="80" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="I11" s="80"/>
       <c r="J11" s="13" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="K11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="n">
@@ -18731,32 +18744,32 @@
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="I12" s="80" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="I13" s="80"/>
       <c r="J13" s="13"/>
@@ -18764,22 +18777,22 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="I14" s="80"/>
       <c r="J14" s="13"/>
@@ -18787,95 +18800,95 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F15" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="I15" s="80"/>
       <c r="J15" s="13" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="K15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="I16" s="80"/>
       <c r="J16" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="K16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="I17" s="80"/>
       <c r="J17" s="13" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="K17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13" t="n">
@@ -18883,7 +18896,7 @@
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="I18" s="80"/>
       <c r="J18" s="13"/>
@@ -21875,7 +21888,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
@@ -21909,14 +21922,14 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="n">
@@ -21932,7 +21945,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>10</v>
@@ -21964,17 +21977,17 @@
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="13" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="n">
@@ -21982,26 +21995,26 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="n">
@@ -22009,16 +22022,16 @@
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B7" s="80"/>
       <c r="C7" s="13" t="s">
@@ -22028,7 +22041,7 @@
         <v>174</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>176</v>
@@ -22036,14 +22049,14 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="J7" s="61"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B8" s="80"/>
       <c r="C8" s="13" t="s">
@@ -22059,17 +22072,17 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>184</v>
@@ -22078,32 +22091,32 @@
         <v>185</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F10" s="66" t="s">
         <v>231</v>
@@ -22113,82 +22126,82 @@
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B11" s="80"/>
       <c r="C11" s="13" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B12" s="80" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="G12" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="K12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B13" s="80" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="n">
@@ -22196,53 +22209,53 @@
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B14" s="80" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="G14" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B15" s="80"/>
       <c r="C15" s="13" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="n">
@@ -22250,47 +22263,47 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="J15" s="61"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="13" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B17" s="80"/>
       <c r="C17" s="13" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="n">
@@ -22298,34 +22311,34 @@
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B18" s="80"/>
       <c r="C18" s="13" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="G18" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>

</xml_diff>

<commit_message>
NAV-188 Load the spectrum validation file in the spectrum finalisation milestone (#73)
* NAV-188 Add data loader to the BDG

* NAV-188 Add the milestone data loader to the DB

* NAV-188 Fix typo

* NAV-188 Spectrum file data loading end-to-end test.

* NAV-188 Fix unit tests.
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="00-Oveview" sheetId="1" state="visible" r:id="rId2"/>
@@ -387,7 +387,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="572">
   <si>
     <t xml:space="preserve">Milestone Title (Visible to User):</t>
   </si>
@@ -1881,6 +1881,9 @@
     <t xml:space="preserve">check_manual_confirmation('EST-S90-11-01-A')</t>
   </si>
   <si>
+    <t xml:space="preserve">Data Loader:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Finalize National HIV Estimates in Spectrum</t>
   </si>
   <si>
@@ -1888,6 +1891,9 @@
   </si>
   <si>
     <t xml:space="preserve">Milestones, 1, 2, 3, 4, 5 and 6 are completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">load_csv_from_zipped_resource('inputs-unaids-spectrum-file', '.*_check.CSV', 'spectrum-validation-file ')</t>
   </si>
   <si>
     <t xml:space="preserve">SPF-01-10</t>
@@ -3239,7 +3245,7 @@
       <selection pane="bottomLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49"/>
@@ -10012,7 +10018,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
@@ -11557,11 +11563,11 @@
   </sheetPr>
   <dimension ref="A1:Y996"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
@@ -12917,7 +12923,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
@@ -14229,7 +14235,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -15815,7 +15821,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -17077,7 +17083,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.41"/>
@@ -18436,18 +18442,19 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="46.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="11.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="32.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="27.43"/>
@@ -18470,21 +18477,27 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>407</v>
+      </c>
       <c r="I1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E2" s="6" t="n">
         <v>0.2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>411</v>
       </c>
       <c r="I2" s="30"/>
     </row>
@@ -18528,66 +18541,66 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="I5" s="80"/>
       <c r="J5" s="13" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="K5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="I6" s="80"/>
       <c r="J6" s="13" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13" t="n">
@@ -18595,31 +18608,31 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="I7" s="80" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="81" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="n">
@@ -18627,26 +18640,26 @@
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="I8" s="80"/>
       <c r="J8" s="13" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="K8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="199.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13" t="n">
@@ -18654,7 +18667,7 @@
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="I9" s="80"/>
       <c r="J9" s="13"/>
@@ -18662,16 +18675,16 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="E10" s="61"/>
       <c r="F10" s="13" t="n">
@@ -18679,51 +18692,51 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="I10" s="80" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="I11" s="80"/>
       <c r="J11" s="13" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="K11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13" t="n">
@@ -18731,32 +18744,32 @@
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="I12" s="80" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="I13" s="80"/>
       <c r="J13" s="13"/>
@@ -18764,22 +18777,22 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="I14" s="80"/>
       <c r="J14" s="13"/>
@@ -18787,95 +18800,95 @@
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="F15" s="13" t="n">
         <v>1</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="13" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="I15" s="80"/>
       <c r="J15" s="13" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="K15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="I16" s="80"/>
       <c r="J16" s="13" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="K16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="I17" s="80"/>
       <c r="J17" s="13" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="K17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13" t="n">
@@ -18883,7 +18896,7 @@
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="13" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="I18" s="80"/>
       <c r="J18" s="13"/>
@@ -21875,7 +21888,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.43"/>
@@ -21909,14 +21922,14 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="7" t="n">
@@ -21932,7 +21945,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="83" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="C4" s="52" t="s">
         <v>10</v>
@@ -21964,17 +21977,17 @@
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B5" s="80"/>
       <c r="C5" s="13" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="n">
@@ -21982,26 +21995,26 @@
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="13" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="B6" s="80" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="n">
@@ -22009,16 +22022,16 @@
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="K6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B7" s="80"/>
       <c r="C7" s="13" t="s">
@@ -22028,7 +22041,7 @@
         <v>174</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>176</v>
@@ -22036,14 +22049,14 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="J7" s="61"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="B8" s="80"/>
       <c r="C8" s="13" t="s">
@@ -22059,17 +22072,17 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>184</v>
@@ -22078,32 +22091,32 @@
         <v>185</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="B10" s="80" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="F10" s="66" t="s">
         <v>231</v>
@@ -22113,82 +22126,82 @@
       </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="B11" s="80"/>
       <c r="C11" s="13" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="F11" s="66" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="B12" s="80" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="E12" s="58" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="G12" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="K12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="B13" s="80" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="n">
@@ -22196,53 +22209,53 @@
       </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B14" s="80" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="G14" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="13" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="B15" s="80"/>
       <c r="C15" s="13" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="n">
@@ -22250,47 +22263,47 @@
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="J15" s="61"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="B16" s="80"/>
       <c r="C16" s="13" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="13" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="13" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B17" s="80"/>
       <c r="C17" s="13" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="n">
@@ -22298,34 +22311,34 @@
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="13" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="B18" s="80"/>
       <c r="C18" s="13" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="G18" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>

</xml_diff>

<commit_message>
NAV-199 New BDG with Naomi checks
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -17,7 +17,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhAJuQuCrSUcWDHjvnrU0Nyiot4Pg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgY3G13jMtTAPFPPdMwQciM5i5Isg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -120,7 +120,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhNGibSaD8hG1aPYAybAzeJZKxv6g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhQRdaztJoEiZyPRyiaOIY4w4Iw+w=="/>
     </ext>
   </extLst>
 </comments>
@@ -242,6 +242,15 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D17">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASdCRYWw
+Jonathan Berry    (2021-12-03 12:11:21)
+@jonathan@strategy4ward.com To check the wording of these automatic spectrum check tasks when he can.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="K18">
       <text>
         <t xml:space="preserve">======
@@ -264,7 +273,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miByJhmzgEBl81JZEBBclzR2Xk33A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIk/v7InulN46/q1ENwBPYMeYRLw=="/>
     </ext>
   </extLst>
 </comments>
@@ -276,6 +285,14 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="E19">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASdCRYWg
+Jonathan Berry    (2021-12-03 12:04:13)
+@jonathan@strategy4ward.com to review the wording of these tasks for  Naomi automatic checks when he can.</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F18">
       <text>
         <t xml:space="preserve">======
@@ -289,14 +306,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJslj5uvmHEvEMtEDbwbds5MVx3A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgkJMrpR5qGHcJ916e/YHH+qqje6A=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="645">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -667,7 +684,7 @@
     <t>Has user updated VMMC data file?</t>
   </si>
   <si>
-    <t xml:space="preserve">*This task is only for VMMC priority countries. If you are not from one of the priority VMMC countries, mark this task complete and click "What's Next".* Before you upload data files to your Inputs Package to ADR, ensure you have updated the data files for the current reporting period.  **Update** your programme data files for VMMC (if relevant). If you produced a VMMC data file last year, UNAIDS has placed that final file in this year's Inputs Package for your convenience. UNAIDS recommends beginning with last year's final Inputs Package and only updating the files for the current reporting period. If you are not using VMMC data for your estimates, you can market this task as complete. You can learn more about the data elements required in Guide 8 Data Quality, Indicator Elements Matrix. </t>
+    <t xml:space="preserve">*This task is only for VMMC priority countries. If you are not from one of the priority VMMC countries, mark this task complete and click "What's Next".* Before you upload data files to your Inputs Package to ADR, ensure you have updated the data files for the current reporting period.  **Update** your programme data files for VMMC (if relevant). UNAIDS recommends beginning with last year's data and only updating as necessary for the current reporting period. If you are not using VMMC data for your estimates, you can market this task as complete. You can learn more about the data elements required in Guide 8 Data Quality, Indicator Elements Matrix. </t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-GEN-05-01-A')</t>
@@ -2283,7 +2300,10 @@
     <t>SPF-13-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Enter PMTCT data for the current reporting year into Spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date PMTCT programme data for the reporting period. These data are required for each Spectrum file. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. Spectrum also provides specific guidance for each regimen in the PMTCT data entry page. *It is highly recommended you finalize your programme data before beginning the Spectrum process.* If edits to PMTCT programme data are required later in the process, you will have to return to this step. For countries with sub-national Spectrum estimates (optional), this step applies to each file. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2313,7 +2333,10 @@
     <t>SPF-14-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Update Adult ART data in Spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date Adult ART programme data for the reporting period for estimating treatment coverage and for estimating incidence. You should update the ART data before running your incidence curve. Data on the number newly initiated on ART and lost to follow up can improve the precision of some of the outputs from Spectrum. If those data are available be sure to include them. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. If edits to the ART programme data are required later in the process, you will have to rerun your incidence curve fitting. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2328,7 +2351,10 @@
     <t>SPF-15-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Update Pediatric ART data in Spectrum for the current reporting period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date Pediatric ART programme data for the reporting period. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. It is highly recommended you finalize your programme data before beginning the Spectrum process. If edits to ART programme data are required later in the process, you will have to return to this step. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2337,6 +2363,9 @@
   </si>
   <si>
     <t>SPF-16-01</t>
+  </si>
+  <si>
+    <t>Spectrum Validation: Update viral load suppression data in Spectrum for the current reporting period for adult females and males and pediatric populations</t>
   </si>
   <si>
     <r>
@@ -2357,7 +2386,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date adult and pediatric viral load suppression programme data for the reporting period. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. It is highly recommended you finalize your programme data before beginning the Spectrum process. Enter the best, most up-to-date viral load suppression data you have for adult female, adult male, and pediatric populations. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2368,7 +2397,10 @@
     <t>SPF-17-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for adult parameters under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum relies on a number of assumptions that are summarized under Advanced Options. These parameters are updated every year as new research and evidence is available on those parameters. For Spectrum on the Desktop update the parameters by selecting Advanced Options &gt; Adult Parameters &gt; Restore defaults. For Spectrum on the web: enter Advanced Options and confirm the default selections for adult parameters. If you see values in red font, the parameters have not been updated. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2379,7 +2411,10 @@
     <t>SPF-18-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for pediatric parameters under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum relies on a number of assumptions that are summarized under Advanced Options. These parameters are updated every year as new research and evidence is available on those parameters. For Spectrum on the Desktop update the parameters by selecting Advanced Options &gt; Pediatric Parameters &gt; Restore defaults. For Spectrum on the web: enter Advanced Options and confirm the default selections for pediatric parameters. If you see values in red font, the parameters have not been updated. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2390,7 +2425,10 @@
     <t>SPF-19-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for Fertility Rate Ratios under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. They must be confirmed for CD4, on ART, and off ART. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2401,7 +2439,10 @@
     <t>SPF-20-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for MTCT probabilities under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "MTCT Transmission Probabilities" are correct for your country. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2412,7 +2453,10 @@
     <t>SPF-21-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for new ART allocation method under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selection for the "allocation method for new ART patients" is correct for your country. To learn more about the Advanced Options, see the Spectrum training materials. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2423,7 +2467,10 @@
     <t>SPF-22-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Upload a completed Shiny 90 file to Spectrum or enter KOS estimates in another format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Each of your Spectrum files requires updated knowledge of status data elements for current estimates year using one of available options - Direct Entry of Case Reports, Shiny 90, CSAVR, ECDC, Manual Entry. Most countries will use Shiny 90. If you have used Shiny 90, you must upload your Shiny 90 model outputs (AIM &gt; Program Statistics &gt; Knowledge of Status &gt; Data Source = Shiny 90 &gt; Load Data).
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2432,6 +2479,9 @@
   </si>
   <si>
     <t>SPF-23-01</t>
+  </si>
+  <si>
+    <t>Spectrum Validation: Confirm your ART and PMTCT coverage does not exceed 100%</t>
   </si>
   <si>
     <r>
@@ -2461,7 +2511,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Occasionally, Spectrum will produce coverage of over 100% for ART or PMTCT services. There are multiple causes for coverage results over 100%. UNAIDS recommends consulting your estimates facilitator and/or UNAIDS to determine how to address coverage issues in your model results. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2472,7 +2522,10 @@
     <t>SPF-24-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Run Uncertainty Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 The uncertainty associated with each result can be estimated using the Uncertainty Analysis tool. Access this tool by choosing ‘Tools’ from the top horizontal menu, then ‘More Tools’, then ‘Uncertainty analysis’. 
 Set the ‘Aggregate data capture year’ to the final year of data and the ‘Number of iterations’ to 300, then click the ‘Process’ button. The model will run 300 simulations by choosing values for the epidemiological parameters from within their confidence intervals. This analysis may take 10-30 minutes. When it is complete, click the ‘Save’ button. After running this analysis you will see uncertainty intervals on all the outputs (as long as you only have one projection open in Spectrum). 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
@@ -2481,15 +2534,6 @@
     <t>check_spectrum_file(['UAvalid'])</t>
   </si>
   <si>
-    <t>SPF-25-CK</t>
-  </si>
-  <si>
-    <t>Are SPF-13-01, SPF-14-01, SPF-15-01, SPF-16-01, SPF-17-01, SPF-18-01, SPF-19-01, SPF-20-01, SPF-21-01, SPF-22-01, SPF-23-01, SPF-24-01 complete?</t>
-  </si>
-  <si>
-    <t>check_not_skipped(['EST-SPF-13-01-A', 'EST-SPF-14-01-A', 'EST-SPF-15-01-A', 'EST-SPF-16-01-A', 'EST-SPF-17-01-A', 'EST-SPF-18-01-A', 'EST-SPF-19-01-A', 'EST-SPF-20-01-A', 'EST-SPF-21-01-A', 'EST-SPF-22-01-A', 'EST-SPF-23-01-A', 'EST-SPF-24-01-A' ])</t>
-  </si>
-  <si>
     <t>SPF-26-01</t>
   </si>
   <si>
@@ -2533,6 +2577,9 @@
     <t>User has a validated, final Spectrum file
 No underlying Spectrum data (e.g., surveillance, survey, or programme data) have changed since the Spectrum file was produced. 
 User has uploaded validated programme data and survey data files to ADR in the required formats</t>
+  </si>
+  <si>
+    <t>load_csv_from_zipped_resource('inputs-unaids-naomi-output-zip', '.*unaids_navigator_checklist.csv', 'naomi-validation-file')</t>
   </si>
   <si>
     <t>Naomi Check File Ref</t>
@@ -2813,6 +2860,109 @@
   </si>
   <si>
     <t>check_manual_confirmation('EST-NAO-14-01-A')</t>
+  </si>
+  <si>
+    <t>NAO-15-01</t>
+  </si>
+  <si>
+    <t>Naomi Validation: Match data inputs for Spectrum and Naomi</t>
+  </si>
+  <si>
+    <t>**Navigator has detected a problem with your Naomi Outputs zip.**
+Some data inputs used by Naomi are disaggregated versions of data inputs for other models such as Spectrum. For example, ART and ANC data used by Naomi are also used by Spectrum. You can learn more about the requirements for each of the models from 'Guide 8' in the UNAIDS training materials (attached below). It is critical that data inputs used by Naomi match the inputs used by Spectrum. Although in some cases disaggregation levels may differ, the sum of the disaggregations must equal those used by Spectrum. If the Naomi data inputs do not match those used in your Spectrum model process, modify them to match. If you have changed inputs used by Spectrum, you must return to Spectrum and begin the process again. If you have altered your Naomi inputs to match those used by Spectrum, you may continue with Naomi. 
+**Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
+  </si>
+  <si>
+    <t>check_naomi_file(['ART_is_Spectrum', 'ANC_is_Spectrum'])</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Ian: run a formal validation to compare the values in the spectrum file and the naomi input files
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF0000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>@Fjelltopp - can ADR compare the Spectrum file's numbers and compare them to the Naomi Input Files?</t>
+    </r>
+  </si>
+  <si>
+    <t>NAO-16-01</t>
+  </si>
+  <si>
+    <t>Naomi Validation: Select or confirm default settings in Naomi model options</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>**Navigator has detected a problem with your Naomi Outputs zip.**
+Naomi is a flexible model which allows countries to customize their subnational outputs. Review the multitude of model options available to users. You can learn more about these options in 'Guide 5, Naomi Quick Start' in UNAIDS estimates training materials</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>**Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
+    </r>
+  </si>
+  <si>
+    <t>check_naomi_file(['Opt_recent_qtr', 'Opt_future_proj_qtr' , 'Opt_area_ID_selected', 'Opt_calendar_survey_match', 'Opt_recent_survey_only', 'Opt_ART_coverage', 'Opt_ANC_data', 'Opt_ART_data', 'Opt_ART_attendance_yes'])</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Ian: Can we run a formal check on the naomi file that is uploaded to the ADR to verify if the standandirsed options a country has used match what is expecetd. This means we need a prepoulated database that contains a list of expected parameters for each country that uses naomi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF0000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>@Fjelltopp - possible this year?</t>
+    </r>
+  </si>
+  <si>
+    <t>NAO-17-01</t>
+  </si>
+  <si>
+    <t>Naomi Validation:  Calibrate the model in Naomi</t>
+  </si>
+  <si>
+    <t>**Navigator has detected a problem with your Naomi Outputs zip.**
+You should calibrate your model for the following four indicators (PLHIV, ART, aware of HIV status and new infections). This is to ensure that the mean aggregate estimates from Spectrum and Naomi are consistent. All these should be adjusted to match your Spectrum file either the national or sub-national Spectrum files with the following age sex stratification: (sex and age &lt;15 /15+ years). Calibration method: use the default which is logistic and which scales the prevalence, ART coverage, proportion unaware, and incidence on the logit scale within each district / sex / age stratum in order to match to Spectrum. This ensures that ART coverage does not go above 100% in any district / sex / age stratification. Further information is available in Guide 5, Naomi Quick Start. 
+**Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
+  </si>
+  <si>
+    <t>check_naomi_file(['Cal_PLHIV', 'Cal_ART', 'Cal_KOS', 'Cal_new_infections', 'Cal_method'])</t>
   </si>
 </sst>
 </file>
@@ -3430,16 +3580,16 @@
     <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -19252,43 +19402,43 @@
       <c r="A17" s="16" t="s">
         <v>488</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>232</v>
+      <c r="B17" s="16" t="s">
+        <v>489</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>233</v>
       </c>
       <c r="D17" s="90" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E17" s="91" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="16" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="I17" s="89" t="s">
         <v>231</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="16" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>492</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>251</v>
+        <v>493</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>494</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>252</v>
       </c>
       <c r="D18" s="90" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>247</v>
@@ -19296,28 +19446,28 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="121" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I18" s="89" t="s">
         <v>250</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="16" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>263</v>
+        <v>498</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>499</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>264</v>
       </c>
       <c r="D19" s="90" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>247</v>
@@ -19325,7 +19475,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="121" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="I19" s="89" t="s">
         <v>262</v>
@@ -19335,22 +19485,22 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>269</v>
+        <v>502</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>503</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D20" s="90" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="121" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="I20" s="89" t="s">
         <v>268</v>
@@ -19360,16 +19510,16 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>503</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>280</v>
+        <v>507</v>
+      </c>
+      <c r="B21" s="122" t="s">
+        <v>508</v>
       </c>
       <c r="C21" s="99" t="s">
         <v>281</v>
       </c>
       <c r="D21" s="100" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="E21" s="101" t="s">
         <v>283</v>
@@ -19377,7 +19527,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="121" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="I21" s="89" t="s">
         <v>279</v>
@@ -19387,16 +19537,16 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>506</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>287</v>
+        <v>511</v>
+      </c>
+      <c r="B22" s="122" t="s">
+        <v>512</v>
       </c>
       <c r="C22" s="99" t="s">
         <v>288</v>
       </c>
       <c r="D22" s="100" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="E22" s="101" t="s">
         <v>283</v>
@@ -19404,7 +19554,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="121" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="I22" s="89" t="s">
         <v>286</v>
@@ -19414,16 +19564,16 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>293</v>
+        <v>515</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>516</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>294</v>
       </c>
       <c r="D23" s="90" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="E23" s="103" t="s">
         <v>283</v>
@@ -19431,7 +19581,7 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="121" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="I23" s="89"/>
       <c r="J23" s="15"/>
@@ -19439,16 +19589,16 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>512</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>299</v>
+        <v>519</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>520</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>300</v>
       </c>
       <c r="D24" s="90" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="E24" s="103" t="s">
         <v>302</v>
@@ -19456,7 +19606,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="121" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="I24" s="89"/>
       <c r="J24" s="15"/>
@@ -19464,16 +19614,16 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>515</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>306</v>
+        <v>523</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>524</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>307</v>
       </c>
       <c r="D25" s="90" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="E25" s="103" t="s">
         <v>283</v>
@@ -19481,7 +19631,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="121" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="I25" s="89" t="s">
         <v>305</v>
@@ -19491,22 +19641,22 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>518</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>430</v>
+        <v>527</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>528</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>431</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="121" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="I26" s="119" t="s">
         <v>434</v>
@@ -19516,22 +19666,22 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>449</v>
+        <v>531</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>532</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="16" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="I27" s="119" t="s">
         <v>453</v>
@@ -19541,22 +19691,22 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>461</v>
+        <v>536</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>537</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>462</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="121" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="I28" s="119" t="s">
         <v>465</v>
@@ -19566,72 +19716,56 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>528</v>
-      </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="122" t="s">
-        <v>529</v>
-      </c>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="81" t="s">
-        <v>530</v>
+        <v>540</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16" t="s">
+        <v>544</v>
       </c>
       <c r="I29" s="119"/>
-      <c r="J29" s="15"/>
+      <c r="J29" s="15" t="s">
+        <v>545</v>
+      </c>
       <c r="K29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>531</v>
+        <v>546</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>534</v>
+        <v>549</v>
       </c>
       <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="15">
+        <v>1.0</v>
+      </c>
       <c r="G30" s="15"/>
       <c r="H30" s="16" t="s">
-        <v>535</v>
+        <v>550</v>
       </c>
       <c r="I30" s="119"/>
-      <c r="J30" s="15" t="s">
-        <v>536</v>
-      </c>
+      <c r="J30" s="15"/>
       <c r="K30" s="15"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>539</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16" t="s">
-        <v>541</v>
-      </c>
-      <c r="I31" s="119"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
+    <row r="31" ht="13.5" customHeight="1">
+      <c r="I31" s="48"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="I32" s="48"/>
@@ -20233,7 +20367,7 @@
     <row r="231" ht="13.5" customHeight="1">
       <c r="I231" s="48"/>
     </row>
-    <row r="232" ht="13.5" customHeight="1">
+    <row r="232" ht="15.75" customHeight="1">
       <c r="I232" s="48"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
@@ -22572,9 +22706,6 @@
     </row>
     <row r="1011" ht="15.75" customHeight="1">
       <c r="I1011" s="48"/>
-    </row>
-    <row r="1012" ht="15.75" customHeight="1">
-      <c r="I1012" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -22604,14 +22735,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.57"/>
-    <col customWidth="1" min="2" max="2" width="11.43"/>
+    <col customWidth="1" min="2" max="2" width="16.14"/>
     <col customWidth="1" min="3" max="3" width="12.29"/>
     <col customWidth="1" min="4" max="4" width="19.43"/>
     <col customWidth="1" min="5" max="5" width="63.0"/>
     <col customWidth="1" min="6" max="6" width="52.86"/>
-    <col customWidth="1" min="7" max="7" width="11.29"/>
+    <col customWidth="1" min="7" max="7" width="16.29"/>
     <col customWidth="1" min="8" max="8" width="20.57"/>
-    <col customWidth="1" min="9" max="9" width="11.29"/>
+    <col customWidth="1" min="9" max="9" width="42.14"/>
     <col customWidth="1" min="10" max="10" width="45.14"/>
     <col customWidth="1" hidden="1" min="11" max="11" width="8.71"/>
     <col customWidth="1" min="12" max="12" width="8.71"/>
@@ -22632,33 +22763,38 @@
       <c r="F1" s="35" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="35" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="37" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="37">
         <v>0.2</v>
       </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
+      <c r="G2" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="125" t="s">
-        <v>545</v>
+      <c r="B4" s="124" t="s">
+        <v>555</v>
       </c>
       <c r="C4" s="85" t="s">
         <v>10</v>
@@ -22690,17 +22826,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>546</v>
+        <v>556</v>
       </c>
       <c r="B5" s="119"/>
       <c r="C5" s="15" t="s">
-        <v>547</v>
+        <v>557</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>548</v>
+        <v>558</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>549</v>
+        <v>559</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15">
@@ -22708,26 +22844,26 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="16" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>555</v>
+        <v>565</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15">
@@ -22735,16 +22871,16 @@
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="16" t="s">
-        <v>556</v>
+        <v>566</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>557</v>
+        <v>567</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="B7" s="119"/>
       <c r="C7" s="15" t="s">
@@ -22754,7 +22890,7 @@
         <v>178</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>559</v>
+        <v>569</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>180</v>
@@ -22762,14 +22898,14 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="16" t="s">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="J7" s="95"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>561</v>
+        <v>571</v>
       </c>
       <c r="B8" s="119"/>
       <c r="C8" s="15" t="s">
@@ -22785,17 +22921,17 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="16" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>564</v>
+        <v>574</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>188</v>
@@ -22804,32 +22940,32 @@
         <v>189</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="16" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>567</v>
+        <v>577</v>
       </c>
       <c r="B10" s="119" t="s">
-        <v>568</v>
+        <v>578</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>569</v>
+        <v>579</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="F10" s="103" t="s">
         <v>247</v>
@@ -22839,82 +22975,82 @@
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="16" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>573</v>
+        <v>583</v>
       </c>
       <c r="B11" s="119"/>
       <c r="C11" s="15" t="s">
-        <v>574</v>
+        <v>584</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
       <c r="F11" s="103" t="s">
-        <v>577</v>
+        <v>587</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="16" t="s">
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="B12" s="119" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="G12" s="15">
         <v>1.0</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="16" t="s">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="K12" s="15"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
       <c r="B13" s="119" t="s">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>589</v>
+        <v>599</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>591</v>
+        <v>601</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15">
@@ -22922,53 +23058,53 @@
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="16" t="s">
-        <v>592</v>
+        <v>602</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="B14" s="119" t="s">
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>597</v>
+        <v>607</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="G14" s="15">
         <v>1.0</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="16" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="B15" s="119"/>
       <c r="C15" s="16" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15">
@@ -22976,47 +23112,47 @@
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="16" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="15"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="B16" s="119"/>
       <c r="C16" s="15" t="s">
-        <v>606</v>
+        <v>616</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>608</v>
+        <v>618</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="16" t="s">
-        <v>609</v>
+        <v>619</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="B17" s="119"/>
       <c r="C17" s="15" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15">
@@ -23024,41 +23160,123 @@
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="16" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="B18" s="119"/>
       <c r="C18" s="15" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>618</v>
+        <v>628</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="G18" s="15">
         <v>1.0</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="16" t="s">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
     </row>
-    <row r="19" ht="12.0" customHeight="1"/>
-    <row r="20" ht="12.0" customHeight="1"/>
-    <row r="21" ht="12.0" customHeight="1"/>
+    <row r="19" ht="12.0" customHeight="1">
+      <c r="A19" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="B19" s="119" t="s">
+        <v>562</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>633</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16" t="s">
+        <v>634</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>635</v>
+      </c>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" ht="49.5" customHeight="1">
+      <c r="A20" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="B20" s="119" t="s">
+        <v>590</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="E20" s="125" t="s">
+        <v>638</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16" t="s">
+        <v>639</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" ht="12.0" customHeight="1">
+      <c r="A21" s="16" t="s">
+        <v>641</v>
+      </c>
+      <c r="B21" s="119" t="s">
+        <v>604</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>642</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>643</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+    </row>
     <row r="22" ht="12.0" customHeight="1"/>
     <row r="23" ht="12.0" customHeight="1"/>
     <row r="24" ht="12.0" customHeight="1"/>
@@ -24034,10 +24252,6 @@
     <row r="994" ht="12.0" customHeight="1"/>
     <row r="995" ht="12.0" customHeight="1"/>
     <row r="996" ht="12.0" customHeight="1"/>
-    <row r="997" ht="12.0" customHeight="1"/>
-    <row r="998" ht="12.0" customHeight="1"/>
-    <row r="999" ht="12.0" customHeight="1"/>
-    <row r="1000" ht="12.0" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -24046,11 +24260,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="E12"/>
+    <hyperlink r:id="rId3" ref="E20"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NAV-199 Add automatic Naomi checks to the BDG (#79)
* NAV-199 Fix Naomi data loader test

* NAV-199 New BDG with Naomi checks

* NAV-199 Add end-to-end test that uses Naomi data loading and conditionals

* NAV-199 Styling tweak
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -17,7 +17,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mhAJuQuCrSUcWDHjvnrU0Nyiot4Pg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId13" roundtripDataSignature="AMtx7mgY3G13jMtTAPFPPdMwQciM5i5Isg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -120,7 +120,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhNGibSaD8hG1aPYAybAzeJZKxv6g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhQRdaztJoEiZyPRyiaOIY4w4Iw+w=="/>
     </ext>
   </extLst>
 </comments>
@@ -242,6 +242,15 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="D17">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASdCRYWw
+Jonathan Berry    (2021-12-03 12:11:21)
+@jonathan@strategy4ward.com To check the wording of these automatic spectrum check tasks when he can.
+_Assigned to Jonathan Pearson_</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="K18">
       <text>
         <t xml:space="preserve">======
@@ -264,7 +273,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miByJhmzgEBl81JZEBBclzR2Xk33A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIk/v7InulN46/q1ENwBPYMeYRLw=="/>
     </ext>
   </extLst>
 </comments>
@@ -276,6 +285,14 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="E19">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAASdCRYWg
+Jonathan Berry    (2021-12-03 12:04:13)
+@jonathan@strategy4ward.com to review the wording of these tasks for  Naomi automatic checks when he can.</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="F18">
       <text>
         <t xml:space="preserve">======
@@ -289,14 +306,14 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJslj5uvmHEvEMtEDbwbds5MVx3A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgkJMrpR5qGHcJ916e/YHH+qqje6A=="/>
     </ext>
   </extLst>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="621">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="645">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -667,7 +684,7 @@
     <t>Has user updated VMMC data file?</t>
   </si>
   <si>
-    <t xml:space="preserve">*This task is only for VMMC priority countries. If you are not from one of the priority VMMC countries, mark this task complete and click "What's Next".* Before you upload data files to your Inputs Package to ADR, ensure you have updated the data files for the current reporting period.  **Update** your programme data files for VMMC (if relevant). If you produced a VMMC data file last year, UNAIDS has placed that final file in this year's Inputs Package for your convenience. UNAIDS recommends beginning with last year's final Inputs Package and only updating the files for the current reporting period. If you are not using VMMC data for your estimates, you can market this task as complete. You can learn more about the data elements required in Guide 8 Data Quality, Indicator Elements Matrix. </t>
+    <t xml:space="preserve">*This task is only for VMMC priority countries. If you are not from one of the priority VMMC countries, mark this task complete and click "What's Next".* Before you upload data files to your Inputs Package to ADR, ensure you have updated the data files for the current reporting period.  **Update** your programme data files for VMMC (if relevant). UNAIDS recommends beginning with last year's data and only updating as necessary for the current reporting period. If you are not using VMMC data for your estimates, you can market this task as complete. You can learn more about the data elements required in Guide 8 Data Quality, Indicator Elements Matrix. </t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-GEN-05-01-A')</t>
@@ -2283,7 +2300,10 @@
     <t>SPF-13-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Enter PMTCT data for the current reporting year into Spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date PMTCT programme data for the reporting period. These data are required for each Spectrum file. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. Spectrum also provides specific guidance for each regimen in the PMTCT data entry page. *It is highly recommended you finalize your programme data before beginning the Spectrum process.* If edits to PMTCT programme data are required later in the process, you will have to return to this step. For countries with sub-national Spectrum estimates (optional), this step applies to each file. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2313,7 +2333,10 @@
     <t>SPF-14-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Update Adult ART data in Spectrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date Adult ART programme data for the reporting period for estimating treatment coverage and for estimating incidence. You should update the ART data before running your incidence curve. Data on the number newly initiated on ART and lost to follow up can improve the precision of some of the outputs from Spectrum. If those data are available be sure to include them. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. If edits to the ART programme data are required later in the process, you will have to rerun your incidence curve fitting. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2328,7 +2351,10 @@
     <t>SPF-15-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Update Pediatric ART data in Spectrum for the current reporting period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date Pediatric ART programme data for the reporting period. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. It is highly recommended you finalize your programme data before beginning the Spectrum process. If edits to ART programme data are required later in the process, you will have to return to this step. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2337,6 +2363,9 @@
   </si>
   <si>
     <t>SPF-16-01</t>
+  </si>
+  <si>
+    <t>Spectrum Validation: Update viral load suppression data in Spectrum for the current reporting period for adult females and males and pediatric populations</t>
   </si>
   <si>
     <r>
@@ -2357,7 +2386,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Spectrum requires up-to-date adult and pediatric viral load suppression programme data for the reporting period. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. It is highly recommended you finalize your programme data before beginning the Spectrum process. Enter the best, most up-to-date viral load suppression data you have for adult female, adult male, and pediatric populations. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2368,7 +2397,10 @@
     <t>SPF-17-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for adult parameters under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum relies on a number of assumptions that are summarized under Advanced Options. These parameters are updated every year as new research and evidence is available on those parameters. For Spectrum on the Desktop update the parameters by selecting Advanced Options &gt; Adult Parameters &gt; Restore defaults. For Spectrum on the web: enter Advanced Options and confirm the default selections for adult parameters. If you see values in red font, the parameters have not been updated. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2379,7 +2411,10 @@
     <t>SPF-18-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for pediatric parameters under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum relies on a number of assumptions that are summarized under Advanced Options. These parameters are updated every year as new research and evidence is available on those parameters. For Spectrum on the Desktop update the parameters by selecting Advanced Options &gt; Pediatric Parameters &gt; Restore defaults. For Spectrum on the web: enter Advanced Options and confirm the default selections for pediatric parameters. If you see values in red font, the parameters have not been updated. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2390,7 +2425,10 @@
     <t>SPF-19-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for Fertility Rate Ratios under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. They must be confirmed for CD4, on ART, and off ART. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2401,7 +2439,10 @@
     <t>SPF-20-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for MTCT probabilities under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "MTCT Transmission Probabilities" are correct for your country. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2412,7 +2453,10 @@
     <t>SPF-21-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Confirm default values for new ART allocation method under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selection for the "allocation method for new ART patients" is correct for your country. To learn more about the Advanced Options, see the Spectrum training materials. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2423,7 +2467,10 @@
     <t>SPF-22-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Upload a completed Shiny 90 file to Spectrum or enter KOS estimates in another format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Each of your Spectrum files requires updated knowledge of status data elements for current estimates year using one of available options - Direct Entry of Case Reports, Shiny 90, CSAVR, ECDC, Manual Entry. Most countries will use Shiny 90. If you have used Shiny 90, you must upload your Shiny 90 model outputs (AIM &gt; Program Statistics &gt; Knowledge of Status &gt; Data Source = Shiny 90 &gt; Load Data).
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2432,6 +2479,9 @@
   </si>
   <si>
     <t>SPF-23-01</t>
+  </si>
+  <si>
+    <t>Spectrum Validation: Confirm your ART and PMTCT coverage does not exceed 100%</t>
   </si>
   <si>
     <r>
@@ -2461,7 +2511,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 Occasionally, Spectrum will produce coverage of over 100% for ART or PMTCT services. There are multiple causes for coverage results over 100%. UNAIDS recommends consulting your estimates facilitator and/or UNAIDS to determine how to address coverage issues in your model results. 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
   </si>
@@ -2472,7 +2522,10 @@
     <t>SPF-24-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Navigator has detected that there is a problem with your Spectrum file. 
+    <t>Spectrum Validation: Run Uncertainty Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 The uncertainty associated with each result can be estimated using the Uncertainty Analysis tool. Access this tool by choosing ‘Tools’ from the top horizontal menu, then ‘More Tools’, then ‘Uncertainty analysis’. 
 Set the ‘Aggregate data capture year’ to the final year of data and the ‘Number of iterations’ to 300, then click the ‘Process’ button. The model will run 300 simulations by choosing values for the epidemiological parameters from within their confidence intervals. This analysis may take 10-30 minutes. When it is complete, click the ‘Save’ button. After running this analysis you will see uncertainty intervals on all the outputs (as long as you only have one projection open in Spectrum). 
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
@@ -2481,15 +2534,6 @@
     <t>check_spectrum_file(['UAvalid'])</t>
   </si>
   <si>
-    <t>SPF-25-CK</t>
-  </si>
-  <si>
-    <t>Are SPF-13-01, SPF-14-01, SPF-15-01, SPF-16-01, SPF-17-01, SPF-18-01, SPF-19-01, SPF-20-01, SPF-21-01, SPF-22-01, SPF-23-01, SPF-24-01 complete?</t>
-  </si>
-  <si>
-    <t>check_not_skipped(['EST-SPF-13-01-A', 'EST-SPF-14-01-A', 'EST-SPF-15-01-A', 'EST-SPF-16-01-A', 'EST-SPF-17-01-A', 'EST-SPF-18-01-A', 'EST-SPF-19-01-A', 'EST-SPF-20-01-A', 'EST-SPF-21-01-A', 'EST-SPF-22-01-A', 'EST-SPF-23-01-A', 'EST-SPF-24-01-A' ])</t>
-  </si>
-  <si>
     <t>SPF-26-01</t>
   </si>
   <si>
@@ -2533,6 +2577,9 @@
     <t>User has a validated, final Spectrum file
 No underlying Spectrum data (e.g., surveillance, survey, or programme data) have changed since the Spectrum file was produced. 
 User has uploaded validated programme data and survey data files to ADR in the required formats</t>
+  </si>
+  <si>
+    <t>load_csv_from_zipped_resource('inputs-unaids-naomi-output-zip', '.*unaids_navigator_checklist.csv', 'naomi-validation-file')</t>
   </si>
   <si>
     <t>Naomi Check File Ref</t>
@@ -2813,6 +2860,109 @@
   </si>
   <si>
     <t>check_manual_confirmation('EST-NAO-14-01-A')</t>
+  </si>
+  <si>
+    <t>NAO-15-01</t>
+  </si>
+  <si>
+    <t>Naomi Validation: Match data inputs for Spectrum and Naomi</t>
+  </si>
+  <si>
+    <t>**Navigator has detected a problem with your Naomi Outputs zip.**
+Some data inputs used by Naomi are disaggregated versions of data inputs for other models such as Spectrum. For example, ART and ANC data used by Naomi are also used by Spectrum. You can learn more about the requirements for each of the models from 'Guide 8' in the UNAIDS training materials (attached below). It is critical that data inputs used by Naomi match the inputs used by Spectrum. Although in some cases disaggregation levels may differ, the sum of the disaggregations must equal those used by Spectrum. If the Naomi data inputs do not match those used in your Spectrum model process, modify them to match. If you have changed inputs used by Spectrum, you must return to Spectrum and begin the process again. If you have altered your Naomi inputs to match those used by Spectrum, you may continue with Naomi. 
+**Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
+  </si>
+  <si>
+    <t>check_naomi_file(['ART_is_Spectrum', 'ANC_is_Spectrum'])</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Ian: run a formal validation to compare the values in the spectrum file and the naomi input files
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF0000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>@Fjelltopp - can ADR compare the Spectrum file's numbers and compare them to the Naomi Input Files?</t>
+    </r>
+  </si>
+  <si>
+    <t>NAO-16-01</t>
+  </si>
+  <si>
+    <t>Naomi Validation: Select or confirm default settings in Naomi model options</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>**Navigator has detected a problem with your Naomi Outputs zip.**
+Naomi is a flexible model which allows countries to customize their subnational outputs. Review the multitude of model options available to users. You can learn more about these options in 'Guide 5, Naomi Quick Start' in UNAIDS estimates training materials</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>**Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
+    </r>
+  </si>
+  <si>
+    <t>check_naomi_file(['Opt_recent_qtr', 'Opt_future_proj_qtr' , 'Opt_area_ID_selected', 'Opt_calendar_survey_match', 'Opt_recent_survey_only', 'Opt_ART_coverage', 'Opt_ANC_data', 'Opt_ART_data', 'Opt_ART_attendance_yes'])</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color theme="1"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t xml:space="preserve">Ian: Can we run a formal check on the naomi file that is uploaded to the ADR to verify if the standandirsed options a country has used match what is expecetd. This means we need a prepoulated database that contains a list of expected parameters for each country that uses naomi
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <color rgb="FFFF0000"/>
+        <sz val="8.0"/>
+      </rPr>
+      <t>@Fjelltopp - possible this year?</t>
+    </r>
+  </si>
+  <si>
+    <t>NAO-17-01</t>
+  </si>
+  <si>
+    <t>Naomi Validation:  Calibrate the model in Naomi</t>
+  </si>
+  <si>
+    <t>**Navigator has detected a problem with your Naomi Outputs zip.**
+You should calibrate your model for the following four indicators (PLHIV, ART, aware of HIV status and new infections). This is to ensure that the mean aggregate estimates from Spectrum and Naomi are consistent. All these should be adjusted to match your Spectrum file either the national or sub-national Spectrum files with the following age sex stratification: (sex and age &lt;15 /15+ years). Calibration method: use the default which is logistic and which scales the prevalence, ART coverage, proportion unaware, and incidence on the logit scale within each district / sex / age stratum in order to match to Spectrum. This ensures that ART coverage does not go above 100% in any district / sex / age stratification. Further information is available in Guide 5, Naomi Quick Start. 
+**Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
+  </si>
+  <si>
+    <t>check_naomi_file(['Cal_PLHIV', 'Cal_ART', 'Cal_KOS', 'Cal_new_infections', 'Cal_method'])</t>
   </si>
 </sst>
 </file>
@@ -3430,16 +3580,16 @@
     <xf borderId="1" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -19252,43 +19402,43 @@
       <c r="A17" s="16" t="s">
         <v>488</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>232</v>
+      <c r="B17" s="16" t="s">
+        <v>489</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>233</v>
       </c>
       <c r="D17" s="90" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E17" s="91" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
       <c r="H17" s="16" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="I17" s="89" t="s">
         <v>231</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="16" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
-        <v>492</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>251</v>
+        <v>493</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>494</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>252</v>
       </c>
       <c r="D18" s="90" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>247</v>
@@ -19296,28 +19446,28 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
       <c r="H18" s="121" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="I18" s="89" t="s">
         <v>250</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="16" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
-        <v>496</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>263</v>
+        <v>498</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>499</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>264</v>
       </c>
       <c r="D19" s="90" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>247</v>
@@ -19325,7 +19475,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
       <c r="H19" s="121" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="I19" s="89" t="s">
         <v>262</v>
@@ -19335,22 +19485,22 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
-        <v>499</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>269</v>
+        <v>502</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>503</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
       <c r="D20" s="90" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
       <c r="H20" s="121" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="I20" s="89" t="s">
         <v>268</v>
@@ -19360,16 +19510,16 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
-        <v>503</v>
-      </c>
-      <c r="B21" s="99" t="s">
-        <v>280</v>
+        <v>507</v>
+      </c>
+      <c r="B21" s="122" t="s">
+        <v>508</v>
       </c>
       <c r="C21" s="99" t="s">
         <v>281</v>
       </c>
       <c r="D21" s="100" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="E21" s="101" t="s">
         <v>283</v>
@@ -19377,7 +19527,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
       <c r="H21" s="121" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="I21" s="89" t="s">
         <v>279</v>
@@ -19387,16 +19537,16 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
-        <v>506</v>
-      </c>
-      <c r="B22" s="99" t="s">
-        <v>287</v>
+        <v>511</v>
+      </c>
+      <c r="B22" s="122" t="s">
+        <v>512</v>
       </c>
       <c r="C22" s="99" t="s">
         <v>288</v>
       </c>
       <c r="D22" s="100" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="E22" s="101" t="s">
         <v>283</v>
@@ -19404,7 +19554,7 @@
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="121" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="I22" s="89" t="s">
         <v>286</v>
@@ -19414,16 +19564,16 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>293</v>
+        <v>515</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>516</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>294</v>
       </c>
       <c r="D23" s="90" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="E23" s="103" t="s">
         <v>283</v>
@@ -19431,7 +19581,7 @@
       <c r="F23" s="15"/>
       <c r="G23" s="15"/>
       <c r="H23" s="121" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="I23" s="89"/>
       <c r="J23" s="15"/>
@@ -19439,16 +19589,16 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="16" t="s">
-        <v>512</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>299</v>
+        <v>519</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>520</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>300</v>
       </c>
       <c r="D24" s="90" t="s">
-        <v>513</v>
+        <v>521</v>
       </c>
       <c r="E24" s="103" t="s">
         <v>302</v>
@@ -19456,7 +19606,7 @@
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="121" t="s">
-        <v>514</v>
+        <v>522</v>
       </c>
       <c r="I24" s="89"/>
       <c r="J24" s="15"/>
@@ -19464,16 +19614,16 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>515</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>306</v>
+        <v>523</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>524</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>307</v>
       </c>
       <c r="D25" s="90" t="s">
-        <v>516</v>
+        <v>525</v>
       </c>
       <c r="E25" s="103" t="s">
         <v>283</v>
@@ -19481,7 +19631,7 @@
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="121" t="s">
-        <v>517</v>
+        <v>526</v>
       </c>
       <c r="I25" s="89" t="s">
         <v>305</v>
@@ -19491,22 +19641,22 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="16" t="s">
-        <v>518</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>430</v>
+        <v>527</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>528</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>431</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>519</v>
+        <v>529</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="121" t="s">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="I26" s="119" t="s">
         <v>434</v>
@@ -19516,22 +19666,22 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="16" t="s">
-        <v>521</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>449</v>
+        <v>531</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>532</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>522</v>
+        <v>533</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>523</v>
+        <v>534</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="16" t="s">
-        <v>524</v>
+        <v>535</v>
       </c>
       <c r="I27" s="119" t="s">
         <v>453</v>
@@ -19541,22 +19691,22 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="16" t="s">
-        <v>525</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>461</v>
+        <v>536</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>537</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>462</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>526</v>
+        <v>538</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="121" t="s">
-        <v>527</v>
+        <v>539</v>
       </c>
       <c r="I28" s="119" t="s">
         <v>465</v>
@@ -19566,72 +19716,56 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="16" t="s">
-        <v>528</v>
-      </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="122" t="s">
-        <v>529</v>
-      </c>
-      <c r="D29" s="112"/>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="81" t="s">
-        <v>530</v>
+        <v>540</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>541</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>543</v>
+      </c>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="16" t="s">
+        <v>544</v>
       </c>
       <c r="I29" s="119"/>
-      <c r="J29" s="15"/>
+      <c r="J29" s="15" t="s">
+        <v>545</v>
+      </c>
       <c r="K29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="16" t="s">
-        <v>531</v>
+        <v>546</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>534</v>
+        <v>549</v>
       </c>
       <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="F30" s="15">
+        <v>1.0</v>
+      </c>
       <c r="G30" s="15"/>
       <c r="H30" s="16" t="s">
-        <v>535</v>
+        <v>550</v>
       </c>
       <c r="I30" s="119"/>
-      <c r="J30" s="15" t="s">
-        <v>536</v>
-      </c>
+      <c r="J30" s="15"/>
       <c r="K30" s="15"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="16" t="s">
-        <v>537</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>538</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>539</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>540</v>
-      </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15">
-        <v>1.0</v>
-      </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16" t="s">
-        <v>541</v>
-      </c>
-      <c r="I31" s="119"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
+    <row r="31" ht="13.5" customHeight="1">
+      <c r="I31" s="48"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="I32" s="48"/>
@@ -20233,7 +20367,7 @@
     <row r="231" ht="13.5" customHeight="1">
       <c r="I231" s="48"/>
     </row>
-    <row r="232" ht="13.5" customHeight="1">
+    <row r="232" ht="15.75" customHeight="1">
       <c r="I232" s="48"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
@@ -22572,9 +22706,6 @@
     </row>
     <row r="1011" ht="15.75" customHeight="1">
       <c r="I1011" s="48"/>
-    </row>
-    <row r="1012" ht="15.75" customHeight="1">
-      <c r="I1012" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -22604,14 +22735,14 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.57"/>
-    <col customWidth="1" min="2" max="2" width="11.43"/>
+    <col customWidth="1" min="2" max="2" width="16.14"/>
     <col customWidth="1" min="3" max="3" width="12.29"/>
     <col customWidth="1" min="4" max="4" width="19.43"/>
     <col customWidth="1" min="5" max="5" width="63.0"/>
     <col customWidth="1" min="6" max="6" width="52.86"/>
-    <col customWidth="1" min="7" max="7" width="11.29"/>
+    <col customWidth="1" min="7" max="7" width="16.29"/>
     <col customWidth="1" min="8" max="8" width="20.57"/>
-    <col customWidth="1" min="9" max="9" width="11.29"/>
+    <col customWidth="1" min="9" max="9" width="42.14"/>
     <col customWidth="1" min="10" max="10" width="45.14"/>
     <col customWidth="1" hidden="1" min="11" max="11" width="8.71"/>
     <col customWidth="1" min="12" max="12" width="8.71"/>
@@ -22632,33 +22763,38 @@
       <c r="F1" s="35" t="s">
         <v>3</v>
       </c>
+      <c r="G1" s="35" t="s">
+        <v>412</v>
+      </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="38" t="s">
-        <v>542</v>
+        <v>551</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>543</v>
+        <v>552</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="37" t="s">
-        <v>544</v>
+        <v>553</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="37">
         <v>0.2</v>
       </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="124"/>
-      <c r="I2" s="124"/>
+      <c r="G2" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="H2" s="123"/>
+      <c r="I2" s="123"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="125" t="s">
-        <v>545</v>
+      <c r="B4" s="124" t="s">
+        <v>555</v>
       </c>
       <c r="C4" s="85" t="s">
         <v>10</v>
@@ -22690,17 +22826,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>546</v>
+        <v>556</v>
       </c>
       <c r="B5" s="119"/>
       <c r="C5" s="15" t="s">
-        <v>547</v>
+        <v>557</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>548</v>
+        <v>558</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>549</v>
+        <v>559</v>
       </c>
       <c r="F5" s="15"/>
       <c r="G5" s="15">
@@ -22708,26 +22844,26 @@
       </c>
       <c r="H5" s="15"/>
       <c r="I5" s="16" t="s">
-        <v>550</v>
+        <v>560</v>
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="B6" s="119" t="s">
-        <v>552</v>
+        <v>562</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>553</v>
+        <v>563</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>554</v>
+        <v>564</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>555</v>
+        <v>565</v>
       </c>
       <c r="F6" s="15"/>
       <c r="G6" s="15">
@@ -22735,16 +22871,16 @@
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="16" t="s">
-        <v>556</v>
+        <v>566</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>557</v>
+        <v>567</v>
       </c>
       <c r="K6" s="15"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>558</v>
+        <v>568</v>
       </c>
       <c r="B7" s="119"/>
       <c r="C7" s="15" t="s">
@@ -22754,7 +22890,7 @@
         <v>178</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>559</v>
+        <v>569</v>
       </c>
       <c r="F7" s="15" t="s">
         <v>180</v>
@@ -22762,14 +22898,14 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
       <c r="I7" s="16" t="s">
-        <v>560</v>
+        <v>570</v>
       </c>
       <c r="J7" s="95"/>
       <c r="K7" s="15"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>561</v>
+        <v>571</v>
       </c>
       <c r="B8" s="119"/>
       <c r="C8" s="15" t="s">
@@ -22785,17 +22921,17 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
       <c r="I8" s="16" t="s">
-        <v>562</v>
+        <v>572</v>
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>564</v>
+        <v>574</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>188</v>
@@ -22804,32 +22940,32 @@
         <v>189</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>565</v>
+        <v>575</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
       <c r="I9" s="16" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>567</v>
+        <v>577</v>
       </c>
       <c r="B10" s="119" t="s">
-        <v>568</v>
+        <v>578</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>569</v>
+        <v>579</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>570</v>
+        <v>580</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>571</v>
+        <v>581</v>
       </c>
       <c r="F10" s="103" t="s">
         <v>247</v>
@@ -22839,82 +22975,82 @@
       </c>
       <c r="H10" s="15"/>
       <c r="I10" s="16" t="s">
-        <v>572</v>
+        <v>582</v>
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="15" t="s">
-        <v>573</v>
+        <v>583</v>
       </c>
       <c r="B11" s="119"/>
       <c r="C11" s="15" t="s">
-        <v>574</v>
+        <v>584</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>575</v>
+        <v>585</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>576</v>
+        <v>586</v>
       </c>
       <c r="F11" s="103" t="s">
-        <v>577</v>
+        <v>587</v>
       </c>
       <c r="G11" s="15"/>
       <c r="H11" s="15"/>
       <c r="I11" s="16" t="s">
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="15" t="s">
-        <v>579</v>
+        <v>589</v>
       </c>
       <c r="B12" s="119" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>581</v>
+        <v>591</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>582</v>
+        <v>592</v>
       </c>
       <c r="E12" s="91" t="s">
-        <v>583</v>
+        <v>593</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>584</v>
+        <v>594</v>
       </c>
       <c r="G12" s="15">
         <v>1.0</v>
       </c>
       <c r="H12" s="15"/>
       <c r="I12" s="16" t="s">
-        <v>585</v>
+        <v>595</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="K12" s="15"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>587</v>
+        <v>597</v>
       </c>
       <c r="B13" s="119" t="s">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>589</v>
+        <v>599</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>591</v>
+        <v>601</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="15">
@@ -22922,53 +23058,53 @@
       </c>
       <c r="H13" s="15"/>
       <c r="I13" s="16" t="s">
-        <v>592</v>
+        <v>602</v>
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="15"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="15" t="s">
-        <v>593</v>
+        <v>603</v>
       </c>
       <c r="B14" s="119" t="s">
-        <v>594</v>
+        <v>604</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>595</v>
+        <v>605</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>597</v>
+        <v>607</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>598</v>
+        <v>608</v>
       </c>
       <c r="G14" s="15">
         <v>1.0</v>
       </c>
       <c r="H14" s="15"/>
       <c r="I14" s="16" t="s">
-        <v>599</v>
+        <v>609</v>
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="15"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="B15" s="119"/>
       <c r="C15" s="16" t="s">
-        <v>601</v>
+        <v>611</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>602</v>
+        <v>612</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>603</v>
+        <v>613</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15">
@@ -22976,47 +23112,47 @@
       </c>
       <c r="H15" s="15"/>
       <c r="I15" s="16" t="s">
-        <v>604</v>
+        <v>614</v>
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="15"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="15" t="s">
-        <v>605</v>
+        <v>615</v>
       </c>
       <c r="B16" s="119"/>
       <c r="C16" s="15" t="s">
-        <v>606</v>
+        <v>616</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>607</v>
+        <v>617</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>608</v>
+        <v>618</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
       <c r="I16" s="16" t="s">
-        <v>609</v>
+        <v>619</v>
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="15"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="15" t="s">
-        <v>610</v>
+        <v>620</v>
       </c>
       <c r="B17" s="119"/>
       <c r="C17" s="15" t="s">
-        <v>611</v>
+        <v>621</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>612</v>
+        <v>622</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>613</v>
+        <v>623</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15">
@@ -23024,41 +23160,123 @@
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="16" t="s">
-        <v>614</v>
+        <v>624</v>
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="15"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="15" t="s">
-        <v>615</v>
+        <v>625</v>
       </c>
       <c r="B18" s="119"/>
       <c r="C18" s="15" t="s">
-        <v>616</v>
+        <v>626</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>617</v>
+        <v>627</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>618</v>
+        <v>628</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>619</v>
+        <v>629</v>
       </c>
       <c r="G18" s="15">
         <v>1.0</v>
       </c>
       <c r="H18" s="15"/>
       <c r="I18" s="16" t="s">
-        <v>620</v>
+        <v>630</v>
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="15"/>
     </row>
-    <row r="19" ht="12.0" customHeight="1"/>
-    <row r="20" ht="12.0" customHeight="1"/>
-    <row r="21" ht="12.0" customHeight="1"/>
+    <row r="19" ht="12.0" customHeight="1">
+      <c r="A19" s="16" t="s">
+        <v>631</v>
+      </c>
+      <c r="B19" s="119" t="s">
+        <v>562</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>632</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>564</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>633</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>247</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="16" t="s">
+        <v>634</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>635</v>
+      </c>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="20" ht="49.5" customHeight="1">
+      <c r="A20" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="B20" s="119" t="s">
+        <v>590</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>592</v>
+      </c>
+      <c r="E20" s="125" t="s">
+        <v>638</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>594</v>
+      </c>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="16" t="s">
+        <v>639</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>640</v>
+      </c>
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" ht="12.0" customHeight="1">
+      <c r="A21" s="16" t="s">
+        <v>641</v>
+      </c>
+      <c r="B21" s="119" t="s">
+        <v>604</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>642</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>606</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>643</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>608</v>
+      </c>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="16" t="s">
+        <v>644</v>
+      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+    </row>
     <row r="22" ht="12.0" customHeight="1"/>
     <row r="23" ht="12.0" customHeight="1"/>
     <row r="24" ht="12.0" customHeight="1"/>
@@ -24034,10 +24252,6 @@
     <row r="994" ht="12.0" customHeight="1"/>
     <row r="995" ht="12.0" customHeight="1"/>
     <row r="996" ht="12.0" customHeight="1"/>
-    <row r="997" ht="12.0" customHeight="1"/>
-    <row r="998" ht="12.0" customHeight="1"/>
-    <row r="999" ht="12.0" customHeight="1"/>
-    <row r="1000" ht="12.0" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -24046,11 +24260,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId2" ref="E12"/>
+    <hyperlink r:id="rId3" ref="E20"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NAV-190 Add blocking step to BDG
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -33,7 +33,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -496,6 +496,53 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">OVV-00-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Under development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always Fail</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Navigator is still under development. 
+It is expected that you will be able to begin using the Navigator by 9am GMT on the 7</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> December 2021. 
+Please check back at this time.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">return_false()</t>
+  </si>
+  <si>
     <t xml:space="preserve">OVV-01-10</t>
   </si>
   <si>
@@ -634,23 +681,6 @@
   </si>
   <si>
     <t xml:space="preserve">06-GenKOSShiny90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OVV-08-02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Under development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Always Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigator is still under development. 
-It is expected that the final milestones will become available by  Friday 10th December 2021 at 9am UTC.
-Please check back at this time.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">return_false()</t>
   </si>
   <si>
     <t xml:space="preserve">OVV-09-01</t>
@@ -2829,7 +2859,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2885,15 +2915,23 @@
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Arial"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -3058,14 +3096,14 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="thin"/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left/>
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
@@ -3160,12 +3198,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3173,6 +3215,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3188,12 +3238,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -3204,16 +3250,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -3224,7 +3262,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3232,23 +3270,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3256,7 +3294,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3264,7 +3302,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3276,7 +3314,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3284,35 +3322,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3320,27 +3358,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3356,7 +3394,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3364,15 +3402,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3396,11 +3434,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3408,15 +3446,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3428,11 +3466,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3440,7 +3478,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3448,7 +3486,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3456,7 +3494,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3537,15 +3575,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X1004"/>
+  <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
+      <selection pane="bottomLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49"/>
@@ -3697,28 +3735,28 @@
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
     </row>
-    <row r="5" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="51.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14" t="n">
+      <c r="E5" s="14"/>
+      <c r="F5" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="6"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
@@ -3735,25 +3773,27 @@
       <c r="X5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
+      <c r="F6" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
@@ -3770,25 +3810,25 @@
       <c r="X6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="19" t="s">
         <v>28</v>
       </c>
+      <c r="B7" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="C7" s="13" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
@@ -3805,27 +3845,25 @@
       <c r="X7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
-        <v>31</v>
+      <c r="A8" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="C8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6" t="s">
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -3842,27 +3880,27 @@
       <c r="X8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="14" t="n">
+      <c r="E9" s="22"/>
+      <c r="F9" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
@@ -3882,20 +3920,24 @@
       <c r="A10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="14" t="n">
+      <c r="D10" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
+      <c r="G10" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
@@ -3913,22 +3955,22 @@
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="14" t="n">
+      <c r="B11" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="5"/>
@@ -3944,24 +3986,24 @@
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
     </row>
-    <row r="12" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+        <v>51</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
@@ -3977,24 +4019,24 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
     </row>
-    <row r="13" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="19.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
+      <c r="B13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
@@ -4012,22 +4054,22 @@
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="14" t="n">
+      <c r="B14" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
@@ -4045,22 +4087,22 @@
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="14" t="n">
+      <c r="B15" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
@@ -4076,27 +4118,23 @@
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
     </row>
-    <row r="16" customFormat="false" ht="42.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="B16" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="20"/>
-      <c r="F16" s="14" t="n">
+      <c r="C16" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G16" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="16"/>
       <c r="I16" s="6"/>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -4117,18 +4155,18 @@
       <c r="A17" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="17" t="s">
         <v>65</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="14" t="n">
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="G17" s="22"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="26"/>
       <c r="I17" s="6"/>
       <c r="K17" s="5"/>
@@ -4150,15 +4188,15 @@
       <c r="A18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="17" t="s">
         <v>68</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="14" t="n">
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="13"/>
@@ -10315,6 +10353,7 @@
     <row r="1002" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1003" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1004" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:C1"/>
@@ -10346,17 +10385,17 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.87"/>
   </cols>
   <sheetData>
@@ -10439,21 +10478,21 @@
       <c r="B5" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="18" t="s">
         <v>76</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>77</v>
       </c>
       <c r="F5" s="32"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="18" t="s">
         <v>79</v>
       </c>
       <c r="K5" s="33"/>
@@ -10480,21 +10519,21 @@
       <c r="B6" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="18" t="s">
         <v>83</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15" t="s">
+      <c r="F6" s="18"/>
+      <c r="G6" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15" t="s">
+      <c r="H6" s="18"/>
+      <c r="I6" s="18" t="s">
         <v>86</v>
       </c>
       <c r="K6" s="33"/>
@@ -10521,21 +10560,21 @@
       <c r="B7" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="18" t="s">
         <v>91</v>
       </c>
       <c r="F7" s="35"/>
       <c r="G7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15" t="s">
+      <c r="H7" s="18"/>
+      <c r="I7" s="18" t="s">
         <v>93</v>
       </c>
       <c r="K7" s="33"/>
@@ -10562,19 +10601,19 @@
       <c r="B8" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="18" t="s">
         <v>91</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15" t="s">
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="s">
         <v>98</v>
       </c>
       <c r="K8" s="33"/>
@@ -10601,19 +10640,19 @@
       <c r="B9" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="18" t="s">
         <v>91</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="6"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="18" t="s">
         <v>103</v>
       </c>
       <c r="K9" s="33"/>
@@ -10640,19 +10679,19 @@
       <c r="B10" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="18" t="s">
         <v>108</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="6"/>
       <c r="H10" s="13"/>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="18" t="s">
         <v>109</v>
       </c>
       <c r="K10" s="33"/>
@@ -10679,19 +10718,19 @@
       <c r="B11" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="18" t="s">
         <v>114</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="6"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="18" t="s">
         <v>115</v>
       </c>
       <c r="K11" s="33"/>
@@ -10718,19 +10757,19 @@
       <c r="B12" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="18" t="s">
         <v>114</v>
       </c>
       <c r="F12" s="35"/>
       <c r="G12" s="6"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="18" t="s">
         <v>120</v>
       </c>
       <c r="K12" s="33"/>
@@ -10757,19 +10796,19 @@
       <c r="B13" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="18" t="s">
         <v>114</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="6"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="18" t="s">
         <v>125</v>
       </c>
       <c r="K13" s="33"/>
@@ -10796,19 +10835,19 @@
       <c r="B14" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="18" t="s">
         <v>114</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="6"/>
       <c r="H14" s="13"/>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="18" t="s">
         <v>130</v>
       </c>
       <c r="K14" s="33"/>
@@ -11895,11 +11934,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="56.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.01"/>
@@ -11984,22 +12023,22 @@
       <c r="A5" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="32"/>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="18"/>
+      <c r="I5" s="18" t="s">
         <v>139</v>
       </c>
     </row>
@@ -12016,10 +12055,10 @@
       <c r="D6" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="32"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="15"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="41" t="s">
         <v>144</v>
       </c>
@@ -12044,20 +12083,20 @@
       <c r="A7" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="32"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15" t="s">
+      <c r="G7" s="25"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18" t="s">
         <v>149</v>
       </c>
       <c r="J7" s="5"/>
@@ -12081,22 +12120,22 @@
       <c r="A8" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="18" t="s">
         <v>153</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>114</v>
       </c>
       <c r="F8" s="32"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15" t="s">
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18" t="s">
         <v>154</v>
       </c>
       <c r="J8" s="5"/>
@@ -12120,22 +12159,22 @@
       <c r="A9" s="13" t="s">
         <v>155</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="18" t="s">
         <v>158</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>114</v>
       </c>
       <c r="F9" s="32"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15" t="s">
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18" t="s">
         <v>159</v>
       </c>
       <c r="J9" s="5"/>
@@ -12198,22 +12237,22 @@
       <c r="A11" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="18" t="s">
         <v>168</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15" t="s">
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18" t="s">
         <v>169</v>
       </c>
       <c r="J11" s="47"/>
@@ -13251,7 +13290,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9"/>
@@ -13356,7 +13395,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="18" t="s">
         <v>177</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -13381,7 +13420,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="18" t="s">
         <v>183</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -13404,7 +13443,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="18" t="s">
         <v>188</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -13416,7 +13455,7 @@
       <c r="D8" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="52" t="n">
         <v>1</v>
       </c>
@@ -13427,19 +13466,19 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="18" t="s">
         <v>193</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="52" t="n">
         <v>1</v>
       </c>
@@ -13450,24 +13489,24 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="53" t="n">
         <v>1</v>
       </c>
       <c r="G10" s="54"/>
-      <c r="H10" s="22"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="13" t="s">
         <v>202</v>
       </c>
@@ -14563,7 +14602,7 @@
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -14573,7 +14612,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="35.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="35.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="31.01"/>
   </cols>
   <sheetData>
@@ -14688,7 +14727,7 @@
       <c r="G6" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="H6" s="20"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13" t="s">
         <v>219</v>
@@ -14787,7 +14826,7 @@
       <c r="H10" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="I10" s="22"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="13" t="s">
         <v>243</v>
       </c>
@@ -14811,7 +14850,7 @@
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="64"/>
-      <c r="I11" s="20"/>
+      <c r="I11" s="14"/>
       <c r="J11" s="13" t="s">
         <v>248</v>
       </c>
@@ -14935,7 +14974,7 @@
       <c r="H16" s="51" t="s">
         <v>276</v>
       </c>
-      <c r="I16" s="22"/>
+      <c r="I16" s="24"/>
       <c r="J16" s="51" t="s">
         <v>277</v>
       </c>
@@ -15065,7 +15104,7 @@
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="64"/>
-      <c r="I21" s="22"/>
+      <c r="I21" s="24"/>
       <c r="J21" s="13" t="s">
         <v>309</v>
       </c>
@@ -16149,7 +16188,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.01"/>
@@ -16157,9 +16196,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="12" style="0" width="8.71"/>
@@ -16347,7 +16386,7 @@
         <v>345</v>
       </c>
       <c r="H9" s="13"/>
-      <c r="I9" s="22"/>
+      <c r="I9" s="24"/>
       <c r="J9" s="13" t="s">
         <v>346</v>
       </c>
@@ -17411,10 +17450,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.43"/>
@@ -18774,7 +18813,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.3"/>
@@ -22520,13 +22559,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="62.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="62.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="52.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.57"/>

</xml_diff>

<commit_message>
NAV-172 Deploy a new version of the BDG
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhXSpO0zDnRWDDj+qpWlZoRJZX+ZA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhGx5s0CeZMjj0InGrvmErvoGtmWg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -93,7 +93,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhrb1YODtM0vmOQbqltQvUSazWi6g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIKUhu8sG/Mj9s1M0mahx+SgkPaA=="/>
     </ext>
   </extLst>
 </comments>
@@ -185,6 +185,30 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A5">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAS0zQkj8
+Jonathan Pearson    (2021-12-09 14:16:50)
+@jonathan@fjelltopp.org - for deletion.
+_Assigned to Jonathan Berry_</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhaiwf6jh+HW7z1kK3cW6DR1x9O7Q=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="D16">
       <text>
         <t xml:space="preserve">======
@@ -222,7 +246,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -256,7 +280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="650">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -1179,7 +1203,7 @@
     <t>ROB-06-01</t>
   </si>
   <si>
-    <t>Review time series results for your ART data file</t>
+    <t>Review time series results for your ANC and ART data file</t>
   </si>
   <si>
     <t>Has user reviewed all plot types for their ART and ANC data files and corrected all anomolies?</t>
@@ -1358,7 +1382,9 @@
     <t>Does the user's Spectrum file have current estimates year data for PMTCT [required / optional data elements available in Indicator Element Matrix]?</t>
   </si>
   <si>
-    <t>Spectrum requires up-to-date PMTCT programme data for the reporting period. These data are required for each Spectrum file. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. Spectrum also provides specific guidance for each regimen in the PMTCT data entry page. *It is highly recommended you finalize your programme data before beginning the Spectrum process.* If edits to PMTCT programme data are required later in the process, you will have to return to this step. For countries with sub-national Spectrum estimates (optional), this step applies to each file.</t>
+    <t>In order to produce updated estimates in Spectrum, updated PMTCT programme data are required. These data are required for each Spectrum file. 
+You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. Spectrum also provides specific guidance for each regimen in the PMTCT data entry page. *It is highly recommended you finalize your programme data before proceeding.* 
+If edits to PMTCT programme data are required later in the process, you will have to return to this step. For countries with sub-national Spectrum estimates (optional), this step applies to each file.</t>
   </si>
   <si>
     <r>
@@ -1404,7 +1430,7 @@
     <t>SPE-07-01</t>
   </si>
   <si>
-    <t>Update ANC testing data in Spectrum</t>
+    <t>Update and review ANC testing data in Spectrum</t>
   </si>
   <si>
     <t>Has user updated ANC testing data in their Spectrum file for current reporting period [required / optional data elements available in Indicator Element Matrix]?</t>
@@ -1569,13 +1595,13 @@
     <t>FRRCD4_default,FRRageNoART_default,FRRageART_default</t>
   </si>
   <si>
-    <t>Confirm default values for Fertility Rate Ratios under Advanced Options</t>
-  </si>
-  <si>
-    <t>Has the user confirmed that the default values for Fertility Rate Ratios under Advanced Options are correct?</t>
-  </si>
-  <si>
-    <t>To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. They must be confirmed for CD4, on ART, and off ART. To learn more about the Advanced Options, see the Spectrum training materials.</t>
+    <t>Update Fertility Rate Ratios or confirm default values are used under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the user updated the Fertility Rate Ratios under Advanced Options? </t>
+  </si>
+  <si>
+    <t>To produce accurate estimates of number of births to women living with HIV, Spectrum requires the correct assumptions about fertility among women living with HIV are selected under Advanced Options. Enter Advanced Options and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. If good quality prevalence from census level ANC data are available, those can be used with the fit local fertility adjustment. The data will be pulled directly from EPP so update your ANC-RT census data in EPP before doing this step.  To learn more about the Advanced Options, see the Spectrum training materials.</t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-SPE-14-01-A')</t>
@@ -1656,6 +1682,7 @@
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <strike/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -1664,15 +1691,16 @@
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <strike/>
         <color theme="1"/>
         <sz val="8.0"/>
-        <u/>
       </rPr>
       <t>not</t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <strike/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -1697,7 +1725,8 @@
     <t>Has the user defined and reviewed the epidemic structure in EPP?</t>
   </si>
   <si>
-    <t xml:space="preserve">EPP requires the country to have a defined epidemic structure. You can see the previously used epidemic structure for your country in Spectrum (Modules&gt;AIM&gt;Incidence&gt;Configuration (EPP)). You may have to choose EPP as the preferred option under Incidence &gt; Incidence Options. 
+    <t xml:space="preserve">Congratulations on finishing the first of two Spectrum milestones. Now you will begin the process of estimating HIV incidence using EPP. 
+EPP requires the country to have a defined epidemic structure. You can see the previously used epidemic structure for your country in Spectrum (Modules&gt;AIM&gt;Incidence&gt;Configuration (EPP)). You may have to choose EPP as the preferred option under Incidence &gt; Incidence Options. 
 If all the information is valid, you can choose "Save and continue", which will take you to EPP's "Define Pops" page. If the epidemic structure is not correct, you can set it up according to data availability for your country. Once completed, choose "Save and continue" to proceed to the next step. </t>
   </si>
   <si>
@@ -1805,7 +1834,7 @@
     <t>S90-01-10</t>
   </si>
   <si>
-    <t>Ensure pediatric and adult ART programme data inputs and incidence estimates for people living with HIV (EPP) have not changed since you completed your sex/age incidence patterns in Spectrum</t>
+    <t>Ensure pediatric and adult ART programme data inputs, incidence estimates (EPP) and sex/age patterns have not changed in Spectrum</t>
   </si>
   <si>
     <t>Programme data for pediatric and adult ART as well as incidence results are up to date?</t>
@@ -1987,13 +2016,13 @@
     <t>SPF-01-10</t>
   </si>
   <si>
-    <t>Confirm PMTCT, ANC, pediatric ART, adult ART programme data inputs have not changed since beginning the EPP process</t>
-  </si>
-  <si>
-    <t>No updates have been made to any Spectrum data files or underlying data to be used by Spectrum before using those files in models which project knowledge of status (population, PMTCT, ANC, ART, breastfeeding patterns)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If any underlying programme data have changed since you completed the first portion of Spectrum, you must update the data entry in Spectrum, rerun EPP curve fits, and rerun Shiny 90. </t>
+    <t>Confirm adult ART programme data and ANC and survey prevalence inputs have not changed since beginning the EPP process</t>
+  </si>
+  <si>
+    <t>No updates have been made to any Spectrum data inputs (population, ART programme data, ART, ANC survey and prevalence ) before estimating incidence in EPP?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If ART or surveillance data have changed since you completed the first portion of Spectrum, you must update the data entry in Spectrum, rerun EPP curve fits and update the sex/age patterns. </t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-SPF-01-10-A')</t>
@@ -2419,6 +2448,9 @@
     <t>Spectrum Validation: Confirm default values for Fertility Rate Ratios under Advanced Options</t>
   </si>
   <si>
+    <t>Has the user confirmed that the default values for Fertility Rate Ratios under Advanced Options are correct?</t>
+  </si>
+  <si>
     <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. They must be confirmed for CD4, on ART, and off ART. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
@@ -3078,7 +3110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3197,6 +3229,12 @@
       <strike/>
       <sz val="8.0"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -3402,7 +3440,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="136">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3682,10 +3720,22 @@
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3707,7 +3757,7 @@
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3718,10 +3768,10 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3984,7 +4034,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.0"/>
     <col customWidth="1" min="2" max="2" width="62.86"/>
-    <col customWidth="1" min="3" max="3" width="21.86"/>
+    <col customWidth="1" min="3" max="3" width="46.14"/>
     <col customWidth="1" min="4" max="4" width="43.71"/>
     <col customWidth="1" min="5" max="5" width="18.29"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
@@ -10624,32 +10674,32 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="46">
         <v>0.2</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>555</v>
-      </c>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
+        <v>556</v>
+      </c>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="128" t="s">
-        <v>556</v>
+      <c r="B4" s="132" t="s">
+        <v>557</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>10</v>
@@ -10681,17 +10731,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="B5" s="123"/>
+        <v>558</v>
+      </c>
+      <c r="B5" s="127"/>
       <c r="C5" s="24" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22">
@@ -10699,45 +10749,45 @@
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="24" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="B6" s="123" t="s">
         <v>563</v>
       </c>
+      <c r="B6" s="127" t="s">
+        <v>564</v>
+      </c>
       <c r="C6" s="22" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F6" s="22"/>
-      <c r="G6" s="22">
-        <v>1.0</v>
+      <c r="G6" s="24">
+        <v>0.0</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="24" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="B7" s="123"/>
+        <v>570</v>
+      </c>
+      <c r="B7" s="127"/>
       <c r="C7" s="22" t="s">
         <v>183</v>
       </c>
@@ -10745,7 +10795,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>186</v>
@@ -10753,42 +10803,42 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="24" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="J7" s="99"/>
       <c r="K7" s="22"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="B8" s="123"/>
+        <v>573</v>
+      </c>
+      <c r="B8" s="127"/>
       <c r="C8" s="22" t="s">
         <v>189</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="129" t="s">
-        <v>573</v>
+      <c r="E8" s="133" t="s">
+        <v>574</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="24" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>576</v>
-      </c>
-      <c r="B9" s="123" t="s">
         <v>577</v>
+      </c>
+      <c r="B9" s="127" t="s">
+        <v>578</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>195</v>
@@ -10797,117 +10847,117 @@
         <v>196</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="24" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="B10" s="123" t="s">
         <v>581</v>
       </c>
+      <c r="B10" s="127" t="s">
+        <v>582</v>
+      </c>
       <c r="C10" s="22" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>584</v>
-      </c>
-      <c r="F10" s="130" t="s">
         <v>585</v>
+      </c>
+      <c r="F10" s="134" t="s">
+        <v>586</v>
       </c>
       <c r="G10" s="22">
         <v>1.0</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="24" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="B11" s="123"/>
+        <v>588</v>
+      </c>
+      <c r="B11" s="127"/>
       <c r="C11" s="22" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="24" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="B12" s="123" t="s">
         <v>594</v>
       </c>
+      <c r="B12" s="127" t="s">
+        <v>595</v>
+      </c>
       <c r="C12" s="22" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="E12" s="131" t="s">
         <v>597</v>
       </c>
+      <c r="E12" s="135" t="s">
+        <v>598</v>
+      </c>
       <c r="F12" s="22" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G12" s="22">
         <v>1.0</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="24" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>601</v>
-      </c>
-      <c r="B13" s="123" t="s">
         <v>602</v>
       </c>
+      <c r="B13" s="127" t="s">
+        <v>603</v>
+      </c>
       <c r="C13" s="22" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
@@ -10915,53 +10965,53 @@
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="24" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="B14" s="123" t="s">
         <v>608</v>
       </c>
+      <c r="B14" s="127" t="s">
+        <v>609</v>
+      </c>
       <c r="C14" s="22" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="G14" s="22">
-        <v>1.0</v>
+        <v>613</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.0</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="24" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>614</v>
-      </c>
-      <c r="B15" s="123"/>
+        <v>615</v>
+      </c>
+      <c r="B15" s="127"/>
       <c r="C15" s="24" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
@@ -10969,47 +11019,47 @@
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="24" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="J15" s="99"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="B16" s="123"/>
+        <v>620</v>
+      </c>
+      <c r="B16" s="127"/>
       <c r="C16" s="22" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="24" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>624</v>
-      </c>
-      <c r="B17" s="123"/>
+        <v>625</v>
+      </c>
+      <c r="B17" s="127"/>
       <c r="C17" s="22" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
@@ -11017,53 +11067,53 @@
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="24" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>629</v>
-      </c>
-      <c r="B18" s="123"/>
+        <v>630</v>
+      </c>
+      <c r="B18" s="127"/>
       <c r="C18" s="22" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="G18" s="22">
         <v>1.0</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="24" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>635</v>
-      </c>
-      <c r="B19" s="123" t="s">
-        <v>563</v>
+        <v>636</v>
+      </c>
+      <c r="B19" s="127" t="s">
+        <v>564</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>257</v>
@@ -11071,65 +11121,65 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="24" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="K19" s="22"/>
     </row>
     <row r="20" ht="49.5" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>640</v>
-      </c>
-      <c r="B20" s="123" t="s">
-        <v>594</v>
+        <v>641</v>
+      </c>
+      <c r="B20" s="127" t="s">
+        <v>595</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="E20" s="131" t="s">
-        <v>642</v>
+        <v>597</v>
+      </c>
+      <c r="E20" s="135" t="s">
+        <v>643</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="24" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="K20" s="22"/>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>645</v>
-      </c>
-      <c r="B21" s="123" t="s">
-        <v>608</v>
+        <v>646</v>
+      </c>
+      <c r="B21" s="127" t="s">
+        <v>609</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="24" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -16569,7 +16619,7 @@
       <c r="A10" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="54" t="s">
         <v>207</v>
       </c>
       <c r="C10" s="50" t="s">
@@ -17913,7 +17963,7 @@
         <v>253</v>
       </c>
       <c r="B11" s="97"/>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>254</v>
       </c>
       <c r="D11" s="22" t="s">
@@ -18115,13 +18165,13 @@
       <c r="B19" s="97" t="s">
         <v>302</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="E19" s="96" t="s">
+      <c r="E19" s="94" t="s">
         <v>305</v>
       </c>
       <c r="F19" s="107" t="s">
@@ -19341,24 +19391,24 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="113" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="114" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="113" t="s">
         <v>331</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="114" t="s">
         <v>332</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="24" t="s">
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="114" t="s">
         <v>333</v>
       </c>
     </row>
@@ -19447,7 +19497,7 @@
       <c r="D9" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="117" t="s">
         <v>354</v>
       </c>
       <c r="F9" s="22">
@@ -20498,12 +20548,13 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E9"/>
+    <hyperlink r:id="rId2" ref="E9"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -20563,7 +20614,7 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="J3" s="114"/>
+      <c r="J3" s="118"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="89" t="s">
@@ -20601,7 +20652,7 @@
       <c r="A5" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>366</v>
       </c>
       <c r="C5" s="68" t="s">
@@ -20616,7 +20667,7 @@
       <c r="H5" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="I5" s="115"/>
+      <c r="I5" s="119"/>
       <c r="J5" s="68"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -20648,24 +20699,24 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="120" t="s">
         <v>377</v>
       </c>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116" t="s">
+      <c r="B7" s="120"/>
+      <c r="C7" s="120" t="s">
         <v>378</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
       <c r="H7" s="84" t="s">
         <v>379</v>
       </c>
-      <c r="I7" s="117" t="s">
+      <c r="I7" s="121" t="s">
         <v>380</v>
       </c>
-      <c r="J7" s="118"/>
+      <c r="J7" s="122"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
@@ -20689,7 +20740,7 @@
         <v>385</v>
       </c>
       <c r="I8" s="96"/>
-      <c r="J8" s="119"/>
+      <c r="J8" s="123"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
@@ -20711,7 +20762,7 @@
         <v>390</v>
       </c>
       <c r="I9" s="96"/>
-      <c r="J9" s="119"/>
+      <c r="J9" s="123"/>
     </row>
     <row r="10" ht="115.5" customHeight="1">
       <c r="A10" s="22" t="s">
@@ -20737,7 +20788,7 @@
       <c r="I10" s="96" t="s">
         <v>396</v>
       </c>
-      <c r="J10" s="119"/>
+      <c r="J10" s="123"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -20759,7 +20810,7 @@
         <v>401</v>
       </c>
       <c r="I11" s="96"/>
-      <c r="J11" s="119"/>
+      <c r="J11" s="123"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
@@ -20785,7 +20836,7 @@
       <c r="I12" s="96" t="s">
         <v>407</v>
       </c>
-      <c r="J12" s="119"/>
+      <c r="J12" s="123"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
@@ -20807,7 +20858,7 @@
         <v>412</v>
       </c>
       <c r="I13" s="96"/>
-      <c r="J13" s="119"/>
+      <c r="J13" s="123"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
@@ -20831,7 +20882,7 @@
         <v>417</v>
       </c>
       <c r="I14" s="96"/>
-      <c r="J14" s="119"/>
+      <c r="J14" s="123"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="C15" s="27"/>
@@ -21873,10 +21924,10 @@
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="121"/>
+      <c r="C1" s="125"/>
       <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
@@ -21895,7 +21946,7 @@
       <c r="B2" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="C2" s="121"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="8" t="s">
         <v>421</v>
       </c>
@@ -21935,7 +21986,7 @@
       <c r="H4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="122" t="s">
+      <c r="I4" s="126" t="s">
         <v>215</v>
       </c>
       <c r="J4" s="89" t="s">
@@ -21949,10 +22000,10 @@
       <c r="A5" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="24" t="s">
         <v>425</v>
       </c>
       <c r="D5" s="24" t="s">
@@ -21964,7 +22015,7 @@
       <c r="H5" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="I5" s="123"/>
+      <c r="I5" s="127"/>
       <c r="J5" s="22" t="s">
         <v>428</v>
       </c>
@@ -21989,7 +22040,7 @@
       <c r="H6" s="24" t="s">
         <v>433</v>
       </c>
-      <c r="I6" s="123"/>
+      <c r="I6" s="127"/>
       <c r="J6" s="22" t="s">
         <v>434</v>
       </c>
@@ -22016,14 +22067,14 @@
       <c r="H7" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="I7" s="123" t="s">
+      <c r="I7" s="127" t="s">
         <v>440</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>441</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="128" t="s">
         <v>442</v>
       </c>
     </row>
@@ -22048,7 +22099,7 @@
       <c r="H8" s="24" t="s">
         <v>447</v>
       </c>
-      <c r="I8" s="123"/>
+      <c r="I8" s="127"/>
       <c r="J8" s="22" t="s">
         <v>448</v>
       </c>
@@ -22075,7 +22126,7 @@
       <c r="H9" s="24" t="s">
         <v>453</v>
       </c>
-      <c r="I9" s="123"/>
+      <c r="I9" s="127"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
@@ -22100,7 +22151,7 @@
       <c r="H10" s="24" t="s">
         <v>458</v>
       </c>
-      <c r="I10" s="123" t="s">
+      <c r="I10" s="127" t="s">
         <v>459</v>
       </c>
       <c r="J10" s="22"/>
@@ -22125,7 +22176,7 @@
       <c r="H11" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="I11" s="123"/>
+      <c r="I11" s="127"/>
       <c r="J11" s="22" t="s">
         <v>465</v>
       </c>
@@ -22152,7 +22203,7 @@
       <c r="H12" s="24" t="s">
         <v>470</v>
       </c>
-      <c r="I12" s="123" t="s">
+      <c r="I12" s="127" t="s">
         <v>471</v>
       </c>
       <c r="J12" s="22"/>
@@ -22177,7 +22228,7 @@
       <c r="H13" s="24" t="s">
         <v>476</v>
       </c>
-      <c r="I13" s="123"/>
+      <c r="I13" s="127"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
@@ -22200,7 +22251,7 @@
       <c r="H14" s="24" t="s">
         <v>481</v>
       </c>
-      <c r="I14" s="123"/>
+      <c r="I14" s="127"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
@@ -22227,7 +22278,7 @@
       <c r="H15" s="24" t="s">
         <v>487</v>
       </c>
-      <c r="I15" s="123"/>
+      <c r="I15" s="127"/>
       <c r="J15" s="24" t="s">
         <v>488</v>
       </c>
@@ -22280,7 +22331,7 @@
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="125" t="s">
+      <c r="H17" s="129" t="s">
         <v>497</v>
       </c>
       <c r="I17" s="93" t="s">
@@ -22309,7 +22360,7 @@
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="125" t="s">
+      <c r="H18" s="129" t="s">
         <v>502</v>
       </c>
       <c r="I18" s="93" t="s">
@@ -22334,7 +22385,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="125" t="s">
+      <c r="H19" s="129" t="s">
         <v>507</v>
       </c>
       <c r="I19" s="93" t="s">
@@ -22347,7 +22398,7 @@
       <c r="A20" s="24" t="s">
         <v>508</v>
       </c>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="130" t="s">
         <v>509</v>
       </c>
       <c r="C20" s="103" t="s">
@@ -22361,7 +22412,7 @@
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="125" t="s">
+      <c r="H20" s="129" t="s">
         <v>511</v>
       </c>
       <c r="I20" s="93"/>
@@ -22372,7 +22423,7 @@
       <c r="A21" s="24" t="s">
         <v>512</v>
       </c>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="130" t="s">
         <v>513</v>
       </c>
       <c r="C21" s="103" t="s">
@@ -22386,7 +22437,7 @@
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="125" t="s">
+      <c r="H21" s="129" t="s">
         <v>515</v>
       </c>
       <c r="I21" s="93" t="s">
@@ -22403,18 +22454,18 @@
         <v>517</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>304</v>
+        <v>518</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E22" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="125" t="s">
-        <v>519</v>
+      <c r="H22" s="129" t="s">
+        <v>520</v>
       </c>
       <c r="I22" s="93"/>
       <c r="J22" s="22"/>
@@ -22422,24 +22473,24 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>310</v>
       </c>
       <c r="D23" s="94" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E23" s="107" t="s">
         <v>312</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="125" t="s">
-        <v>523</v>
+      <c r="H23" s="129" t="s">
+        <v>524</v>
       </c>
       <c r="I23" s="93"/>
       <c r="J23" s="22"/>
@@ -22447,24 +22498,24 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>317</v>
       </c>
       <c r="D24" s="94" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E24" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="125" t="s">
-        <v>527</v>
+      <c r="H24" s="129" t="s">
+        <v>528</v>
       </c>
       <c r="I24" s="93" t="s">
         <v>315</v>
@@ -22474,24 +22525,24 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>437</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="125" t="s">
-        <v>531</v>
-      </c>
-      <c r="I25" s="123" t="s">
+      <c r="H25" s="129" t="s">
+        <v>532</v>
+      </c>
+      <c r="I25" s="127" t="s">
         <v>440</v>
       </c>
       <c r="J25" s="22"/>
@@ -22499,24 +22550,24 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="24" t="s">
-        <v>536</v>
-      </c>
-      <c r="I26" s="123" t="s">
+        <v>537</v>
+      </c>
+      <c r="I26" s="127" t="s">
         <v>459</v>
       </c>
       <c r="J26" s="22"/>
@@ -22524,24 +22575,24 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>468</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="125" t="s">
-        <v>540</v>
-      </c>
-      <c r="I27" s="123" t="s">
+      <c r="H27" s="129" t="s">
+        <v>541</v>
+      </c>
+      <c r="I27" s="127" t="s">
         <v>471</v>
       </c>
       <c r="J27" s="22"/>
@@ -22549,41 +22600,41 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="24" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="24" t="s">
-        <v>545</v>
-      </c>
-      <c r="I28" s="123"/>
+        <v>546</v>
+      </c>
+      <c r="I28" s="127"/>
       <c r="J28" s="22" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="K28" s="22"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22">
@@ -22591,9 +22642,9 @@
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="24" t="s">
-        <v>551</v>
-      </c>
-      <c r="I29" s="123"/>
+        <v>552</v>
+      </c>
+      <c r="I29" s="127"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
     </row>

</xml_diff>

<commit_message>
NAV-172 Deploy a new version of the BDG (#90)
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhXSpO0zDnRWDDj+qpWlZoRJZX+ZA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhGx5s0CeZMjj0InGrvmErvoGtmWg=="/>
     </ext>
   </extLst>
 </workbook>
@@ -93,7 +93,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhrb1YODtM0vmOQbqltQvUSazWi6g=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIKUhu8sG/Mj9s1M0mahx+SgkPaA=="/>
     </ext>
   </extLst>
 </comments>
@@ -185,6 +185,30 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="A5">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAS0zQkj8
+Jonathan Pearson    (2021-12-09 14:16:50)
+@jonathan@fjelltopp.org - for deletion.
+_Assigned to Jonathan Berry_</t>
+      </text>
+    </comment>
+  </commentList>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhaiwf6jh+HW7z1kK3cW6DR1x9O7Q=="/>
+    </ext>
+  </extLst>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
     <comment authorId="0" ref="D16">
       <text>
         <t xml:space="preserve">======
@@ -222,7 +246,7 @@
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -256,7 +280,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="649">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="650">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -1179,7 +1203,7 @@
     <t>ROB-06-01</t>
   </si>
   <si>
-    <t>Review time series results for your ART data file</t>
+    <t>Review time series results for your ANC and ART data file</t>
   </si>
   <si>
     <t>Has user reviewed all plot types for their ART and ANC data files and corrected all anomolies?</t>
@@ -1358,7 +1382,9 @@
     <t>Does the user's Spectrum file have current estimates year data for PMTCT [required / optional data elements available in Indicator Element Matrix]?</t>
   </si>
   <si>
-    <t>Spectrum requires up-to-date PMTCT programme data for the reporting period. These data are required for each Spectrum file. You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. Spectrum also provides specific guidance for each regimen in the PMTCT data entry page. *It is highly recommended you finalize your programme data before beginning the Spectrum process.* If edits to PMTCT programme data are required later in the process, you will have to return to this step. For countries with sub-national Spectrum estimates (optional), this step applies to each file.</t>
+    <t>In order to produce updated estimates in Spectrum, updated PMTCT programme data are required. These data are required for each Spectrum file. 
+You can find all required data elements in the Guide 8, Data quality, Indicator Element Matrix. Spectrum also provides specific guidance for each regimen in the PMTCT data entry page. *It is highly recommended you finalize your programme data before proceeding.* 
+If edits to PMTCT programme data are required later in the process, you will have to return to this step. For countries with sub-national Spectrum estimates (optional), this step applies to each file.</t>
   </si>
   <si>
     <r>
@@ -1404,7 +1430,7 @@
     <t>SPE-07-01</t>
   </si>
   <si>
-    <t>Update ANC testing data in Spectrum</t>
+    <t>Update and review ANC testing data in Spectrum</t>
   </si>
   <si>
     <t>Has user updated ANC testing data in their Spectrum file for current reporting period [required / optional data elements available in Indicator Element Matrix]?</t>
@@ -1569,13 +1595,13 @@
     <t>FRRCD4_default,FRRageNoART_default,FRRageART_default</t>
   </si>
   <si>
-    <t>Confirm default values for Fertility Rate Ratios under Advanced Options</t>
-  </si>
-  <si>
-    <t>Has the user confirmed that the default values for Fertility Rate Ratios under Advanced Options are correct?</t>
-  </si>
-  <si>
-    <t>To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. They must be confirmed for CD4, on ART, and off ART. To learn more about the Advanced Options, see the Spectrum training materials.</t>
+    <t>Update Fertility Rate Ratios or confirm default values are used under Advanced Options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has the user updated the Fertility Rate Ratios under Advanced Options? </t>
+  </si>
+  <si>
+    <t>To produce accurate estimates of number of births to women living with HIV, Spectrum requires the correct assumptions about fertility among women living with HIV are selected under Advanced Options. Enter Advanced Options and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. If good quality prevalence from census level ANC data are available, those can be used with the fit local fertility adjustment. The data will be pulled directly from EPP so update your ANC-RT census data in EPP before doing this step.  To learn more about the Advanced Options, see the Spectrum training materials.</t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-SPE-14-01-A')</t>
@@ -1656,6 +1682,7 @@
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <strike/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -1664,15 +1691,16 @@
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <strike/>
         <color theme="1"/>
         <sz val="8.0"/>
-        <u/>
       </rPr>
       <t>not</t>
     </r>
     <r>
       <rPr>
         <rFont val="Calibri"/>
+        <strike/>
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
@@ -1697,7 +1725,8 @@
     <t>Has the user defined and reviewed the epidemic structure in EPP?</t>
   </si>
   <si>
-    <t xml:space="preserve">EPP requires the country to have a defined epidemic structure. You can see the previously used epidemic structure for your country in Spectrum (Modules&gt;AIM&gt;Incidence&gt;Configuration (EPP)). You may have to choose EPP as the preferred option under Incidence &gt; Incidence Options. 
+    <t xml:space="preserve">Congratulations on finishing the first of two Spectrum milestones. Now you will begin the process of estimating HIV incidence using EPP. 
+EPP requires the country to have a defined epidemic structure. You can see the previously used epidemic structure for your country in Spectrum (Modules&gt;AIM&gt;Incidence&gt;Configuration (EPP)). You may have to choose EPP as the preferred option under Incidence &gt; Incidence Options. 
 If all the information is valid, you can choose "Save and continue", which will take you to EPP's "Define Pops" page. If the epidemic structure is not correct, you can set it up according to data availability for your country. Once completed, choose "Save and continue" to proceed to the next step. </t>
   </si>
   <si>
@@ -1805,7 +1834,7 @@
     <t>S90-01-10</t>
   </si>
   <si>
-    <t>Ensure pediatric and adult ART programme data inputs and incidence estimates for people living with HIV (EPP) have not changed since you completed your sex/age incidence patterns in Spectrum</t>
+    <t>Ensure pediatric and adult ART programme data inputs, incidence estimates (EPP) and sex/age patterns have not changed in Spectrum</t>
   </si>
   <si>
     <t>Programme data for pediatric and adult ART as well as incidence results are up to date?</t>
@@ -1987,13 +2016,13 @@
     <t>SPF-01-10</t>
   </si>
   <si>
-    <t>Confirm PMTCT, ANC, pediatric ART, adult ART programme data inputs have not changed since beginning the EPP process</t>
-  </si>
-  <si>
-    <t>No updates have been made to any Spectrum data files or underlying data to be used by Spectrum before using those files in models which project knowledge of status (population, PMTCT, ANC, ART, breastfeeding patterns)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If any underlying programme data have changed since you completed the first portion of Spectrum, you must update the data entry in Spectrum, rerun EPP curve fits, and rerun Shiny 90. </t>
+    <t>Confirm adult ART programme data and ANC and survey prevalence inputs have not changed since beginning the EPP process</t>
+  </si>
+  <si>
+    <t>No updates have been made to any Spectrum data inputs (population, ART programme data, ART, ANC survey and prevalence ) before estimating incidence in EPP?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If ART or surveillance data have changed since you completed the first portion of Spectrum, you must update the data entry in Spectrum, rerun EPP curve fits and update the sex/age patterns. </t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-SPF-01-10-A')</t>
@@ -2419,6 +2448,9 @@
     <t>Spectrum Validation: Confirm default values for Fertility Rate Ratios under Advanced Options</t>
   </si>
   <si>
+    <t>Has the user confirmed that the default values for Fertility Rate Ratios under Advanced Options are correct?</t>
+  </si>
+  <si>
     <t xml:space="preserve">**Navigator has detected that there is a problem with your Spectrum file. **
 To produce accurate estimates, Spectrum requires the correct options are selected under Advanced Options. Enter Advanced Options in Spectrum Web and confirm the default selections for the "HIV-related fertility reductions" are correct for your country. They must be confirmed for CD4, on ART, and off ART. To learn more about the Advanced Options, see the Spectrum training materials.
 Please ensure you correct this in your Spectrum file **and then reupload the file to the ADR** in order to complete this task. </t>
@@ -3078,7 +3110,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3197,6 +3229,12 @@
       <strike/>
       <sz val="8.0"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -3402,7 +3440,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="136">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3682,10 +3720,22 @@
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3707,7 +3757,7 @@
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3718,10 +3768,10 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -3984,7 +4034,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.0"/>
     <col customWidth="1" min="2" max="2" width="62.86"/>
-    <col customWidth="1" min="3" max="3" width="21.86"/>
+    <col customWidth="1" min="3" max="3" width="46.14"/>
     <col customWidth="1" min="4" max="4" width="43.71"/>
     <col customWidth="1" min="5" max="5" width="18.29"/>
     <col customWidth="1" min="6" max="6" width="11.57"/>
@@ -10624,32 +10674,32 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="46">
         <v>0.2</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>555</v>
-      </c>
-      <c r="H2" s="127"/>
-      <c r="I2" s="127"/>
+        <v>556</v>
+      </c>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="128" t="s">
-        <v>556</v>
+      <c r="B4" s="132" t="s">
+        <v>557</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>10</v>
@@ -10681,17 +10731,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>557</v>
-      </c>
-      <c r="B5" s="123"/>
+        <v>558</v>
+      </c>
+      <c r="B5" s="127"/>
       <c r="C5" s="24" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22">
@@ -10699,45 +10749,45 @@
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="24" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>562</v>
-      </c>
-      <c r="B6" s="123" t="s">
         <v>563</v>
       </c>
+      <c r="B6" s="127" t="s">
+        <v>564</v>
+      </c>
       <c r="C6" s="22" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F6" s="22"/>
-      <c r="G6" s="22">
-        <v>1.0</v>
+      <c r="G6" s="24">
+        <v>0.0</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="24" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>569</v>
-      </c>
-      <c r="B7" s="123"/>
+        <v>570</v>
+      </c>
+      <c r="B7" s="127"/>
       <c r="C7" s="22" t="s">
         <v>183</v>
       </c>
@@ -10745,7 +10795,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>186</v>
@@ -10753,42 +10803,42 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="24" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="J7" s="99"/>
       <c r="K7" s="22"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>572</v>
-      </c>
-      <c r="B8" s="123"/>
+        <v>573</v>
+      </c>
+      <c r="B8" s="127"/>
       <c r="C8" s="22" t="s">
         <v>189</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="129" t="s">
-        <v>573</v>
+      <c r="E8" s="133" t="s">
+        <v>574</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="24" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>576</v>
-      </c>
-      <c r="B9" s="123" t="s">
         <v>577</v>
+      </c>
+      <c r="B9" s="127" t="s">
+        <v>578</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>195</v>
@@ -10797,117 +10847,117 @@
         <v>196</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="24" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>580</v>
-      </c>
-      <c r="B10" s="123" t="s">
         <v>581</v>
       </c>
+      <c r="B10" s="127" t="s">
+        <v>582</v>
+      </c>
       <c r="C10" s="22" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>584</v>
-      </c>
-      <c r="F10" s="130" t="s">
         <v>585</v>
+      </c>
+      <c r="F10" s="134" t="s">
+        <v>586</v>
       </c>
       <c r="G10" s="22">
         <v>1.0</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="24" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>587</v>
-      </c>
-      <c r="B11" s="123"/>
+        <v>588</v>
+      </c>
+      <c r="B11" s="127"/>
       <c r="C11" s="22" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="24" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>593</v>
-      </c>
-      <c r="B12" s="123" t="s">
         <v>594</v>
       </c>
+      <c r="B12" s="127" t="s">
+        <v>595</v>
+      </c>
       <c r="C12" s="22" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="E12" s="131" t="s">
         <v>597</v>
       </c>
+      <c r="E12" s="135" t="s">
+        <v>598</v>
+      </c>
       <c r="F12" s="22" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G12" s="22">
         <v>1.0</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="24" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>601</v>
-      </c>
-      <c r="B13" s="123" t="s">
         <v>602</v>
       </c>
+      <c r="B13" s="127" t="s">
+        <v>603</v>
+      </c>
       <c r="C13" s="22" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
@@ -10915,53 +10965,53 @@
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="24" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>607</v>
-      </c>
-      <c r="B14" s="123" t="s">
         <v>608</v>
       </c>
+      <c r="B14" s="127" t="s">
+        <v>609</v>
+      </c>
       <c r="C14" s="22" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>612</v>
-      </c>
-      <c r="G14" s="22">
-        <v>1.0</v>
+        <v>613</v>
+      </c>
+      <c r="G14" s="24">
+        <v>0.0</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="24" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>614</v>
-      </c>
-      <c r="B15" s="123"/>
+        <v>615</v>
+      </c>
+      <c r="B15" s="127"/>
       <c r="C15" s="24" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
@@ -10969,47 +11019,47 @@
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="24" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="J15" s="99"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>619</v>
-      </c>
-      <c r="B16" s="123"/>
+        <v>620</v>
+      </c>
+      <c r="B16" s="127"/>
       <c r="C16" s="22" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="24" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>624</v>
-      </c>
-      <c r="B17" s="123"/>
+        <v>625</v>
+      </c>
+      <c r="B17" s="127"/>
       <c r="C17" s="22" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
@@ -11017,53 +11067,53 @@
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="24" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>629</v>
-      </c>
-      <c r="B18" s="123"/>
+        <v>630</v>
+      </c>
+      <c r="B18" s="127"/>
       <c r="C18" s="22" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="G18" s="22">
         <v>1.0</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="24" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>635</v>
-      </c>
-      <c r="B19" s="123" t="s">
-        <v>563</v>
+        <v>636</v>
+      </c>
+      <c r="B19" s="127" t="s">
+        <v>564</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>257</v>
@@ -11071,65 +11121,65 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="24" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="K19" s="22"/>
     </row>
     <row r="20" ht="49.5" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>640</v>
-      </c>
-      <c r="B20" s="123" t="s">
-        <v>594</v>
+        <v>641</v>
+      </c>
+      <c r="B20" s="127" t="s">
+        <v>595</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="E20" s="131" t="s">
-        <v>642</v>
+        <v>597</v>
+      </c>
+      <c r="E20" s="135" t="s">
+        <v>643</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="24" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="K20" s="22"/>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>645</v>
-      </c>
-      <c r="B21" s="123" t="s">
-        <v>608</v>
+        <v>646</v>
+      </c>
+      <c r="B21" s="127" t="s">
+        <v>609</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="24" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -16569,7 +16619,7 @@
       <c r="A10" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="54" t="s">
         <v>207</v>
       </c>
       <c r="C10" s="50" t="s">
@@ -17913,7 +17963,7 @@
         <v>253</v>
       </c>
       <c r="B11" s="97"/>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="24" t="s">
         <v>254</v>
       </c>
       <c r="D11" s="22" t="s">
@@ -18115,13 +18165,13 @@
       <c r="B19" s="97" t="s">
         <v>302</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="E19" s="96" t="s">
+      <c r="E19" s="94" t="s">
         <v>305</v>
       </c>
       <c r="F19" s="107" t="s">
@@ -19341,24 +19391,24 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="113" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="114" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="113" t="s">
         <v>331</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="114" t="s">
         <v>332</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="24" t="s">
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="116"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="114" t="s">
         <v>333</v>
       </c>
     </row>
@@ -19447,7 +19497,7 @@
       <c r="D9" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E9" s="113" t="s">
+      <c r="E9" s="117" t="s">
         <v>354</v>
       </c>
       <c r="F9" s="22">
@@ -20498,12 +20548,13 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="E9"/>
+    <hyperlink r:id="rId2" ref="E9"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -20563,7 +20614,7 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="J3" s="114"/>
+      <c r="J3" s="118"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="89" t="s">
@@ -20601,7 +20652,7 @@
       <c r="A5" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>366</v>
       </c>
       <c r="C5" s="68" t="s">
@@ -20616,7 +20667,7 @@
       <c r="H5" s="24" t="s">
         <v>369</v>
       </c>
-      <c r="I5" s="115"/>
+      <c r="I5" s="119"/>
       <c r="J5" s="68"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
@@ -20648,24 +20699,24 @@
       <c r="J6" s="22"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="120" t="s">
         <v>377</v>
       </c>
-      <c r="B7" s="116"/>
-      <c r="C7" s="116" t="s">
+      <c r="B7" s="120"/>
+      <c r="C7" s="120" t="s">
         <v>378</v>
       </c>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
       <c r="H7" s="84" t="s">
         <v>379</v>
       </c>
-      <c r="I7" s="117" t="s">
+      <c r="I7" s="121" t="s">
         <v>380</v>
       </c>
-      <c r="J7" s="118"/>
+      <c r="J7" s="122"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
@@ -20689,7 +20740,7 @@
         <v>385</v>
       </c>
       <c r="I8" s="96"/>
-      <c r="J8" s="119"/>
+      <c r="J8" s="123"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
@@ -20711,7 +20762,7 @@
         <v>390</v>
       </c>
       <c r="I9" s="96"/>
-      <c r="J9" s="119"/>
+      <c r="J9" s="123"/>
     </row>
     <row r="10" ht="115.5" customHeight="1">
       <c r="A10" s="22" t="s">
@@ -20737,7 +20788,7 @@
       <c r="I10" s="96" t="s">
         <v>396</v>
       </c>
-      <c r="J10" s="119"/>
+      <c r="J10" s="123"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
@@ -20759,7 +20810,7 @@
         <v>401</v>
       </c>
       <c r="I11" s="96"/>
-      <c r="J11" s="119"/>
+      <c r="J11" s="123"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
@@ -20785,7 +20836,7 @@
       <c r="I12" s="96" t="s">
         <v>407</v>
       </c>
-      <c r="J12" s="119"/>
+      <c r="J12" s="123"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
@@ -20807,7 +20858,7 @@
         <v>412</v>
       </c>
       <c r="I13" s="96"/>
-      <c r="J13" s="119"/>
+      <c r="J13" s="123"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
@@ -20831,7 +20882,7 @@
         <v>417</v>
       </c>
       <c r="I14" s="96"/>
-      <c r="J14" s="119"/>
+      <c r="J14" s="123"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="C15" s="27"/>
@@ -21873,10 +21924,10 @@
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="121"/>
+      <c r="C1" s="125"/>
       <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
@@ -21895,7 +21946,7 @@
       <c r="B2" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="C2" s="121"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="8" t="s">
         <v>421</v>
       </c>
@@ -21935,7 +21986,7 @@
       <c r="H4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="122" t="s">
+      <c r="I4" s="126" t="s">
         <v>215</v>
       </c>
       <c r="J4" s="89" t="s">
@@ -21949,10 +22000,10 @@
       <c r="A5" s="22" t="s">
         <v>423</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="24" t="s">
         <v>425</v>
       </c>
       <c r="D5" s="24" t="s">
@@ -21964,7 +22015,7 @@
       <c r="H5" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="I5" s="123"/>
+      <c r="I5" s="127"/>
       <c r="J5" s="22" t="s">
         <v>428</v>
       </c>
@@ -21989,7 +22040,7 @@
       <c r="H6" s="24" t="s">
         <v>433</v>
       </c>
-      <c r="I6" s="123"/>
+      <c r="I6" s="127"/>
       <c r="J6" s="22" t="s">
         <v>434</v>
       </c>
@@ -22016,14 +22067,14 @@
       <c r="H7" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="I7" s="123" t="s">
+      <c r="I7" s="127" t="s">
         <v>440</v>
       </c>
       <c r="J7" s="22" t="s">
         <v>441</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="L7" s="124" t="s">
+      <c r="L7" s="128" t="s">
         <v>442</v>
       </c>
     </row>
@@ -22048,7 +22099,7 @@
       <c r="H8" s="24" t="s">
         <v>447</v>
       </c>
-      <c r="I8" s="123"/>
+      <c r="I8" s="127"/>
       <c r="J8" s="22" t="s">
         <v>448</v>
       </c>
@@ -22075,7 +22126,7 @@
       <c r="H9" s="24" t="s">
         <v>453</v>
       </c>
-      <c r="I9" s="123"/>
+      <c r="I9" s="127"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
@@ -22100,7 +22151,7 @@
       <c r="H10" s="24" t="s">
         <v>458</v>
       </c>
-      <c r="I10" s="123" t="s">
+      <c r="I10" s="127" t="s">
         <v>459</v>
       </c>
       <c r="J10" s="22"/>
@@ -22125,7 +22176,7 @@
       <c r="H11" s="24" t="s">
         <v>464</v>
       </c>
-      <c r="I11" s="123"/>
+      <c r="I11" s="127"/>
       <c r="J11" s="22" t="s">
         <v>465</v>
       </c>
@@ -22152,7 +22203,7 @@
       <c r="H12" s="24" t="s">
         <v>470</v>
       </c>
-      <c r="I12" s="123" t="s">
+      <c r="I12" s="127" t="s">
         <v>471</v>
       </c>
       <c r="J12" s="22"/>
@@ -22177,7 +22228,7 @@
       <c r="H13" s="24" t="s">
         <v>476</v>
       </c>
-      <c r="I13" s="123"/>
+      <c r="I13" s="127"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
@@ -22200,7 +22251,7 @@
       <c r="H14" s="24" t="s">
         <v>481</v>
       </c>
-      <c r="I14" s="123"/>
+      <c r="I14" s="127"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
@@ -22227,7 +22278,7 @@
       <c r="H15" s="24" t="s">
         <v>487</v>
       </c>
-      <c r="I15" s="123"/>
+      <c r="I15" s="127"/>
       <c r="J15" s="24" t="s">
         <v>488</v>
       </c>
@@ -22280,7 +22331,7 @@
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="125" t="s">
+      <c r="H17" s="129" t="s">
         <v>497</v>
       </c>
       <c r="I17" s="93" t="s">
@@ -22309,7 +22360,7 @@
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="125" t="s">
+      <c r="H18" s="129" t="s">
         <v>502</v>
       </c>
       <c r="I18" s="93" t="s">
@@ -22334,7 +22385,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="125" t="s">
+      <c r="H19" s="129" t="s">
         <v>507</v>
       </c>
       <c r="I19" s="93" t="s">
@@ -22347,7 +22398,7 @@
       <c r="A20" s="24" t="s">
         <v>508</v>
       </c>
-      <c r="B20" s="126" t="s">
+      <c r="B20" s="130" t="s">
         <v>509</v>
       </c>
       <c r="C20" s="103" t="s">
@@ -22361,7 +22412,7 @@
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="125" t="s">
+      <c r="H20" s="129" t="s">
         <v>511</v>
       </c>
       <c r="I20" s="93"/>
@@ -22372,7 +22423,7 @@
       <c r="A21" s="24" t="s">
         <v>512</v>
       </c>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="130" t="s">
         <v>513</v>
       </c>
       <c r="C21" s="103" t="s">
@@ -22386,7 +22437,7 @@
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="125" t="s">
+      <c r="H21" s="129" t="s">
         <v>515</v>
       </c>
       <c r="I21" s="93" t="s">
@@ -22403,18 +22454,18 @@
         <v>517</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>304</v>
+        <v>518</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E22" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="125" t="s">
-        <v>519</v>
+      <c r="H22" s="129" t="s">
+        <v>520</v>
       </c>
       <c r="I22" s="93"/>
       <c r="J22" s="22"/>
@@ -22422,24 +22473,24 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>310</v>
       </c>
       <c r="D23" s="94" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E23" s="107" t="s">
         <v>312</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="125" t="s">
-        <v>523</v>
+      <c r="H23" s="129" t="s">
+        <v>524</v>
       </c>
       <c r="I23" s="93"/>
       <c r="J23" s="22"/>
@@ -22447,24 +22498,24 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>317</v>
       </c>
       <c r="D24" s="94" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="E24" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="125" t="s">
-        <v>527</v>
+      <c r="H24" s="129" t="s">
+        <v>528</v>
       </c>
       <c r="I24" s="93" t="s">
         <v>315</v>
@@ -22474,24 +22525,24 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>437</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="125" t="s">
-        <v>531</v>
-      </c>
-      <c r="I25" s="123" t="s">
+      <c r="H25" s="129" t="s">
+        <v>532</v>
+      </c>
+      <c r="I25" s="127" t="s">
         <v>440</v>
       </c>
       <c r="J25" s="22"/>
@@ -22499,24 +22550,24 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="24" t="s">
-        <v>536</v>
-      </c>
-      <c r="I26" s="123" t="s">
+        <v>537</v>
+      </c>
+      <c r="I26" s="127" t="s">
         <v>459</v>
       </c>
       <c r="J26" s="22"/>
@@ -22524,24 +22575,24 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>468</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="125" t="s">
-        <v>540</v>
-      </c>
-      <c r="I27" s="123" t="s">
+      <c r="H27" s="129" t="s">
+        <v>541</v>
+      </c>
+      <c r="I27" s="127" t="s">
         <v>471</v>
       </c>
       <c r="J27" s="22"/>
@@ -22549,41 +22600,41 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="24" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="24" t="s">
-        <v>545</v>
-      </c>
-      <c r="I28" s="123"/>
+        <v>546</v>
+      </c>
+      <c r="I28" s="127"/>
       <c r="J28" s="22" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="K28" s="22"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22">
@@ -22591,9 +22642,9 @@
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="24" t="s">
-        <v>551</v>
-      </c>
-      <c r="I29" s="123"/>
+        <v>552</v>
+      </c>
+      <c r="I29" s="127"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
     </row>

</xml_diff>

<commit_message>
NAV-172 New BDG version
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhGx5s0CeZMjj0InGrvmErvoGtmWg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mijv/Yi2GmeSQjMjGB0S/7X8CYI/A=="/>
     </ext>
   </extLst>
 </workbook>
@@ -93,7 +93,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIKUhu8sG/Mj9s1M0mahx+SgkPaA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJ0JgbOCBuUu1yDls2+Zyj6eJPHA=="/>
     </ext>
   </extLst>
 </comments>
@@ -185,30 +185,6 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A5">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAS0zQkj8
-Jonathan Pearson    (2021-12-09 14:16:50)
-@jonathan@fjelltopp.org - for deletion.
-_Assigned to Jonathan Berry_</t>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhaiwf6jh+HW7z1kK3cW6DR1x9O7Q=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
     <comment authorId="0" ref="D16">
       <text>
         <t xml:space="preserve">======
@@ -246,7 +222,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -280,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="645">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -1671,49 +1647,6 @@
   </si>
   <si>
     <t>S4 Follow-up</t>
-  </si>
-  <si>
-    <t>EPP-01-10</t>
-  </si>
-  <si>
-    <t>Ensure pediatric and adult ART programme data inputs have not changed since you completed the first Spectrum milestone</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <strike/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve">Programme data for pediatric ART and adult ART have </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <strike/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t>not</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <strike/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve"> changed since the first Spectrum milestone was completed?</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Congratulations on finishing the first of two Spectrum milestones. Now you will begin the process of estimating HIV incidence using EPP. 
-Before you begin, you should be sure that Spectrum has your best, most up-to-date ART data. 
-*If any underlying ART programme data have changed in your source files since you completed the first portion of Spectrum, you must return to the task in Spectrum where you enter your adult and pediatric ART data and then return to EPP.* </t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-EPP-01-10-A')</t>
   </si>
   <si>
     <t>EPP-02-01</t>
@@ -3110,7 +3043,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3229,12 +3162,6 @@
       <strike/>
       <sz val="8.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -3440,7 +3367,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="132">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3720,22 +3647,10 @@
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3757,7 +3672,7 @@
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3768,10 +3683,10 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -10669,37 +10584,37 @@
         <v>3</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="46">
         <v>0.2</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>556</v>
-      </c>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
+        <v>551</v>
+      </c>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="132" t="s">
-        <v>557</v>
+      <c r="B4" s="128" t="s">
+        <v>552</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>10</v>
@@ -10731,17 +10646,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>558</v>
-      </c>
-      <c r="B5" s="127"/>
+        <v>553</v>
+      </c>
+      <c r="B5" s="123"/>
       <c r="C5" s="24" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22">
@@ -10749,26 +10664,26 @@
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="24" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="B6" s="127" t="s">
-        <v>564</v>
+        <v>558</v>
+      </c>
+      <c r="B6" s="123" t="s">
+        <v>559</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="24">
@@ -10776,18 +10691,18 @@
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="24" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="B7" s="127"/>
+        <v>565</v>
+      </c>
+      <c r="B7" s="123"/>
       <c r="C7" s="22" t="s">
         <v>183</v>
       </c>
@@ -10795,7 +10710,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>186</v>
@@ -10803,42 +10718,42 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="24" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="J7" s="99"/>
       <c r="K7" s="22"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="B8" s="127"/>
+        <v>568</v>
+      </c>
+      <c r="B8" s="123"/>
       <c r="C8" s="22" t="s">
         <v>189</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="133" t="s">
-        <v>574</v>
+      <c r="E8" s="129" t="s">
+        <v>569</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="24" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>577</v>
-      </c>
-      <c r="B9" s="127" t="s">
-        <v>578</v>
+        <v>572</v>
+      </c>
+      <c r="B9" s="123" t="s">
+        <v>573</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>195</v>
@@ -10847,117 +10762,117 @@
         <v>196</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="24" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="B10" s="123" t="s">
+        <v>577</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="F10" s="130" t="s">
         <v>581</v>
-      </c>
-      <c r="B10" s="127" t="s">
-        <v>582</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>583</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>585</v>
-      </c>
-      <c r="F10" s="134" t="s">
-        <v>586</v>
       </c>
       <c r="G10" s="22">
         <v>1.0</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="24" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="B11" s="127"/>
+        <v>583</v>
+      </c>
+      <c r="B11" s="123"/>
       <c r="C11" s="22" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="24" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="B12" s="123" t="s">
+        <v>590</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>592</v>
+      </c>
+      <c r="E12" s="131" t="s">
+        <v>593</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>594</v>
-      </c>
-      <c r="B12" s="127" t="s">
-        <v>595</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="E12" s="135" t="s">
-        <v>598</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>599</v>
       </c>
       <c r="G12" s="22">
         <v>1.0</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="24" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="B13" s="127" t="s">
-        <v>603</v>
+        <v>597</v>
+      </c>
+      <c r="B13" s="123" t="s">
+        <v>598</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
@@ -10965,53 +10880,53 @@
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="24" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="B14" s="123" t="s">
+        <v>604</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="F14" s="22" t="s">
         <v>608</v>
-      </c>
-      <c r="B14" s="127" t="s">
-        <v>609</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>610</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>611</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>612</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>613</v>
       </c>
       <c r="G14" s="24">
         <v>0.0</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="24" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>615</v>
-      </c>
-      <c r="B15" s="127"/>
+        <v>610</v>
+      </c>
+      <c r="B15" s="123"/>
       <c r="C15" s="24" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
@@ -11019,47 +10934,47 @@
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="24" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="J15" s="99"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="B16" s="127"/>
+        <v>615</v>
+      </c>
+      <c r="B16" s="123"/>
       <c r="C16" s="22" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="24" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>625</v>
-      </c>
-      <c r="B17" s="127"/>
+        <v>620</v>
+      </c>
+      <c r="B17" s="123"/>
       <c r="C17" s="22" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
@@ -11067,53 +10982,53 @@
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="24" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="B18" s="127"/>
+        <v>625</v>
+      </c>
+      <c r="B18" s="123"/>
       <c r="C18" s="22" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="G18" s="22">
         <v>1.0</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="24" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>636</v>
-      </c>
-      <c r="B19" s="127" t="s">
-        <v>564</v>
+        <v>631</v>
+      </c>
+      <c r="B19" s="123" t="s">
+        <v>559</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>257</v>
@@ -11121,65 +11036,65 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="24" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="K19" s="22"/>
     </row>
     <row r="20" ht="49.5" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>641</v>
-      </c>
-      <c r="B20" s="127" t="s">
-        <v>595</v>
+        <v>636</v>
+      </c>
+      <c r="B20" s="123" t="s">
+        <v>590</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="E20" s="135" t="s">
-        <v>643</v>
+        <v>592</v>
+      </c>
+      <c r="E20" s="131" t="s">
+        <v>638</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="24" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="K20" s="22"/>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>646</v>
-      </c>
-      <c r="B21" s="127" t="s">
-        <v>609</v>
+        <v>641</v>
+      </c>
+      <c r="B21" s="123" t="s">
+        <v>604</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="24" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -19391,44 +19306,46 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="22" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="114" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="96" t="s">
         <v>333</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="24" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="D6" s="24" t="s">
         <v>337</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>338</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="96" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
@@ -19450,10 +19367,10 @@
         <v>343</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="96" t="s">
-        <v>338</v>
-      </c>
+      <c r="F7" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="96"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="24" t="s">
@@ -19473,85 +19390,62 @@
       <c r="D8" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="113" t="s">
+        <v>349</v>
+      </c>
       <c r="F8" s="22">
         <v>1.0</v>
       </c>
-      <c r="G8" s="96"/>
+      <c r="G8" s="96" t="s">
+        <v>350</v>
+      </c>
       <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="I8" s="21"/>
       <c r="J8" s="24" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="E9" s="117" t="s">
         <v>354</v>
       </c>
+      <c r="D9" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="E9" s="22"/>
       <c r="F9" s="22">
         <v>1.0</v>
       </c>
-      <c r="G9" s="96" t="s">
-        <v>355</v>
-      </c>
+      <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="24" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>360</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="24" t="s">
-        <v>361</v>
-      </c>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="77"/>
-      <c r="R10" s="77"/>
-      <c r="S10" s="77"/>
-      <c r="T10" s="77"/>
-      <c r="U10" s="77"/>
-      <c r="V10" s="77"/>
-      <c r="W10" s="77"/>
-      <c r="X10" s="77"/>
-      <c r="Y10" s="77"/>
-      <c r="Z10" s="77"/>
-    </row>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77"/>
+      <c r="S9" s="77"/>
+      <c r="T9" s="77"/>
+      <c r="U9" s="77"/>
+      <c r="V9" s="77"/>
+      <c r="W9" s="77"/>
+      <c r="X9" s="77"/>
+      <c r="Y9" s="77"/>
+      <c r="Z9" s="77"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -19760,7 +19654,7 @@
     <row r="216" ht="14.25" customHeight="1"/>
     <row r="217" ht="14.25" customHeight="1"/>
     <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
@@ -20540,7 +20434,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -20548,13 +20441,12 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="E9"/>
+    <hyperlink r:id="rId1" ref="E8"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20599,14 +20491,14 @@
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -20614,7 +20506,7 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="J3" s="118"/>
+      <c r="J3" s="114"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="89" t="s">
@@ -20650,86 +20542,86 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C5" s="68" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D5" s="68" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E5" s="99"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="I5" s="119"/>
+        <v>364</v>
+      </c>
+      <c r="I5" s="115"/>
       <c r="J5" s="68"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F6" s="22">
         <v>1.0</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="I6" s="94" t="s">
+        <v>371</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="116" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="84" t="s">
+        <v>374</v>
+      </c>
+      <c r="I7" s="117" t="s">
         <v>375</v>
       </c>
-      <c r="I6" s="94" t="s">
-        <v>376</v>
-      </c>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="120" t="s">
-        <v>377</v>
-      </c>
-      <c r="B7" s="120"/>
-      <c r="C7" s="120" t="s">
-        <v>378</v>
-      </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="84" t="s">
-        <v>379</v>
-      </c>
-      <c r="I7" s="121" t="s">
-        <v>380</v>
-      </c>
-      <c r="J7" s="122"/>
+      <c r="J7" s="118"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22">
@@ -20737,45 +20629,45 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="24" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="I8" s="96"/>
-      <c r="J8" s="123"/>
+      <c r="J8" s="119"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="24" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="I9" s="96"/>
-      <c r="J9" s="123"/>
+      <c r="J9" s="119"/>
     </row>
     <row r="10" ht="115.5" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22">
@@ -20783,47 +20675,47 @@
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="24" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I10" s="96" t="s">
-        <v>396</v>
-      </c>
-      <c r="J10" s="123"/>
+        <v>391</v>
+      </c>
+      <c r="J10" s="119"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="I11" s="96"/>
-      <c r="J11" s="123"/>
+      <c r="J11" s="119"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22">
@@ -20831,47 +20723,47 @@
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="I12" s="96" t="s">
-        <v>407</v>
-      </c>
-      <c r="J12" s="123"/>
+        <v>402</v>
+      </c>
+      <c r="J12" s="119"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="24" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I13" s="96"/>
-      <c r="J13" s="123"/>
+      <c r="J13" s="119"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22">
@@ -20879,10 +20771,10 @@
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="24" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I14" s="96"/>
-      <c r="J14" s="123"/>
+      <c r="J14" s="119"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="C15" s="27"/>
@@ -21924,10 +21816,10 @@
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="125"/>
+      <c r="C1" s="121"/>
       <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
@@ -21935,26 +21827,26 @@
         <v>3</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="I1" s="44"/>
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="C2" s="125"/>
+        <v>415</v>
+      </c>
+      <c r="C2" s="121"/>
       <c r="D2" s="8" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E2" s="47">
         <v>0.2</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I2" s="44"/>
     </row>
@@ -21986,7 +21878,7 @@
       <c r="H4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="126" t="s">
+      <c r="I4" s="122" t="s">
         <v>215</v>
       </c>
       <c r="J4" s="89" t="s">
@@ -21998,66 +21890,66 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="24" t="s">
-        <v>427</v>
-      </c>
-      <c r="I5" s="127"/>
+        <v>422</v>
+      </c>
+      <c r="I5" s="123"/>
       <c r="J5" s="22" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="24" t="s">
-        <v>433</v>
-      </c>
-      <c r="I6" s="127"/>
+        <v>428</v>
+      </c>
+      <c r="I6" s="123"/>
       <c r="J6" s="22" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22">
@@ -22065,31 +21957,31 @@
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="24" t="s">
-        <v>439</v>
-      </c>
-      <c r="I7" s="127" t="s">
-        <v>440</v>
+        <v>434</v>
+      </c>
+      <c r="I7" s="123" t="s">
+        <v>435</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="L7" s="128" t="s">
-        <v>442</v>
+      <c r="L7" s="124" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22">
@@ -22097,26 +21989,26 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="24" t="s">
-        <v>447</v>
-      </c>
-      <c r="I8" s="127"/>
+        <v>442</v>
+      </c>
+      <c r="I8" s="123"/>
       <c r="J8" s="22" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="199.5" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22">
@@ -22124,24 +22016,24 @@
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="24" t="s">
-        <v>453</v>
-      </c>
-      <c r="I9" s="127"/>
+        <v>448</v>
+      </c>
+      <c r="I9" s="123"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E10" s="99"/>
       <c r="F10" s="22">
@@ -22149,51 +22041,51 @@
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="24" t="s">
-        <v>458</v>
-      </c>
-      <c r="I10" s="127" t="s">
-        <v>459</v>
+        <v>453</v>
+      </c>
+      <c r="I10" s="123" t="s">
+        <v>454</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="24" t="s">
-        <v>464</v>
-      </c>
-      <c r="I11" s="127"/>
+        <v>459</v>
+      </c>
+      <c r="I11" s="123"/>
       <c r="J11" s="22" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22">
@@ -22201,167 +22093,167 @@
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="24" t="s">
-        <v>470</v>
-      </c>
-      <c r="I12" s="127" t="s">
-        <v>471</v>
+        <v>465</v>
+      </c>
+      <c r="I12" s="123" t="s">
+        <v>466</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="24" t="s">
-        <v>476</v>
-      </c>
-      <c r="I13" s="127"/>
+        <v>471</v>
+      </c>
+      <c r="I13" s="123"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="24" t="s">
-        <v>481</v>
-      </c>
-      <c r="I14" s="127"/>
+        <v>476</v>
+      </c>
+      <c r="I14" s="123"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E15" s="95" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="F15" s="22">
         <v>1.0</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="24" t="s">
-        <v>487</v>
-      </c>
-      <c r="I15" s="127"/>
+        <v>482</v>
+      </c>
+      <c r="I15" s="123"/>
       <c r="J15" s="24" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>243</v>
       </c>
       <c r="D16" s="94" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="E16" s="95" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="24" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="I16" s="93" t="s">
         <v>241</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="24" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="24" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>262</v>
       </c>
       <c r="D17" s="94" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>257</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="129" t="s">
-        <v>497</v>
+      <c r="H17" s="125" t="s">
+        <v>492</v>
       </c>
       <c r="I17" s="93" t="s">
         <v>260</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="24" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>274</v>
       </c>
       <c r="D18" s="94" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>257</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="129" t="s">
-        <v>502</v>
+      <c r="H18" s="125" t="s">
+        <v>497</v>
       </c>
       <c r="I18" s="93" t="s">
         <v>272</v>
@@ -22371,22 +22263,22 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D19" s="94" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="129" t="s">
-        <v>507</v>
+      <c r="H19" s="125" t="s">
+        <v>502</v>
       </c>
       <c r="I19" s="93" t="s">
         <v>278</v>
@@ -22396,24 +22288,24 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="B20" s="130" t="s">
-        <v>509</v>
+        <v>503</v>
+      </c>
+      <c r="B20" s="126" t="s">
+        <v>504</v>
       </c>
       <c r="C20" s="103" t="s">
         <v>291</v>
       </c>
       <c r="D20" s="104" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E20" s="105" t="s">
         <v>293</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="129" t="s">
-        <v>511</v>
+      <c r="H20" s="125" t="s">
+        <v>506</v>
       </c>
       <c r="I20" s="93"/>
       <c r="J20" s="22"/>
@@ -22421,24 +22313,24 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>512</v>
-      </c>
-      <c r="B21" s="130" t="s">
-        <v>513</v>
+        <v>507</v>
+      </c>
+      <c r="B21" s="126" t="s">
+        <v>508</v>
       </c>
       <c r="C21" s="103" t="s">
         <v>298</v>
       </c>
       <c r="D21" s="104" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E21" s="105" t="s">
         <v>293</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="129" t="s">
-        <v>515</v>
+      <c r="H21" s="125" t="s">
+        <v>510</v>
       </c>
       <c r="I21" s="93" t="s">
         <v>296</v>
@@ -22448,24 +22340,24 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="24" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="E22" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="129" t="s">
-        <v>520</v>
+      <c r="H22" s="125" t="s">
+        <v>515</v>
       </c>
       <c r="I22" s="93"/>
       <c r="J22" s="22"/>
@@ -22473,24 +22365,24 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>310</v>
       </c>
       <c r="D23" s="94" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="E23" s="107" t="s">
         <v>312</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="129" t="s">
-        <v>524</v>
+      <c r="H23" s="125" t="s">
+        <v>519</v>
       </c>
       <c r="I23" s="93"/>
       <c r="J23" s="22"/>
@@ -22498,24 +22390,24 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>317</v>
       </c>
       <c r="D24" s="94" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="E24" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="129" t="s">
-        <v>528</v>
+      <c r="H24" s="125" t="s">
+        <v>523</v>
       </c>
       <c r="I24" s="93" t="s">
         <v>315</v>
@@ -22525,116 +22417,116 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="129" t="s">
-        <v>532</v>
-      </c>
-      <c r="I25" s="127" t="s">
-        <v>440</v>
+      <c r="H25" s="125" t="s">
+        <v>527</v>
+      </c>
+      <c r="I25" s="123" t="s">
+        <v>435</v>
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="24" t="s">
-        <v>537</v>
-      </c>
-      <c r="I26" s="127" t="s">
-        <v>459</v>
+        <v>532</v>
+      </c>
+      <c r="I26" s="123" t="s">
+        <v>454</v>
       </c>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="129" t="s">
-        <v>541</v>
-      </c>
-      <c r="I27" s="127" t="s">
-        <v>471</v>
+      <c r="H27" s="125" t="s">
+        <v>536</v>
+      </c>
+      <c r="I27" s="123" t="s">
+        <v>466</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="24" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="24" t="s">
-        <v>546</v>
-      </c>
-      <c r="I28" s="127"/>
+        <v>541</v>
+      </c>
+      <c r="I28" s="123"/>
       <c r="J28" s="22" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="K28" s="22"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22">
@@ -22642,9 +22534,9 @@
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="24" t="s">
-        <v>552</v>
-      </c>
-      <c r="I29" s="127"/>
+        <v>547</v>
+      </c>
+      <c r="I29" s="123"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
     </row>

</xml_diff>

<commit_message>
NAV-172 New BDG version (#92)
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mhGx5s0CeZMjj0InGrvmErvoGtmWg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mijv/Yi2GmeSQjMjGB0S/7X8CYI/A=="/>
     </ext>
   </extLst>
 </workbook>
@@ -93,7 +93,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miIKUhu8sG/Mj9s1M0mahx+SgkPaA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJ0JgbOCBuUu1yDls2+Zyj6eJPHA=="/>
     </ext>
   </extLst>
 </comments>
@@ -185,30 +185,6 @@
     <author/>
   </authors>
   <commentList>
-    <comment authorId="0" ref="A5">
-      <text>
-        <t xml:space="preserve">======
-ID#AAAAS0zQkj8
-Jonathan Pearson    (2021-12-09 14:16:50)
-@jonathan@fjelltopp.org - for deletion.
-_Assigned to Jonathan Berry_</t>
-      </text>
-    </comment>
-  </commentList>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhaiwf6jh+HW7z1kK3cW6DR1x9O7Q=="/>
-    </ext>
-  </extLst>
-</comments>
-</file>
-
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
     <comment authorId="0" ref="D16">
       <text>
         <t xml:space="preserve">======
@@ -246,7 +222,7 @@
 </comments>
 </file>
 
-<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
@@ -280,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="645">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -1671,49 +1647,6 @@
   </si>
   <si>
     <t>S4 Follow-up</t>
-  </si>
-  <si>
-    <t>EPP-01-10</t>
-  </si>
-  <si>
-    <t>Ensure pediatric and adult ART programme data inputs have not changed since you completed the first Spectrum milestone</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <strike/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve">Programme data for pediatric ART and adult ART have </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <strike/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t>not</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <strike/>
-        <color theme="1"/>
-        <sz val="8.0"/>
-      </rPr>
-      <t xml:space="preserve"> changed since the first Spectrum milestone was completed?</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Congratulations on finishing the first of two Spectrum milestones. Now you will begin the process of estimating HIV incidence using EPP. 
-Before you begin, you should be sure that Spectrum has your best, most up-to-date ART data. 
-*If any underlying ART programme data have changed in your source files since you completed the first portion of Spectrum, you must return to the task in Spectrum where you enter your adult and pediatric ART data and then return to EPP.* </t>
-  </si>
-  <si>
-    <t>check_manual_confirmation('EST-EPP-01-10-A')</t>
   </si>
   <si>
     <t>EPP-02-01</t>
@@ -3110,7 +3043,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="29">
+  <fonts count="28">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -3229,12 +3162,6 @@
       <strike/>
       <sz val="8.0"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -3440,7 +3367,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="132">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3720,22 +3647,10 @@
     <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="24" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3757,7 +3672,7 @@
     <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="26" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="25" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
@@ -3768,10 +3683,10 @@
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="8" fontId="20" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="26" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -10669,37 +10584,37 @@
         <v>3</v>
       </c>
       <c r="G1" s="29" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="46">
         <v>0.2</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>556</v>
-      </c>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
+        <v>551</v>
+      </c>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
     </row>
     <row r="3" ht="12.0" customHeight="1"/>
     <row r="4" ht="12.0" customHeight="1">
       <c r="A4" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="132" t="s">
-        <v>557</v>
+      <c r="B4" s="128" t="s">
+        <v>552</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>10</v>
@@ -10731,17 +10646,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>558</v>
-      </c>
-      <c r="B5" s="127"/>
+        <v>553</v>
+      </c>
+      <c r="B5" s="123"/>
       <c r="C5" s="24" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22">
@@ -10749,26 +10664,26 @@
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="24" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>563</v>
-      </c>
-      <c r="B6" s="127" t="s">
-        <v>564</v>
+        <v>558</v>
+      </c>
+      <c r="B6" s="123" t="s">
+        <v>559</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="24">
@@ -10776,18 +10691,18 @@
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="24" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>570</v>
-      </c>
-      <c r="B7" s="127"/>
+        <v>565</v>
+      </c>
+      <c r="B7" s="123"/>
       <c r="C7" s="22" t="s">
         <v>183</v>
       </c>
@@ -10795,7 +10710,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>186</v>
@@ -10803,42 +10718,42 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="24" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="J7" s="99"/>
       <c r="K7" s="22"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>573</v>
-      </c>
-      <c r="B8" s="127"/>
+        <v>568</v>
+      </c>
+      <c r="B8" s="123"/>
       <c r="C8" s="22" t="s">
         <v>189</v>
       </c>
       <c r="D8" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="E8" s="133" t="s">
-        <v>574</v>
+      <c r="E8" s="129" t="s">
+        <v>569</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="24" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>577</v>
-      </c>
-      <c r="B9" s="127" t="s">
-        <v>578</v>
+        <v>572</v>
+      </c>
+      <c r="B9" s="123" t="s">
+        <v>573</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>195</v>
@@ -10847,117 +10762,117 @@
         <v>196</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="24" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="22" t="s">
+        <v>576</v>
+      </c>
+      <c r="B10" s="123" t="s">
+        <v>577</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>578</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>579</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>580</v>
+      </c>
+      <c r="F10" s="130" t="s">
         <v>581</v>
-      </c>
-      <c r="B10" s="127" t="s">
-        <v>582</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>583</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>584</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>585</v>
-      </c>
-      <c r="F10" s="134" t="s">
-        <v>586</v>
       </c>
       <c r="G10" s="22">
         <v>1.0</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="24" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>588</v>
-      </c>
-      <c r="B11" s="127"/>
+        <v>583</v>
+      </c>
+      <c r="B11" s="123"/>
       <c r="C11" s="22" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="24" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="22" t="s">
+        <v>589</v>
+      </c>
+      <c r="B12" s="123" t="s">
+        <v>590</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>592</v>
+      </c>
+      <c r="E12" s="131" t="s">
+        <v>593</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>594</v>
-      </c>
-      <c r="B12" s="127" t="s">
-        <v>595</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>596</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="E12" s="135" t="s">
-        <v>598</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>599</v>
       </c>
       <c r="G12" s="22">
         <v>1.0</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="24" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>602</v>
-      </c>
-      <c r="B13" s="127" t="s">
-        <v>603</v>
+        <v>597</v>
+      </c>
+      <c r="B13" s="123" t="s">
+        <v>598</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
@@ -10965,53 +10880,53 @@
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="24" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="22" t="s">
+        <v>603</v>
+      </c>
+      <c r="B14" s="123" t="s">
+        <v>604</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>605</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>606</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="F14" s="22" t="s">
         <v>608</v>
-      </c>
-      <c r="B14" s="127" t="s">
-        <v>609</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>610</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>611</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>612</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>613</v>
       </c>
       <c r="G14" s="24">
         <v>0.0</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="24" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>615</v>
-      </c>
-      <c r="B15" s="127"/>
+        <v>610</v>
+      </c>
+      <c r="B15" s="123"/>
       <c r="C15" s="24" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
@@ -11019,47 +10934,47 @@
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="24" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="J15" s="99"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>620</v>
-      </c>
-      <c r="B16" s="127"/>
+        <v>615</v>
+      </c>
+      <c r="B16" s="123"/>
       <c r="C16" s="22" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="24" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>625</v>
-      </c>
-      <c r="B17" s="127"/>
+        <v>620</v>
+      </c>
+      <c r="B17" s="123"/>
       <c r="C17" s="22" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
@@ -11067,53 +10982,53 @@
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="24" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="B18" s="127"/>
+        <v>625</v>
+      </c>
+      <c r="B18" s="123"/>
       <c r="C18" s="22" t="s">
-        <v>631</v>
+        <v>626</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="G18" s="22">
         <v>1.0</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="24" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>636</v>
-      </c>
-      <c r="B19" s="127" t="s">
-        <v>564</v>
+        <v>631</v>
+      </c>
+      <c r="B19" s="123" t="s">
+        <v>559</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>257</v>
@@ -11121,65 +11036,65 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="24" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="K19" s="22"/>
     </row>
     <row r="20" ht="49.5" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>641</v>
-      </c>
-      <c r="B20" s="127" t="s">
-        <v>595</v>
+        <v>636</v>
+      </c>
+      <c r="B20" s="123" t="s">
+        <v>590</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>597</v>
-      </c>
-      <c r="E20" s="135" t="s">
-        <v>643</v>
+        <v>592</v>
+      </c>
+      <c r="E20" s="131" t="s">
+        <v>638</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="24" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="K20" s="22"/>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>646</v>
-      </c>
-      <c r="B21" s="127" t="s">
-        <v>609</v>
+        <v>641</v>
+      </c>
+      <c r="B21" s="123" t="s">
+        <v>604</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="24" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -19391,44 +19306,46 @@
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="22" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="114" t="s">
+      <c r="B5" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="113" t="s">
+      <c r="C5" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="D5" s="114" t="s">
+      <c r="D5" s="24" t="s">
         <v>332</v>
       </c>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="115"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="113"/>
-      <c r="J5" s="114" t="s">
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="96" t="s">
         <v>333</v>
+      </c>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="24" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="D6" s="24" t="s">
         <v>337</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>338</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="96" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
@@ -19450,10 +19367,10 @@
         <v>343</v>
       </c>
       <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="96" t="s">
-        <v>338</v>
-      </c>
+      <c r="F7" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="96"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="J7" s="24" t="s">
@@ -19473,85 +19390,62 @@
       <c r="D8" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="E8" s="22"/>
+      <c r="E8" s="113" t="s">
+        <v>349</v>
+      </c>
       <c r="F8" s="22">
         <v>1.0</v>
       </c>
-      <c r="G8" s="96"/>
+      <c r="G8" s="96" t="s">
+        <v>350</v>
+      </c>
       <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="I8" s="21"/>
       <c r="J8" s="24" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="E9" s="117" t="s">
         <v>354</v>
       </c>
+      <c r="D9" s="24" t="s">
+        <v>355</v>
+      </c>
+      <c r="E9" s="22"/>
       <c r="F9" s="22">
         <v>1.0</v>
       </c>
-      <c r="G9" s="96" t="s">
-        <v>355</v>
-      </c>
+      <c r="G9" s="22"/>
       <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
+      <c r="I9" s="22"/>
       <c r="J9" s="24" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>360</v>
-      </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="24" t="s">
-        <v>361</v>
-      </c>
-      <c r="K10" s="77"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="77"/>
-      <c r="P10" s="77"/>
-      <c r="Q10" s="77"/>
-      <c r="R10" s="77"/>
-      <c r="S10" s="77"/>
-      <c r="T10" s="77"/>
-      <c r="U10" s="77"/>
-      <c r="V10" s="77"/>
-      <c r="W10" s="77"/>
-      <c r="X10" s="77"/>
-      <c r="Y10" s="77"/>
-      <c r="Z10" s="77"/>
-    </row>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+      <c r="N9" s="77"/>
+      <c r="O9" s="77"/>
+      <c r="P9" s="77"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="77"/>
+      <c r="S9" s="77"/>
+      <c r="T9" s="77"/>
+      <c r="U9" s="77"/>
+      <c r="V9" s="77"/>
+      <c r="W9" s="77"/>
+      <c r="X9" s="77"/>
+      <c r="Y9" s="77"/>
+      <c r="Z9" s="77"/>
+    </row>
+    <row r="10" ht="14.25" customHeight="1"/>
     <row r="11" ht="14.25" customHeight="1"/>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
@@ -19760,7 +19654,7 @@
     <row r="216" ht="14.25" customHeight="1"/>
     <row r="217" ht="14.25" customHeight="1"/>
     <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
     <row r="220" ht="15.75" customHeight="1"/>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
@@ -20540,7 +20434,6 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
-    <row r="999" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
@@ -20548,13 +20441,12 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId2" ref="E9"/>
+    <hyperlink r:id="rId1" ref="E8"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20599,14 +20491,14 @@
     </row>
     <row r="2" ht="82.5" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="47">
@@ -20614,7 +20506,7 @@
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="J3" s="118"/>
+      <c r="J3" s="114"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="89" t="s">
@@ -20650,86 +20542,86 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C5" s="68" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D5" s="68" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="E5" s="99"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="24" t="s">
-        <v>369</v>
-      </c>
-      <c r="I5" s="119"/>
+        <v>364</v>
+      </c>
+      <c r="I5" s="115"/>
       <c r="J5" s="68"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="E6" s="22" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="F6" s="22">
         <v>1.0</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="I6" s="94" t="s">
+        <v>371</v>
+      </c>
+      <c r="J6" s="22"/>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="116" t="s">
+        <v>372</v>
+      </c>
+      <c r="B7" s="116"/>
+      <c r="C7" s="116" t="s">
+        <v>373</v>
+      </c>
+      <c r="D7" s="116"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="84" t="s">
+        <v>374</v>
+      </c>
+      <c r="I7" s="117" t="s">
         <v>375</v>
       </c>
-      <c r="I6" s="94" t="s">
-        <v>376</v>
-      </c>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="120" t="s">
-        <v>377</v>
-      </c>
-      <c r="B7" s="120"/>
-      <c r="C7" s="120" t="s">
-        <v>378</v>
-      </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="84" t="s">
-        <v>379</v>
-      </c>
-      <c r="I7" s="121" t="s">
-        <v>380</v>
-      </c>
-      <c r="J7" s="122"/>
+      <c r="J7" s="118"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22">
@@ -20737,45 +20629,45 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="24" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="I8" s="96"/>
-      <c r="J8" s="123"/>
+      <c r="J8" s="119"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="24" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="I9" s="96"/>
-      <c r="J9" s="123"/>
+      <c r="J9" s="119"/>
     </row>
     <row r="10" ht="115.5" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22">
@@ -20783,47 +20675,47 @@
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="24" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I10" s="96" t="s">
-        <v>396</v>
-      </c>
-      <c r="J10" s="123"/>
+        <v>391</v>
+      </c>
+      <c r="J10" s="119"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="24" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="I11" s="96"/>
-      <c r="J11" s="123"/>
+      <c r="J11" s="119"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22">
@@ -20831,47 +20723,47 @@
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="24" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="I12" s="96" t="s">
-        <v>407</v>
-      </c>
-      <c r="J12" s="123"/>
+        <v>402</v>
+      </c>
+      <c r="J12" s="119"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="24" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="I13" s="96"/>
-      <c r="J13" s="123"/>
+      <c r="J13" s="119"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22">
@@ -20879,10 +20771,10 @@
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="24" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I14" s="96"/>
-      <c r="J14" s="123"/>
+      <c r="J14" s="119"/>
     </row>
     <row r="15" ht="14.25" customHeight="1">
       <c r="C15" s="27"/>
@@ -21924,10 +21816,10 @@
       <c r="A1" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="125"/>
+      <c r="C1" s="121"/>
       <c r="D1" s="28" t="s">
         <v>2</v>
       </c>
@@ -21935,26 +21827,26 @@
         <v>3</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="I1" s="44"/>
     </row>
     <row r="2" ht="75.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>420</v>
-      </c>
-      <c r="C2" s="125"/>
+        <v>415</v>
+      </c>
+      <c r="C2" s="121"/>
       <c r="D2" s="8" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E2" s="47">
         <v>0.2</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="I2" s="44"/>
     </row>
@@ -21986,7 +21878,7 @@
       <c r="H4" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="126" t="s">
+      <c r="I4" s="122" t="s">
         <v>215</v>
       </c>
       <c r="J4" s="89" t="s">
@@ -21998,66 +21890,66 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="24" t="s">
-        <v>427</v>
-      </c>
-      <c r="I5" s="127"/>
+        <v>422</v>
+      </c>
+      <c r="I5" s="123"/>
       <c r="J5" s="22" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="24" t="s">
-        <v>433</v>
-      </c>
-      <c r="I6" s="127"/>
+        <v>428</v>
+      </c>
+      <c r="I6" s="123"/>
       <c r="J6" s="22" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22">
@@ -22065,31 +21957,31 @@
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="24" t="s">
-        <v>439</v>
-      </c>
-      <c r="I7" s="127" t="s">
-        <v>440</v>
+        <v>434</v>
+      </c>
+      <c r="I7" s="123" t="s">
+        <v>435</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="K7" s="22"/>
-      <c r="L7" s="128" t="s">
-        <v>442</v>
+      <c r="L7" s="124" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22">
@@ -22097,26 +21989,26 @@
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="24" t="s">
-        <v>447</v>
-      </c>
-      <c r="I8" s="127"/>
+        <v>442</v>
+      </c>
+      <c r="I8" s="123"/>
       <c r="J8" s="22" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="199.5" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22">
@@ -22124,24 +22016,24 @@
       </c>
       <c r="G9" s="22"/>
       <c r="H9" s="24" t="s">
-        <v>453</v>
-      </c>
-      <c r="I9" s="127"/>
+        <v>448</v>
+      </c>
+      <c r="I9" s="123"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="E10" s="99"/>
       <c r="F10" s="22">
@@ -22149,51 +22041,51 @@
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="24" t="s">
-        <v>458</v>
-      </c>
-      <c r="I10" s="127" t="s">
-        <v>459</v>
+        <v>453</v>
+      </c>
+      <c r="I10" s="123" t="s">
+        <v>454</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
       <c r="H11" s="24" t="s">
-        <v>464</v>
-      </c>
-      <c r="I11" s="127"/>
+        <v>459</v>
+      </c>
+      <c r="I11" s="123"/>
       <c r="J11" s="22" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22">
@@ -22201,167 +22093,167 @@
       </c>
       <c r="G12" s="22"/>
       <c r="H12" s="24" t="s">
-        <v>470</v>
-      </c>
-      <c r="I12" s="127" t="s">
-        <v>471</v>
+        <v>465</v>
+      </c>
+      <c r="I12" s="123" t="s">
+        <v>466</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
       <c r="H13" s="24" t="s">
-        <v>476</v>
-      </c>
-      <c r="I13" s="127"/>
+        <v>471</v>
+      </c>
+      <c r="I13" s="123"/>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
       <c r="H14" s="24" t="s">
-        <v>481</v>
-      </c>
-      <c r="I14" s="127"/>
+        <v>476</v>
+      </c>
+      <c r="I14" s="123"/>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E15" s="95" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="F15" s="22">
         <v>1.0</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="24" t="s">
-        <v>487</v>
-      </c>
-      <c r="I15" s="127"/>
+        <v>482</v>
+      </c>
+      <c r="I15" s="123"/>
       <c r="J15" s="24" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>243</v>
       </c>
       <c r="D16" s="94" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="E16" s="95" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="24" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="I16" s="93" t="s">
         <v>241</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="24" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="24" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>262</v>
       </c>
       <c r="D17" s="94" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>257</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
-      <c r="H17" s="129" t="s">
-        <v>497</v>
+      <c r="H17" s="125" t="s">
+        <v>492</v>
       </c>
       <c r="I17" s="93" t="s">
         <v>260</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="24" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>274</v>
       </c>
       <c r="D18" s="94" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E18" s="22" t="s">
         <v>257</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
-      <c r="H18" s="129" t="s">
-        <v>502</v>
+      <c r="H18" s="125" t="s">
+        <v>497</v>
       </c>
       <c r="I18" s="93" t="s">
         <v>272</v>
@@ -22371,22 +22263,22 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D19" s="94" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
-      <c r="H19" s="129" t="s">
-        <v>507</v>
+      <c r="H19" s="125" t="s">
+        <v>502</v>
       </c>
       <c r="I19" s="93" t="s">
         <v>278</v>
@@ -22396,24 +22288,24 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>508</v>
-      </c>
-      <c r="B20" s="130" t="s">
-        <v>509</v>
+        <v>503</v>
+      </c>
+      <c r="B20" s="126" t="s">
+        <v>504</v>
       </c>
       <c r="C20" s="103" t="s">
         <v>291</v>
       </c>
       <c r="D20" s="104" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E20" s="105" t="s">
         <v>293</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
-      <c r="H20" s="129" t="s">
-        <v>511</v>
+      <c r="H20" s="125" t="s">
+        <v>506</v>
       </c>
       <c r="I20" s="93"/>
       <c r="J20" s="22"/>
@@ -22421,24 +22313,24 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>512</v>
-      </c>
-      <c r="B21" s="130" t="s">
-        <v>513</v>
+        <v>507</v>
+      </c>
+      <c r="B21" s="126" t="s">
+        <v>508</v>
       </c>
       <c r="C21" s="103" t="s">
         <v>298</v>
       </c>
       <c r="D21" s="104" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="E21" s="105" t="s">
         <v>293</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
-      <c r="H21" s="129" t="s">
-        <v>515</v>
+      <c r="H21" s="125" t="s">
+        <v>510</v>
       </c>
       <c r="I21" s="93" t="s">
         <v>296</v>
@@ -22448,24 +22340,24 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="24" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="E22" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F22" s="22"/>
       <c r="G22" s="22"/>
-      <c r="H22" s="129" t="s">
-        <v>520</v>
+      <c r="H22" s="125" t="s">
+        <v>515</v>
       </c>
       <c r="I22" s="93"/>
       <c r="J22" s="22"/>
@@ -22473,24 +22365,24 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>310</v>
       </c>
       <c r="D23" s="94" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="E23" s="107" t="s">
         <v>312</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="22"/>
-      <c r="H23" s="129" t="s">
-        <v>524</v>
+      <c r="H23" s="125" t="s">
+        <v>519</v>
       </c>
       <c r="I23" s="93"/>
       <c r="J23" s="22"/>
@@ -22498,24 +22390,24 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>317</v>
       </c>
       <c r="D24" s="94" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="E24" s="107" t="s">
         <v>293</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="22"/>
-      <c r="H24" s="129" t="s">
-        <v>528</v>
+      <c r="H24" s="125" t="s">
+        <v>523</v>
       </c>
       <c r="I24" s="93" t="s">
         <v>315</v>
@@ -22525,116 +22417,116 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
       <c r="G25" s="22"/>
-      <c r="H25" s="129" t="s">
-        <v>532</v>
-      </c>
-      <c r="I25" s="127" t="s">
-        <v>440</v>
+      <c r="H25" s="125" t="s">
+        <v>527</v>
+      </c>
+      <c r="I25" s="123" t="s">
+        <v>435</v>
       </c>
       <c r="J25" s="22"/>
       <c r="K25" s="22"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="22"/>
       <c r="H26" s="24" t="s">
-        <v>537</v>
-      </c>
-      <c r="I26" s="127" t="s">
-        <v>459</v>
+        <v>532</v>
+      </c>
+      <c r="I26" s="123" t="s">
+        <v>454</v>
       </c>
       <c r="J26" s="22"/>
       <c r="K26" s="22"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="D27" s="24" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
       <c r="G27" s="22"/>
-      <c r="H27" s="129" t="s">
-        <v>541</v>
-      </c>
-      <c r="I27" s="127" t="s">
-        <v>471</v>
+      <c r="H27" s="125" t="s">
+        <v>536</v>
+      </c>
+      <c r="I27" s="123" t="s">
+        <v>466</v>
       </c>
       <c r="J27" s="22"/>
       <c r="K27" s="22"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="24" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="24" t="s">
-        <v>546</v>
-      </c>
-      <c r="I28" s="127"/>
+        <v>541</v>
+      </c>
+      <c r="I28" s="123"/>
       <c r="J28" s="22" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="K28" s="22"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22">
@@ -22642,9 +22534,9 @@
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="24" t="s">
-        <v>552</v>
-      </c>
-      <c r="I29" s="127"/>
+        <v>547</v>
+      </c>
+      <c r="I29" s="123"/>
       <c r="J29" s="22"/>
       <c r="K29" s="22"/>
     </row>

</xml_diff>

<commit_message>
NAV-172 New BDG (#93)
* NAV-172 Update BDG

* NAV-172 Add new calibration check to the naomi checklist

* NAV-172 Silently pass validation conditional for non-existant indicators

* NAV-172 Fix unit tests for new validation conditional behaviour

* NAV-172 Fix unit tests for new Naomi validation file

* NAV-172 New casette for end to end test including new BDG steps

* NAV-172 Fix linting
</commit_message>
<xml_diff>
--- a/Estimates 22 BDG [Final].xlsx
+++ b/Estimates 22 BDG [Final].xlsx
@@ -18,7 +18,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mijv/Yi2GmeSQjMjGB0S/7X8CYI/A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId14" roundtripDataSignature="AMtx7mgEJWHwflgbFsau28RIk7+4PPZXOA=="/>
     </ext>
   </extLst>
 </workbook>
@@ -93,7 +93,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgJ0JgbOCBuUu1yDls2+Zyj6eJPHA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjzjTuoRlIIKOQ6XItBD1oh5rK1sw=="/>
     </ext>
   </extLst>
 </comments>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="651">
   <si>
     <t>Milestone Title (Visible to User):</t>
   </si>
@@ -2490,6 +2490,21 @@
     <t>check_spectrum_file(['UAvalid'])</t>
   </si>
   <si>
+    <t>SPF-25-01</t>
+  </si>
+  <si>
+    <t>Upload KP workbook into Spectrum</t>
+  </si>
+  <si>
+    <t>Has the user uploaded their KP workbook into Spectrum</t>
+  </si>
+  <si>
+    <t>A new feature added in 2022 was the review of available key population data. These data will be used in future years to improve the models. In 2022 it will not impact the model. This task requires that you review the prepopulated key population data, update with any missing data, and create national-level estimates of KP size, HIV prevalence, and new HIV infections.  Once you are complete you should upload the file into Spectrum under Program Statistics &gt; Key Populations.  Remember that this step has no impact on your Spectrum estimates.</t>
+  </si>
+  <si>
+    <t>check_manual_confirmation('EST-SPF-25-01-A')</t>
+  </si>
+  <si>
     <t>SPF-26-01</t>
   </si>
   <si>
@@ -2518,8 +2533,9 @@
     <t xml:space="preserve">User is producing district-level HIV estimates? </t>
   </si>
   <si>
-    <t>If you are not producing district-level estimates, congratulations, you have completed the estimates process. You may use results for national reporting or other needs. 
-*If you require estimates to inform your PEPFAR Data Pack or DMPPT, you must product district-level estimates using Naomi.*</t>
+    <t xml:space="preserve">If you are not producing district-level estimates, congratulations, you have completed the estimates process. You may use results for national reporting or other needs. 
+*If you require estimates to inform your PEPFAR Data Pack or DMPPT, you must product district-level estimates using Naomi.*
+If you are planning to produce district-level estimates, mark this task complete and click the "What's Next?" button to proceed to the Naomi milestone. </t>
   </si>
   <si>
     <t>check_manual_confirmation('EST-SPF-27-01-A')</t>
@@ -3028,6 +3044,9 @@
     <t>NAO-17-01</t>
   </si>
   <si>
+    <t>Cal_PLHIV,Cal_ART,Cal_KOS,Cal_new_infections,Cal_method, Cal_Population</t>
+  </si>
+  <si>
     <t>Naomi Validation:  Calibrate the model in Naomi</t>
   </si>
   <si>
@@ -3036,7 +3055,7 @@
 **Please ensure you address this in your Naomi model run and then reupload your Naomi Outputs zip to the ADR in order to complete this task.**</t>
   </si>
   <si>
-    <t>check_naomi_file(['Cal_PLHIV', 'Cal_ART', 'Cal_KOS', 'Cal_new_infections', 'Cal_method'])</t>
+    <t>check_naomi_file(['Cal_PLHIV', 'Cal_ART', 'Cal_KOS', 'Cal_new_infections', 'Cal_method', 'Cal_Population'])</t>
   </si>
 </sst>
 </file>
@@ -3367,7 +3386,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="133">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -3690,6 +3709,9 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10589,21 +10611,21 @@
     </row>
     <row r="2" ht="12.0" customHeight="1">
       <c r="A2" s="47" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="46" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="46">
         <v>0.2</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="H2" s="127"/>
       <c r="I2" s="127"/>
@@ -10614,7 +10636,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="128" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="C4" s="89" t="s">
         <v>10</v>
@@ -10646,17 +10668,17 @@
     </row>
     <row r="5" ht="12.0" customHeight="1">
       <c r="A5" s="22" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="B5" s="123"/>
       <c r="C5" s="24" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="E5" s="24" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="22">
@@ -10664,26 +10686,26 @@
       </c>
       <c r="H5" s="22"/>
       <c r="I5" s="24" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" ht="12.0" customHeight="1">
       <c r="A6" s="22" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="B6" s="123" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="E6" s="24" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="F6" s="22"/>
       <c r="G6" s="24">
@@ -10691,16 +10713,16 @@
       </c>
       <c r="H6" s="22"/>
       <c r="I6" s="24" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="K6" s="22"/>
     </row>
     <row r="7" ht="12.0" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="B7" s="123"/>
       <c r="C7" s="22" t="s">
@@ -10710,7 +10732,7 @@
         <v>184</v>
       </c>
       <c r="E7" s="24" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="F7" s="22" t="s">
         <v>186</v>
@@ -10718,14 +10740,14 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="24" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="J7" s="99"/>
       <c r="K7" s="22"/>
     </row>
     <row r="8" ht="12.0" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="B8" s="123"/>
       <c r="C8" s="22" t="s">
@@ -10735,25 +10757,25 @@
         <v>190</v>
       </c>
       <c r="E8" s="129" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
       <c r="I8" s="24" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="J8" s="22"/>
       <c r="K8" s="22"/>
     </row>
     <row r="9" ht="12.0" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="B9" s="123" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>195</v>
@@ -10762,117 +10784,117 @@
         <v>196</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
       <c r="I9" s="24" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
     </row>
     <row r="10" ht="12.0" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="B10" s="123" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="E10" s="24" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="F10" s="130" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="G10" s="22">
         <v>1.0</v>
       </c>
       <c r="H10" s="22"/>
       <c r="I10" s="24" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22"/>
     </row>
     <row r="11" ht="12.0" customHeight="1">
       <c r="A11" s="22" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="B11" s="123"/>
       <c r="C11" s="22" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="F11" s="107" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="24" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
     </row>
     <row r="12" ht="49.5" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="B12" s="123" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="E12" s="131" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="G12" s="22">
         <v>1.0</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="24" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="K12" s="22"/>
     </row>
     <row r="13" ht="12.0" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="B13" s="123" t="s">
-        <v>598</v>
+        <v>603</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>599</v>
+        <v>604</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>601</v>
+        <v>606</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22">
@@ -10880,53 +10902,53 @@
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="24" t="s">
-        <v>602</v>
+        <v>607</v>
       </c>
       <c r="J13" s="22"/>
       <c r="K13" s="22"/>
     </row>
     <row r="14" ht="12.0" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>603</v>
+        <v>608</v>
       </c>
       <c r="B14" s="123" t="s">
-        <v>604</v>
+        <v>609</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>605</v>
+        <v>610</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="G14" s="24">
         <v>0.0</v>
       </c>
       <c r="H14" s="22"/>
       <c r="I14" s="24" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="J14" s="22"/>
       <c r="K14" s="22"/>
     </row>
     <row r="15" ht="12.0" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="B15" s="123"/>
       <c r="C15" s="24" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>613</v>
+        <v>618</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22">
@@ -10934,47 +10956,47 @@
       </c>
       <c r="H15" s="22"/>
       <c r="I15" s="24" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="J15" s="99"/>
       <c r="K15" s="22"/>
     </row>
     <row r="16" ht="12.0" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="B16" s="123"/>
       <c r="C16" s="22" t="s">
-        <v>616</v>
+        <v>621</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>617</v>
+        <v>622</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="24" t="s">
-        <v>619</v>
+        <v>624</v>
       </c>
       <c r="J16" s="22"/>
       <c r="K16" s="22"/>
     </row>
     <row r="17" ht="12.0" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>620</v>
+        <v>625</v>
       </c>
       <c r="B17" s="123"/>
       <c r="C17" s="22" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22">
@@ -10982,53 +11004,53 @@
       </c>
       <c r="H17" s="22"/>
       <c r="I17" s="24" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="J17" s="22"/>
       <c r="K17" s="22"/>
     </row>
     <row r="18" ht="12.0" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>625</v>
+        <v>630</v>
       </c>
       <c r="B18" s="123"/>
       <c r="C18" s="22" t="s">
-        <v>626</v>
+        <v>631</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="E18" s="22" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
       <c r="G18" s="22">
         <v>1.0</v>
       </c>
       <c r="H18" s="22"/>
       <c r="I18" s="24" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="J18" s="22"/>
       <c r="K18" s="22"/>
     </row>
     <row r="19" ht="12.0" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>631</v>
+        <v>636</v>
       </c>
       <c r="B19" s="123" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>632</v>
+        <v>637</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="E19" s="24" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="F19" s="24" t="s">
         <v>257</v>
@@ -11036,65 +11058,65 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="I19" s="24" t="s">
-        <v>634</v>
+        <v>639</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>635</v>
+        <v>640</v>
       </c>
       <c r="K19" s="22"/>
     </row>
     <row r="20" ht="49.5" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>636</v>
+        <v>641</v>
       </c>
       <c r="B20" s="123" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>637</v>
+        <v>642</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="E20" s="131" t="s">
-        <v>638</v>
+        <v>643</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="G20" s="22"/>
       <c r="H20" s="22"/>
       <c r="I20" s="24" t="s">
-        <v>639</v>
+        <v>644</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>640</v>
+        <v>645</v>
       </c>
       <c r="K20" s="22"/>
     </row>
     <row r="21" ht="12.0" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>641</v>
-      </c>
-      <c r="B21" s="123" t="s">
-        <v>604</v>
+        <v>646</v>
+      </c>
+      <c r="B21" s="132" t="s">
+        <v>647</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>642</v>
+        <v>648</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>606</v>
+        <v>611</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>643</v>
+        <v>649</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="24" t="s">
-        <v>644</v>
+        <v>650</v>
       </c>
       <c r="J21" s="22"/>
       <c r="K21" s="22"/>
@@ -22494,54 +22516,76 @@
       <c r="A28" s="24" t="s">
         <v>537</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="24" t="s">
         <v>538</v>
       </c>
-      <c r="C28" s="22" t="s">
+      <c r="C28" s="24" t="s">
         <v>539</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="24" t="s">
         <v>540</v>
       </c>
-      <c r="E28" s="22"/>
+      <c r="E28" s="107" t="s">
+        <v>293</v>
+      </c>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
       <c r="H28" s="24" t="s">
         <v>541</v>
       </c>
       <c r="I28" s="123"/>
-      <c r="J28" s="22" t="s">
-        <v>542</v>
-      </c>
+      <c r="J28" s="22"/>
       <c r="K28" s="22"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="24" t="s">
+        <v>542</v>
+      </c>
+      <c r="B29" s="22" t="s">
         <v>543</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="C29" s="22" t="s">
         <v>544</v>
       </c>
-      <c r="C29" s="22" t="s">
+      <c r="D29" s="22" t="s">
         <v>545</v>
       </c>
-      <c r="D29" s="24" t="s">
-        <v>546</v>
-      </c>
       <c r="E29" s="22"/>
-      <c r="F29" s="22">
-        <v>1.0</v>
-      </c>
+      <c r="F29" s="22"/>
       <c r="G29" s="22"/>
       <c r="H29" s="24" t="s">
+        <v>546</v>
+      </c>
+      <c r="I29" s="123"/>
+      <c r="J29" s="22" t="s">
         <v>547</v>
       </c>
-      <c r="I29" s="123"/>
-      <c r="J29" s="22"/>
       <c r="K29" s="22"/>
     </row>
-    <row r="30" ht="13.5" customHeight="1">
-      <c r="I30" s="44"/>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="24" t="s">
+        <v>548</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="C30" s="22" t="s">
+        <v>550</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>551</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="G30" s="22"/>
+      <c r="H30" s="24" t="s">
+        <v>552</v>
+      </c>
+      <c r="I30" s="123"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="I31" s="44"/>
@@ -23143,7 +23187,7 @@
     <row r="230" ht="13.5" customHeight="1">
       <c r="I230" s="44"/>
     </row>
-    <row r="231" ht="15.75" customHeight="1">
+    <row r="231" ht="13.5" customHeight="1">
       <c r="I231" s="44"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
@@ -25482,6 +25526,9 @@
     </row>
     <row r="1010" ht="15.75" customHeight="1">
       <c r="I1010" s="44"/>
+    </row>
+    <row r="1011" ht="15.75" customHeight="1">
+      <c r="I1011" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>